<commit_message>
TM-4802 formatting Created/Modified Fields to DateTime with TZ, fixing bad rendering of Data in *Room* and *Comments* (overwriting headers) refactoring code
git-svn-id: https://opsvcs.tdsops.com/repos/tdstm/trunk@7387 fecba46a-3362-0410-80e5-8c76cdb905a0
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="15360" tabRatio="782"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -6205,14 +6205,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -6256,6 +6253,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1540">
     <cellStyle name="_JDI DCM Runbook Hour by Hour EMA Comm Systems (Bundle 2) 11-JUL-07" xfId="1"/>
@@ -8228,7 +8228,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8272,7 +8272,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8316,7 +8316,7 @@
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="68" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
@@ -8324,7 +8324,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="68" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -8332,7 +8332,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="68" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -8340,7 +8340,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="68" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -8348,7 +8348,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="68" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -8356,7 +8356,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="68" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="33">
@@ -8364,7 +8364,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="68" t="s">
         <v>271</v>
       </c>
       <c r="B9" t="s">
@@ -8372,7 +8372,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="71" t="s">
+      <c r="A10" s="68" t="s">
         <v>272</v>
       </c>
       <c r="B10" t="s">
@@ -8412,24 +8412,24 @@
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
       <c r="E15" s="35"/>
-      <c r="F15" s="75" t="s">
+      <c r="F15" s="72" t="s">
         <v>233</v>
       </c>
-      <c r="G15" s="75"/>
+      <c r="G15" s="72"/>
     </row>
     <row r="16" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36"/>
-      <c r="B16" s="74" t="s">
+      <c r="B16" s="71" t="s">
         <v>234</v>
       </c>
-      <c r="C16" s="74"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="37" t="s">
         <v>262</v>
       </c>
       <c r="E16" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="61" t="s">
         <v>264</v>
       </c>
       <c r="G16" s="37" t="s">
@@ -8504,7 +8504,7 @@
       </c>
       <c r="F19" s="44"/>
       <c r="G19" s="44"/>
-      <c r="I19" s="61" t="s">
+      <c r="I19" s="58" t="s">
         <v>257</v>
       </c>
       <c r="J19" t="s">
@@ -8538,7 +8538,7 @@
         <f>COUNTIF(Devices!B:EL,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Devices!B:EL,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Devices!B:EL,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Devices!B:EL,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="I20" s="62" t="s">
+      <c r="I20" s="59" t="s">
         <v>258</v>
       </c>
       <c r="J20" t="s">
@@ -8884,24 +8884,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="19.5" style="73" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="73"/>
+    <col min="1" max="5" width="19.5" style="70" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="70"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="69" t="s">
         <v>273</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="69" t="s">
         <v>274</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="69" t="s">
         <v>275</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="69" t="s">
         <v>276</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="69" t="s">
         <v>277</v>
       </c>
     </row>
@@ -8920,9 +8920,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EK1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="AE1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8943,9 +8943,9 @@
     <col min="39" max="39" width="13.5" style="11" customWidth="1"/>
     <col min="40" max="40" width="8.6640625" customWidth="1"/>
     <col min="41" max="41" width="10.5" customWidth="1"/>
-    <col min="42" max="42" width="13.5" style="58" customWidth="1"/>
+    <col min="42" max="42" width="13.5" style="56" customWidth="1"/>
     <col min="43" max="43" width="11.83203125" style="11" customWidth="1"/>
-    <col min="44" max="44" width="12.1640625" style="53" customWidth="1"/>
+    <col min="44" max="44" width="12.1640625" style="77" customWidth="1"/>
     <col min="45" max="45" width="11.1640625" customWidth="1"/>
     <col min="46" max="73" width="9.6640625" customWidth="1"/>
     <col min="74" max="74" width="9.6640625" style="13" customWidth="1"/>
@@ -8958,7 +8958,7 @@
       <c r="A1" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="57" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="15" t="s">
@@ -9021,7 +9021,7 @@
       <c r="V1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="56" t="s">
+      <c r="W1" s="54" t="s">
         <v>160</v>
       </c>
       <c r="X1" s="15" t="s">
@@ -9060,7 +9060,7 @@
       <c r="AI1" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="AJ1" s="57" t="s">
+      <c r="AJ1" s="55" t="s">
         <v>172</v>
       </c>
       <c r="AK1" s="18" t="s">
@@ -9069,7 +9069,7 @@
       <c r="AL1" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="AM1" s="57" t="s">
+      <c r="AM1" s="55" t="s">
         <v>175</v>
       </c>
       <c r="AN1" s="18" t="s">
@@ -9078,13 +9078,13 @@
       <c r="AO1" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="AP1" s="57" t="s">
+      <c r="AP1" s="55" t="s">
         <v>178</v>
       </c>
       <c r="AQ1" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="AR1" s="52" t="s">
+      <c r="AR1" s="76" t="s">
         <v>49</v>
       </c>
       <c r="AS1" s="8" t="s">
@@ -9398,9 +9398,9 @@
   </sheetPr>
   <dimension ref="A1:EK1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="AD1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9441,7 +9441,7 @@
     <col min="40" max="41" width="8.6640625" style="4" customWidth="1"/>
     <col min="42" max="42" width="14" style="4" customWidth="1"/>
     <col min="43" max="43" width="11.1640625" style="4" customWidth="1"/>
-    <col min="44" max="44" width="12.1640625" style="59" customWidth="1"/>
+    <col min="44" max="44" width="12.1640625" style="78" customWidth="1"/>
     <col min="45" max="45" width="10.5" style="4" customWidth="1"/>
     <col min="46" max="110" width="9.6640625" style="5" customWidth="1"/>
     <col min="111" max="111" width="9.6640625" style="4" customWidth="1"/>
@@ -9452,10 +9452,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:141" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="53" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
@@ -9581,7 +9581,7 @@
       <c r="AQ1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AR1" s="52" t="s">
+      <c r="AR1" s="76" t="s">
         <v>49</v>
       </c>
       <c r="AS1" s="8" t="s">
@@ -9906,7 +9906,7 @@
     <col min="13" max="13" width="12.1640625" customWidth="1"/>
     <col min="15" max="15" width="8.6640625" style="11" customWidth="1"/>
     <col min="16" max="16" width="12.1640625" style="11" customWidth="1"/>
-    <col min="17" max="17" width="12.83203125" style="50" customWidth="1"/>
+    <col min="17" max="17" width="12.83203125" style="33" customWidth="1"/>
     <col min="18" max="18" width="11.33203125" customWidth="1"/>
     <col min="19" max="42" width="9.6640625" customWidth="1"/>
     <col min="43" max="43" width="9.6640625" style="13" customWidth="1"/>
@@ -9964,7 +9964,7 @@
       <c r="P1" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="76" t="s">
         <v>49</v>
       </c>
       <c r="R1" s="8" t="s">
@@ -10291,7 +10291,7 @@
     <col min="15" max="15" width="10.33203125" customWidth="1"/>
     <col min="16" max="16" width="10.5" style="11" customWidth="1"/>
     <col min="17" max="17" width="12" style="11" customWidth="1"/>
-    <col min="18" max="18" width="12" style="50" customWidth="1"/>
+    <col min="18" max="18" width="12" style="33" customWidth="1"/>
     <col min="19" max="19" width="11.1640625" customWidth="1"/>
     <col min="20" max="43" width="9.6640625" customWidth="1"/>
     <col min="44" max="44" width="9.6640625" style="13" customWidth="1"/>
@@ -10322,7 +10322,7 @@
       <c r="G1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="63" t="s">
+      <c r="H1" s="60" t="s">
         <v>261</v>
       </c>
       <c r="I1" s="19" t="s">
@@ -10352,7 +10352,7 @@
       <c r="Q1" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="52" t="s">
+      <c r="R1" s="76" t="s">
         <v>49</v>
       </c>
       <c r="S1" s="8" t="s">
@@ -10903,13 +10903,13 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.6640625" style="5"/>
-    <col min="2" max="2" width="7.83203125" style="68" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" style="65" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" style="5"/>
-    <col min="5" max="5" width="8.33203125" style="68" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="65" customWidth="1"/>
     <col min="6" max="6" width="24.5" style="5" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="5"/>
-    <col min="8" max="8" width="24.1640625" style="70" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" style="67" customWidth="1"/>
     <col min="9" max="9" width="9.6640625" style="5"/>
     <col min="10" max="10" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.83203125" style="5" customWidth="1"/>
@@ -10918,56 +10918,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="73" t="s">
         <v>217</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="77" t="s">
+      <c r="C1" s="74"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="74" t="s">
         <v>218</v>
       </c>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="69"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="66"/>
       <c r="J1" s="5" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="65" t="s">
+    <row r="2" spans="1:12" s="63" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="62" t="s">
         <v>219</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="64" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="62" t="s">
         <v>221</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="62" t="s">
         <v>222</v>
       </c>
-      <c r="E2" s="67" t="s">
+      <c r="E2" s="64" t="s">
         <v>220</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="F2" s="62" t="s">
         <v>221</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="G2" s="62" t="s">
         <v>222</v>
       </c>
-      <c r="H2" s="67" t="s">
+      <c r="H2" s="64" t="s">
         <v>223</v>
       </c>
-      <c r="I2" s="65" t="s">
+      <c r="I2" s="62" t="s">
         <v>224</v>
       </c>
-      <c r="J2" s="65" t="s">
+      <c r="J2" s="62" t="s">
         <v>225</v>
       </c>
-      <c r="K2" s="65" t="s">
+      <c r="K2" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="L2" s="65" t="s">
+      <c r="L2" s="62" t="s">
         <v>227</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TM-5265 Changed spreadsheet templates for Asset Export and Runbook to disable the 1904 dates
git-svn-id: https://opsvcs.tdsops.com/repos/tdstm/trunk@7453 fecba46a-3362-0410-80e5-8c76cdb905a0
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
-  <workbookPr date1904="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/octavio/Documents/TDS/tranman/src/web-app/templates/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="782"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -43,13 +38,13 @@
     <definedName name="ProjectManager">Title!$B$5</definedName>
     <definedName name="ProjectName">Title!$C$4</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -6238,24 +6233,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1049"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1540">
     <cellStyle name="_JDI DCM Runbook Hour by Hour EMA Comm Systems (Bundle 2) 11-JUL-07" xfId="1"/>
@@ -8228,7 +8223,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8272,7 +8267,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8296,26 +8291,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="38.33203125" customWidth="1"/>
-    <col min="10" max="10" width="2.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="38.28515625" customWidth="1"/>
+    <col min="10" max="10" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="18">
       <c r="A1" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" s="68" t="s">
         <v>0</v>
       </c>
@@ -8323,7 +8320,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="A4" s="68" t="s">
         <v>1</v>
       </c>
@@ -8331,7 +8328,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="68" t="s">
         <v>2</v>
       </c>
@@ -8339,7 +8336,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="A6" s="68" t="s">
         <v>5</v>
       </c>
@@ -8347,7 +8344,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="A7" s="68" t="s">
         <v>4</v>
       </c>
@@ -8355,7 +8352,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7">
       <c r="A8" s="68" t="s">
         <v>3</v>
       </c>
@@ -8363,7 +8360,7 @@
         <v>38295</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7">
       <c r="A9" s="68" t="s">
         <v>271</v>
       </c>
@@ -8371,7 +8368,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7">
       <c r="A10" s="68" t="s">
         <v>272</v>
       </c>
@@ -8379,10 +8376,10 @@
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7">
       <c r="B12" t="s">
         <v>236</v>
       </c>
@@ -8391,7 +8388,7 @@
       <c r="F12" s="38"/>
       <c r="G12" s="38"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7">
       <c r="B13" t="s">
         <v>269</v>
       </c>
@@ -8400,29 +8397,29 @@
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7">
       <c r="D14" s="38"/>
       <c r="E14" s="38"/>
       <c r="F14" s="38"/>
       <c r="G14" s="38"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15" customHeight="1">
       <c r="A15" s="34"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
       <c r="E15" s="35"/>
-      <c r="F15" s="72" t="s">
+      <c r="F15" s="75" t="s">
         <v>233</v>
       </c>
-      <c r="G15" s="72"/>
+      <c r="G15" s="75"/>
     </row>
-    <row r="16" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="28" customHeight="1">
       <c r="A16" s="36"/>
-      <c r="B16" s="71" t="s">
+      <c r="B16" s="74" t="s">
         <v>234</v>
       </c>
-      <c r="C16" s="71"/>
+      <c r="C16" s="74"/>
       <c r="D16" s="37" t="s">
         <v>262</v>
       </c>
@@ -8436,7 +8433,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="20" customHeight="1">
       <c r="A17" s="39">
         <f>COUNTA(Applications!B:B)-1</f>
         <v>0</v>
@@ -8464,7 +8461,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" ht="20" customHeight="1">
       <c r="A18">
         <f>COUNTIF(Applications!R:R,"Master")</f>
         <v>0</v>
@@ -8486,7 +8483,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" ht="20" customHeight="1">
       <c r="A19">
         <f>A17-A18</f>
         <v>0</v>
@@ -8514,7 +8511,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="20" customHeight="1">
       <c r="A20" s="39">
         <f>COUNTA(Devices!B:B)-1</f>
         <v>0</v>
@@ -8548,7 +8545,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" ht="20" customHeight="1">
       <c r="A21">
         <f>COUNTIF(Devices!H:H,"Server")+COUNTIF(Devices!H:H,"VM")+COUNTIF(Devices!H:H,"Blade")+COUNTIF(Devices!H:H,"Appliance")</f>
         <v>0</v>
@@ -8567,7 +8564,7 @@
       <c r="F21" s="44"/>
       <c r="G21" s="44"/>
     </row>
-    <row r="22" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="20" customHeight="1">
       <c r="A22" s="39">
         <f>COUNTA(Databases!B:B)-1</f>
         <v>0</v>
@@ -8592,7 +8589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="20" customHeight="1">
       <c r="A23" s="39">
         <f>COUNTA(Storage!B:B)-1</f>
         <v>0</v>
@@ -8617,7 +8614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="20" customHeight="1">
       <c r="A24" s="39">
         <f>COUNTA(Dependencies!D:D)-1</f>
         <v>0</v>
@@ -8642,7 +8639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" ht="20" customHeight="1">
       <c r="A25">
         <f>COUNTIF(Dependencies!H:H,"Master")</f>
         <v>0</v>
@@ -8655,7 +8652,7 @@
       <c r="F25" s="38"/>
       <c r="G25" s="38"/>
     </row>
-    <row r="26" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" ht="20" customHeight="1">
       <c r="A26">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Application")-A25</f>
         <v>0</v>
@@ -8668,7 +8665,7 @@
       <c r="F26" s="38"/>
       <c r="G26" s="38"/>
     </row>
-    <row r="27" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" ht="20" customHeight="1">
       <c r="A27">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!H:H,"Runs On")</f>
         <v>0</v>
@@ -8681,7 +8678,7 @@
       <c r="F27" s="38"/>
       <c r="G27" s="38"/>
     </row>
-    <row r="28" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" ht="20" customHeight="1">
       <c r="A28">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Database")</f>
         <v>0</v>
@@ -8694,7 +8691,7 @@
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
     </row>
-    <row r="29" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" ht="20" customHeight="1">
       <c r="A29">
         <f>COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Server")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Blade")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"VM")</f>
         <v>0</v>
@@ -8707,7 +8704,7 @@
       <c r="F29" s="38"/>
       <c r="G29" s="38"/>
     </row>
-    <row r="30" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11" ht="20" customHeight="1">
       <c r="A30">
         <f>COUNTIF(Dependencies!H:H,"Storage")</f>
         <v>0</v>
@@ -8720,7 +8717,7 @@
       <c r="F30" s="38"/>
       <c r="G30" s="38"/>
     </row>
-    <row r="31" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="20" customHeight="1">
       <c r="A31" s="39">
         <f>COUNTA(Room!B:B)-1</f>
         <v>0</v>
@@ -8733,7 +8730,7 @@
       <c r="F31" s="46"/>
       <c r="G31" s="46"/>
     </row>
-    <row r="32" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="20" customHeight="1">
       <c r="A32" s="39">
         <f>COUNTA(Rack!B:B)-1</f>
         <v>0</v>
@@ -8746,7 +8743,7 @@
       <c r="F32" s="46"/>
       <c r="G32" s="46"/>
     </row>
-    <row r="33" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="20" customHeight="1">
       <c r="A33" s="39">
         <f>COUNTA(Cabling!B:B)-2</f>
         <v>0</v>
@@ -8759,7 +8756,7 @@
       <c r="F33" s="46"/>
       <c r="G33" s="46"/>
     </row>
-    <row r="34" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="20" customHeight="1">
       <c r="A34" s="40">
         <f>COUNTA(Comments!B:B)-1</f>
         <v>0</v>
@@ -8772,21 +8769,21 @@
       <c r="F34" s="46"/>
       <c r="G34" s="46"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="46" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="47" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="48" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="45" spans="1:7" ht="21" customHeight="1"/>
+    <row r="46" spans="1:7" ht="21" customHeight="1"/>
+    <row r="47" spans="1:7" ht="21" customHeight="1"/>
+    <row r="48" spans="1:7" ht="21" customHeight="1"/>
+    <row r="49" ht="21" customHeight="1"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataConsolidate/>
@@ -8820,6 +8817,11 @@
     <ignoredError sqref="D17:D24 E18 F17:F24 G17:G24 A17:A34" emptyCellReference="1"/>
     <ignoredError sqref="E21" formula="1" emptyCellReference="1"/>
   </ignoredErrors>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8831,18 +8833,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="16" style="11" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="12" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="22" customWidth="1"/>
-    <col min="6" max="6" width="51.83203125" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="9.6640625" style="22"/>
+    <col min="3" max="3" width="20.140625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" style="22" customWidth="1"/>
+    <col min="7" max="16384" width="9.7109375" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6">
       <c r="A1" s="31" t="s">
         <v>228</v>
       </c>
@@ -8871,6 +8873,11 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8882,13 +8889,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="5" width="19.5" style="70" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="70"/>
+    <col min="1" max="5" width="19.42578125" style="70" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="70"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5">
       <c r="A1" s="69" t="s">
         <v>273</v>
       </c>
@@ -8913,6 +8920,11 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8925,36 +8937,36 @@
       <selection pane="bottomLeft" activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="11"/>
+    <col min="1" max="1" width="9.7109375" style="11"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" style="12"/>
-    <col min="16" max="16" width="11.83203125" style="12" customWidth="1"/>
-    <col min="20" max="20" width="11.1640625" customWidth="1"/>
-    <col min="23" max="23" width="9.6640625" style="11"/>
-    <col min="28" max="28" width="17.33203125" customWidth="1"/>
-    <col min="33" max="33" width="9.83203125" style="11" customWidth="1"/>
-    <col min="34" max="34" width="11.5" customWidth="1"/>
-    <col min="35" max="35" width="13.5" customWidth="1"/>
-    <col min="36" max="36" width="16.1640625" style="11" customWidth="1"/>
-    <col min="37" max="37" width="9.5" customWidth="1"/>
-    <col min="38" max="38" width="11.5" customWidth="1"/>
-    <col min="39" max="39" width="13.5" style="11" customWidth="1"/>
-    <col min="40" max="40" width="8.6640625" customWidth="1"/>
-    <col min="41" max="41" width="10.5" customWidth="1"/>
-    <col min="42" max="42" width="13.5" style="56" customWidth="1"/>
-    <col min="43" max="43" width="11.83203125" style="11" customWidth="1"/>
-    <col min="44" max="44" width="12.1640625" style="77" customWidth="1"/>
-    <col min="45" max="45" width="11.1640625" customWidth="1"/>
-    <col min="46" max="73" width="9.6640625" customWidth="1"/>
-    <col min="74" max="74" width="9.6640625" style="13" customWidth="1"/>
-    <col min="75" max="109" width="9.6640625" customWidth="1"/>
-    <col min="110" max="110" width="9.6640625" style="13" customWidth="1"/>
-    <col min="111" max="141" width="9.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" style="12"/>
+    <col min="16" max="16" width="11.85546875" style="12" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" style="11"/>
+    <col min="28" max="28" width="17.28515625" customWidth="1"/>
+    <col min="33" max="33" width="9.85546875" style="11" customWidth="1"/>
+    <col min="34" max="34" width="11.42578125" customWidth="1"/>
+    <col min="35" max="35" width="13.42578125" customWidth="1"/>
+    <col min="36" max="36" width="16.140625" style="11" customWidth="1"/>
+    <col min="37" max="37" width="9.42578125" customWidth="1"/>
+    <col min="38" max="38" width="11.42578125" customWidth="1"/>
+    <col min="39" max="39" width="13.42578125" style="11" customWidth="1"/>
+    <col min="40" max="40" width="8.7109375" customWidth="1"/>
+    <col min="41" max="41" width="10.42578125" customWidth="1"/>
+    <col min="42" max="42" width="13.42578125" style="56" customWidth="1"/>
+    <col min="43" max="43" width="11.85546875" style="11" customWidth="1"/>
+    <col min="44" max="44" width="12.140625" style="72" customWidth="1"/>
+    <col min="45" max="45" width="11.140625" customWidth="1"/>
+    <col min="46" max="73" width="9.7109375" customWidth="1"/>
+    <col min="74" max="74" width="9.7109375" style="13" customWidth="1"/>
+    <col min="75" max="109" width="9.7109375" customWidth="1"/>
+    <col min="110" max="110" width="9.7109375" style="13" customWidth="1"/>
+    <col min="111" max="141" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:141" s="17" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:141" s="17" customFormat="1">
       <c r="A1" s="47" t="s">
         <v>147</v>
       </c>
@@ -9084,7 +9096,7 @@
       <c r="AQ1" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="AR1" s="76" t="s">
+      <c r="AR1" s="71" t="s">
         <v>49</v>
       </c>
       <c r="AS1" s="8" t="s">
@@ -9388,6 +9400,11 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9403,55 +9420,55 @@
       <selection pane="bottomLeft" activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="5" customWidth="1"/>
     <col min="4" max="4" width="13" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" style="5" customWidth="1"/>
-    <col min="8" max="9" width="12.1640625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="9.5" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="5" customWidth="1"/>
-    <col min="12" max="13" width="10.33203125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="9.83203125" style="5" customWidth="1"/>
-    <col min="15" max="15" width="10.5" style="4" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" style="5" customWidth="1"/>
-    <col min="17" max="17" width="18.83203125" style="4" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" style="5" customWidth="1"/>
-    <col min="19" max="19" width="8.5" style="5" customWidth="1"/>
-    <col min="20" max="20" width="11.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="5" customWidth="1"/>
+    <col min="8" max="9" width="12.140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="5" customWidth="1"/>
+    <col min="12" max="13" width="10.28515625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" style="5" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" style="5" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" style="5" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="5" customWidth="1"/>
     <col min="21" max="21" width="11" style="5"/>
     <col min="22" max="22" width="10" style="4" customWidth="1"/>
     <col min="23" max="23" width="11" style="5"/>
-    <col min="24" max="24" width="15.6640625" style="4" customWidth="1"/>
-    <col min="25" max="25" width="12.1640625" style="5" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" style="4" customWidth="1"/>
+    <col min="25" max="25" width="12.140625" style="5" customWidth="1"/>
     <col min="26" max="26" width="12" style="6" customWidth="1"/>
     <col min="27" max="27" width="11" style="6"/>
-    <col min="28" max="28" width="12.83203125" style="5" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" style="5" customWidth="1"/>
     <col min="29" max="30" width="11" style="5"/>
-    <col min="31" max="31" width="11.5" style="5" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="5" customWidth="1"/>
     <col min="32" max="32" width="11" style="5"/>
-    <col min="33" max="33" width="8.83203125" style="5" customWidth="1"/>
+    <col min="33" max="33" width="8.85546875" style="5" customWidth="1"/>
     <col min="34" max="36" width="11" style="5"/>
     <col min="37" max="38" width="11" style="4"/>
-    <col min="39" max="39" width="12.83203125" style="4" customWidth="1"/>
-    <col min="40" max="41" width="8.6640625" style="4" customWidth="1"/>
+    <col min="39" max="39" width="12.85546875" style="4" customWidth="1"/>
+    <col min="40" max="41" width="8.7109375" style="4" customWidth="1"/>
     <col min="42" max="42" width="14" style="4" customWidth="1"/>
-    <col min="43" max="43" width="11.1640625" style="4" customWidth="1"/>
-    <col min="44" max="44" width="12.1640625" style="78" customWidth="1"/>
-    <col min="45" max="45" width="10.5" style="4" customWidth="1"/>
-    <col min="46" max="110" width="9.6640625" style="5" customWidth="1"/>
-    <col min="111" max="111" width="9.6640625" style="4" customWidth="1"/>
-    <col min="112" max="112" width="9.6640625" style="5" customWidth="1"/>
-    <col min="113" max="113" width="9.6640625" style="4" customWidth="1"/>
-    <col min="114" max="141" width="9.6640625" style="5" customWidth="1"/>
+    <col min="43" max="43" width="11.140625" style="4" customWidth="1"/>
+    <col min="44" max="44" width="12.140625" style="73" customWidth="1"/>
+    <col min="45" max="45" width="10.42578125" style="4" customWidth="1"/>
+    <col min="46" max="110" width="9.7109375" style="5" customWidth="1"/>
+    <col min="111" max="111" width="9.7109375" style="4" customWidth="1"/>
+    <col min="112" max="112" width="9.7109375" style="5" customWidth="1"/>
+    <col min="113" max="113" width="9.7109375" style="4" customWidth="1"/>
+    <col min="114" max="141" width="9.7109375" style="5" customWidth="1"/>
     <col min="142" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:141" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:141" s="8" customFormat="1">
       <c r="A1" s="52" t="s">
         <v>6</v>
       </c>
@@ -9581,7 +9598,7 @@
       <c r="AQ1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AR1" s="76" t="s">
+      <c r="AR1" s="71" t="s">
         <v>49</v>
       </c>
       <c r="AS1" s="8" t="s">
@@ -9882,6 +9899,11 @@
   <pageMargins left="0.25" right="0.25" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9894,28 +9916,28 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="11"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="11"/>
-    <col min="6" max="6" width="16.5" style="11" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="12"/>
-    <col min="10" max="10" width="16.1640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="11"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="11"/>
+    <col min="6" max="6" width="16.42578125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="12"/>
+    <col min="10" max="10" width="16.140625" style="12" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="13" max="13" width="12.1640625" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="11" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="11" customWidth="1"/>
-    <col min="17" max="17" width="12.83203125" style="33" customWidth="1"/>
-    <col min="18" max="18" width="11.33203125" customWidth="1"/>
-    <col min="19" max="42" width="9.6640625" customWidth="1"/>
-    <col min="43" max="43" width="9.6640625" style="13" customWidth="1"/>
-    <col min="44" max="82" width="9.6640625" customWidth="1"/>
-    <col min="83" max="83" width="9.6640625" style="13"/>
-    <col min="85" max="86" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" style="11" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" style="11" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="33" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" customWidth="1"/>
+    <col min="19" max="42" width="9.7109375" customWidth="1"/>
+    <col min="43" max="43" width="9.7109375" style="13" customWidth="1"/>
+    <col min="44" max="82" width="9.7109375" customWidth="1"/>
+    <col min="83" max="83" width="9.7109375" style="13"/>
+    <col min="85" max="86" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:114" s="17" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:114" s="17" customFormat="1">
       <c r="A1" s="47" t="s">
         <v>179</v>
       </c>
@@ -9964,7 +9986,7 @@
       <c r="P1" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="76" t="s">
+      <c r="Q1" s="71" t="s">
         <v>49</v>
       </c>
       <c r="R1" s="8" t="s">
@@ -10268,6 +10290,11 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10280,27 +10307,27 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="11"/>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="11"/>
-    <col min="6" max="6" width="14.6640625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="22"/>
+    <col min="1" max="1" width="8.7109375" style="11"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="11"/>
+    <col min="6" max="6" width="14.7109375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="22"/>
     <col min="10" max="11" width="10" style="12" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" customWidth="1"/>
-    <col min="16" max="16" width="10.5" style="11" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="11" customWidth="1"/>
     <col min="17" max="17" width="12" style="11" customWidth="1"/>
     <col min="18" max="18" width="12" style="33" customWidth="1"/>
-    <col min="19" max="19" width="11.1640625" customWidth="1"/>
-    <col min="20" max="43" width="9.6640625" customWidth="1"/>
-    <col min="44" max="44" width="9.6640625" style="13" customWidth="1"/>
-    <col min="45" max="83" width="9.6640625" customWidth="1"/>
-    <col min="84" max="84" width="9.6640625" style="13" customWidth="1"/>
-    <col min="85" max="115" width="9.6640625" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" customWidth="1"/>
+    <col min="20" max="43" width="9.7109375" customWidth="1"/>
+    <col min="44" max="44" width="9.7109375" style="13" customWidth="1"/>
+    <col min="45" max="83" width="9.7109375" customWidth="1"/>
+    <col min="84" max="84" width="9.7109375" style="13" customWidth="1"/>
+    <col min="85" max="115" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:115" s="17" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:115" s="17" customFormat="1">
       <c r="A1" s="47" t="s">
         <v>181</v>
       </c>
@@ -10352,7 +10379,7 @@
       <c r="Q1" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="76" t="s">
+      <c r="R1" s="71" t="s">
         <v>49</v>
       </c>
       <c r="S1" s="8" t="s">
@@ -10652,6 +10679,11 @@
   <autoFilter ref="A1:DK1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10664,22 +10696,22 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="8.6640625" style="11"/>
-    <col min="3" max="3" width="13.5" style="11" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="22" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="11" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="22" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" customWidth="1"/>
-    <col min="11" max="11" width="8.1640625" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" customWidth="1"/>
+    <col min="1" max="2" width="8.7109375" style="11"/>
+    <col min="3" max="3" width="13.42578125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="22" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" s="26" customFormat="1">
       <c r="A1" s="23" t="s">
         <v>182</v>
       </c>
@@ -10734,6 +10766,11 @@
   <autoFilter ref="A1:P1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10746,23 +10783,23 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="11"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
-    <col min="4" max="5" width="14.5" style="13" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.5" customWidth="1"/>
-    <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="11"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="5" width="14.42578125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="19.5" style="2" customWidth="1"/>
-    <col min="12" max="12" width="25.33203125" style="50" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" style="50" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" style="50" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" s="29" customFormat="1">
       <c r="A1" s="23" t="s">
         <v>197</v>
       </c>
@@ -10812,6 +10849,11 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10824,22 +10866,22 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.5" style="11" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="13" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="13" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="13" customWidth="1"/>
     <col min="11" max="11" width="12" style="13" customWidth="1"/>
-    <col min="12" max="12" width="13.5" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" s="28" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>208</v>
       </c>
@@ -10889,6 +10931,11 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10900,40 +10947,40 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="5"/>
-    <col min="2" max="2" width="7.83203125" style="65" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="5"/>
-    <col min="5" max="5" width="8.33203125" style="65" customWidth="1"/>
-    <col min="6" max="6" width="24.5" style="5" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="5"/>
-    <col min="8" max="8" width="24.1640625" style="67" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="5"/>
-    <col min="10" max="10" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="15.5" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="9.6640625" style="5"/>
+    <col min="1" max="1" width="9.7109375" style="5"/>
+    <col min="2" max="2" width="7.85546875" style="65" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="5"/>
+    <col min="5" max="5" width="8.28515625" style="65" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="5"/>
+    <col min="8" max="8" width="24.140625" style="67" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="5"/>
+    <col min="10" max="10" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="9.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B1" s="73" t="s">
+    <row r="1" spans="1:12">
+      <c r="B1" s="76" t="s">
         <v>217</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="74" t="s">
+      <c r="C1" s="77"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="77" t="s">
         <v>218</v>
       </c>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
       <c r="H1" s="66"/>
       <c r="J1" s="5" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="63" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" s="63" customFormat="1">
       <c r="A2" s="62" t="s">
         <v>219</v>
       </c>
@@ -10984,5 +11031,10 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TM-4584 Fixed Export of Version to Text Cell, Fixed Import when number to Formated Number (we need to deep test this since the old version trunked the value to INTEGER) Fixed the XLS Template (Bad positioning and column cell data type)
git-svn-id: https://opsvcs.tdsops.com/repos/tdstm/trunk@7651 fecba46a-3362-0410-80e5-8c76cdb905a0
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/octavio/Documents/TDS/tranman/trunk/web-app/templates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="782"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15540" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -38,13 +43,13 @@
     <definedName name="ProjectManager">Title!$B$5</definedName>
     <definedName name="ProjectName">Title!$C$4</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -6125,7 +6130,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -6251,6 +6256,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1540">
     <cellStyle name="_JDI DCM Runbook Hour by Hour EMA Comm Systems (Bundle 2) 11-JUL-07" xfId="1"/>
@@ -8223,7 +8229,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8267,7 +8273,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8295,24 +8301,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="38.28515625" customWidth="1"/>
-    <col min="10" max="10" width="2.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="38.33203125" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="68" t="s">
         <v>0</v>
       </c>
@@ -8320,7 +8326,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="68" t="s">
         <v>1</v>
       </c>
@@ -8328,7 +8334,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="68" t="s">
         <v>2</v>
       </c>
@@ -8336,7 +8342,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="68" t="s">
         <v>5</v>
       </c>
@@ -8344,7 +8350,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="68" t="s">
         <v>4</v>
       </c>
@@ -8352,7 +8358,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="68" t="s">
         <v>3</v>
       </c>
@@ -8360,7 +8366,7 @@
         <v>38295</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="68" t="s">
         <v>271</v>
       </c>
@@ -8368,7 +8374,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="68" t="s">
         <v>272</v>
       </c>
@@ -8376,10 +8382,10 @@
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>236</v>
       </c>
@@ -8388,7 +8394,7 @@
       <c r="F12" s="38"/>
       <c r="G12" s="38"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>269</v>
       </c>
@@ -8397,13 +8403,13 @@
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="D14" s="38"/>
       <c r="E14" s="38"/>
       <c r="F14" s="38"/>
       <c r="G14" s="38"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="34"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
@@ -8414,7 +8420,7 @@
       </c>
       <c r="G15" s="75"/>
     </row>
-    <row r="16" spans="1:7" ht="28" customHeight="1">
+    <row r="16" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36"/>
       <c r="B16" s="74" t="s">
         <v>234</v>
@@ -8433,7 +8439,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="20" customHeight="1">
+    <row r="17" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="39">
         <f>COUNTA(Applications!B:B)-1</f>
         <v>0</v>
@@ -8461,7 +8467,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="20" customHeight="1">
+    <row r="18" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18">
         <f>COUNTIF(Applications!R:R,"Master")</f>
         <v>0</v>
@@ -8483,7 +8489,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="20" customHeight="1">
+    <row r="19" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19">
         <f>A17-A18</f>
         <v>0</v>
@@ -8511,7 +8517,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="20" customHeight="1">
+    <row r="20" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="39">
         <f>COUNTA(Devices!B:B)-1</f>
         <v>0</v>
@@ -8545,7 +8551,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="20" customHeight="1">
+    <row r="21" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21">
         <f>COUNTIF(Devices!H:H,"Server")+COUNTIF(Devices!H:H,"VM")+COUNTIF(Devices!H:H,"Blade")+COUNTIF(Devices!H:H,"Appliance")</f>
         <v>0</v>
@@ -8564,7 +8570,7 @@
       <c r="F21" s="44"/>
       <c r="G21" s="44"/>
     </row>
-    <row r="22" spans="1:11" ht="20" customHeight="1">
+    <row r="22" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="39">
         <f>COUNTA(Databases!B:B)-1</f>
         <v>0</v>
@@ -8589,7 +8595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="20" customHeight="1">
+    <row r="23" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="39">
         <f>COUNTA(Storage!B:B)-1</f>
         <v>0</v>
@@ -8614,7 +8620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="20" customHeight="1">
+    <row r="24" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="39">
         <f>COUNTA(Dependencies!D:D)-1</f>
         <v>0</v>
@@ -8639,7 +8645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="20" customHeight="1">
+    <row r="25" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25">
         <f>COUNTIF(Dependencies!H:H,"Master")</f>
         <v>0</v>
@@ -8652,7 +8658,7 @@
       <c r="F25" s="38"/>
       <c r="G25" s="38"/>
     </row>
-    <row r="26" spans="1:11" ht="20" customHeight="1">
+    <row r="26" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Application")-A25</f>
         <v>0</v>
@@ -8665,7 +8671,7 @@
       <c r="F26" s="38"/>
       <c r="G26" s="38"/>
     </row>
-    <row r="27" spans="1:11" ht="20" customHeight="1">
+    <row r="27" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!H:H,"Runs On")</f>
         <v>0</v>
@@ -8678,7 +8684,7 @@
       <c r="F27" s="38"/>
       <c r="G27" s="38"/>
     </row>
-    <row r="28" spans="1:11" ht="20" customHeight="1">
+    <row r="28" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Database")</f>
         <v>0</v>
@@ -8691,7 +8697,7 @@
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
     </row>
-    <row r="29" spans="1:11" ht="20" customHeight="1">
+    <row r="29" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29">
         <f>COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Server")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Blade")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"VM")</f>
         <v>0</v>
@@ -8704,7 +8710,7 @@
       <c r="F29" s="38"/>
       <c r="G29" s="38"/>
     </row>
-    <row r="30" spans="1:11" ht="20" customHeight="1">
+    <row r="30" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30">
         <f>COUNTIF(Dependencies!H:H,"Storage")</f>
         <v>0</v>
@@ -8717,7 +8723,7 @@
       <c r="F30" s="38"/>
       <c r="G30" s="38"/>
     </row>
-    <row r="31" spans="1:11" ht="20" customHeight="1">
+    <row r="31" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="39">
         <f>COUNTA(Room!B:B)-1</f>
         <v>0</v>
@@ -8730,7 +8736,7 @@
       <c r="F31" s="46"/>
       <c r="G31" s="46"/>
     </row>
-    <row r="32" spans="1:11" ht="20" customHeight="1">
+    <row r="32" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="39">
         <f>COUNTA(Rack!B:B)-1</f>
         <v>0</v>
@@ -8743,7 +8749,7 @@
       <c r="F32" s="46"/>
       <c r="G32" s="46"/>
     </row>
-    <row r="33" spans="1:7" ht="20" customHeight="1">
+    <row r="33" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="39">
         <f>COUNTA(Cabling!B:B)-2</f>
         <v>0</v>
@@ -8756,7 +8762,7 @@
       <c r="F33" s="46"/>
       <c r="G33" s="46"/>
     </row>
-    <row r="34" spans="1:7" ht="20" customHeight="1">
+    <row r="34" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="40">
         <f>COUNTA(Comments!B:B)-1</f>
         <v>0</v>
@@ -8769,21 +8775,21 @@
       <c r="F34" s="46"/>
       <c r="G34" s="46"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="21" customHeight="1"/>
-    <row r="46" spans="1:7" ht="21" customHeight="1"/>
-    <row r="47" spans="1:7" ht="21" customHeight="1"/>
-    <row r="48" spans="1:7" ht="21" customHeight="1"/>
-    <row r="49" ht="21" customHeight="1"/>
+    <row r="45" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="46" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="47" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="48" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataConsolidate/>
@@ -8817,11 +8823,6 @@
     <ignoredError sqref="D17:D24 E18 F17:F24 G17:G24 A17:A34" emptyCellReference="1"/>
     <ignoredError sqref="E21" formula="1" emptyCellReference="1"/>
   </ignoredErrors>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8833,18 +8834,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="13" customWidth="1"/>
     <col min="2" max="2" width="16" style="11" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="9.7109375" style="22"/>
+    <col min="3" max="3" width="20.1640625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="17.5" style="12" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="22" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" style="22" customWidth="1"/>
+    <col min="7" max="16384" width="9.6640625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
         <v>228</v>
       </c>
@@ -8873,11 +8874,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8889,13 +8885,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="19.42578125" style="70" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="70"/>
+    <col min="1" max="5" width="19.5" style="70" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="70"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="69" t="s">
         <v>273</v>
       </c>
@@ -8920,11 +8916,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8932,41 +8923,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EK1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="AE1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE2" sqref="AE2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="11"/>
+    <col min="1" max="1" width="9.6640625" style="11"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" style="12"/>
-    <col min="16" max="16" width="11.85546875" style="12" customWidth="1"/>
-    <col min="20" max="20" width="11.140625" customWidth="1"/>
-    <col min="23" max="23" width="9.7109375" style="11"/>
-    <col min="28" max="28" width="17.28515625" customWidth="1"/>
-    <col min="33" max="33" width="9.85546875" style="11" customWidth="1"/>
-    <col min="34" max="34" width="11.42578125" customWidth="1"/>
-    <col min="35" max="35" width="13.42578125" customWidth="1"/>
-    <col min="36" max="36" width="16.140625" style="11" customWidth="1"/>
-    <col min="37" max="37" width="9.42578125" customWidth="1"/>
-    <col min="38" max="38" width="11.42578125" customWidth="1"/>
-    <col min="39" max="39" width="13.42578125" style="11" customWidth="1"/>
-    <col min="40" max="40" width="8.7109375" customWidth="1"/>
-    <col min="41" max="41" width="10.42578125" customWidth="1"/>
-    <col min="42" max="42" width="13.42578125" style="56" customWidth="1"/>
-    <col min="43" max="43" width="11.85546875" style="11" customWidth="1"/>
-    <col min="44" max="44" width="12.140625" style="72" customWidth="1"/>
-    <col min="45" max="45" width="11.140625" customWidth="1"/>
-    <col min="46" max="73" width="9.7109375" customWidth="1"/>
-    <col min="74" max="74" width="9.7109375" style="13" customWidth="1"/>
-    <col min="75" max="109" width="9.7109375" customWidth="1"/>
-    <col min="110" max="110" width="9.7109375" style="13" customWidth="1"/>
-    <col min="111" max="141" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="2"/>
+    <col min="15" max="15" width="9.6640625" style="12"/>
+    <col min="16" max="16" width="11.83203125" style="12" customWidth="1"/>
+    <col min="20" max="20" width="11.1640625" customWidth="1"/>
+    <col min="23" max="23" width="9.6640625" style="11"/>
+    <col min="28" max="28" width="17.33203125" customWidth="1"/>
+    <col min="33" max="33" width="9.83203125" style="11" customWidth="1"/>
+    <col min="34" max="34" width="11.5" customWidth="1"/>
+    <col min="35" max="35" width="13.5" customWidth="1"/>
+    <col min="36" max="36" width="16.1640625" style="11" customWidth="1"/>
+    <col min="37" max="37" width="9.5" customWidth="1"/>
+    <col min="38" max="38" width="11.5" customWidth="1"/>
+    <col min="39" max="39" width="13.5" style="11" customWidth="1"/>
+    <col min="40" max="40" width="8.6640625" customWidth="1"/>
+    <col min="41" max="41" width="10.5" customWidth="1"/>
+    <col min="42" max="42" width="13.5" style="56" customWidth="1"/>
+    <col min="43" max="43" width="11.83203125" style="11" customWidth="1"/>
+    <col min="44" max="44" width="12.1640625" style="72" customWidth="1"/>
+    <col min="45" max="45" width="11.1640625" customWidth="1"/>
+    <col min="46" max="73" width="9.6640625" customWidth="1"/>
+    <col min="74" max="74" width="9.6640625" style="13" customWidth="1"/>
+    <col min="75" max="109" width="9.6640625" customWidth="1"/>
+    <col min="110" max="110" width="9.6640625" style="13" customWidth="1"/>
+    <col min="111" max="141" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:141" s="17" customFormat="1">
+    <row r="1" spans="1:141" s="17" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="47" t="s">
         <v>147</v>
       </c>
@@ -8976,7 +8968,7 @@
       <c r="C1" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="79" t="s">
         <v>149</v>
       </c>
       <c r="E1" s="15" t="s">
@@ -9400,11 +9392,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9415,60 +9402,60 @@
   </sheetPr>
   <dimension ref="A1:EK1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="AD1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD2" sqref="AD2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="13" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="5" customWidth="1"/>
-    <col min="8" max="9" width="12.140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="5" customWidth="1"/>
-    <col min="12" max="13" width="10.28515625" style="5" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" style="5" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="4" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="18.85546875" style="4" customWidth="1"/>
-    <col min="18" max="18" width="13.28515625" style="5" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" style="5" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="5" customWidth="1"/>
+    <col min="8" max="9" width="12.1640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="9.5" style="5" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="5" customWidth="1"/>
+    <col min="12" max="13" width="10.33203125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="9.83203125" style="5" customWidth="1"/>
+    <col min="15" max="15" width="10.5" style="4" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" style="5" customWidth="1"/>
+    <col min="17" max="17" width="18.83203125" style="4" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" style="5" customWidth="1"/>
+    <col min="19" max="19" width="8.5" style="5" customWidth="1"/>
+    <col min="20" max="20" width="11.5" style="5" customWidth="1"/>
     <col min="21" max="21" width="11" style="5"/>
     <col min="22" max="22" width="10" style="4" customWidth="1"/>
     <col min="23" max="23" width="11" style="5"/>
-    <col min="24" max="24" width="15.7109375" style="4" customWidth="1"/>
-    <col min="25" max="25" width="12.140625" style="5" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" style="4" customWidth="1"/>
+    <col min="25" max="25" width="12.1640625" style="5" customWidth="1"/>
     <col min="26" max="26" width="12" style="6" customWidth="1"/>
     <col min="27" max="27" width="11" style="6"/>
-    <col min="28" max="28" width="12.85546875" style="5" customWidth="1"/>
+    <col min="28" max="28" width="12.83203125" style="5" customWidth="1"/>
     <col min="29" max="30" width="11" style="5"/>
-    <col min="31" max="31" width="11.42578125" style="5" customWidth="1"/>
+    <col min="31" max="31" width="11.5" style="5" customWidth="1"/>
     <col min="32" max="32" width="11" style="5"/>
-    <col min="33" max="33" width="8.85546875" style="5" customWidth="1"/>
+    <col min="33" max="33" width="8.83203125" style="5" customWidth="1"/>
     <col min="34" max="36" width="11" style="5"/>
     <col min="37" max="38" width="11" style="4"/>
-    <col min="39" max="39" width="12.85546875" style="4" customWidth="1"/>
-    <col min="40" max="41" width="8.7109375" style="4" customWidth="1"/>
+    <col min="39" max="39" width="12.83203125" style="4" customWidth="1"/>
+    <col min="40" max="41" width="8.6640625" style="4" customWidth="1"/>
     <col min="42" max="42" width="14" style="4" customWidth="1"/>
-    <col min="43" max="43" width="11.140625" style="4" customWidth="1"/>
-    <col min="44" max="44" width="12.140625" style="73" customWidth="1"/>
-    <col min="45" max="45" width="10.42578125" style="4" customWidth="1"/>
-    <col min="46" max="110" width="9.7109375" style="5" customWidth="1"/>
-    <col min="111" max="111" width="9.7109375" style="4" customWidth="1"/>
-    <col min="112" max="112" width="9.7109375" style="5" customWidth="1"/>
-    <col min="113" max="113" width="9.7109375" style="4" customWidth="1"/>
-    <col min="114" max="141" width="9.7109375" style="5" customWidth="1"/>
+    <col min="43" max="43" width="11.1640625" style="4" customWidth="1"/>
+    <col min="44" max="44" width="12.1640625" style="73" customWidth="1"/>
+    <col min="45" max="45" width="10.5" style="4" customWidth="1"/>
+    <col min="46" max="110" width="9.6640625" style="5" customWidth="1"/>
+    <col min="111" max="111" width="9.6640625" style="4" customWidth="1"/>
+    <col min="112" max="112" width="9.6640625" style="5" customWidth="1"/>
+    <col min="113" max="113" width="9.6640625" style="4" customWidth="1"/>
+    <col min="114" max="141" width="9.6640625" style="5" customWidth="1"/>
     <col min="142" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:141" s="8" customFormat="1">
+    <row r="1" spans="1:141" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="52" t="s">
         <v>6</v>
       </c>
@@ -9899,11 +9886,6 @@
   <pageMargins left="0.25" right="0.25" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9916,28 +9898,28 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="11"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="11"/>
-    <col min="6" max="6" width="16.42578125" style="11" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="12"/>
-    <col min="10" max="10" width="16.140625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="11"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="11"/>
+    <col min="6" max="6" width="16.5" style="11" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="12"/>
+    <col min="10" max="10" width="16.1640625" style="12" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="11" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" style="11" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" style="33" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" customWidth="1"/>
-    <col min="19" max="42" width="9.7109375" customWidth="1"/>
-    <col min="43" max="43" width="9.7109375" style="13" customWidth="1"/>
-    <col min="44" max="82" width="9.7109375" customWidth="1"/>
-    <col min="83" max="83" width="9.7109375" style="13"/>
-    <col min="85" max="86" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" customWidth="1"/>
+    <col min="15" max="15" width="8.6640625" style="11" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" style="11" customWidth="1"/>
+    <col min="17" max="17" width="12.83203125" style="33" customWidth="1"/>
+    <col min="18" max="18" width="11.33203125" customWidth="1"/>
+    <col min="19" max="42" width="9.6640625" customWidth="1"/>
+    <col min="43" max="43" width="9.6640625" style="13" customWidth="1"/>
+    <col min="44" max="82" width="9.6640625" customWidth="1"/>
+    <col min="83" max="83" width="9.6640625" style="13"/>
+    <col min="85" max="86" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:114" s="17" customFormat="1">
+    <row r="1" spans="1:114" s="17" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="47" t="s">
         <v>179</v>
       </c>
@@ -10290,11 +10272,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -10307,27 +10284,27 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="11"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="11"/>
-    <col min="6" max="6" width="14.7109375" style="11" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="22"/>
+    <col min="1" max="1" width="8.6640625" style="11"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="11"/>
+    <col min="6" max="6" width="14.6640625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="22"/>
     <col min="10" max="11" width="10" style="12" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" style="11" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" customWidth="1"/>
+    <col min="16" max="16" width="10.5" style="11" customWidth="1"/>
     <col min="17" max="17" width="12" style="11" customWidth="1"/>
     <col min="18" max="18" width="12" style="33" customWidth="1"/>
-    <col min="19" max="19" width="11.140625" customWidth="1"/>
-    <col min="20" max="43" width="9.7109375" customWidth="1"/>
-    <col min="44" max="44" width="9.7109375" style="13" customWidth="1"/>
-    <col min="45" max="83" width="9.7109375" customWidth="1"/>
-    <col min="84" max="84" width="9.7109375" style="13" customWidth="1"/>
-    <col min="85" max="115" width="9.7109375" customWidth="1"/>
+    <col min="19" max="19" width="11.1640625" customWidth="1"/>
+    <col min="20" max="43" width="9.6640625" customWidth="1"/>
+    <col min="44" max="44" width="9.6640625" style="13" customWidth="1"/>
+    <col min="45" max="83" width="9.6640625" customWidth="1"/>
+    <col min="84" max="84" width="9.6640625" style="13" customWidth="1"/>
+    <col min="85" max="115" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:115" s="17" customFormat="1">
+    <row r="1" spans="1:115" s="17" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="47" t="s">
         <v>181</v>
       </c>
@@ -10679,11 +10656,6 @@
   <autoFilter ref="A1:DK1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -10696,22 +10668,22 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="8.7109375" style="11"/>
-    <col min="3" max="3" width="13.42578125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="22" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" customWidth="1"/>
+    <col min="1" max="2" width="8.6640625" style="11"/>
+    <col min="3" max="3" width="13.5" style="11" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="22" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="11" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" customWidth="1"/>
+    <col min="11" max="11" width="8.1640625" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="26" customFormat="1">
+    <row r="1" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="23" t="s">
         <v>182</v>
       </c>
@@ -10766,11 +10738,6 @@
   <autoFilter ref="A1:P1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -10783,23 +10750,23 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="11"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="5" width="14.42578125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="11"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="4" max="5" width="14.5" style="13" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="26.5" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="25.28515625" style="50" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="50" customWidth="1"/>
+    <col min="11" max="11" width="19.5" style="2" customWidth="1"/>
+    <col min="12" max="12" width="25.33203125" style="50" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" style="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="29" customFormat="1">
+    <row r="1" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="23" t="s">
         <v>197</v>
       </c>
@@ -10849,11 +10816,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -10866,22 +10828,22 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="13" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="11" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="13" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="13" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="13" customWidth="1"/>
     <col min="11" max="11" width="12" style="13" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="28" customFormat="1">
+    <row r="1" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>208</v>
       </c>
@@ -10931,11 +10893,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -10947,24 +10904,24 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="5"/>
-    <col min="2" max="2" width="7.85546875" style="65" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="5"/>
-    <col min="5" max="5" width="8.28515625" style="65" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="5"/>
-    <col min="8" max="8" width="24.140625" style="67" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="5"/>
-    <col min="10" max="10" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="9.7109375" style="5"/>
+    <col min="1" max="1" width="9.6640625" style="5"/>
+    <col min="2" max="2" width="7.83203125" style="65" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="5"/>
+    <col min="5" max="5" width="8.33203125" style="65" customWidth="1"/>
+    <col min="6" max="6" width="24.5" style="5" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="5"/>
+    <col min="8" max="8" width="24.1640625" style="67" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="5"/>
+    <col min="10" max="10" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="15.5" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="9.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B1" s="76" t="s">
         <v>217</v>
       </c>
@@ -10980,7 +10937,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="63" customFormat="1">
+    <row r="2" spans="1:12" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="62" t="s">
         <v>219</v>
       </c>
@@ -11031,10 +10988,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TM-4231 Some changes for the TDS Master Templates.
git-svn-id: https://opsvcs.tdsops.com/repos/tdstm/trunk@8365 fecba46a-3362-0410-80e5-8c76cdb905a0
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/octavio/Documents/TDS/tranman/trunk/web-app/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtruitt\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15540" tabRatio="782"/>
+    <workbookView xWindow="240" yWindow="456" windowWidth="25356" windowHeight="15540" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <definedName name="ProjectManager">Title!$B$5</definedName>
     <definedName name="ProjectName">Title!$C$4</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -61,7 +61,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="V1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -976,7 +976,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="d\ mmm\ yy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
@@ -992,10 +992,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1112,22 +1114,26 @@
       <b/>
       <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -6130,7 +6136,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -6241,6 +6247,16 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -6256,7 +6272,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1540">
     <cellStyle name="_JDI DCM Runbook Hour by Hour EMA Comm Systems (Bundle 2) 11-JUL-07" xfId="1"/>
@@ -7919,6 +7934,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -8229,7 +8247,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8273,7 +8291,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8301,24 +8319,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="38.33203125" customWidth="1"/>
-    <col min="10" max="10" width="2.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="7" max="7" width="11.6328125" customWidth="1"/>
+    <col min="9" max="9" width="38.36328125" customWidth="1"/>
+    <col min="10" max="10" width="2.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="68" t="s">
         <v>0</v>
       </c>
@@ -8326,7 +8344,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="68" t="s">
         <v>1</v>
       </c>
@@ -8334,7 +8352,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="68" t="s">
         <v>2</v>
       </c>
@@ -8342,7 +8360,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="68" t="s">
         <v>5</v>
       </c>
@@ -8350,7 +8368,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="68" t="s">
         <v>4</v>
       </c>
@@ -8358,7 +8376,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="68" t="s">
         <v>3</v>
       </c>
@@ -8366,7 +8384,7 @@
         <v>38295</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="68" t="s">
         <v>271</v>
       </c>
@@ -8374,7 +8392,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="68" t="s">
         <v>272</v>
       </c>
@@ -8382,10 +8400,10 @@
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>236</v>
       </c>
@@ -8394,7 +8412,7 @@
       <c r="F12" s="38"/>
       <c r="G12" s="38"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>269</v>
       </c>
@@ -8403,29 +8421,29 @@
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D14" s="38"/>
       <c r="E14" s="38"/>
       <c r="F14" s="38"/>
       <c r="G14" s="38"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="34"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
       <c r="E15" s="35"/>
-      <c r="F15" s="75" t="s">
+      <c r="F15" s="81" t="s">
         <v>233</v>
       </c>
-      <c r="G15" s="75"/>
+      <c r="G15" s="81"/>
     </row>
-    <row r="16" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="36"/>
-      <c r="B16" s="74" t="s">
+      <c r="B16" s="80" t="s">
         <v>234</v>
       </c>
-      <c r="C16" s="74"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="37" t="s">
         <v>262</v>
       </c>
@@ -8439,7 +8457,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="39">
         <f>COUNTA(Applications!B:B)-1</f>
         <v>0</v>
@@ -8467,7 +8485,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <f>COUNTIF(Applications!R:R,"Master")</f>
         <v>0</v>
@@ -8489,7 +8507,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <f>A17-A18</f>
         <v>0</v>
@@ -8517,7 +8535,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="39">
         <f>COUNTA(Devices!B:B)-1</f>
         <v>0</v>
@@ -8551,7 +8569,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <f>COUNTIF(Devices!H:H,"Server")+COUNTIF(Devices!H:H,"VM")+COUNTIF(Devices!H:H,"Blade")+COUNTIF(Devices!H:H,"Appliance")</f>
         <v>0</v>
@@ -8570,7 +8588,7 @@
       <c r="F21" s="44"/>
       <c r="G21" s="44"/>
     </row>
-    <row r="22" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="39">
         <f>COUNTA(Databases!B:B)-1</f>
         <v>0</v>
@@ -8595,7 +8613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="39">
         <f>COUNTA(Storage!B:B)-1</f>
         <v>0</v>
@@ -8620,7 +8638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="39">
         <f>COUNTA(Dependencies!D:D)-1</f>
         <v>0</v>
@@ -8645,7 +8663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <f>COUNTIF(Dependencies!H:H,"Master")</f>
         <v>0</v>
@@ -8658,7 +8676,7 @@
       <c r="F25" s="38"/>
       <c r="G25" s="38"/>
     </row>
-    <row r="26" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Application")-A25</f>
         <v>0</v>
@@ -8671,7 +8689,7 @@
       <c r="F26" s="38"/>
       <c r="G26" s="38"/>
     </row>
-    <row r="27" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!H:H,"Runs On")</f>
         <v>0</v>
@@ -8684,7 +8702,7 @@
       <c r="F27" s="38"/>
       <c r="G27" s="38"/>
     </row>
-    <row r="28" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Database")</f>
         <v>0</v>
@@ -8697,7 +8715,7 @@
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
     </row>
-    <row r="29" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <f>COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Server")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Blade")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"VM")</f>
         <v>0</v>
@@ -8710,7 +8728,7 @@
       <c r="F29" s="38"/>
       <c r="G29" s="38"/>
     </row>
-    <row r="30" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <f>COUNTIF(Dependencies!H:H,"Storage")</f>
         <v>0</v>
@@ -8723,7 +8741,7 @@
       <c r="F30" s="38"/>
       <c r="G30" s="38"/>
     </row>
-    <row r="31" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="39">
         <f>COUNTA(Room!B:B)-1</f>
         <v>0</v>
@@ -8736,7 +8754,7 @@
       <c r="F31" s="46"/>
       <c r="G31" s="46"/>
     </row>
-    <row r="32" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="39">
         <f>COUNTA(Rack!B:B)-1</f>
         <v>0</v>
@@ -8749,7 +8767,7 @@
       <c r="F32" s="46"/>
       <c r="G32" s="46"/>
     </row>
-    <row r="33" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="39">
         <f>COUNTA(Cabling!B:B)-2</f>
         <v>0</v>
@@ -8762,7 +8780,7 @@
       <c r="F33" s="46"/>
       <c r="G33" s="46"/>
     </row>
-    <row r="34" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="40">
         <f>COUNTA(Comments!B:B)-1</f>
         <v>0</v>
@@ -8775,21 +8793,21 @@
       <c r="F34" s="46"/>
       <c r="G34" s="46"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="46" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="47" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="48" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="45" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataConsolidate/>
@@ -8834,25 +8852,25 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="16.6328125" style="13" customWidth="1"/>
     <col min="2" max="2" width="16" style="11" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="12" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="22" customWidth="1"/>
-    <col min="6" max="6" width="51.83203125" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="9.6640625" style="22"/>
+    <col min="3" max="3" width="20.1796875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="51.81640625" style="22" customWidth="1"/>
+    <col min="7" max="16384" width="9.6328125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="75" t="s">
         <v>229</v>
       </c>
       <c r="D1" s="31" t="s">
@@ -8885,13 +8903,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="19.5" style="70" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="70"/>
+    <col min="1" max="5" width="19.453125" style="70" customWidth="1"/>
+    <col min="6" max="16384" width="11.453125" style="70"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
         <v>273</v>
       </c>
@@ -8928,37 +8946,37 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="11"/>
+    <col min="1" max="1" width="9.6328125" style="11"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="2"/>
-    <col min="15" max="15" width="9.6640625" style="12"/>
-    <col min="16" max="16" width="11.83203125" style="12" customWidth="1"/>
-    <col min="20" max="20" width="11.1640625" customWidth="1"/>
-    <col min="23" max="23" width="9.6640625" style="11"/>
-    <col min="28" max="28" width="17.33203125" customWidth="1"/>
-    <col min="33" max="33" width="9.83203125" style="11" customWidth="1"/>
-    <col min="34" max="34" width="11.5" customWidth="1"/>
-    <col min="35" max="35" width="13.5" customWidth="1"/>
-    <col min="36" max="36" width="16.1640625" style="11" customWidth="1"/>
-    <col min="37" max="37" width="9.5" customWidth="1"/>
-    <col min="38" max="38" width="11.5" customWidth="1"/>
-    <col min="39" max="39" width="13.5" style="11" customWidth="1"/>
-    <col min="40" max="40" width="8.6640625" customWidth="1"/>
-    <col min="41" max="41" width="10.5" customWidth="1"/>
-    <col min="42" max="42" width="13.5" style="56" customWidth="1"/>
-    <col min="43" max="43" width="11.83203125" style="11" customWidth="1"/>
-    <col min="44" max="44" width="12.1640625" style="72" customWidth="1"/>
-    <col min="45" max="45" width="11.1640625" customWidth="1"/>
-    <col min="46" max="73" width="9.6640625" customWidth="1"/>
-    <col min="74" max="74" width="9.6640625" style="13" customWidth="1"/>
-    <col min="75" max="109" width="9.6640625" customWidth="1"/>
-    <col min="110" max="110" width="9.6640625" style="13" customWidth="1"/>
-    <col min="111" max="141" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" style="2"/>
+    <col min="15" max="15" width="9.6328125" style="12"/>
+    <col min="16" max="16" width="11.81640625" style="12" customWidth="1"/>
+    <col min="20" max="20" width="11.1796875" customWidth="1"/>
+    <col min="23" max="23" width="9.6328125" style="11"/>
+    <col min="28" max="28" width="17.36328125" customWidth="1"/>
+    <col min="33" max="33" width="9.81640625" style="11" customWidth="1"/>
+    <col min="34" max="34" width="11.453125" customWidth="1"/>
+    <col min="35" max="35" width="13.453125" customWidth="1"/>
+    <col min="36" max="36" width="16.1796875" style="11" customWidth="1"/>
+    <col min="37" max="37" width="9.453125" customWidth="1"/>
+    <col min="38" max="38" width="11.453125" customWidth="1"/>
+    <col min="39" max="39" width="13.453125" style="11" customWidth="1"/>
+    <col min="40" max="40" width="8.6328125" customWidth="1"/>
+    <col min="41" max="41" width="10.453125" customWidth="1"/>
+    <col min="42" max="42" width="13.453125" style="56" customWidth="1"/>
+    <col min="43" max="43" width="11.81640625" style="11" customWidth="1"/>
+    <col min="44" max="44" width="12.1796875" style="72" customWidth="1"/>
+    <col min="45" max="45" width="11.1796875" customWidth="1"/>
+    <col min="46" max="73" width="9.6328125" customWidth="1"/>
+    <col min="74" max="74" width="9.6328125" style="13" customWidth="1"/>
+    <col min="75" max="109" width="9.6328125" customWidth="1"/>
+    <col min="110" max="110" width="9.6328125" style="13" customWidth="1"/>
+    <col min="111" max="141" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:141" s="17" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:141" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
         <v>147</v>
       </c>
@@ -8968,7 +8986,7 @@
       <c r="C1" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="74" t="s">
         <v>149</v>
       </c>
       <c r="E1" s="15" t="s">
@@ -9397,7 +9415,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:EK1"/>
@@ -9407,55 +9425,55 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" style="5" customWidth="1"/>
     <col min="4" max="4" width="13" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" style="5" customWidth="1"/>
-    <col min="8" max="9" width="12.1640625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="9.5" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="5" customWidth="1"/>
-    <col min="12" max="13" width="10.33203125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="9.83203125" style="5" customWidth="1"/>
-    <col min="15" max="15" width="10.5" style="4" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" style="5" customWidth="1"/>
-    <col min="17" max="17" width="18.83203125" style="4" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" style="5" customWidth="1"/>
-    <col min="19" max="19" width="8.5" style="5" customWidth="1"/>
-    <col min="20" max="20" width="11.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" style="5" customWidth="1"/>
+    <col min="8" max="9" width="12.1796875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="9.453125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" style="5" customWidth="1"/>
+    <col min="12" max="13" width="10.36328125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="10.453125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="11.36328125" style="5" customWidth="1"/>
+    <col min="17" max="17" width="18.81640625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="13.36328125" style="5" customWidth="1"/>
+    <col min="19" max="19" width="8.453125" style="5" customWidth="1"/>
+    <col min="20" max="20" width="11.453125" style="5" customWidth="1"/>
     <col min="21" max="21" width="11" style="5"/>
     <col min="22" max="22" width="10" style="4" customWidth="1"/>
     <col min="23" max="23" width="11" style="5"/>
-    <col min="24" max="24" width="15.6640625" style="4" customWidth="1"/>
-    <col min="25" max="25" width="12.1640625" style="5" customWidth="1"/>
+    <col min="24" max="24" width="15.6328125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="12.1796875" style="5" customWidth="1"/>
     <col min="26" max="26" width="12" style="6" customWidth="1"/>
     <col min="27" max="27" width="11" style="6"/>
-    <col min="28" max="28" width="12.83203125" style="5" customWidth="1"/>
+    <col min="28" max="28" width="12.81640625" style="5" customWidth="1"/>
     <col min="29" max="30" width="11" style="5"/>
-    <col min="31" max="31" width="11.5" style="5" customWidth="1"/>
+    <col min="31" max="31" width="11.453125" style="5" customWidth="1"/>
     <col min="32" max="32" width="11" style="5"/>
-    <col min="33" max="33" width="8.83203125" style="5" customWidth="1"/>
+    <col min="33" max="33" width="8.81640625" style="5" customWidth="1"/>
     <col min="34" max="36" width="11" style="5"/>
     <col min="37" max="38" width="11" style="4"/>
-    <col min="39" max="39" width="12.83203125" style="4" customWidth="1"/>
-    <col min="40" max="41" width="8.6640625" style="4" customWidth="1"/>
+    <col min="39" max="39" width="12.81640625" style="4" customWidth="1"/>
+    <col min="40" max="41" width="8.6328125" style="4" customWidth="1"/>
     <col min="42" max="42" width="14" style="4" customWidth="1"/>
-    <col min="43" max="43" width="11.1640625" style="4" customWidth="1"/>
-    <col min="44" max="44" width="12.1640625" style="73" customWidth="1"/>
-    <col min="45" max="45" width="10.5" style="4" customWidth="1"/>
-    <col min="46" max="110" width="9.6640625" style="5" customWidth="1"/>
-    <col min="111" max="111" width="9.6640625" style="4" customWidth="1"/>
-    <col min="112" max="112" width="9.6640625" style="5" customWidth="1"/>
-    <col min="113" max="113" width="9.6640625" style="4" customWidth="1"/>
-    <col min="114" max="141" width="9.6640625" style="5" customWidth="1"/>
+    <col min="43" max="43" width="11.1796875" style="4" customWidth="1"/>
+    <col min="44" max="44" width="12.1796875" style="73" customWidth="1"/>
+    <col min="45" max="45" width="10.453125" style="4" customWidth="1"/>
+    <col min="46" max="110" width="9.6328125" style="5" customWidth="1"/>
+    <col min="111" max="111" width="9.6328125" style="4" customWidth="1"/>
+    <col min="112" max="112" width="9.6328125" style="5" customWidth="1"/>
+    <col min="113" max="113" width="9.6328125" style="4" customWidth="1"/>
+    <col min="114" max="141" width="9.6328125" style="5" customWidth="1"/>
     <col min="142" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:141" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:141" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="52" t="s">
         <v>6</v>
       </c>
@@ -9898,28 +9916,28 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="11"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="11"/>
-    <col min="6" max="6" width="16.5" style="11" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="12"/>
-    <col min="10" max="10" width="16.1640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="9.6328125" style="11"/>
+    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" style="11"/>
+    <col min="6" max="6" width="16.453125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="9.6328125" style="12"/>
+    <col min="10" max="10" width="16.1796875" style="12" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="13" max="13" width="12.1640625" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="11" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="11" customWidth="1"/>
-    <col min="17" max="17" width="12.83203125" style="33" customWidth="1"/>
-    <col min="18" max="18" width="11.33203125" customWidth="1"/>
-    <col min="19" max="42" width="9.6640625" customWidth="1"/>
-    <col min="43" max="43" width="9.6640625" style="13" customWidth="1"/>
-    <col min="44" max="82" width="9.6640625" customWidth="1"/>
-    <col min="83" max="83" width="9.6640625" style="13"/>
-    <col min="85" max="86" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.1796875" customWidth="1"/>
+    <col min="15" max="15" width="8.6328125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="12.1796875" style="11" customWidth="1"/>
+    <col min="17" max="17" width="12.81640625" style="33" customWidth="1"/>
+    <col min="18" max="18" width="11.36328125" customWidth="1"/>
+    <col min="19" max="42" width="9.6328125" customWidth="1"/>
+    <col min="43" max="43" width="9.6328125" style="13" customWidth="1"/>
+    <col min="44" max="82" width="9.6328125" customWidth="1"/>
+    <col min="83" max="83" width="9.6328125" style="13"/>
+    <col min="85" max="86" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:114" s="17" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:114" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
         <v>179</v>
       </c>
@@ -10284,27 +10302,27 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="11"/>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="11"/>
-    <col min="6" max="6" width="14.6640625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="22"/>
+    <col min="1" max="1" width="8.6328125" style="11"/>
+    <col min="2" max="2" width="21.1796875" customWidth="1"/>
+    <col min="4" max="4" width="8.6328125" style="11"/>
+    <col min="6" max="6" width="14.6328125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="8.6328125" style="22"/>
     <col min="10" max="11" width="10" style="12" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" customWidth="1"/>
-    <col min="16" max="16" width="10.5" style="11" customWidth="1"/>
+    <col min="15" max="15" width="10.36328125" customWidth="1"/>
+    <col min="16" max="16" width="10.453125" style="11" customWidth="1"/>
     <col min="17" max="17" width="12" style="11" customWidth="1"/>
     <col min="18" max="18" width="12" style="33" customWidth="1"/>
-    <col min="19" max="19" width="11.1640625" customWidth="1"/>
-    <col min="20" max="43" width="9.6640625" customWidth="1"/>
-    <col min="44" max="44" width="9.6640625" style="13" customWidth="1"/>
-    <col min="45" max="83" width="9.6640625" customWidth="1"/>
-    <col min="84" max="84" width="9.6640625" style="13" customWidth="1"/>
-    <col min="85" max="115" width="9.6640625" customWidth="1"/>
+    <col min="19" max="19" width="11.1796875" customWidth="1"/>
+    <col min="20" max="43" width="9.6328125" customWidth="1"/>
+    <col min="44" max="44" width="9.6328125" style="13" customWidth="1"/>
+    <col min="45" max="83" width="9.6328125" customWidth="1"/>
+    <col min="84" max="84" width="9.6328125" style="13" customWidth="1"/>
+    <col min="85" max="115" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:115" s="17" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:115" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
         <v>181</v>
       </c>
@@ -10668,29 +10686,29 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.6640625" style="11"/>
-    <col min="3" max="3" width="13.5" style="11" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="22" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="11" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="22" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" customWidth="1"/>
-    <col min="11" max="11" width="8.1640625" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" customWidth="1"/>
+    <col min="1" max="2" width="8.6328125" style="11"/>
+    <col min="3" max="3" width="13.453125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" style="22" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" style="22" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" customWidth="1"/>
+    <col min="10" max="10" width="17.81640625" customWidth="1"/>
+    <col min="11" max="11" width="8.1796875" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="76" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="76" t="s">
         <v>184</v>
       </c>
       <c r="D1" s="24" t="s">
@@ -10708,10 +10726,10 @@
       <c r="H1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="77" t="s">
         <v>189</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="77" t="s">
         <v>190</v>
       </c>
       <c r="K1" s="26" t="s">
@@ -10750,23 +10768,23 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="11"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
-    <col min="4" max="5" width="14.5" style="13" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.5" customWidth="1"/>
-    <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.6328125" style="11"/>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" customWidth="1"/>
+    <col min="4" max="5" width="14.453125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" customWidth="1"/>
+    <col min="7" max="7" width="26.453125" customWidth="1"/>
+    <col min="8" max="8" width="21.453125" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="19.5" style="2" customWidth="1"/>
-    <col min="12" max="12" width="25.33203125" style="50" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" style="50" customWidth="1"/>
+    <col min="11" max="11" width="19.453125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="25.36328125" style="50" customWidth="1"/>
+    <col min="13" max="13" width="16.81640625" style="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>197</v>
       </c>
@@ -10828,22 +10846,22 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5" style="11" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="13" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="4" max="5" width="16.36328125" customWidth="1"/>
+    <col min="6" max="6" width="11.36328125" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="13.36328125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" style="13" customWidth="1"/>
     <col min="11" max="11" width="12" style="13" customWidth="1"/>
-    <col min="12" max="12" width="13.5" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>208</v>
       </c>
@@ -10904,50 +10922,50 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="5"/>
-    <col min="2" max="2" width="7.83203125" style="65" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="5"/>
-    <col min="5" max="5" width="8.33203125" style="65" customWidth="1"/>
-    <col min="6" max="6" width="24.5" style="5" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="5"/>
-    <col min="8" max="8" width="24.1640625" style="67" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="5"/>
-    <col min="10" max="10" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="15.5" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="9.6640625" style="5"/>
+    <col min="1" max="1" width="9.6328125" style="5"/>
+    <col min="2" max="2" width="7.81640625" style="65" customWidth="1"/>
+    <col min="3" max="3" width="22.36328125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" style="5"/>
+    <col min="5" max="5" width="8.36328125" style="65" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="9.6328125" style="5"/>
+    <col min="8" max="8" width="24.1796875" style="67" customWidth="1"/>
+    <col min="9" max="9" width="9.6328125" style="5"/>
+    <col min="10" max="10" width="14.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="9.6328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B1" s="76" t="s">
+    <row r="1" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1" s="82" t="s">
         <v>217</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="77" t="s">
+      <c r="C1" s="83"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="83" t="s">
         <v>218</v>
       </c>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
       <c r="H1" s="66"/>
       <c r="J1" s="5" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="63" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="62" t="s">
+    <row r="2" spans="1:12" s="63" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="78" t="s">
         <v>219</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="79" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="78" t="s">
         <v>221</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="78" t="s">
         <v>222</v>
       </c>
       <c r="E2" s="64" t="s">
@@ -10983,7 +11001,7 @@
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
TM-6596 Change the Asset Export template to freeze on asset names and column headers
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtruitt\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="456" windowWidth="25356" windowHeight="15540" tabRatio="782"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15540" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -45,11 +40,11 @@
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -61,7 +56,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -976,7 +971,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="d\ mmm\ yy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
@@ -8247,7 +8242,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8291,7 +8286,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8319,24 +8314,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
-    <col min="7" max="7" width="11.6328125" customWidth="1"/>
-    <col min="9" max="9" width="38.36328125" customWidth="1"/>
-    <col min="10" max="10" width="2.36328125" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="38.42578125" customWidth="1"/>
+    <col min="10" max="10" width="2.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18">
       <c r="A1" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="68" t="s">
         <v>0</v>
       </c>
@@ -8344,7 +8339,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="68" t="s">
         <v>1</v>
       </c>
@@ -8352,7 +8347,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="68" t="s">
         <v>2</v>
       </c>
@@ -8360,7 +8355,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="68" t="s">
         <v>5</v>
       </c>
@@ -8368,7 +8363,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="68" t="s">
         <v>4</v>
       </c>
@@ -8376,7 +8371,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="68" t="s">
         <v>3</v>
       </c>
@@ -8384,7 +8379,7 @@
         <v>38295</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="68" t="s">
         <v>271</v>
       </c>
@@ -8392,7 +8387,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="68" t="s">
         <v>272</v>
       </c>
@@ -8400,10 +8395,10 @@
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="B12" t="s">
         <v>236</v>
       </c>
@@ -8412,7 +8407,7 @@
       <c r="F12" s="38"/>
       <c r="G12" s="38"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="B13" t="s">
         <v>269</v>
       </c>
@@ -8421,13 +8416,13 @@
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="D14" s="38"/>
       <c r="E14" s="38"/>
       <c r="F14" s="38"/>
       <c r="G14" s="38"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15" customHeight="1">
       <c r="A15" s="34"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
@@ -8438,7 +8433,7 @@
       </c>
       <c r="G15" s="81"/>
     </row>
-    <row r="16" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="28" customHeight="1">
       <c r="A16" s="36"/>
       <c r="B16" s="80" t="s">
         <v>234</v>
@@ -8457,7 +8452,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="20" customHeight="1">
       <c r="A17" s="39">
         <f>COUNTA(Applications!B:B)-1</f>
         <v>0</v>
@@ -8485,7 +8480,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="20" customHeight="1">
       <c r="A18">
         <f>COUNTIF(Applications!R:R,"Master")</f>
         <v>0</v>
@@ -8507,7 +8502,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="20" customHeight="1">
       <c r="A19">
         <f>A17-A18</f>
         <v>0</v>
@@ -8535,7 +8530,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="20" customHeight="1">
       <c r="A20" s="39">
         <f>COUNTA(Devices!B:B)-1</f>
         <v>0</v>
@@ -8569,7 +8564,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="20" customHeight="1">
       <c r="A21">
         <f>COUNTIF(Devices!H:H,"Server")+COUNTIF(Devices!H:H,"VM")+COUNTIF(Devices!H:H,"Blade")+COUNTIF(Devices!H:H,"Appliance")</f>
         <v>0</v>
@@ -8588,7 +8583,7 @@
       <c r="F21" s="44"/>
       <c r="G21" s="44"/>
     </row>
-    <row r="22" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="20" customHeight="1">
       <c r="A22" s="39">
         <f>COUNTA(Databases!B:B)-1</f>
         <v>0</v>
@@ -8613,7 +8608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="20" customHeight="1">
       <c r="A23" s="39">
         <f>COUNTA(Storage!B:B)-1</f>
         <v>0</v>
@@ -8638,7 +8633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="20" customHeight="1">
       <c r="A24" s="39">
         <f>COUNTA(Dependencies!D:D)-1</f>
         <v>0</v>
@@ -8663,7 +8658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="20" customHeight="1">
       <c r="A25">
         <f>COUNTIF(Dependencies!H:H,"Master")</f>
         <v>0</v>
@@ -8676,7 +8671,7 @@
       <c r="F25" s="38"/>
       <c r="G25" s="38"/>
     </row>
-    <row r="26" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="20" customHeight="1">
       <c r="A26">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Application")-A25</f>
         <v>0</v>
@@ -8689,7 +8684,7 @@
       <c r="F26" s="38"/>
       <c r="G26" s="38"/>
     </row>
-    <row r="27" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="20" customHeight="1">
       <c r="A27">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!H:H,"Runs On")</f>
         <v>0</v>
@@ -8702,7 +8697,7 @@
       <c r="F27" s="38"/>
       <c r="G27" s="38"/>
     </row>
-    <row r="28" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="20" customHeight="1">
       <c r="A28">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Database")</f>
         <v>0</v>
@@ -8715,7 +8710,7 @@
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
     </row>
-    <row r="29" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="20" customHeight="1">
       <c r="A29">
         <f>COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Server")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Blade")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"VM")</f>
         <v>0</v>
@@ -8728,7 +8723,7 @@
       <c r="F29" s="38"/>
       <c r="G29" s="38"/>
     </row>
-    <row r="30" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="20" customHeight="1">
       <c r="A30">
         <f>COUNTIF(Dependencies!H:H,"Storage")</f>
         <v>0</v>
@@ -8741,7 +8736,7 @@
       <c r="F30" s="38"/>
       <c r="G30" s="38"/>
     </row>
-    <row r="31" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="20" customHeight="1">
       <c r="A31" s="39">
         <f>COUNTA(Room!B:B)-1</f>
         <v>0</v>
@@ -8754,7 +8749,7 @@
       <c r="F31" s="46"/>
       <c r="G31" s="46"/>
     </row>
-    <row r="32" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="20" customHeight="1">
       <c r="A32" s="39">
         <f>COUNTA(Rack!B:B)-1</f>
         <v>0</v>
@@ -8767,7 +8762,7 @@
       <c r="F32" s="46"/>
       <c r="G32" s="46"/>
     </row>
-    <row r="33" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="20" customHeight="1">
       <c r="A33" s="39">
         <f>COUNTA(Cabling!B:B)-2</f>
         <v>0</v>
@@ -8780,7 +8775,7 @@
       <c r="F33" s="46"/>
       <c r="G33" s="46"/>
     </row>
-    <row r="34" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="20" customHeight="1">
       <c r="A34" s="40">
         <f>COUNTA(Comments!B:B)-1</f>
         <v>0</v>
@@ -8793,21 +8788,21 @@
       <c r="F34" s="46"/>
       <c r="G34" s="46"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:7" ht="21" customHeight="1"/>
+    <row r="46" spans="1:7" ht="21" customHeight="1"/>
+    <row r="47" spans="1:7" ht="21" customHeight="1"/>
+    <row r="48" spans="1:7" ht="21" customHeight="1"/>
+    <row r="49" ht="21" customHeight="1"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataConsolidate/>
@@ -8841,6 +8836,11 @@
     <ignoredError sqref="D17:D24 E18 F17:F24 G17:G24 A17:A34" emptyCellReference="1"/>
     <ignoredError sqref="E21" formula="1" emptyCellReference="1"/>
   </ignoredErrors>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8852,18 +8852,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="13" customWidth="1"/>
     <col min="2" max="2" width="16" style="11" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="51.81640625" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="9.6328125" style="22"/>
+    <col min="3" max="3" width="20.140625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" style="22" customWidth="1"/>
+    <col min="7" max="16384" width="9.5703125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="31" t="s">
         <v>228</v>
       </c>
@@ -8892,6 +8892,11 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8903,13 +8908,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="5" width="19.453125" style="70" customWidth="1"/>
-    <col min="6" max="16384" width="11.453125" style="70"/>
+    <col min="1" max="5" width="19.42578125" style="70" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="70"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="69" t="s">
         <v>273</v>
       </c>
@@ -8934,6 +8939,11 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8942,41 +8952,43 @@
   <dimension ref="A1:EK1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" style="11"/>
+    <col min="1" max="1" width="9.5703125" style="11"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" style="2"/>
-    <col min="15" max="15" width="9.6328125" style="12"/>
-    <col min="16" max="16" width="11.81640625" style="12" customWidth="1"/>
-    <col min="20" max="20" width="11.1796875" customWidth="1"/>
-    <col min="23" max="23" width="9.6328125" style="11"/>
-    <col min="28" max="28" width="17.36328125" customWidth="1"/>
-    <col min="33" max="33" width="9.81640625" style="11" customWidth="1"/>
-    <col min="34" max="34" width="11.453125" customWidth="1"/>
-    <col min="35" max="35" width="13.453125" customWidth="1"/>
-    <col min="36" max="36" width="16.1796875" style="11" customWidth="1"/>
-    <col min="37" max="37" width="9.453125" customWidth="1"/>
-    <col min="38" max="38" width="11.453125" customWidth="1"/>
-    <col min="39" max="39" width="13.453125" style="11" customWidth="1"/>
-    <col min="40" max="40" width="8.6328125" customWidth="1"/>
-    <col min="41" max="41" width="10.453125" customWidth="1"/>
-    <col min="42" max="42" width="13.453125" style="56" customWidth="1"/>
-    <col min="43" max="43" width="11.81640625" style="11" customWidth="1"/>
-    <col min="44" max="44" width="12.1796875" style="72" customWidth="1"/>
-    <col min="45" max="45" width="11.1796875" customWidth="1"/>
-    <col min="46" max="73" width="9.6328125" customWidth="1"/>
-    <col min="74" max="74" width="9.6328125" style="13" customWidth="1"/>
-    <col min="75" max="109" width="9.6328125" customWidth="1"/>
-    <col min="110" max="110" width="9.6328125" style="13" customWidth="1"/>
-    <col min="111" max="141" width="9.6328125" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="2"/>
+    <col min="15" max="15" width="9.5703125" style="12"/>
+    <col min="16" max="16" width="11.85546875" style="12" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" style="11"/>
+    <col min="28" max="28" width="17.42578125" customWidth="1"/>
+    <col min="33" max="33" width="9.85546875" style="11" customWidth="1"/>
+    <col min="34" max="34" width="11.42578125" customWidth="1"/>
+    <col min="35" max="35" width="13.42578125" customWidth="1"/>
+    <col min="36" max="36" width="16.140625" style="11" customWidth="1"/>
+    <col min="37" max="37" width="9.42578125" customWidth="1"/>
+    <col min="38" max="38" width="11.42578125" customWidth="1"/>
+    <col min="39" max="39" width="13.42578125" style="11" customWidth="1"/>
+    <col min="40" max="40" width="8.5703125" customWidth="1"/>
+    <col min="41" max="41" width="10.42578125" customWidth="1"/>
+    <col min="42" max="42" width="13.42578125" style="56" customWidth="1"/>
+    <col min="43" max="43" width="11.85546875" style="11" customWidth="1"/>
+    <col min="44" max="44" width="12.140625" style="72" customWidth="1"/>
+    <col min="45" max="45" width="11.140625" customWidth="1"/>
+    <col min="46" max="73" width="9.5703125" customWidth="1"/>
+    <col min="74" max="74" width="9.5703125" style="13" customWidth="1"/>
+    <col min="75" max="109" width="9.5703125" customWidth="1"/>
+    <col min="110" max="110" width="9.5703125" style="13" customWidth="1"/>
+    <col min="111" max="141" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:141" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:141" s="17" customFormat="1">
       <c r="A1" s="47" t="s">
         <v>147</v>
       </c>
@@ -9410,70 +9422,77 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:EK1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="5" customWidth="1"/>
     <col min="4" max="4" width="13" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" style="5" customWidth="1"/>
-    <col min="8" max="9" width="12.1796875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="9.453125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" style="5" customWidth="1"/>
-    <col min="12" max="13" width="10.36328125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="9.81640625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="10.453125" style="4" customWidth="1"/>
-    <col min="16" max="16" width="11.36328125" style="5" customWidth="1"/>
-    <col min="17" max="17" width="18.81640625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="13.36328125" style="5" customWidth="1"/>
-    <col min="19" max="19" width="8.453125" style="5" customWidth="1"/>
-    <col min="20" max="20" width="11.453125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="5" customWidth="1"/>
+    <col min="8" max="9" width="12.140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="5" customWidth="1"/>
+    <col min="12" max="13" width="10.42578125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" style="5" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="5" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" style="5" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" style="5" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="5" customWidth="1"/>
     <col min="21" max="21" width="11" style="5"/>
     <col min="22" max="22" width="10" style="4" customWidth="1"/>
     <col min="23" max="23" width="11" style="5"/>
-    <col min="24" max="24" width="15.6328125" style="4" customWidth="1"/>
-    <col min="25" max="25" width="12.1796875" style="5" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="12.140625" style="5" customWidth="1"/>
     <col min="26" max="26" width="12" style="6" customWidth="1"/>
     <col min="27" max="27" width="11" style="6"/>
-    <col min="28" max="28" width="12.81640625" style="5" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" style="5" customWidth="1"/>
     <col min="29" max="30" width="11" style="5"/>
-    <col min="31" max="31" width="11.453125" style="5" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="5" customWidth="1"/>
     <col min="32" max="32" width="11" style="5"/>
-    <col min="33" max="33" width="8.81640625" style="5" customWidth="1"/>
+    <col min="33" max="33" width="8.85546875" style="5" customWidth="1"/>
     <col min="34" max="36" width="11" style="5"/>
     <col min="37" max="38" width="11" style="4"/>
-    <col min="39" max="39" width="12.81640625" style="4" customWidth="1"/>
-    <col min="40" max="41" width="8.6328125" style="4" customWidth="1"/>
+    <col min="39" max="39" width="12.85546875" style="4" customWidth="1"/>
+    <col min="40" max="41" width="8.5703125" style="4" customWidth="1"/>
     <col min="42" max="42" width="14" style="4" customWidth="1"/>
-    <col min="43" max="43" width="11.1796875" style="4" customWidth="1"/>
-    <col min="44" max="44" width="12.1796875" style="73" customWidth="1"/>
-    <col min="45" max="45" width="10.453125" style="4" customWidth="1"/>
-    <col min="46" max="110" width="9.6328125" style="5" customWidth="1"/>
-    <col min="111" max="111" width="9.6328125" style="4" customWidth="1"/>
-    <col min="112" max="112" width="9.6328125" style="5" customWidth="1"/>
-    <col min="113" max="113" width="9.6328125" style="4" customWidth="1"/>
-    <col min="114" max="141" width="9.6328125" style="5" customWidth="1"/>
+    <col min="43" max="43" width="11.140625" style="4" customWidth="1"/>
+    <col min="44" max="44" width="12.140625" style="73" customWidth="1"/>
+    <col min="45" max="45" width="10.42578125" style="4" customWidth="1"/>
+    <col min="46" max="110" width="9.5703125" style="5" customWidth="1"/>
+    <col min="111" max="111" width="9.5703125" style="4" customWidth="1"/>
+    <col min="112" max="112" width="9.5703125" style="5" customWidth="1"/>
+    <col min="113" max="113" width="9.5703125" style="4" customWidth="1"/>
+    <col min="114" max="141" width="9.5703125" style="5" customWidth="1"/>
     <col min="142" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:141" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:141" s="8" customFormat="1">
       <c r="A1" s="52" t="s">
         <v>6</v>
       </c>
@@ -9904,6 +9923,11 @@
   <pageMargins left="0.25" right="0.25" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9912,32 +9936,34 @@
   <dimension ref="A1:DJ1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" style="11"/>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" style="11"/>
-    <col min="6" max="6" width="16.453125" style="11" customWidth="1"/>
-    <col min="9" max="9" width="9.6328125" style="12"/>
-    <col min="10" max="10" width="16.1796875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="11"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="11"/>
+    <col min="6" max="6" width="16.42578125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" style="12"/>
+    <col min="10" max="10" width="16.140625" style="12" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="13" max="13" width="12.1796875" customWidth="1"/>
-    <col min="15" max="15" width="8.6328125" style="11" customWidth="1"/>
-    <col min="16" max="16" width="12.1796875" style="11" customWidth="1"/>
-    <col min="17" max="17" width="12.81640625" style="33" customWidth="1"/>
-    <col min="18" max="18" width="11.36328125" customWidth="1"/>
-    <col min="19" max="42" width="9.6328125" customWidth="1"/>
-    <col min="43" max="43" width="9.6328125" style="13" customWidth="1"/>
-    <col min="44" max="82" width="9.6328125" customWidth="1"/>
-    <col min="83" max="83" width="9.6328125" style="13"/>
-    <col min="85" max="86" width="9.6328125" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" style="11" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="33" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="42" width="9.5703125" customWidth="1"/>
+    <col min="43" max="43" width="9.5703125" style="13" customWidth="1"/>
+    <col min="44" max="82" width="9.5703125" customWidth="1"/>
+    <col min="83" max="83" width="9.5703125" style="13"/>
+    <col min="85" max="86" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:114" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:114" s="17" customFormat="1">
       <c r="A1" s="47" t="s">
         <v>179</v>
       </c>
@@ -10290,6 +10316,11 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10298,31 +10329,33 @@
   <dimension ref="A1:DK1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.6328125" style="11"/>
-    <col min="2" max="2" width="21.1796875" customWidth="1"/>
-    <col min="4" max="4" width="8.6328125" style="11"/>
-    <col min="6" max="6" width="14.6328125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="8.6328125" style="22"/>
+    <col min="1" max="1" width="8.5703125" style="11"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="11"/>
+    <col min="6" max="6" width="14.5703125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="22"/>
     <col min="10" max="11" width="10" style="12" customWidth="1"/>
-    <col min="15" max="15" width="10.36328125" customWidth="1"/>
-    <col min="16" max="16" width="10.453125" style="11" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="11" customWidth="1"/>
     <col min="17" max="17" width="12" style="11" customWidth="1"/>
     <col min="18" max="18" width="12" style="33" customWidth="1"/>
-    <col min="19" max="19" width="11.1796875" customWidth="1"/>
-    <col min="20" max="43" width="9.6328125" customWidth="1"/>
-    <col min="44" max="44" width="9.6328125" style="13" customWidth="1"/>
-    <col min="45" max="83" width="9.6328125" customWidth="1"/>
-    <col min="84" max="84" width="9.6328125" style="13" customWidth="1"/>
-    <col min="85" max="115" width="9.6328125" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" customWidth="1"/>
+    <col min="20" max="43" width="9.5703125" customWidth="1"/>
+    <col min="44" max="44" width="9.5703125" style="13" customWidth="1"/>
+    <col min="45" max="83" width="9.5703125" customWidth="1"/>
+    <col min="84" max="84" width="9.5703125" style="13" customWidth="1"/>
+    <col min="85" max="115" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:115" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:115" s="17" customFormat="1">
       <c r="A1" s="47" t="s">
         <v>181</v>
       </c>
@@ -10674,6 +10707,11 @@
   <autoFilter ref="A1:DK1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10686,22 +10724,22 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="8.6328125" style="11"/>
-    <col min="3" max="3" width="13.453125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="16.1796875" style="22" customWidth="1"/>
-    <col min="7" max="7" width="14.6328125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="14.1796875" style="22" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" customWidth="1"/>
-    <col min="10" max="10" width="17.81640625" customWidth="1"/>
-    <col min="11" max="11" width="8.1796875" customWidth="1"/>
-    <col min="12" max="12" width="12.1796875" customWidth="1"/>
+    <col min="1" max="2" width="8.5703125" style="11"/>
+    <col min="3" max="3" width="13.42578125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="26" customFormat="1">
       <c r="A1" s="23" t="s">
         <v>182</v>
       </c>
@@ -10756,6 +10794,11 @@
   <autoFilter ref="A1:P1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10764,27 +10807,29 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" style="11"/>
-    <col min="2" max="2" width="22.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" customWidth="1"/>
-    <col min="4" max="5" width="14.453125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" customWidth="1"/>
-    <col min="7" max="7" width="26.453125" customWidth="1"/>
-    <col min="8" max="8" width="21.453125" customWidth="1"/>
-    <col min="9" max="9" width="13.1796875" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="11"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="5" width="14.42578125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="19.453125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="25.36328125" style="50" customWidth="1"/>
-    <col min="13" max="13" width="16.81640625" style="50" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="25.42578125" style="50" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="29" customFormat="1">
       <c r="A1" s="23" t="s">
         <v>197</v>
       </c>
@@ -10834,6 +10879,11 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10842,26 +10892,27 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.453125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" customWidth="1"/>
-    <col min="4" max="5" width="16.36328125" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="13.6328125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="13" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="13" customWidth="1"/>
     <col min="11" max="11" width="12" style="13" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="28" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>208</v>
       </c>
@@ -10911,6 +10962,11 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10922,24 +10978,24 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" style="5"/>
-    <col min="2" max="2" width="7.81640625" style="65" customWidth="1"/>
-    <col min="3" max="3" width="22.36328125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" style="5"/>
-    <col min="5" max="5" width="8.36328125" style="65" customWidth="1"/>
-    <col min="6" max="6" width="24.453125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" style="5"/>
-    <col min="8" max="8" width="24.1796875" style="67" customWidth="1"/>
-    <col min="9" max="9" width="9.6328125" style="5"/>
-    <col min="10" max="10" width="14.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.81640625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="15.453125" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="9.6328125" style="5"/>
+    <col min="1" max="1" width="9.5703125" style="5"/>
+    <col min="2" max="2" width="7.85546875" style="65" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="5"/>
+    <col min="5" max="5" width="8.42578125" style="65" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="5"/>
+    <col min="8" max="8" width="24.140625" style="67" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" style="5"/>
+    <col min="10" max="10" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="9.5703125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="B1" s="82" t="s">
         <v>217</v>
       </c>
@@ -10955,7 +11011,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="63" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="63" customFormat="1">
       <c r="A2" s="78" t="s">
         <v>219</v>
       </c>
@@ -11001,10 +11057,15 @@
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TM-6586 Asset Export : removed the Custom1..Custom96 from each of the Asset tabs
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -38,7 +38,7 @@
     <definedName name="ProjectManager">Title!$B$5</definedName>
     <definedName name="ProjectName">Title!$C$4</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="182">
   <si>
     <t>Customer:</t>
   </si>
@@ -284,294 +284,6 @@
   </si>
   <si>
     <t>Modified By</t>
-  </si>
-  <si>
-    <t>Custom1</t>
-  </si>
-  <si>
-    <t>Custom2</t>
-  </si>
-  <si>
-    <t>Custom3</t>
-  </si>
-  <si>
-    <t>Custom4</t>
-  </si>
-  <si>
-    <t>Custom5</t>
-  </si>
-  <si>
-    <t>Custom6</t>
-  </si>
-  <si>
-    <t>Custom7</t>
-  </si>
-  <si>
-    <t>Custom8</t>
-  </si>
-  <si>
-    <t>Custom9</t>
-  </si>
-  <si>
-    <t>Custom10</t>
-  </si>
-  <si>
-    <t>Custom11</t>
-  </si>
-  <si>
-    <t>Custom12</t>
-  </si>
-  <si>
-    <t>Custom13</t>
-  </si>
-  <si>
-    <t>Custom14</t>
-  </si>
-  <si>
-    <t>Custom15</t>
-  </si>
-  <si>
-    <t>Custom16</t>
-  </si>
-  <si>
-    <t>Custom17</t>
-  </si>
-  <si>
-    <t>Custom18</t>
-  </si>
-  <si>
-    <t>Custom19</t>
-  </si>
-  <si>
-    <t>Custom20</t>
-  </si>
-  <si>
-    <t>Custom21</t>
-  </si>
-  <si>
-    <t>Custom22</t>
-  </si>
-  <si>
-    <t>Custom23</t>
-  </si>
-  <si>
-    <t>Custom24</t>
-  </si>
-  <si>
-    <t>Custom25</t>
-  </si>
-  <si>
-    <t>Custom26</t>
-  </si>
-  <si>
-    <t>Custom27</t>
-  </si>
-  <si>
-    <t>Custom28</t>
-  </si>
-  <si>
-    <t>Custom29</t>
-  </si>
-  <si>
-    <t>Custom30</t>
-  </si>
-  <si>
-    <t>Custom31</t>
-  </si>
-  <si>
-    <t>Custom32</t>
-  </si>
-  <si>
-    <t>Custom33</t>
-  </si>
-  <si>
-    <t>Custom34</t>
-  </si>
-  <si>
-    <t>Custom35</t>
-  </si>
-  <si>
-    <t>Custom36</t>
-  </si>
-  <si>
-    <t>Custom37</t>
-  </si>
-  <si>
-    <t>Custom38</t>
-  </si>
-  <si>
-    <t>Custom39</t>
-  </si>
-  <si>
-    <t>Custom40</t>
-  </si>
-  <si>
-    <t>Custom41</t>
-  </si>
-  <si>
-    <t>Custom42</t>
-  </si>
-  <si>
-    <t>Custom43</t>
-  </si>
-  <si>
-    <t>Custom44</t>
-  </si>
-  <si>
-    <t>Custom45</t>
-  </si>
-  <si>
-    <t>Custom46</t>
-  </si>
-  <si>
-    <t>Custom47</t>
-  </si>
-  <si>
-    <t>Custom48</t>
-  </si>
-  <si>
-    <t>Custom49</t>
-  </si>
-  <si>
-    <t>Custom50</t>
-  </si>
-  <si>
-    <t>Custom51</t>
-  </si>
-  <si>
-    <t>Custom52</t>
-  </si>
-  <si>
-    <t>Custom53</t>
-  </si>
-  <si>
-    <t>Custom54</t>
-  </si>
-  <si>
-    <t>Custom55</t>
-  </si>
-  <si>
-    <t>Custom56</t>
-  </si>
-  <si>
-    <t>Custom57</t>
-  </si>
-  <si>
-    <t>Custom58</t>
-  </si>
-  <si>
-    <t>Custom59</t>
-  </si>
-  <si>
-    <t>Custom60</t>
-  </si>
-  <si>
-    <t>Custom61</t>
-  </si>
-  <si>
-    <t>Custom62</t>
-  </si>
-  <si>
-    <t>Custom63</t>
-  </si>
-  <si>
-    <t>Custom64</t>
-  </si>
-  <si>
-    <t>Custom65</t>
-  </si>
-  <si>
-    <t>Custom66</t>
-  </si>
-  <si>
-    <t>Custom67</t>
-  </si>
-  <si>
-    <t>Custom68</t>
-  </si>
-  <si>
-    <t>Custom69</t>
-  </si>
-  <si>
-    <t>Custom70</t>
-  </si>
-  <si>
-    <t>Custom71</t>
-  </si>
-  <si>
-    <t>Custom72</t>
-  </si>
-  <si>
-    <t>Custom73</t>
-  </si>
-  <si>
-    <t>Custom74</t>
-  </si>
-  <si>
-    <t>Custom75</t>
-  </si>
-  <si>
-    <t>Custom76</t>
-  </si>
-  <si>
-    <t>Custom77</t>
-  </si>
-  <si>
-    <t>Custom78</t>
-  </si>
-  <si>
-    <t>Custom79</t>
-  </si>
-  <si>
-    <t>Custom80</t>
-  </si>
-  <si>
-    <t>Custom81</t>
-  </si>
-  <si>
-    <t>Custom82</t>
-  </si>
-  <si>
-    <t>Custom83</t>
-  </si>
-  <si>
-    <t>Custom84</t>
-  </si>
-  <si>
-    <t>Custom85</t>
-  </si>
-  <si>
-    <t>Custom86</t>
-  </si>
-  <si>
-    <t>Custom87</t>
-  </si>
-  <si>
-    <t>Custom88</t>
-  </si>
-  <si>
-    <t>Custom89</t>
-  </si>
-  <si>
-    <t>Custom90</t>
-  </si>
-  <si>
-    <t>Custom91</t>
-  </si>
-  <si>
-    <t>Custom92</t>
-  </si>
-  <si>
-    <t>Custom93</t>
-  </si>
-  <si>
-    <t>Custom94</t>
-  </si>
-  <si>
-    <t>Custom95</t>
-  </si>
-  <si>
-    <t>Custom96</t>
   </si>
   <si>
     <t>appId</t>
@@ -8325,7 +8037,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18">
       <c r="A1" s="1" t="s">
-        <v>237</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -8336,7 +8048,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>268</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -8344,7 +8056,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>268</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -8352,7 +8064,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>268</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -8360,7 +8072,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>268</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -8368,7 +8080,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>268</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -8381,18 +8093,18 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="68" t="s">
-        <v>271</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
-        <v>268</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="68" t="s">
-        <v>272</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s">
-        <v>268</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -8400,7 +8112,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="B12" t="s">
-        <v>236</v>
+        <v>140</v>
       </c>
       <c r="D12" s="38"/>
       <c r="E12" s="38"/>
@@ -8409,7 +8121,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
-        <v>269</v>
+        <v>173</v>
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="38"/>
@@ -8429,27 +8141,27 @@
       <c r="D15" s="35"/>
       <c r="E15" s="35"/>
       <c r="F15" s="81" t="s">
-        <v>233</v>
+        <v>137</v>
       </c>
       <c r="G15" s="81"/>
     </row>
     <row r="16" spans="1:7" ht="28" customHeight="1">
       <c r="A16" s="36"/>
       <c r="B16" s="80" t="s">
-        <v>234</v>
+        <v>138</v>
       </c>
       <c r="C16" s="80"/>
       <c r="D16" s="37" t="s">
-        <v>262</v>
+        <v>166</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>235</v>
+        <v>139</v>
       </c>
       <c r="F16" s="61" t="s">
-        <v>264</v>
+        <v>168</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>265</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="20" customHeight="1">
@@ -8458,7 +8170,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="39" t="s">
-        <v>238</v>
+        <v>142</v>
       </c>
       <c r="D17" s="41">
         <f>COUNTA(Applications!A:A)-1</f>
@@ -8477,7 +8189,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="39" t="s">
-        <v>255</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="20" customHeight="1">
@@ -8486,7 +8198,7 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>239</v>
+        <v>143</v>
       </c>
       <c r="D18" s="43">
         <f>COUNTIFS(Applications!A:A,"&gt;0",Applications!R:R,"Master")</f>
@@ -8499,7 +8211,7 @@
       <c r="F18" s="44"/>
       <c r="G18" s="44"/>
       <c r="I18" t="s">
-        <v>256</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="20" customHeight="1">
@@ -8508,7 +8220,7 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>240</v>
+        <v>144</v>
       </c>
       <c r="D19" s="43">
         <f>IF(ISNUMBER(D17),D17-D18,"")</f>
@@ -8521,13 +8233,13 @@
       <c r="F19" s="44"/>
       <c r="G19" s="44"/>
       <c r="I19" s="58" t="s">
-        <v>257</v>
+        <v>161</v>
       </c>
       <c r="J19" t="s">
-        <v>263</v>
+        <v>167</v>
       </c>
       <c r="K19" t="s">
-        <v>259</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="20" customHeight="1">
@@ -8536,7 +8248,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>241</v>
+        <v>145</v>
       </c>
       <c r="D20" s="41">
         <f>COUNTA(Devices!A:A)-1</f>
@@ -8555,13 +8267,13 @@
         <v>0</v>
       </c>
       <c r="I20" s="59" t="s">
-        <v>258</v>
+        <v>162</v>
       </c>
       <c r="J20" t="s">
-        <v>263</v>
+        <v>167</v>
       </c>
       <c r="K20" t="s">
-        <v>260</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="20" customHeight="1">
@@ -8570,7 +8282,7 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>242</v>
+        <v>146</v>
       </c>
       <c r="D21" s="43">
         <f>COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!H:H,"Server")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!H:H,"Blade")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!H:H,"VM")++COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!H:H,"Appliance")</f>
@@ -8589,7 +8301,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>243</v>
+        <v>147</v>
       </c>
       <c r="D22" s="41">
         <f>COUNTA(Databases!A:A)-1</f>
@@ -8614,7 +8326,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>244</v>
+        <v>148</v>
       </c>
       <c r="D23" s="41">
         <f>COUNTA(Storage!A:A)-1</f>
@@ -8639,7 +8351,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>245</v>
+        <v>149</v>
       </c>
       <c r="D24" s="41">
         <f>COUNTA(Dependencies!A:A)-1</f>
@@ -8664,7 +8376,7 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>246</v>
+        <v>150</v>
       </c>
       <c r="D25" s="38"/>
       <c r="E25" s="38"/>
@@ -8677,7 +8389,7 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>247</v>
+        <v>151</v>
       </c>
       <c r="D26" s="38"/>
       <c r="E26" s="38"/>
@@ -8690,7 +8402,7 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>248</v>
+        <v>152</v>
       </c>
       <c r="D27" s="38"/>
       <c r="E27" s="38"/>
@@ -8703,7 +8415,7 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>249</v>
+        <v>153</v>
       </c>
       <c r="D28" s="38"/>
       <c r="E28" s="38"/>
@@ -8716,7 +8428,7 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>250</v>
+        <v>154</v>
       </c>
       <c r="D29" s="38"/>
       <c r="E29" s="38"/>
@@ -8729,7 +8441,7 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>251</v>
+        <v>155</v>
       </c>
       <c r="D30" s="38"/>
       <c r="E30" s="38"/>
@@ -8742,7 +8454,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>210</v>
+        <v>114</v>
       </c>
       <c r="D31" s="46"/>
       <c r="E31" s="46"/>
@@ -8755,7 +8467,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>252</v>
+        <v>156</v>
       </c>
       <c r="D32" s="46"/>
       <c r="E32" s="46"/>
@@ -8768,7 +8480,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>253</v>
+        <v>157</v>
       </c>
       <c r="D33" s="46"/>
       <c r="E33" s="46"/>
@@ -8781,7 +8493,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>254</v>
+        <v>158</v>
       </c>
       <c r="D34" s="46"/>
       <c r="E34" s="46"/>
@@ -8790,12 +8502,12 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>267</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>266</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="21" customHeight="1"/>
@@ -8865,22 +8577,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="31" t="s">
-        <v>228</v>
+        <v>132</v>
       </c>
       <c r="B1" s="75" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="75" t="s">
-        <v>229</v>
+        <v>133</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>230</v>
+        <v>134</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>231</v>
+        <v>135</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>232</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -8916,19 +8628,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="69" t="s">
-        <v>273</v>
+        <v>177</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>274</v>
+        <v>178</v>
       </c>
       <c r="C1" s="69" t="s">
-        <v>275</v>
+        <v>179</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>276</v>
+        <v>180</v>
       </c>
       <c r="E1" s="69" t="s">
-        <v>277</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -8990,28 +8702,28 @@
   <sheetData>
     <row r="1" spans="1:141" s="17" customFormat="1">
       <c r="A1" s="47" t="s">
-        <v>147</v>
+        <v>51</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>148</v>
+        <v>52</v>
       </c>
       <c r="D1" s="74" t="s">
-        <v>149</v>
+        <v>53</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>150</v>
+        <v>54</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>151</v>
+        <v>55</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>152</v>
+        <v>56</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>153</v>
+        <v>57</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>14</v>
@@ -9020,16 +8732,16 @@
         <v>30</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>154</v>
+        <v>58</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>156</v>
+        <v>60</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="O1" s="16" t="s">
         <v>31</v>
@@ -9038,13 +8750,13 @@
         <v>32</v>
       </c>
       <c r="Q1" s="15" t="s">
-        <v>158</v>
+        <v>62</v>
       </c>
       <c r="R1" s="15" t="s">
         <v>33</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>159</v>
+        <v>63</v>
       </c>
       <c r="T1" s="17" t="s">
         <v>35</v>
@@ -9056,64 +8768,64 @@
         <v>37</v>
       </c>
       <c r="W1" s="54" t="s">
-        <v>160</v>
+        <v>64</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>161</v>
+        <v>65</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>162</v>
+        <v>66</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>163</v>
+        <v>67</v>
       </c>
       <c r="AA1" s="15" t="s">
-        <v>164</v>
+        <v>68</v>
       </c>
       <c r="AB1" s="17" t="s">
-        <v>165</v>
+        <v>69</v>
       </c>
       <c r="AC1" s="17" t="s">
-        <v>166</v>
+        <v>70</v>
       </c>
       <c r="AD1" s="17" t="s">
-        <v>167</v>
+        <v>71</v>
       </c>
       <c r="AE1" s="17" t="s">
-        <v>168</v>
+        <v>72</v>
       </c>
       <c r="AF1" s="17" t="s">
-        <v>169</v>
+        <v>73</v>
       </c>
       <c r="AG1" s="7" t="s">
         <v>43</v>
       </c>
       <c r="AH1" s="8" t="s">
-        <v>170</v>
+        <v>74</v>
       </c>
       <c r="AI1" s="8" t="s">
-        <v>171</v>
+        <v>75</v>
       </c>
       <c r="AJ1" s="55" t="s">
-        <v>172</v>
+        <v>76</v>
       </c>
       <c r="AK1" s="18" t="s">
-        <v>173</v>
+        <v>77</v>
       </c>
       <c r="AL1" s="18" t="s">
-        <v>174</v>
+        <v>78</v>
       </c>
       <c r="AM1" s="55" t="s">
-        <v>175</v>
+        <v>79</v>
       </c>
       <c r="AN1" s="18" t="s">
-        <v>176</v>
+        <v>80</v>
       </c>
       <c r="AO1" s="18" t="s">
-        <v>177</v>
+        <v>81</v>
       </c>
       <c r="AP1" s="55" t="s">
-        <v>178</v>
+        <v>82</v>
       </c>
       <c r="AQ1" s="14" t="s">
         <v>44</v>
@@ -9124,294 +8836,78 @@
       <c r="AS1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AT1" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="AU1" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV1" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AW1" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="AX1" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="AY1" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="AZ1" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="BA1" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="BB1" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC1" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="BD1" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="BE1" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="BF1" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BG1" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="BH1" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="BI1" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="BJ1" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="BK1" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="BL1" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="BM1" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="BN1" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="BO1" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="BP1" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="BQ1" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="BR1" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="BS1" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="BT1" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="BU1" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="BV1" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="BW1" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="BX1" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="BY1" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="BZ1" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="CA1" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="CB1" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="CC1" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="CD1" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="CE1" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="CF1" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="CG1" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="CH1" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="CI1" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="CJ1" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="CK1" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="CL1" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="CM1" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="CN1" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="CO1" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="CP1" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="CQ1" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="CR1" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="CS1" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="CT1" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="CU1" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="CV1" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="CW1" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="CX1" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="CY1" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="CZ1" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="DA1" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="DB1" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="DC1" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="DD1" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="DE1" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="DF1" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="DG1" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="DH1" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="DI1" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="DJ1" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="DK1" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="DL1" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="DM1" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="DN1" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="DO1" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="DP1" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="DQ1" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="DR1" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="DS1" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="DT1" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="DU1" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="DV1" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="DW1" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="DX1" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="DY1" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="DZ1" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="EA1" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="EB1" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="EC1" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="ED1" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="EE1" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="EF1" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="EG1" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="EH1" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="EI1" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="EJ1" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="EK1" s="8" t="s">
-        <v>146</v>
-      </c>
+      <c r="BR1" s="8"/>
+      <c r="BS1" s="8"/>
+      <c r="BT1" s="8"/>
+      <c r="BU1" s="8"/>
+      <c r="BV1" s="8"/>
+      <c r="BW1" s="8"/>
+      <c r="BX1" s="8"/>
+      <c r="BY1" s="8"/>
+      <c r="BZ1" s="8"/>
+      <c r="CA1" s="8"/>
+      <c r="CB1" s="8"/>
+      <c r="CC1" s="8"/>
+      <c r="CD1" s="8"/>
+      <c r="CE1" s="8"/>
+      <c r="CF1" s="8"/>
+      <c r="CG1" s="8"/>
+      <c r="CH1" s="8"/>
+      <c r="CI1" s="8"/>
+      <c r="CJ1" s="8"/>
+      <c r="CK1" s="8"/>
+      <c r="CL1" s="8"/>
+      <c r="CM1" s="8"/>
+      <c r="CN1" s="8"/>
+      <c r="CO1" s="8"/>
+      <c r="CP1" s="8"/>
+      <c r="CQ1" s="8"/>
+      <c r="CR1" s="8"/>
+      <c r="CS1" s="8"/>
+      <c r="CT1" s="8"/>
+      <c r="CU1" s="8"/>
+      <c r="CV1" s="8"/>
+      <c r="CW1" s="8"/>
+      <c r="CX1" s="8"/>
+      <c r="CY1" s="8"/>
+      <c r="CZ1" s="8"/>
+      <c r="DA1" s="8"/>
+      <c r="DB1" s="8"/>
+      <c r="DC1" s="8"/>
+      <c r="DD1" s="8"/>
+      <c r="DE1" s="8"/>
+      <c r="DF1" s="8"/>
+      <c r="DG1" s="8"/>
+      <c r="DH1" s="8"/>
+      <c r="DI1" s="8"/>
+      <c r="DJ1" s="8"/>
+      <c r="DK1" s="8"/>
+      <c r="DL1" s="8"/>
+      <c r="DM1" s="8"/>
+      <c r="DN1" s="8"/>
+      <c r="DO1" s="8"/>
+      <c r="DP1" s="8"/>
+      <c r="DQ1" s="8"/>
+      <c r="DR1" s="8"/>
+      <c r="DS1" s="8"/>
+      <c r="DT1" s="8"/>
+      <c r="DU1" s="8"/>
+      <c r="DV1" s="8"/>
+      <c r="DW1" s="8"/>
+      <c r="DX1" s="8"/>
+      <c r="DY1" s="8"/>
+      <c r="DZ1" s="8"/>
+      <c r="EA1" s="8"/>
+      <c r="EB1" s="8"/>
+      <c r="EC1" s="8"/>
+      <c r="ED1" s="8"/>
+      <c r="EE1" s="8"/>
+      <c r="EF1" s="8"/>
+      <c r="EG1" s="8"/>
+      <c r="EH1" s="8"/>
+      <c r="EI1" s="8"/>
+      <c r="EJ1" s="8"/>
+      <c r="EK1" s="8"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -9435,18 +8931,18 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EK1"/>
+  <dimension ref="A1:DI1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9" style="4" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" style="5" customWidth="1"/>
     <col min="4" max="4" width="13" style="5" customWidth="1"/>
@@ -9492,7 +8988,7 @@
     <col min="142" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:141" s="8" customFormat="1">
+    <row r="1" spans="1:45" s="8" customFormat="1">
       <c r="A1" s="52" t="s">
         <v>6</v>
       </c>
@@ -9627,294 +9123,6 @@
       </c>
       <c r="AS1" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="AT1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="AU1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="AW1" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="AX1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="AY1" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="AZ1" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="BA1" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="BB1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC1" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="BD1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="BE1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="BF1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="BG1" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="BH1" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="BI1" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="BJ1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BK1" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="BL1" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="BM1" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="BN1" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="BO1" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="BP1" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="BQ1" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="BR1" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="BS1" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="BT1" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="BU1" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="BV1" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="BW1" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="BX1" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="BY1" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="BZ1" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="CA1" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="CB1" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="CC1" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="CD1" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="CE1" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="CF1" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="CG1" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="CH1" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="CI1" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="CJ1" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="CK1" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="CL1" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="CM1" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="CN1" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="CO1" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="CP1" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="CQ1" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="CR1" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="CS1" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="CT1" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="CU1" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="CV1" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="CW1" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="CX1" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="CY1" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="CZ1" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="DA1" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="DB1" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="DC1" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="DD1" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="DE1" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="DF1" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="DG1" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="DH1" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="DI1" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="DJ1" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="DK1" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="DL1" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="DM1" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="DN1" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="DO1" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="DP1" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="DQ1" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="DR1" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="DS1" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="DT1" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="DU1" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="DV1" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="DW1" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="DX1" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="DY1" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="DZ1" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="EA1" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="EB1" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="EC1" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="ED1" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="EE1" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="EF1" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="EG1" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="EH1" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="EI1" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="EJ1" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="EK1" s="8" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -9965,13 +9173,13 @@
   <sheetData>
     <row r="1" spans="1:114" s="17" customFormat="1">
       <c r="A1" s="47" t="s">
-        <v>179</v>
+        <v>83</v>
       </c>
       <c r="B1" s="48" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>180</v>
+        <v>84</v>
       </c>
       <c r="D1" s="20" t="s">
         <v>45</v>
@@ -10018,294 +9226,78 @@
       <c r="R1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="T1" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="U1" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="V1" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="W1" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="X1" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y1" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z1" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA1" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB1" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC1" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD1" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE1" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF1" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG1" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH1" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI1" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ1" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK1" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL1" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM1" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN1" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="AO1" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="AP1" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="AQ1" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="AR1" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="AS1" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="AT1" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="AU1" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AV1" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AW1" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AX1" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="AY1" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="AZ1" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="BA1" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="BB1" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="BC1" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="BD1" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE1" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="BF1" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="BG1" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="BH1" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="BI1" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="BJ1" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="BK1" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="BL1" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="BM1" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="BN1" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="BO1" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="BP1" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="BQ1" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="BR1" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="BS1" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="BT1" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="BU1" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="BV1" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="BW1" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="BX1" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="BY1" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="BZ1" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="CA1" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="CB1" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="CC1" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="CD1" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="CE1" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="CF1" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="CG1" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="CH1" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="CI1" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="CJ1" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="CK1" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="CL1" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="CM1" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="CN1" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="CO1" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="CP1" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="CQ1" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="CR1" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="CS1" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="CT1" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="CU1" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="CV1" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="CW1" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="CX1" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="CY1" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="CZ1" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="DA1" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="DB1" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="DC1" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="DD1" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="DE1" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="DF1" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="DG1" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="DH1" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="DI1" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="DJ1" s="8" t="s">
-        <v>146</v>
-      </c>
+      <c r="AQ1" s="8"/>
+      <c r="AR1" s="8"/>
+      <c r="AS1" s="8"/>
+      <c r="AT1" s="8"/>
+      <c r="AU1" s="8"/>
+      <c r="AV1" s="8"/>
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="8"/>
+      <c r="AY1" s="8"/>
+      <c r="AZ1" s="8"/>
+      <c r="BA1" s="8"/>
+      <c r="BB1" s="8"/>
+      <c r="BC1" s="8"/>
+      <c r="BD1" s="8"/>
+      <c r="BE1" s="8"/>
+      <c r="BF1" s="8"/>
+      <c r="BG1" s="8"/>
+      <c r="BH1" s="8"/>
+      <c r="BI1" s="8"/>
+      <c r="BJ1" s="8"/>
+      <c r="BK1" s="8"/>
+      <c r="BL1" s="8"/>
+      <c r="BM1" s="8"/>
+      <c r="BN1" s="8"/>
+      <c r="BO1" s="8"/>
+      <c r="BP1" s="8"/>
+      <c r="BQ1" s="8"/>
+      <c r="BR1" s="8"/>
+      <c r="BS1" s="8"/>
+      <c r="BT1" s="8"/>
+      <c r="BU1" s="8"/>
+      <c r="BV1" s="8"/>
+      <c r="BW1" s="8"/>
+      <c r="BX1" s="8"/>
+      <c r="BY1" s="8"/>
+      <c r="BZ1" s="8"/>
+      <c r="CA1" s="8"/>
+      <c r="CB1" s="8"/>
+      <c r="CC1" s="8"/>
+      <c r="CD1" s="8"/>
+      <c r="CE1" s="8"/>
+      <c r="CF1" s="8"/>
+      <c r="CG1" s="8"/>
+      <c r="CH1" s="8"/>
+      <c r="CI1" s="8"/>
+      <c r="CJ1" s="8"/>
+      <c r="CK1" s="8"/>
+      <c r="CL1" s="8"/>
+      <c r="CM1" s="8"/>
+      <c r="CN1" s="8"/>
+      <c r="CO1" s="8"/>
+      <c r="CP1" s="8"/>
+      <c r="CQ1" s="8"/>
+      <c r="CR1" s="8"/>
+      <c r="CS1" s="8"/>
+      <c r="CT1" s="8"/>
+      <c r="CU1" s="8"/>
+      <c r="CV1" s="8"/>
+      <c r="CW1" s="8"/>
+      <c r="CX1" s="8"/>
+      <c r="CY1" s="8"/>
+      <c r="CZ1" s="8"/>
+      <c r="DA1" s="8"/>
+      <c r="DB1" s="8"/>
+      <c r="DC1" s="8"/>
+      <c r="DD1" s="8"/>
+      <c r="DE1" s="8"/>
+      <c r="DF1" s="8"/>
+      <c r="DG1" s="8"/>
+      <c r="DH1" s="8"/>
+      <c r="DI1" s="8"/>
+      <c r="DJ1" s="8"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -10357,13 +9349,13 @@
   <sheetData>
     <row r="1" spans="1:115" s="17" customFormat="1">
       <c r="A1" s="47" t="s">
-        <v>181</v>
+        <v>85</v>
       </c>
       <c r="B1" s="48" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>180</v>
+        <v>84</v>
       </c>
       <c r="D1" s="20" t="s">
         <v>45</v>
@@ -10378,7 +9370,7 @@
         <v>14</v>
       </c>
       <c r="H1" s="60" t="s">
-        <v>261</v>
+        <v>165</v>
       </c>
       <c r="I1" s="19" t="s">
         <v>30</v>
@@ -10413,294 +9405,102 @@
       <c r="S1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="T1" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="U1" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="V1" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="W1" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="X1" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y1" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z1" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA1" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB1" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC1" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD1" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE1" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF1" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG1" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="AH1" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="AI1" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ1" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="AK1" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="AL1" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="AM1" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="AN1" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="AO1" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="AP1" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ1" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="AR1" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="AS1" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="AT1" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="AU1" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="AV1" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AW1" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AX1" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AY1" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="AZ1" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="BA1" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="BB1" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="BC1" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="BD1" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="BE1" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="BF1" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="BG1" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="BH1" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="BI1" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="BJ1" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="BK1" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="BL1" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="BM1" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="BN1" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="BO1" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="BP1" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="BQ1" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="BR1" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="BS1" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="BT1" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="BU1" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="BV1" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="BW1" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="BX1" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="BY1" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="BZ1" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="CA1" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="CB1" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="CC1" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="CD1" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="CE1" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="CF1" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="CG1" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="CH1" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="CI1" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="CJ1" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="CK1" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="CL1" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="CM1" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="CN1" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="CO1" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="CP1" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="CQ1" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="CR1" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="CS1" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="CT1" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="CU1" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="CV1" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="CW1" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="CX1" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="CY1" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="CZ1" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="DA1" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="DB1" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="DC1" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="DD1" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="DE1" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="DF1" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="DG1" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="DH1" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="DI1" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="DJ1" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="DK1" s="8" t="s">
-        <v>146</v>
-      </c>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="19"/>
+      <c r="AI1" s="19"/>
+      <c r="AJ1" s="19"/>
+      <c r="AK1" s="19"/>
+      <c r="AL1" s="19"/>
+      <c r="AM1" s="19"/>
+      <c r="AN1" s="19"/>
+      <c r="AO1" s="19"/>
+      <c r="AP1" s="19"/>
+      <c r="AQ1" s="19"/>
+      <c r="AR1" s="8"/>
+      <c r="AS1" s="8"/>
+      <c r="AT1" s="8"/>
+      <c r="AU1" s="8"/>
+      <c r="AV1" s="8"/>
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="8"/>
+      <c r="AY1" s="8"/>
+      <c r="AZ1" s="8"/>
+      <c r="BA1" s="8"/>
+      <c r="BB1" s="8"/>
+      <c r="BC1" s="8"/>
+      <c r="BD1" s="8"/>
+      <c r="BE1" s="8"/>
+      <c r="BF1" s="8"/>
+      <c r="BG1" s="8"/>
+      <c r="BH1" s="8"/>
+      <c r="BI1" s="8"/>
+      <c r="BJ1" s="8"/>
+      <c r="BK1" s="8"/>
+      <c r="BL1" s="8"/>
+      <c r="BM1" s="8"/>
+      <c r="BN1" s="8"/>
+      <c r="BO1" s="8"/>
+      <c r="BP1" s="8"/>
+      <c r="BQ1" s="8"/>
+      <c r="BR1" s="8"/>
+      <c r="BS1" s="8"/>
+      <c r="BT1" s="8"/>
+      <c r="BU1" s="8"/>
+      <c r="BV1" s="8"/>
+      <c r="BW1" s="8"/>
+      <c r="BX1" s="8"/>
+      <c r="BY1" s="8"/>
+      <c r="BZ1" s="8"/>
+      <c r="CA1" s="8"/>
+      <c r="CB1" s="8"/>
+      <c r="CC1" s="8"/>
+      <c r="CD1" s="8"/>
+      <c r="CE1" s="8"/>
+      <c r="CF1" s="8"/>
+      <c r="CG1" s="8"/>
+      <c r="CH1" s="8"/>
+      <c r="CI1" s="8"/>
+      <c r="CJ1" s="8"/>
+      <c r="CK1" s="8"/>
+      <c r="CL1" s="8"/>
+      <c r="CM1" s="8"/>
+      <c r="CN1" s="8"/>
+      <c r="CO1" s="8"/>
+      <c r="CP1" s="8"/>
+      <c r="CQ1" s="8"/>
+      <c r="CR1" s="8"/>
+      <c r="CS1" s="8"/>
+      <c r="CT1" s="8"/>
+      <c r="CU1" s="8"/>
+      <c r="CV1" s="8"/>
+      <c r="CW1" s="8"/>
+      <c r="CX1" s="8"/>
+      <c r="CY1" s="8"/>
+      <c r="CZ1" s="8"/>
+      <c r="DA1" s="8"/>
+      <c r="DB1" s="8"/>
+      <c r="DC1" s="8"/>
+      <c r="DD1" s="8"/>
+      <c r="DE1" s="8"/>
+      <c r="DF1" s="8"/>
+      <c r="DG1" s="8"/>
+      <c r="DH1" s="8"/>
+      <c r="DI1" s="8"/>
+      <c r="DJ1" s="8"/>
+      <c r="DK1" s="8"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -10741,52 +9541,52 @@
   <sheetData>
     <row r="1" spans="1:16" s="26" customFormat="1">
       <c r="A1" s="23" t="s">
-        <v>182</v>
+        <v>86</v>
       </c>
       <c r="B1" s="76" t="s">
-        <v>183</v>
+        <v>87</v>
       </c>
       <c r="C1" s="76" t="s">
-        <v>184</v>
+        <v>88</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>185</v>
+        <v>89</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>186</v>
+        <v>90</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>187</v>
+        <v>91</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>188</v>
+        <v>92</v>
       </c>
       <c r="H1" s="24" t="s">
         <v>13</v>
       </c>
       <c r="I1" s="77" t="s">
-        <v>189</v>
+        <v>93</v>
       </c>
       <c r="J1" s="77" t="s">
-        <v>190</v>
+        <v>94</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>191</v>
+        <v>95</v>
       </c>
       <c r="L1" s="26" t="s">
-        <v>192</v>
+        <v>96</v>
       </c>
       <c r="M1" s="26" t="s">
-        <v>193</v>
+        <v>97</v>
       </c>
       <c r="N1" s="26" t="s">
-        <v>194</v>
+        <v>98</v>
       </c>
       <c r="O1" s="26" t="s">
-        <v>195</v>
+        <v>99</v>
       </c>
       <c r="P1" s="26" t="s">
-        <v>196</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -10831,43 +9631,43 @@
   <sheetData>
     <row r="1" spans="1:13" s="29" customFormat="1">
       <c r="A1" s="23" t="s">
-        <v>197</v>
+        <v>101</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>198</v>
+        <v>102</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>199</v>
+        <v>103</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>200</v>
+        <v>104</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>152</v>
+        <v>56</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>201</v>
+        <v>105</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>202</v>
+        <v>106</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>203</v>
+        <v>107</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>204</v>
+        <v>108</v>
       </c>
       <c r="K1" s="51" t="s">
-        <v>205</v>
+        <v>109</v>
       </c>
       <c r="L1" s="49" t="s">
-        <v>206</v>
+        <v>110</v>
       </c>
       <c r="M1" s="49" t="s">
-        <v>207</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -10914,43 +9714,43 @@
   <sheetData>
     <row r="1" spans="1:13" s="28" customFormat="1">
       <c r="A1" s="10" t="s">
-        <v>208</v>
+        <v>112</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>209</v>
+        <v>113</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>198</v>
+        <v>102</v>
       </c>
       <c r="D1" s="28" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>210</v>
+        <v>114</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>152</v>
+        <v>56</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>211</v>
+        <v>115</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>212</v>
+        <v>116</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>213</v>
+        <v>117</v>
       </c>
       <c r="J1" s="30" t="s">
-        <v>214</v>
+        <v>118</v>
       </c>
       <c r="K1" s="30" t="s">
-        <v>215</v>
+        <v>119</v>
       </c>
       <c r="L1" s="28" t="s">
         <v>13</v>
       </c>
       <c r="M1" s="28" t="s">
-        <v>216</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -10997,56 +9797,56 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="B1" s="82" t="s">
-        <v>217</v>
+        <v>121</v>
       </c>
       <c r="C1" s="83"/>
       <c r="D1" s="84"/>
       <c r="E1" s="83" t="s">
-        <v>218</v>
+        <v>122</v>
       </c>
       <c r="F1" s="83"/>
       <c r="G1" s="83"/>
       <c r="H1" s="66"/>
       <c r="J1" s="5" t="s">
-        <v>270</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="63" customFormat="1">
       <c r="A2" s="78" t="s">
-        <v>219</v>
+        <v>123</v>
       </c>
       <c r="B2" s="79" t="s">
-        <v>220</v>
+        <v>124</v>
       </c>
       <c r="C2" s="78" t="s">
-        <v>221</v>
+        <v>125</v>
       </c>
       <c r="D2" s="78" t="s">
-        <v>222</v>
+        <v>126</v>
       </c>
       <c r="E2" s="64" t="s">
-        <v>220</v>
+        <v>124</v>
       </c>
       <c r="F2" s="62" t="s">
-        <v>221</v>
+        <v>125</v>
       </c>
       <c r="G2" s="62" t="s">
-        <v>222</v>
+        <v>126</v>
       </c>
       <c r="H2" s="64" t="s">
-        <v>223</v>
+        <v>127</v>
       </c>
       <c r="I2" s="62" t="s">
-        <v>224</v>
+        <v>128</v>
       </c>
       <c r="J2" s="62" t="s">
-        <v>225</v>
+        <v>129</v>
       </c>
       <c r="K2" s="62" t="s">
-        <v>226</v>
+        <v>130</v>
       </c>
       <c r="L2" s="62" t="s">
-        <v>227</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TM-6688 Changed the headings to the Asset tabs to match the Field Spec Labels. Updated the CSV and regenerated the combined.json.
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15540" tabRatio="782"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="26340" windowHeight="14400" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,15 @@
     <sheet name="Validation" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Applications!$A$1:$EK$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Applications!$A$1:$EH$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Cabling!$A$2:$L$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Comments!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Databases!$A$1:$DJ$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Databases!$A$1:$DI$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Dependencies!$A$1:$P$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Devices!$A$1:$EK$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Devices!$A$1:$EJ$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Rack!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Room!$A$1:$M$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Storage!$A$1:$DK$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Storage!$A$1:$DH$1</definedName>
     <definedName name="_xlfn_COUNTIFS">#N/A</definedName>
     <definedName name="CustomerName">Title!$B$3</definedName>
     <definedName name="ExportDatetime">Title!$B$8</definedName>
@@ -56,21 +56,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="8"/>
-            <rFont val="Times New Roman"/>
-            <family val="1"/>
-          </rPr>
-          <t>The source location/datacenter where the asset will be moved from</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -98,40 +84,30 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="8"/>
-            <rFont val="Times New Roman"/>
-            <family val="1"/>
-          </rPr>
-          <t>The U position that the asset is located at in rack before the move.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="8"/>
-            <rFont val="Verdana"/>
-            <family val="2"/>
-          </rPr>
-          <t>Position in the cabinet U1 is on the bottom</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="fieldSettingsDefines.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:data:dev:src:tdstm:misc:fieldSettingsDefines.csv" comma="1">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="179">
   <si>
     <t>Customer:</t>
   </si>
@@ -157,15 +133,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>ShortName</t>
-  </si>
-  <si>
-    <t>S/N</t>
-  </si>
-  <si>
-    <t>AssetTag</t>
-  </si>
-  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -178,60 +145,18 @@
     <t>Description</t>
   </si>
   <si>
-    <t>IP</t>
-  </si>
-  <si>
     <t>OS</t>
   </si>
   <si>
-    <t>SourceLoc</t>
-  </si>
-  <si>
-    <t>SourceRoom</t>
-  </si>
-  <si>
-    <t>SourceRack</t>
-  </si>
-  <si>
-    <t>SourcePos</t>
-  </si>
-  <si>
-    <t>Source Blade</t>
-  </si>
-  <si>
     <t>Source Blade Position</t>
   </si>
   <si>
-    <t>VirtualHost</t>
-  </si>
-  <si>
-    <t>TargetLoc</t>
-  </si>
-  <si>
-    <t>TargetRoom</t>
-  </si>
-  <si>
-    <t>TargetRack</t>
-  </si>
-  <si>
-    <t>TargetPos</t>
-  </si>
-  <si>
-    <t>Target Blade</t>
-  </si>
-  <si>
     <t>Target Blade Position</t>
   </si>
   <si>
     <t>SupportType</t>
   </si>
   <si>
-    <t>Retire</t>
-  </si>
-  <si>
-    <t>MaintExp</t>
-  </si>
-  <si>
     <t>Environment</t>
   </si>
   <si>
@@ -241,12 +166,6 @@
     <t>Validation</t>
   </si>
   <si>
-    <t>MoveBundle</t>
-  </si>
-  <si>
-    <t>PlanStatus</t>
-  </si>
-  <si>
     <t>Truck</t>
   </si>
   <si>
@@ -256,18 +175,9 @@
     <t>Shelf</t>
   </si>
   <si>
-    <t>RailType</t>
-  </si>
-  <si>
-    <t>usize</t>
-  </si>
-  <si>
     <t>DepGroup</t>
   </si>
   <si>
-    <t>ExternalRefId</t>
-  </si>
-  <si>
     <t>Size</t>
   </si>
   <si>
@@ -283,9 +193,6 @@
     <t>Modified Date</t>
   </si>
   <si>
-    <t>Modified By</t>
-  </si>
-  <si>
     <t>appId</t>
   </si>
   <si>
@@ -298,88 +205,19 @@
     <t>Technology</t>
   </si>
   <si>
-    <t>AccessType</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
     <t>License</t>
   </si>
   <si>
-    <t>SME</t>
-  </si>
-  <si>
     <t>SME2</t>
   </si>
   <si>
-    <t>BusinessUnit</t>
-  </si>
-  <si>
-    <t>AppOwner</t>
-  </si>
-  <si>
     <t>Function</t>
   </si>
   <si>
     <t>Criticality</t>
-  </si>
-  <si>
-    <t>TotalUsers</t>
-  </si>
-  <si>
-    <t>UserLocations</t>
-  </si>
-  <si>
-    <t>Frequency</t>
-  </si>
-  <si>
-    <t>RPO</t>
-  </si>
-  <si>
-    <t>RTO</t>
-  </si>
-  <si>
-    <t>DowntimeTolerance</t>
-  </si>
-  <si>
-    <t>Latency</t>
-  </si>
-  <si>
-    <t>TestProc</t>
-  </si>
-  <si>
-    <t>StartupProc</t>
-  </si>
-  <si>
-    <t>Url</t>
-  </si>
-  <si>
-    <t>ShutdownBy</t>
-  </si>
-  <si>
-    <t>ShutdownFixed</t>
-  </si>
-  <si>
-    <t>ShutdownDuration</t>
-  </si>
-  <si>
-    <t>StartupBy</t>
-  </si>
-  <si>
-    <t>StartupFixed</t>
-  </si>
-  <si>
-    <t>StartupDuration</t>
-  </si>
-  <si>
-    <t>TestingBy</t>
-  </si>
-  <si>
-    <t>TestingFixed</t>
-  </si>
-  <si>
-    <t>TestingDuration</t>
   </si>
   <si>
     <t>dbId</t>
@@ -678,6 +516,135 @@
   </si>
   <si>
     <t>Dep Status</t>
+  </si>
+  <si>
+    <t>Asset Tag</t>
+  </si>
+  <si>
+    <t>External Ref Id</t>
+  </si>
+  <si>
+    <t>Maint Expiration</t>
+  </si>
+  <si>
+    <t>Rail Type</t>
+  </si>
+  <si>
+    <t>Retire Date</t>
+  </si>
+  <si>
+    <t>Serial #</t>
+  </si>
+  <si>
+    <t>Alternate Name</t>
+  </si>
+  <si>
+    <t>Source Location</t>
+  </si>
+  <si>
+    <t>Source Position</t>
+  </si>
+  <si>
+    <t>Source Room</t>
+  </si>
+  <si>
+    <t>Target Location</t>
+  </si>
+  <si>
+    <t>Target Position</t>
+  </si>
+  <si>
+    <t>Target Room</t>
+  </si>
+  <si>
+    <t>Usize</t>
+  </si>
+  <si>
+    <t>App Owner</t>
+  </si>
+  <si>
+    <t>Business Unit</t>
+  </si>
+  <si>
+    <t>DR RPO</t>
+  </si>
+  <si>
+    <t>DR RTO</t>
+  </si>
+  <si>
+    <t>Latency OK</t>
+  </si>
+  <si>
+    <t>Bundle</t>
+  </si>
+  <si>
+    <t>Shutdown By</t>
+  </si>
+  <si>
+    <t>Shutdown Duration</t>
+  </si>
+  <si>
+    <t>Shutdown Fixed</t>
+  </si>
+  <si>
+    <t>SME1</t>
+  </si>
+  <si>
+    <t>Startup By</t>
+  </si>
+  <si>
+    <t>Startup Duration</t>
+  </si>
+  <si>
+    <t>Startup Fixed</t>
+  </si>
+  <si>
+    <t>Startup Proc OK</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Testing By</t>
+  </si>
+  <si>
+    <t>Testing Duration</t>
+  </si>
+  <si>
+    <t>Testing Fixed</t>
+  </si>
+  <si>
+    <t>Test Proc OK</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Use Frequency</t>
+  </si>
+  <si>
+    <t>Source Chassis</t>
+  </si>
+  <si>
+    <t>Target Chassis</t>
+  </si>
+  <si>
+    <t>Device Type</t>
+  </si>
+  <si>
+    <t>IP Address</t>
+  </si>
+  <si>
+    <t>Target Rack</t>
+  </si>
+  <si>
+    <t>Source Rack</t>
+  </si>
+  <si>
+    <t>User Count</t>
+  </si>
+  <si>
+    <t>User Locations</t>
   </si>
 </sst>
 </file>
@@ -690,7 +657,7 @@
     <numFmt numFmtId="166" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -806,13 +773,6 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
@@ -840,6 +800,26 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -979,7 +959,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1540">
+  <cellStyleXfs count="1694">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -4796,59 +4776,59 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -4857,28 +4837,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
@@ -5007,7 +4987,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -5842,8 +5822,162 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -5853,14 +5987,11 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -5884,50 +6015,48 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5944,7 +6073,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1539" applyFont="1" applyAlignment="1">
@@ -5954,10 +6083,9 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5967,7 +6095,7 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5979,8 +6107,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1540">
+  <cellStyles count="1694">
     <cellStyle name="_JDI DCM Runbook Hour by Hour EMA Comm Systems (Bundle 2) 11-JUL-07" xfId="1"/>
     <cellStyle name="_JDI DCM Runbook Hour by Hour EMA Comm Systems (Bundle 2) 11-JUL-07_Title" xfId="2"/>
     <cellStyle name="_Momentive Migration Runbook Move Event 2B 09-08-2007 v2 31" xfId="3"/>
@@ -6186,6 +6325,160 @@
     <cellStyle name="EMC Table Text Example" xfId="203"/>
     <cellStyle name="EMC Table Text_Title" xfId="204"/>
     <cellStyle name="EMC Title" xfId="205"/>
+    <cellStyle name="Followed Hyperlink" xfId="1541" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1543" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1545" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1547" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1549" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1551" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1553" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1555" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1557" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1559" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1561" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1563" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1565" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1567" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1569" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1571" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1573" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1575" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1577" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1579" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1581" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1583" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1585" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1587" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1589" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1591" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1593" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1595" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1597" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1599" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1601" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1603" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1605" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1607" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1609" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1611" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1613" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1615" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1617" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1619" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1621" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1623" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1625" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1627" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1629" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1631" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1633" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1635" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1637" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1639" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1641" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1643" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1645" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1647" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1649" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1651" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1653" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1655" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1657" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1659" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1661" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1663" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1665" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1667" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1669" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1671" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1673" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1675" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1677" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1679" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1681" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1683" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1685" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1687" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1689" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1691" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1693" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1540" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1542" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1544" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1546" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1548" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1550" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1552" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1554" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1556" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1558" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1560" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1562" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1564" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1566" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1568" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1570" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1574" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1576" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1578" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1580" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1582" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1584" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1586" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1588" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1590" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1592" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1600" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1602" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1604" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1606" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1608" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1610" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1612" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1614" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1616" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1618" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1620" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1622" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1624" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1626" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1628" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1630" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1632" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1634" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1636" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1638" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1640" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1642" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1644" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1646" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1648" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1650" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1652" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1654" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1656" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1658" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1660" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1662" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1664" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1666" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1668" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1670" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1672" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1674" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1676" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1678" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1680" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1682" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1684" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1686" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1688" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1690" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1692" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 10" xfId="206"/>
     <cellStyle name="Hyperlink 11" xfId="207"/>
     <cellStyle name="Hyperlink 12" xfId="208"/>
@@ -8037,74 +8330,74 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="63" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="63" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="63" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="63" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="63" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="30">
         <v>38295</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="68" t="s">
-        <v>175</v>
+      <c r="A9" s="63" t="s">
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="68" t="s">
-        <v>176</v>
+      <c r="A10" s="63" t="s">
+        <v>130</v>
       </c>
       <c r="B10" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -8112,84 +8405,84 @@
     </row>
     <row r="12" spans="1:7">
       <c r="B12" t="s">
-        <v>140</v>
-      </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
+        <v>94</v>
+      </c>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
-        <v>173</v>
-      </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
+        <v>127</v>
+      </c>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="81" t="s">
-        <v>137</v>
-      </c>
-      <c r="G15" s="81"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="75" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="75"/>
     </row>
     <row r="16" spans="1:7" ht="28" customHeight="1">
-      <c r="A16" s="36"/>
-      <c r="B16" s="80" t="s">
-        <v>138</v>
-      </c>
-      <c r="C16" s="80"/>
-      <c r="D16" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="F16" s="61" t="s">
-        <v>168</v>
-      </c>
-      <c r="G16" s="37" t="s">
-        <v>169</v>
+      <c r="A16" s="33"/>
+      <c r="B16" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="74"/>
+      <c r="D16" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="20" customHeight="1">
-      <c r="A17" s="39">
+      <c r="A17" s="36">
         <f>COUNTA(Applications!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B17" s="39" t="s">
-        <v>142</v>
-      </c>
-      <c r="D17" s="41">
+      <c r="B17" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="38">
         <f>COUNTA(Applications!A:A)-1</f>
         <v>0</v>
       </c>
-      <c r="E17" s="41">
+      <c r="E17" s="38">
         <f>A17-D17</f>
         <v>0</v>
       </c>
-      <c r="F17" s="42">
-        <f>COUNTIF(Applications!B:EK,REPT("?",254)&amp;"*")</f>
+      <c r="F17" s="39">
+        <f>COUNTIF(Applications!B:EH,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="G17" s="42">
-        <f>COUNTIF(Applications!B:EL,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Applications!B:EL,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Applications!B:EL,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Applications!B:EL,"*"&amp;CHAR(39)&amp;"*")</f>
+      <c r="G17" s="39">
+        <f>COUNTIF(Applications!B:EI,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Applications!B:EI,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Applications!B:EI,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Applications!B:EI,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="I17" s="39" t="s">
-        <v>159</v>
+      <c r="I17" s="36" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="20" customHeight="1">
@@ -8198,20 +8491,20 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>143</v>
-      </c>
-      <c r="D18" s="43">
+        <v>97</v>
+      </c>
+      <c r="D18" s="40">
         <f>COUNTIFS(Applications!A:A,"&gt;0",Applications!R:R,"Master")</f>
         <v>0</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="40">
         <f>COUNTIFS(Applications!B:B,"&lt;&gt;''",Applications!R:R,"Master")-D18</f>
         <v>0</v>
       </c>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
       <c r="I18" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="20" customHeight="1">
@@ -8220,152 +8513,152 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
-      </c>
-      <c r="D19" s="43">
+        <v>98</v>
+      </c>
+      <c r="D19" s="40">
         <f>IF(ISNUMBER(D17),D17-D18,"")</f>
         <v>0</v>
       </c>
-      <c r="E19" s="43">
+      <c r="E19" s="40">
         <f>IF(ISNUMBER(E17),E17-E18,"")</f>
         <v>0</v>
       </c>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="I19" s="58" t="s">
-        <v>161</v>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="I19" s="53" t="s">
+        <v>115</v>
       </c>
       <c r="J19" t="s">
-        <v>167</v>
+        <v>121</v>
       </c>
       <c r="K19" t="s">
-        <v>163</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="20" customHeight="1">
-      <c r="A20" s="39">
+      <c r="A20" s="36">
         <f>COUNTA(Devices!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B20" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="D20" s="41">
+      <c r="B20" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="38">
         <f>COUNTA(Devices!A:A)-1</f>
         <v>0</v>
       </c>
-      <c r="E20" s="41">
+      <c r="E20" s="38">
         <f>A20-D20</f>
         <v>0</v>
       </c>
-      <c r="F20" s="42">
-        <f>COUNTIF(Devices!B:EK,REPT("?",254)&amp;"*")</f>
+      <c r="F20" s="39">
+        <f>COUNTIF(Devices!B:EJ,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="G20" s="42">
-        <f>COUNTIF(Devices!B:EL,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Devices!B:EL,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Devices!B:EL,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Devices!B:EL,"*"&amp;CHAR(39)&amp;"*")</f>
+      <c r="G20" s="39">
+        <f>COUNTIF(Devices!B:EK,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Devices!B:EK,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Devices!B:EK,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Devices!B:EK,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="I20" s="59" t="s">
-        <v>162</v>
+      <c r="I20" s="54" t="s">
+        <v>116</v>
       </c>
       <c r="J20" t="s">
-        <v>167</v>
+        <v>121</v>
       </c>
       <c r="K20" t="s">
-        <v>164</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="20" customHeight="1">
       <c r="A21">
-        <f>COUNTIF(Devices!H:H,"Server")+COUNTIF(Devices!H:H,"VM")+COUNTIF(Devices!H:H,"Blade")+COUNTIF(Devices!H:H,"Appliance")</f>
+        <f>COUNTIF(Devices!J:J,"Server")+COUNTIF(Devices!J:J,"VM")+COUNTIF(Devices!J:J,"Blade")+COUNTIF(Devices!J:J,"Appliance")</f>
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>146</v>
-      </c>
-      <c r="D21" s="43">
-        <f>COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!H:H,"Server")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!H:H,"Blade")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!H:H,"VM")++COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!H:H,"Appliance")</f>
+        <v>100</v>
+      </c>
+      <c r="D21" s="40">
+        <f>COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!J:J,"Server")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!J:J,"Blade")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!J:J,"VM")++COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!J:J,"Appliance")</f>
         <v>0</v>
       </c>
-      <c r="E21" s="43">
-        <f>COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!H:H,"Server")+COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!H:H,"Blade")+COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!H:H,"VM")++COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!H:H,"Appliance")</f>
+      <c r="E21" s="40">
+        <f>COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!J:J,"Server")+COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!J:J,"Blade")+COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!J:J,"VM")++COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!J:J,"Appliance")</f>
         <v>0</v>
       </c>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
     </row>
     <row r="22" spans="1:11" ht="20" customHeight="1">
-      <c r="A22" s="39">
+      <c r="A22" s="36">
         <f>COUNTA(Databases!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B22" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="D22" s="41">
+      <c r="B22" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="38">
         <f>COUNTA(Databases!A:A)-1</f>
         <v>0</v>
       </c>
-      <c r="E22" s="41">
+      <c r="E22" s="38">
         <f>A22-D22</f>
         <v>0</v>
       </c>
-      <c r="F22" s="42">
-        <f>COUNTIF(Databases!B:EK,REPT("?",254)&amp;"*")</f>
+      <c r="F22" s="39">
+        <f>COUNTIF(Databases!B:EJ,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="G22" s="42">
-        <f>COUNTIF(Databases!B:EL,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Databases!B:EL,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Databases!B:EL,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Databases!B:EL,"*"&amp;CHAR(39)&amp;"*")</f>
+      <c r="G22" s="39">
+        <f>COUNTIF(Databases!B:EK,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Databases!B:EK,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Databases!B:EK,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Databases!B:EK,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="20" customHeight="1">
-      <c r="A23" s="39">
+      <c r="A23" s="36">
         <f>COUNTA(Storage!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B23" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="D23" s="41">
+      <c r="B23" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="38">
         <f>COUNTA(Storage!A:A)-1</f>
         <v>0</v>
       </c>
-      <c r="E23" s="41">
+      <c r="E23" s="38">
         <f>A23-D23</f>
         <v>0</v>
       </c>
-      <c r="F23" s="42">
-        <f>COUNTIF(Storage!B:EL,REPT("?",254)&amp;"*")</f>
+      <c r="F23" s="39">
+        <f>COUNTIF(Storage!B:EI,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="G23" s="42">
-        <f>COUNTIF(Storage!B:EM,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Storage!B:EM,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Storage!B:EM,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Storage!B:EM,"*"&amp;CHAR(39)&amp;"*")</f>
+      <c r="G23" s="39">
+        <f>COUNTIF(Storage!B:EJ,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Storage!B:EJ,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Storage!B:EJ,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Storage!B:EJ,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="20" customHeight="1">
-      <c r="A24" s="39">
+      <c r="A24" s="36">
         <f>COUNTA(Dependencies!D:D)-1</f>
         <v>0</v>
       </c>
-      <c r="B24" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="D24" s="41">
+      <c r="B24" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="38">
         <f>COUNTA(Dependencies!A:A)-1</f>
         <v>0</v>
       </c>
-      <c r="E24" s="41">
+      <c r="E24" s="38">
         <f>A24-D24</f>
         <v>0</v>
       </c>
-      <c r="F24" s="42">
-        <f>COUNTIF(Storage!B:EL,REPT("?",254)&amp;"*")</f>
+      <c r="F24" s="39">
+        <f>COUNTIF(Storage!B:EI,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="G24" s="45">
+      <c r="G24" s="42">
         <f>COUNTIF(Dependencies!B:EL,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Dependencies!B:EL,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Dependencies!B:EL,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Dependencies!B:EL,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
@@ -8376,12 +8669,12 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>150</v>
-      </c>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
+        <v>104</v>
+      </c>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
     </row>
     <row r="26" spans="1:11" ht="20" customHeight="1">
       <c r="A26">
@@ -8389,12 +8682,12 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>151</v>
-      </c>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
+        <v>105</v>
+      </c>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
     </row>
     <row r="27" spans="1:11" ht="20" customHeight="1">
       <c r="A27">
@@ -8402,12 +8695,12 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>152</v>
-      </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
+        <v>106</v>
+      </c>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
     </row>
     <row r="28" spans="1:11" ht="20" customHeight="1">
       <c r="A28">
@@ -8415,12 +8708,12 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>153</v>
-      </c>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
+        <v>107</v>
+      </c>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
     </row>
     <row r="29" spans="1:11" ht="20" customHeight="1">
       <c r="A29">
@@ -8428,12 +8721,12 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>154</v>
-      </c>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
+        <v>108</v>
+      </c>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
     </row>
     <row r="30" spans="1:11" ht="20" customHeight="1">
       <c r="A30">
@@ -8441,73 +8734,73 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>155</v>
-      </c>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
+        <v>109</v>
+      </c>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
     </row>
     <row r="31" spans="1:11" ht="20" customHeight="1">
-      <c r="A31" s="39">
+      <c r="A31" s="36">
         <f>COUNTA(Room!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B31" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
+      <c r="B31" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
     </row>
     <row r="32" spans="1:11" ht="20" customHeight="1">
-      <c r="A32" s="39">
+      <c r="A32" s="36">
         <f>COUNTA(Rack!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B32" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
+      <c r="B32" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
     </row>
     <row r="33" spans="1:7" ht="20" customHeight="1">
-      <c r="A33" s="39">
+      <c r="A33" s="36">
         <f>COUNTA(Cabling!B:B)-2</f>
         <v>0</v>
       </c>
-      <c r="B33" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="46"/>
+      <c r="B33" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
     </row>
     <row r="34" spans="1:7" ht="20" customHeight="1">
-      <c r="A34" s="40">
+      <c r="A34" s="37">
         <f>COUNTA(Comments!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B34" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
+      <c r="B34" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>171</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="21" customHeight="1"/>
@@ -8566,33 +8859,33 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="16" style="11" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="9.5703125" style="22"/>
+    <col min="1" max="1" width="16.5703125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="16" style="10" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" style="19" customWidth="1"/>
+    <col min="7" max="16384" width="9.5703125" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="75" t="s">
+      <c r="A1" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="75" t="s">
-        <v>133</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>136</v>
+      <c r="C1" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -8622,25 +8915,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="5" width="19.42578125" style="70" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="70"/>
+    <col min="1" max="5" width="19.42578125" style="65" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="65"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="69" t="s">
-        <v>177</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>178</v>
-      </c>
-      <c r="C1" s="69" t="s">
-        <v>179</v>
-      </c>
-      <c r="D1" s="69" t="s">
-        <v>180</v>
-      </c>
-      <c r="E1" s="69" t="s">
-        <v>181</v>
+      <c r="A1" s="64" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="64" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="64" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="64" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="64" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -8661,7 +8954,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EK1"/>
+  <dimension ref="A1:EH1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -8672,170 +8965,169 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="11"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="2"/>
-    <col min="15" max="15" width="9.5703125" style="12"/>
-    <col min="16" max="16" width="11.85546875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="10" customWidth="1"/>
+    <col min="2" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="2"/>
+    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" style="11" customWidth="1"/>
     <col min="20" max="20" width="11.140625" customWidth="1"/>
-    <col min="23" max="23" width="9.5703125" style="11"/>
-    <col min="28" max="28" width="17.42578125" customWidth="1"/>
-    <col min="33" max="33" width="9.85546875" style="11" customWidth="1"/>
-    <col min="34" max="34" width="11.42578125" customWidth="1"/>
-    <col min="35" max="35" width="13.42578125" customWidth="1"/>
-    <col min="36" max="36" width="16.140625" style="11" customWidth="1"/>
-    <col min="37" max="37" width="9.42578125" customWidth="1"/>
-    <col min="38" max="38" width="11.42578125" customWidth="1"/>
-    <col min="39" max="39" width="13.42578125" style="11" customWidth="1"/>
-    <col min="40" max="40" width="8.5703125" customWidth="1"/>
-    <col min="41" max="41" width="10.42578125" customWidth="1"/>
-    <col min="42" max="42" width="13.42578125" style="56" customWidth="1"/>
-    <col min="43" max="43" width="11.85546875" style="11" customWidth="1"/>
-    <col min="44" max="44" width="12.140625" style="72" customWidth="1"/>
-    <col min="45" max="45" width="11.140625" customWidth="1"/>
-    <col min="46" max="73" width="9.5703125" customWidth="1"/>
-    <col min="74" max="74" width="9.5703125" style="13" customWidth="1"/>
-    <col min="75" max="109" width="9.5703125" customWidth="1"/>
-    <col min="110" max="110" width="9.5703125" style="13" customWidth="1"/>
-    <col min="111" max="141" width="9.5703125" customWidth="1"/>
+    <col min="22" max="22" width="9.5703125" style="10"/>
+    <col min="26" max="26" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.85546875" style="10" customWidth="1"/>
+    <col min="32" max="32" width="13" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.140625" style="10" customWidth="1"/>
+    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.42578125" style="10" customWidth="1"/>
+    <col min="38" max="38" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.42578125" style="52" customWidth="1"/>
+    <col min="41" max="41" width="11.85546875" style="10" customWidth="1"/>
+    <col min="42" max="42" width="12.140625" style="67" customWidth="1"/>
+    <col min="43" max="70" width="9.5703125" customWidth="1"/>
+    <col min="71" max="71" width="9.5703125" style="12" customWidth="1"/>
+    <col min="72" max="106" width="9.5703125" customWidth="1"/>
+    <col min="107" max="107" width="9.5703125" style="12" customWidth="1"/>
+    <col min="108" max="138" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:141" s="17" customFormat="1">
-      <c r="A1" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="57" t="s">
+    <row r="1" spans="1:138" s="84" customFormat="1" ht="14" customHeight="1">
+      <c r="A1" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" s="74" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="15" t="s">
+      <c r="C1" s="81" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="81" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="81" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="N1" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="O1" s="16" t="s">
+      <c r="G1" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="H1" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="R1" s="15" t="s">
+      <c r="I1" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="T1" s="17" t="s">
+      <c r="J1" s="81" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" s="81" t="s">
+        <v>159</v>
+      </c>
+      <c r="L1" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="81" t="s">
+        <v>151</v>
+      </c>
+      <c r="N1" s="81" t="s">
+        <v>150</v>
+      </c>
+      <c r="O1" s="83" t="s">
+        <v>140</v>
+      </c>
+      <c r="P1" s="83" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q1" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="R1" s="81" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="W1" s="54" t="s">
-        <v>64</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y1" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z1" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA1" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB1" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC1" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD1" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE1" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF1" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH1" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="AI1" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="AJ1" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK1" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL1" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="AM1" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="AO1" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="AP1" s="55" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ1" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="AR1" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="AS1" s="8" t="s">
-        <v>50</v>
-      </c>
+      <c r="T1" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="81" t="s">
+        <v>133</v>
+      </c>
+      <c r="V1" s="85" t="s">
+        <v>177</v>
+      </c>
+      <c r="W1" s="81" t="s">
+        <v>178</v>
+      </c>
+      <c r="X1" s="81" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y1" s="81" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z1" s="81" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA1" s="84" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB1" s="84" t="s">
+        <v>168</v>
+      </c>
+      <c r="AC1" s="84" t="s">
+        <v>163</v>
+      </c>
+      <c r="AD1" s="84" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF1" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="AG1" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH1" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="AI1" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AJ1" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="AK1" s="51" t="s">
+        <v>161</v>
+      </c>
+      <c r="AL1" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="AM1" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="AN1" s="51" t="s">
+        <v>166</v>
+      </c>
+      <c r="AO1" s="86" t="s">
+        <v>137</v>
+      </c>
+      <c r="AP1" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="BO1" s="8"/>
+      <c r="BP1" s="8"/>
+      <c r="BQ1" s="8"/>
       <c r="BR1" s="8"/>
       <c r="BS1" s="8"/>
       <c r="BT1" s="8"/>
@@ -8905,13 +9197,10 @@
       <c r="EF1" s="8"/>
       <c r="EG1" s="8"/>
       <c r="EH1" s="8"/>
-      <c r="EI1" s="8"/>
-      <c r="EJ1" s="8"/>
-      <c r="EK1" s="8"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <autoFilter ref="A1:EK1"/>
+  <autoFilter ref="A1:EH1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -8931,7 +9220,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DI1"/>
+  <dimension ref="A1:DH1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -8942,192 +9231,185 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="5" customWidth="1"/>
-    <col min="8" max="9" width="12.140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="5" customWidth="1"/>
-    <col min="12" max="13" width="10.42578125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" style="5" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="4" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" style="5" customWidth="1"/>
-    <col min="17" max="17" width="18.85546875" style="4" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" style="5" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" style="5" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="20.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="13" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" style="4" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" style="5" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" style="5"/>
     <col min="22" max="22" width="10" style="4" customWidth="1"/>
-    <col min="23" max="23" width="11" style="5"/>
+    <col min="23" max="23" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="15.5703125" style="4" customWidth="1"/>
     <col min="25" max="25" width="12.140625" style="5" customWidth="1"/>
     <col min="26" max="26" width="12" style="6" customWidth="1"/>
     <col min="27" max="27" width="11" style="6"/>
     <col min="28" max="28" width="12.85546875" style="5" customWidth="1"/>
-    <col min="29" max="30" width="11" style="5"/>
-    <col min="31" max="31" width="11.42578125" style="5" customWidth="1"/>
-    <col min="32" max="32" width="11" style="5"/>
-    <col min="33" max="33" width="8.85546875" style="5" customWidth="1"/>
-    <col min="34" max="36" width="11" style="5"/>
-    <col min="37" max="38" width="11" style="4"/>
-    <col min="39" max="39" width="12.85546875" style="4" customWidth="1"/>
-    <col min="40" max="41" width="8.5703125" style="4" customWidth="1"/>
-    <col min="42" max="42" width="14" style="4" customWidth="1"/>
-    <col min="43" max="43" width="11.140625" style="4" customWidth="1"/>
-    <col min="44" max="44" width="12.140625" style="73" customWidth="1"/>
-    <col min="45" max="45" width="10.42578125" style="4" customWidth="1"/>
-    <col min="46" max="110" width="9.5703125" style="5" customWidth="1"/>
-    <col min="111" max="111" width="9.5703125" style="4" customWidth="1"/>
-    <col min="112" max="112" width="9.5703125" style="5" customWidth="1"/>
-    <col min="113" max="113" width="9.5703125" style="4" customWidth="1"/>
-    <col min="114" max="141" width="9.5703125" style="5" customWidth="1"/>
-    <col min="142" max="16384" width="11" style="5"/>
+    <col min="29" max="31" width="11" style="5"/>
+    <col min="32" max="32" width="8.85546875" style="5" customWidth="1"/>
+    <col min="33" max="35" width="11" style="5"/>
+    <col min="36" max="37" width="11" style="4"/>
+    <col min="38" max="38" width="12.85546875" style="4" customWidth="1"/>
+    <col min="39" max="40" width="8.5703125" style="4" customWidth="1"/>
+    <col min="41" max="41" width="14" style="4" customWidth="1"/>
+    <col min="42" max="42" width="11.140625" style="4" customWidth="1"/>
+    <col min="43" max="43" width="12.140625" style="68" customWidth="1"/>
+    <col min="44" max="44" width="10.42578125" style="4" customWidth="1"/>
+    <col min="45" max="109" width="9.5703125" style="5" customWidth="1"/>
+    <col min="110" max="110" width="9.5703125" style="4" customWidth="1"/>
+    <col min="111" max="111" width="9.5703125" style="5" customWidth="1"/>
+    <col min="112" max="112" width="9.5703125" style="4" customWidth="1"/>
+    <col min="113" max="140" width="9.5703125" style="5" customWidth="1"/>
+    <col min="141" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="8" customFormat="1">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:43" s="8" customFormat="1" ht="14" customHeight="1">
+      <c r="A1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="50" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="8" t="s">
+      <c r="J1" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="M1" s="87" t="s">
+        <v>143</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="P1" s="87" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q1" s="88" t="s">
+        <v>171</v>
+      </c>
+      <c r="R1" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="S1" s="87" t="s">
+        <v>146</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="V1" s="87" t="s">
+        <v>147</v>
+      </c>
+      <c r="W1" s="87" t="s">
+        <v>172</v>
+      </c>
+      <c r="X1" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="Z1" s="87" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA1" s="87" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="AF1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="AG1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="AH1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="AI1" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AK1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="AL1" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="AM1" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="AN1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="AO1" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="AP1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="AQ1" s="87" t="s">
         <v>27</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="X1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD1" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF1" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG1" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH1" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ1" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AK1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM1" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN1" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="AO1" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AP1" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="AQ1" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="AR1" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="AS1" s="8" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <autoFilter ref="A1:EK1"/>
+  <autoFilter ref="A1:EJ1"/>
   <pageMargins left="0.25" right="0.25" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>
@@ -9141,7 +9423,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DJ1"/>
+  <dimension ref="A1:DI1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -9152,80 +9434,78 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="11"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="11"/>
-    <col min="6" max="6" width="16.42578125" style="11" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" style="12"/>
-    <col min="10" max="10" width="16.140625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" style="11" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" style="11" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" style="33" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" customWidth="1"/>
-    <col min="19" max="42" width="9.5703125" customWidth="1"/>
-    <col min="43" max="43" width="9.5703125" style="13" customWidth="1"/>
-    <col min="44" max="82" width="9.5703125" customWidth="1"/>
-    <col min="83" max="83" width="9.5703125" style="13"/>
-    <col min="85" max="86" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="10" customWidth="1"/>
+    <col min="2" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="10"/>
+    <col min="8" max="8" width="13.140625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="11"/>
+    <col min="11" max="11" width="16.140625" style="11" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" style="10" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" style="10" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="30" customWidth="1"/>
+    <col min="18" max="41" width="9.5703125" customWidth="1"/>
+    <col min="42" max="42" width="9.5703125" style="12" customWidth="1"/>
+    <col min="43" max="81" width="9.5703125" customWidth="1"/>
+    <col min="82" max="82" width="9.5703125" style="12"/>
+    <col min="84" max="85" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:114" s="17" customFormat="1">
-      <c r="A1" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="48" t="s">
+    <row r="1" spans="1:113" s="14" customFormat="1" ht="14" customHeight="1">
+      <c r="A1" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="17" t="s">
-        <v>37</v>
+      <c r="C1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>133</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>50</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q1" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP1" s="8"/>
       <c r="AQ1" s="8"/>
       <c r="AR1" s="8"/>
       <c r="AS1" s="8"/>
@@ -9297,11 +9577,10 @@
       <c r="DG1" s="8"/>
       <c r="DH1" s="8"/>
       <c r="DI1" s="8"/>
-      <c r="DJ1" s="8"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <autoFilter ref="A1:DJ1"/>
+  <autoFilter ref="A1:DI1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -9318,117 +9597,113 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DK1"/>
+  <dimension ref="A1:DH1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="11"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="11"/>
-    <col min="6" max="6" width="14.5703125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="22"/>
-    <col min="10" max="11" width="10" style="12" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" style="11" customWidth="1"/>
-    <col min="17" max="17" width="12" style="11" customWidth="1"/>
-    <col min="18" max="18" width="12" style="33" customWidth="1"/>
-    <col min="19" max="19" width="11.140625" customWidth="1"/>
-    <col min="20" max="43" width="9.5703125" customWidth="1"/>
-    <col min="44" max="44" width="9.5703125" style="13" customWidth="1"/>
-    <col min="45" max="83" width="9.5703125" customWidth="1"/>
-    <col min="84" max="84" width="9.5703125" style="13" customWidth="1"/>
-    <col min="85" max="115" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="10" customWidth="1"/>
+    <col min="2" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="10"/>
+    <col min="9" max="9" width="14.5703125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="10" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="17" max="40" width="9.5703125" customWidth="1"/>
+    <col min="41" max="41" width="9.5703125" style="12" customWidth="1"/>
+    <col min="42" max="80" width="9.5703125" customWidth="1"/>
+    <col min="81" max="81" width="9.5703125" style="12" customWidth="1"/>
+    <col min="82" max="112" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:115" s="17" customFormat="1">
-      <c r="A1" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="48" t="s">
+    <row r="1" spans="1:112" s="14" customFormat="1" ht="14" customHeight="1">
+      <c r="A1" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="60" t="s">
-        <v>165</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q1" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="19"/>
-      <c r="AH1" s="19"/>
-      <c r="AI1" s="19"/>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="19"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="19"/>
-      <c r="AP1" s="19"/>
-      <c r="AQ1" s="19"/>
+      <c r="C1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="P1" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="16"/>
+      <c r="AM1" s="16"/>
+      <c r="AN1" s="16"/>
+      <c r="AO1" s="8"/>
+      <c r="AP1" s="8"/>
+      <c r="AQ1" s="8"/>
       <c r="AR1" s="8"/>
       <c r="AS1" s="8"/>
       <c r="AT1" s="8"/>
@@ -9498,13 +9773,10 @@
       <c r="DF1" s="8"/>
       <c r="DG1" s="8"/>
       <c r="DH1" s="8"/>
-      <c r="DI1" s="8"/>
-      <c r="DJ1" s="8"/>
-      <c r="DK1" s="8"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <autoFilter ref="A1:DK1"/>
+  <autoFilter ref="A1:DH1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
@@ -9526,67 +9798,67 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="8.5703125" style="11"/>
-    <col min="3" max="3" width="13.42578125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="22" customWidth="1"/>
+    <col min="1" max="2" width="8.5703125" style="10"/>
+    <col min="3" max="3" width="13.42578125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="19" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="19" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="19" customWidth="1"/>
     <col min="9" max="9" width="14.140625" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" customWidth="1"/>
     <col min="11" max="11" width="8.140625" customWidth="1"/>
     <col min="12" max="12" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="26" customFormat="1">
-      <c r="A1" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="B1" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="77" t="s">
-        <v>93</v>
-      </c>
-      <c r="J1" s="77" t="s">
-        <v>94</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="P1" s="26" t="s">
-        <v>100</v>
+    <row r="1" spans="1:16" s="23" customFormat="1">
+      <c r="A1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="70" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="71" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -9615,59 +9887,59 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="11"/>
+    <col min="1" max="1" width="9.5703125" style="10"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="5" width="14.42578125" style="13" customWidth="1"/>
+    <col min="4" max="5" width="14.42578125" style="12" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="7" width="26.42578125" customWidth="1"/>
     <col min="8" max="8" width="21.42578125" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="19.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="25.42578125" style="50" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="50" customWidth="1"/>
+    <col min="12" max="12" width="25.42578125" style="47" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="29" customFormat="1">
-      <c r="A1" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" s="26" t="s">
+    <row r="1" spans="1:13" s="26" customFormat="1">
+      <c r="A1" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="26" t="s">
+      <c r="C1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" s="51" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="M1" s="49" t="s">
-        <v>111</v>
+      <c r="D1" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="46" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -9700,57 +9972,57 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="10" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="13" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="12" style="13" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="12" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="12" style="12" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="28" customFormat="1">
-      <c r="A1" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="28" t="s">
+    <row r="1" spans="1:13" s="25" customFormat="1">
+      <c r="A1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>120</v>
+      <c r="D1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -9781,13 +10053,13 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="5"/>
-    <col min="2" max="2" width="7.85546875" style="65" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="60" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" style="5"/>
-    <col min="5" max="5" width="8.42578125" style="65" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="60" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" style="5"/>
-    <col min="8" max="8" width="24.140625" style="67" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" style="62" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" style="5"/>
     <col min="10" max="10" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" style="5" customWidth="1"/>
@@ -9796,57 +10068,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="B1" s="82" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" s="83"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="83" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="66"/>
+      <c r="B1" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="77"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="77" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="61"/>
       <c r="J1" s="5" t="s">
-        <v>174</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="63" customFormat="1">
-      <c r="A2" s="78" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="79" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="78" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" s="78" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" s="64" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" s="62" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="62" t="s">
-        <v>126</v>
-      </c>
-      <c r="H2" s="64" t="s">
-        <v>127</v>
-      </c>
-      <c r="I2" s="62" t="s">
-        <v>128</v>
-      </c>
-      <c r="J2" s="62" t="s">
-        <v>129</v>
-      </c>
-      <c r="K2" s="62" t="s">
-        <v>130</v>
-      </c>
-      <c r="L2" s="62" t="s">
-        <v>131</v>
+    <row r="2" spans="1:12" s="58" customFormat="1">
+      <c r="A2" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="73" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="72" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="72" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="57" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TM-6586 Made a number of small tweaks where I was getting a syntax error with a call to forEach.
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -959,7 +959,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1694">
+  <cellStyleXfs count="1698">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -5822,6 +5822,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6092,21 +6096,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -6118,8 +6107,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1694">
+  <cellStyles count="1698">
     <cellStyle name="_JDI DCM Runbook Hour by Hour EMA Comm Systems (Bundle 2) 11-JUL-07" xfId="1"/>
     <cellStyle name="_JDI DCM Runbook Hour by Hour EMA Comm Systems (Bundle 2) 11-JUL-07_Title" xfId="2"/>
     <cellStyle name="_Momentive Migration Runbook Move Event 2B 09-08-2007 v2 31" xfId="3"/>
@@ -6402,6 +6406,8 @@
     <cellStyle name="Followed Hyperlink" xfId="1689" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1691" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1693" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1695" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1697" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1540" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1542" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1544" builtinId="8" hidden="1"/>
@@ -6479,6 +6485,8 @@
     <cellStyle name="Hyperlink" xfId="1688" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1690" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1692" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1694" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1696" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 10" xfId="206"/>
     <cellStyle name="Hyperlink 11" xfId="207"/>
     <cellStyle name="Hyperlink 12" xfId="208"/>
@@ -8433,17 +8441,17 @@
       <c r="C15" s="31"/>
       <c r="D15" s="32"/>
       <c r="E15" s="32"/>
-      <c r="F15" s="75" t="s">
+      <c r="F15" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="G15" s="75"/>
+      <c r="G15" s="86"/>
     </row>
     <row r="16" spans="1:7" ht="28" customHeight="1">
       <c r="A16" s="33"/>
-      <c r="B16" s="74" t="s">
+      <c r="B16" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="74"/>
+      <c r="C16" s="85"/>
       <c r="D16" s="34" t="s">
         <v>120</v>
       </c>
@@ -8970,8 +8978,8 @@
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" style="2"/>
-    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.85546875" style="11" customWidth="1"/>
     <col min="20" max="20" width="11.140625" customWidth="1"/>
@@ -8998,95 +9006,95 @@
     <col min="108" max="138" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:138" s="84" customFormat="1" ht="14" customHeight="1">
-      <c r="A1" s="79" t="s">
+    <row r="1" spans="1:138" s="79" customFormat="1" ht="14" customHeight="1">
+      <c r="A1" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="76" t="s">
         <v>155</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="82" t="s">
+      <c r="F1" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="G1" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="81" t="s">
+      <c r="H1" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="81" t="s">
+      <c r="I1" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="81" t="s">
+      <c r="J1" s="76" t="s">
         <v>164</v>
       </c>
-      <c r="K1" s="81" t="s">
+      <c r="K1" s="76" t="s">
+        <v>151</v>
+      </c>
+      <c r="L1" s="76" t="s">
+        <v>150</v>
+      </c>
+      <c r="M1" s="76" t="s">
         <v>159</v>
       </c>
-      <c r="L1" s="81" t="s">
+      <c r="N1" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="81" t="s">
-        <v>151</v>
-      </c>
-      <c r="N1" s="81" t="s">
-        <v>150</v>
-      </c>
-      <c r="O1" s="83" t="s">
+      <c r="O1" s="78" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="83" t="s">
+      <c r="P1" s="78" t="s">
         <v>138</v>
       </c>
-      <c r="Q1" s="81" t="s">
+      <c r="Q1" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="81" t="s">
+      <c r="R1" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="81" t="s">
+      <c r="S1" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="84" t="s">
+      <c r="T1" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="81" t="s">
+      <c r="U1" s="76" t="s">
         <v>133</v>
       </c>
-      <c r="V1" s="85" t="s">
+      <c r="V1" s="80" t="s">
         <v>177</v>
       </c>
-      <c r="W1" s="81" t="s">
+      <c r="W1" s="76" t="s">
         <v>178</v>
       </c>
-      <c r="X1" s="81" t="s">
+      <c r="X1" s="76" t="s">
         <v>170</v>
       </c>
-      <c r="Y1" s="81" t="s">
+      <c r="Y1" s="76" t="s">
         <v>152</v>
       </c>
-      <c r="Z1" s="81" t="s">
+      <c r="Z1" s="76" t="s">
         <v>153</v>
       </c>
-      <c r="AA1" s="84" t="s">
+      <c r="AA1" s="79" t="s">
         <v>154</v>
       </c>
-      <c r="AB1" s="84" t="s">
+      <c r="AB1" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="AC1" s="84" t="s">
+      <c r="AC1" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="AD1" s="84" t="s">
+      <c r="AD1" s="79" t="s">
         <v>169</v>
       </c>
       <c r="AE1" s="7" t="s">
@@ -9119,7 +9127,7 @@
       <c r="AN1" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="AO1" s="86" t="s">
+      <c r="AO1" s="81" t="s">
         <v>137</v>
       </c>
       <c r="AP1" s="66" t="s">
@@ -9307,13 +9315,13 @@
       <c r="J1" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="K1" s="87" t="s">
+      <c r="K1" s="82" t="s">
         <v>174</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="87" t="s">
+      <c r="M1" s="82" t="s">
         <v>143</v>
       </c>
       <c r="N1" s="8" t="s">
@@ -9322,16 +9330,16 @@
       <c r="O1" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="P1" s="87" t="s">
+      <c r="P1" s="82" t="s">
         <v>144</v>
       </c>
-      <c r="Q1" s="88" t="s">
+      <c r="Q1" s="83" t="s">
         <v>171</v>
       </c>
-      <c r="R1" s="87" t="s">
+      <c r="R1" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="87" t="s">
+      <c r="S1" s="82" t="s">
         <v>146</v>
       </c>
       <c r="T1" s="8" t="s">
@@ -9340,22 +9348,22 @@
       <c r="U1" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="V1" s="87" t="s">
+      <c r="V1" s="82" t="s">
         <v>147</v>
       </c>
-      <c r="W1" s="87" t="s">
+      <c r="W1" s="82" t="s">
         <v>172</v>
       </c>
-      <c r="X1" s="87" t="s">
+      <c r="X1" s="82" t="s">
         <v>14</v>
       </c>
       <c r="Y1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="87" t="s">
+      <c r="Z1" s="82" t="s">
         <v>140</v>
       </c>
-      <c r="AA1" s="87" t="s">
+      <c r="AA1" s="82" t="s">
         <v>138</v>
       </c>
       <c r="AB1" s="8" t="s">
@@ -9391,19 +9399,19 @@
       <c r="AL1" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="AM1" s="89" t="s">
+      <c r="AM1" s="84" t="s">
         <v>23</v>
       </c>
       <c r="AN1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AO1" s="87" t="s">
+      <c r="AO1" s="82" t="s">
         <v>25</v>
       </c>
       <c r="AP1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AQ1" s="87" t="s">
+      <c r="AQ1" s="82" t="s">
         <v>27</v>
       </c>
     </row>
@@ -10068,16 +10076,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="77" t="s">
+      <c r="C1" s="88"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
       <c r="H1" s="61"/>
       <c r="J1" s="5" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
TM-6720 Fixed issue with Security Warning in Asset Export Spreadsheet. Changed the first column to be Id consistently for the assets.
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="26340" windowHeight="14400" tabRatio="782"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="13120" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Comments!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Databases!$A$1:$DI$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Dependencies!$A$1:$P$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Devices!$A$1:$EJ$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Devices!$A$1:$EI$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Rack!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Room!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Storage!$A$1:$DH$1</definedName>
@@ -56,6 +56,20 @@
     <author/>
   </authors>
   <commentList>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="8"/>
+            <rFont val="Times New Roman"/>
+            <family val="1"/>
+          </rPr>
+          <t>The source location/datacenter where the asset will be moved from</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="N1" authorId="0">
       <text>
         <r>
@@ -84,30 +98,40 @@
         </r>
       </text>
     </comment>
+    <comment ref="P1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="8"/>
+            <rFont val="Times New Roman"/>
+            <family val="1"/>
+          </rPr>
+          <t>The U position that the asset is located at in rack before the move.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="8"/>
+            <rFont val="Verdana"/>
+            <family val="2"/>
+          </rPr>
+          <t>Position in the cabinet U1 is on the bottom</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="fieldSettingsDefines.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="Macintosh HD:data:dev:src:tdstm:misc:fieldSettingsDefines.csv" comma="1">
-      <textFields count="7">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="176">
   <si>
     <t>Customer:</t>
   </si>
@@ -187,15 +211,9 @@
     <t>Rate Of Change</t>
   </si>
   <si>
-    <t>Application</t>
-  </si>
-  <si>
     <t>Modified Date</t>
   </si>
   <si>
-    <t>appId</t>
-  </si>
-  <si>
     <t>Vendor</t>
   </si>
   <si>
@@ -220,13 +238,7 @@
     <t>Criticality</t>
   </si>
   <si>
-    <t>dbId</t>
-  </si>
-  <si>
     <t>Format</t>
-  </si>
-  <si>
-    <t>filesId</t>
   </si>
   <si>
     <t>AssetDependencyId</t>
@@ -518,133 +530,136 @@
     <t>Dep Status</t>
   </si>
   <si>
+    <t>Bundle</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>SME1</t>
+  </si>
+  <si>
+    <t>Business Unit</t>
+  </si>
+  <si>
+    <t>App Owner</t>
+  </si>
+  <si>
+    <t>Retire Date</t>
+  </si>
+  <si>
+    <t>Maint Expiration</t>
+  </si>
+  <si>
+    <t>User Count</t>
+  </si>
+  <si>
+    <t>User Locations</t>
+  </si>
+  <si>
+    <t>Use Frequency</t>
+  </si>
+  <si>
+    <t>DR RPO</t>
+  </si>
+  <si>
+    <t>DR RTO</t>
+  </si>
+  <si>
+    <t>Latency OK</t>
+  </si>
+  <si>
+    <t>Test Proc OK</t>
+  </si>
+  <si>
+    <t>Startup Proc OK</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Shutdown By</t>
+  </si>
+  <si>
+    <t>Shutdown Fixed</t>
+  </si>
+  <si>
+    <t>Shutdown Duration</t>
+  </si>
+  <si>
+    <t>Startup By</t>
+  </si>
+  <si>
+    <t>Startup Fixed</t>
+  </si>
+  <si>
+    <t>Startup Duration</t>
+  </si>
+  <si>
+    <t>Testing By</t>
+  </si>
+  <si>
+    <t>Testing Fixed</t>
+  </si>
+  <si>
+    <t>Testing Duration</t>
+  </si>
+  <si>
+    <t>External Ref Id</t>
+  </si>
+  <si>
+    <t>Alternate Name</t>
+  </si>
+  <si>
+    <t>Serial #</t>
+  </si>
+  <si>
     <t>Asset Tag</t>
   </si>
   <si>
-    <t>External Ref Id</t>
-  </si>
-  <si>
-    <t>Maint Expiration</t>
+    <t>Device Type</t>
+  </si>
+  <si>
+    <t>IP Address</t>
+  </si>
+  <si>
+    <t>Source Location</t>
+  </si>
+  <si>
+    <t>Source Room</t>
+  </si>
+  <si>
+    <t>Source Rack</t>
+  </si>
+  <si>
+    <t>Source Position</t>
+  </si>
+  <si>
+    <t>Source Chassis</t>
+  </si>
+  <si>
+    <t>Target Location</t>
+  </si>
+  <si>
+    <t>Target Room</t>
+  </si>
+  <si>
+    <t>Target Rack</t>
+  </si>
+  <si>
+    <t>Target Position</t>
+  </si>
+  <si>
+    <t>Target Chassis</t>
   </si>
   <si>
     <t>Rail Type</t>
   </si>
   <si>
-    <t>Retire Date</t>
-  </si>
-  <si>
-    <t>Serial #</t>
-  </si>
-  <si>
-    <t>Alternate Name</t>
-  </si>
-  <si>
-    <t>Source Location</t>
-  </si>
-  <si>
-    <t>Source Position</t>
-  </si>
-  <si>
-    <t>Source Room</t>
-  </si>
-  <si>
-    <t>Target Location</t>
-  </si>
-  <si>
-    <t>Target Position</t>
-  </si>
-  <si>
-    <t>Target Room</t>
-  </si>
-  <si>
     <t>Usize</t>
   </si>
   <si>
-    <t>App Owner</t>
-  </si>
-  <si>
-    <t>Business Unit</t>
-  </si>
-  <si>
-    <t>DR RPO</t>
-  </si>
-  <si>
-    <t>DR RTO</t>
-  </si>
-  <si>
-    <t>Latency OK</t>
-  </si>
-  <si>
-    <t>Bundle</t>
-  </si>
-  <si>
-    <t>Shutdown By</t>
-  </si>
-  <si>
-    <t>Shutdown Duration</t>
-  </si>
-  <si>
-    <t>Shutdown Fixed</t>
-  </si>
-  <si>
-    <t>SME1</t>
-  </si>
-  <si>
-    <t>Startup By</t>
-  </si>
-  <si>
-    <t>Startup Duration</t>
-  </si>
-  <si>
-    <t>Startup Fixed</t>
-  </si>
-  <si>
-    <t>Startup Proc OK</t>
-  </si>
-  <si>
-    <t>Support</t>
-  </si>
-  <si>
-    <t>Testing By</t>
-  </si>
-  <si>
-    <t>Testing Duration</t>
-  </si>
-  <si>
-    <t>Testing Fixed</t>
-  </si>
-  <si>
-    <t>Test Proc OK</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Use Frequency</t>
-  </si>
-  <si>
-    <t>Source Chassis</t>
-  </si>
-  <si>
-    <t>Target Chassis</t>
-  </si>
-  <si>
-    <t>Device Type</t>
-  </si>
-  <si>
-    <t>IP Address</t>
-  </si>
-  <si>
-    <t>Target Rack</t>
-  </si>
-  <si>
-    <t>Source Rack</t>
-  </si>
-  <si>
-    <t>User Count</t>
-  </si>
-  <si>
-    <t>User Locations</t>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -773,6 +788,13 @@
       <family val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
@@ -814,12 +836,6 @@
       <sz val="10"/>
       <color theme="11"/>
       <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -959,7 +975,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1698">
+  <cellStyleXfs count="1568">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -4776,59 +4792,59 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -4837,28 +4853,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
@@ -4987,7 +5003,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -5822,166 +5838,36 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -5991,11 +5877,13 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6019,48 +5907,50 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6077,7 +5967,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1539" applyFont="1" applyAlignment="1">
@@ -6087,30 +5977,22 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6123,7 +6005,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1698">
+  <cellStyles count="1568">
     <cellStyle name="_JDI DCM Runbook Hour by Hour EMA Comm Systems (Bundle 2) 11-JUL-07" xfId="1"/>
     <cellStyle name="_JDI DCM Runbook Hour by Hour EMA Comm Systems (Bundle 2) 11-JUL-07_Title" xfId="2"/>
     <cellStyle name="_Momentive Migration Runbook Move Event 2B 09-08-2007 v2 31" xfId="3"/>
@@ -6343,71 +6225,6 @@
     <cellStyle name="Followed Hyperlink" xfId="1563" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1565" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1567" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1569" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1571" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1573" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1575" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1577" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1579" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1581" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1583" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1585" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1587" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1589" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1591" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1593" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1595" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1597" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1599" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1601" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1603" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1605" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1607" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1609" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1611" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1613" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1615" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1617" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1619" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1621" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1623" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1625" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1627" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1629" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1631" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1633" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1635" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1637" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1639" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1641" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1643" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1645" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1647" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1649" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1651" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1653" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1655" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1657" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1659" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1661" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1663" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1665" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1667" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1669" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1671" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1673" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1675" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1677" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1679" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1681" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1683" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1685" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1687" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1689" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1691" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1693" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1695" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1697" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1540" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1542" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1544" builtinId="8" hidden="1"/>
@@ -6422,71 +6239,6 @@
     <cellStyle name="Hyperlink" xfId="1562" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1564" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1566" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1568" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1570" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1572" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1574" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1576" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1578" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1580" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1582" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1584" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1586" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1588" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1590" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1592" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1594" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1596" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1598" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1600" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1602" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1604" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1606" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1608" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1610" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1612" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1614" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1616" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1618" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1620" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1622" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1624" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1626" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1628" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1630" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1632" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1634" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1636" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1638" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1640" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1642" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1644" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1646" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1648" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1650" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1652" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1654" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1656" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1658" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1660" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1662" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1664" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1666" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1668" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1670" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1672" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1674" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1676" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1678" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1680" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1682" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1684" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1686" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1688" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1690" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1692" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1694" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1696" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 10" xfId="206"/>
     <cellStyle name="Hyperlink 11" xfId="207"/>
     <cellStyle name="Hyperlink 12" xfId="208"/>
@@ -8338,74 +8090,74 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="67" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="67" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="67" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="32">
         <v>38295</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="63" t="s">
-        <v>129</v>
+      <c r="A9" s="67" t="s">
+        <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="63" t="s">
-        <v>130</v>
+      <c r="A10" s="67" t="s">
+        <v>126</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -8413,84 +8165,84 @@
     </row>
     <row r="12" spans="1:7">
       <c r="B12" t="s">
-        <v>94</v>
-      </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
+        <v>90</v>
+      </c>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
+        <v>123</v>
+      </c>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="86" t="s">
-        <v>91</v>
-      </c>
-      <c r="G15" s="86"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="82"/>
     </row>
     <row r="16" spans="1:7" ht="28" customHeight="1">
-      <c r="A16" s="33"/>
-      <c r="B16" s="85" t="s">
-        <v>92</v>
-      </c>
-      <c r="C16" s="85"/>
-      <c r="D16" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="E16" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="F16" s="56" t="s">
-        <v>122</v>
-      </c>
-      <c r="G16" s="34" t="s">
-        <v>123</v>
+      <c r="A16" s="35"/>
+      <c r="B16" s="81" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="81"/>
+      <c r="D16" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="20" customHeight="1">
-      <c r="A17" s="36">
+      <c r="A17" s="38">
         <f>COUNTA(Applications!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B17" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="D17" s="38">
+      <c r="B17" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="40">
         <f>COUNTA(Applications!A:A)-1</f>
         <v>0</v>
       </c>
-      <c r="E17" s="38">
+      <c r="E17" s="40">
         <f>A17-D17</f>
         <v>0</v>
       </c>
-      <c r="F17" s="39">
+      <c r="F17" s="41">
         <f>COUNTIF(Applications!B:EH,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="G17" s="39">
+      <c r="G17" s="41">
         <f>COUNTIF(Applications!B:EI,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Applications!B:EI,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Applications!B:EI,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Applications!B:EI,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="I17" s="36" t="s">
-        <v>113</v>
+      <c r="I17" s="38" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="20" customHeight="1">
@@ -8499,20 +8251,20 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="40">
+        <v>93</v>
+      </c>
+      <c r="D18" s="42">
         <f>COUNTIFS(Applications!A:A,"&gt;0",Applications!R:R,"Master")</f>
         <v>0</v>
       </c>
-      <c r="E18" s="40">
+      <c r="E18" s="42">
         <f>COUNTIFS(Applications!B:B,"&lt;&gt;''",Applications!R:R,"Master")-D18</f>
         <v>0</v>
       </c>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
       <c r="I18" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="20" customHeight="1">
@@ -8521,60 +8273,60 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D19" s="40">
+        <v>94</v>
+      </c>
+      <c r="D19" s="42">
         <f>IF(ISNUMBER(D17),D17-D18,"")</f>
         <v>0</v>
       </c>
-      <c r="E19" s="40">
+      <c r="E19" s="42">
         <f>IF(ISNUMBER(E17),E17-E18,"")</f>
         <v>0</v>
       </c>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="I19" s="53" t="s">
-        <v>115</v>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="I19" s="57" t="s">
+        <v>111</v>
       </c>
       <c r="J19" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K19" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="20" customHeight="1">
-      <c r="A20" s="36">
+      <c r="A20" s="38">
         <f>COUNTA(Devices!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B20" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="38">
+      <c r="B20" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="40">
         <f>COUNTA(Devices!A:A)-1</f>
         <v>0</v>
       </c>
-      <c r="E20" s="38">
+      <c r="E20" s="40">
         <f>A20-D20</f>
         <v>0</v>
       </c>
-      <c r="F20" s="39">
-        <f>COUNTIF(Devices!B:EJ,REPT("?",254)&amp;"*")</f>
+      <c r="F20" s="41">
+        <f>COUNTIF(Devices!B:EI,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="G20" s="39">
-        <f>COUNTIF(Devices!B:EK,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Devices!B:EK,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Devices!B:EK,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Devices!B:EK,"*"&amp;CHAR(39)&amp;"*")</f>
+      <c r="G20" s="41">
+        <f>COUNTIF(Devices!B:EJ,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Devices!B:EJ,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Devices!B:EJ,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Devices!B:EJ,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="I20" s="54" t="s">
-        <v>116</v>
+      <c r="I20" s="58" t="s">
+        <v>112</v>
       </c>
       <c r="J20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="20" customHeight="1">
@@ -8583,90 +8335,90 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" s="40">
+        <v>96</v>
+      </c>
+      <c r="D21" s="42">
         <f>COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!J:J,"Server")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!J:J,"Blade")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!J:J,"VM")++COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!J:J,"Appliance")</f>
         <v>0</v>
       </c>
-      <c r="E21" s="40">
+      <c r="E21" s="42">
         <f>COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!J:J,"Server")+COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!J:J,"Blade")+COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!J:J,"VM")++COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!J:J,"Appliance")</f>
         <v>0</v>
       </c>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
     </row>
     <row r="22" spans="1:11" ht="20" customHeight="1">
-      <c r="A22" s="36">
+      <c r="A22" s="38">
         <f>COUNTA(Databases!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B22" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="38">
+      <c r="B22" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="40">
         <f>COUNTA(Databases!A:A)-1</f>
         <v>0</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E22" s="40">
         <f>A22-D22</f>
         <v>0</v>
       </c>
-      <c r="F22" s="39">
+      <c r="F22" s="41">
         <f>COUNTIF(Databases!B:EJ,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="G22" s="39">
+      <c r="G22" s="41">
         <f>COUNTIF(Databases!B:EK,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Databases!B:EK,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Databases!B:EK,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Databases!B:EK,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="20" customHeight="1">
-      <c r="A23" s="36">
+      <c r="A23" s="38">
         <f>COUNTA(Storage!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B23" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="D23" s="38">
+      <c r="B23" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="40">
         <f>COUNTA(Storage!A:A)-1</f>
         <v>0</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="40">
         <f>A23-D23</f>
         <v>0</v>
       </c>
-      <c r="F23" s="39">
+      <c r="F23" s="41">
         <f>COUNTIF(Storage!B:EI,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="G23" s="39">
+      <c r="G23" s="41">
         <f>COUNTIF(Storage!B:EJ,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Storage!B:EJ,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Storage!B:EJ,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Storage!B:EJ,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="20" customHeight="1">
-      <c r="A24" s="36">
+      <c r="A24" s="38">
         <f>COUNTA(Dependencies!D:D)-1</f>
         <v>0</v>
       </c>
-      <c r="B24" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" s="38">
+      <c r="B24" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="40">
         <f>COUNTA(Dependencies!A:A)-1</f>
         <v>0</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E24" s="40">
         <f>A24-D24</f>
         <v>0</v>
       </c>
-      <c r="F24" s="39">
+      <c r="F24" s="41">
         <f>COUNTIF(Storage!B:EI,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="G24" s="42">
+      <c r="G24" s="44">
         <f>COUNTIF(Dependencies!B:EL,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Dependencies!B:EL,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Dependencies!B:EL,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Dependencies!B:EL,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
@@ -8677,12 +8429,12 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
-      </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
+        <v>100</v>
+      </c>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
     </row>
     <row r="26" spans="1:11" ht="20" customHeight="1">
       <c r="A26">
@@ -8690,12 +8442,12 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
+        <v>101</v>
+      </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
     </row>
     <row r="27" spans="1:11" ht="20" customHeight="1">
       <c r="A27">
@@ -8703,12 +8455,12 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
-      </c>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
+        <v>102</v>
+      </c>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
     </row>
     <row r="28" spans="1:11" ht="20" customHeight="1">
       <c r="A28">
@@ -8716,12 +8468,12 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
-      </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
+        <v>103</v>
+      </c>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
     </row>
     <row r="29" spans="1:11" ht="20" customHeight="1">
       <c r="A29">
@@ -8729,12 +8481,12 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
+        <v>104</v>
+      </c>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
     </row>
     <row r="30" spans="1:11" ht="20" customHeight="1">
       <c r="A30">
@@ -8742,73 +8494,73 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
+        <v>105</v>
+      </c>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
     </row>
     <row r="31" spans="1:11" ht="20" customHeight="1">
-      <c r="A31" s="36">
+      <c r="A31" s="38">
         <f>COUNTA(Room!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B31" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
+      <c r="B31" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
     </row>
     <row r="32" spans="1:11" ht="20" customHeight="1">
-      <c r="A32" s="36">
+      <c r="A32" s="38">
         <f>COUNTA(Rack!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B32" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
+      <c r="B32" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
     </row>
     <row r="33" spans="1:7" ht="20" customHeight="1">
-      <c r="A33" s="36">
+      <c r="A33" s="38">
         <f>COUNTA(Cabling!B:B)-2</f>
         <v>0</v>
       </c>
-      <c r="B33" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
+      <c r="B33" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
     </row>
     <row r="34" spans="1:7" ht="20" customHeight="1">
-      <c r="A34" s="37">
+      <c r="A34" s="39">
         <f>COUNTA(Comments!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B34" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
+      <c r="B34" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="21" customHeight="1"/>
@@ -8867,33 +8619,33 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="16" style="10" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="19" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="19" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" style="19" customWidth="1"/>
-    <col min="7" max="16384" width="9.5703125" style="19"/>
+    <col min="1" max="1" width="16.5703125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="16" style="11" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="21" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" style="21" customWidth="1"/>
+    <col min="7" max="16384" width="9.5703125" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="31" t="s">
         <v>86</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="69" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -8923,25 +8675,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="5" width="19.42578125" style="65" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="65"/>
+    <col min="1" max="5" width="19.42578125" style="69" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="69"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="68" t="s">
         <v>131</v>
-      </c>
-      <c r="B1" s="64" t="s">
-        <v>132</v>
-      </c>
-      <c r="C1" s="64" t="s">
-        <v>133</v>
-      </c>
-      <c r="D1" s="64" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" s="64" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -8973,165 +8725,158 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="11" customWidth="1"/>
     <col min="2" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" style="2"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" style="11" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" style="12"/>
+    <col min="16" max="16" width="11.85546875" style="12" customWidth="1"/>
     <col min="20" max="20" width="11.140625" customWidth="1"/>
-    <col min="22" max="22" width="9.5703125" style="10"/>
-    <col min="26" max="26" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.85546875" style="10" customWidth="1"/>
-    <col min="32" max="32" width="13" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.140625" style="10" customWidth="1"/>
-    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.42578125" style="10" customWidth="1"/>
-    <col min="38" max="38" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.42578125" style="52" customWidth="1"/>
-    <col min="41" max="41" width="11.85546875" style="10" customWidth="1"/>
-    <col min="42" max="42" width="12.140625" style="67" customWidth="1"/>
+    <col min="22" max="22" width="9.5703125" style="11"/>
+    <col min="31" max="31" width="9.85546875" style="11" customWidth="1"/>
+    <col min="32" max="32" width="11.42578125" customWidth="1"/>
+    <col min="33" max="33" width="13.42578125" customWidth="1"/>
+    <col min="34" max="34" width="16.140625" style="11" customWidth="1"/>
+    <col min="35" max="35" width="9.42578125" customWidth="1"/>
+    <col min="36" max="36" width="11.42578125" customWidth="1"/>
+    <col min="37" max="37" width="13.42578125" style="11" customWidth="1"/>
+    <col min="38" max="38" width="8.5703125" customWidth="1"/>
+    <col min="39" max="39" width="10.42578125" customWidth="1"/>
+    <col min="40" max="40" width="13.42578125" style="55" customWidth="1"/>
+    <col min="41" max="41" width="11.85546875" style="11" customWidth="1"/>
+    <col min="42" max="42" width="12.140625" style="71" customWidth="1"/>
     <col min="43" max="70" width="9.5703125" customWidth="1"/>
-    <col min="71" max="71" width="9.5703125" style="12" customWidth="1"/>
+    <col min="71" max="71" width="9.5703125" style="13" customWidth="1"/>
     <col min="72" max="106" width="9.5703125" customWidth="1"/>
-    <col min="107" max="107" width="9.5703125" style="12" customWidth="1"/>
+    <col min="107" max="107" width="9.5703125" style="13" customWidth="1"/>
     <col min="108" max="138" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:138" s="79" customFormat="1" ht="14" customHeight="1">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:138" s="16" customFormat="1">
+      <c r="A1" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="75" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="76" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="76" t="s">
-        <v>155</v>
-      </c>
-      <c r="E1" s="76" t="s">
+      <c r="G1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="H1" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="76" t="s">
+      <c r="I1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="76" t="s">
+      <c r="J1" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="79" t="s">
+        <v>135</v>
+      </c>
+      <c r="L1" s="79" t="s">
+        <v>136</v>
+      </c>
+      <c r="M1" s="79" t="s">
+        <v>134</v>
+      </c>
+      <c r="N1" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="76" t="s">
+      <c r="O1" s="80" t="s">
+        <v>137</v>
+      </c>
+      <c r="P1" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="76" t="s">
-        <v>164</v>
-      </c>
-      <c r="K1" s="76" t="s">
-        <v>151</v>
-      </c>
-      <c r="L1" s="76" t="s">
-        <v>150</v>
-      </c>
-      <c r="M1" s="76" t="s">
-        <v>159</v>
-      </c>
-      <c r="N1" s="76" t="s">
+      <c r="R1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="78" t="s">
+      <c r="T1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="V1" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="W1" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="78" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q1" s="76" t="s">
-        <v>35</v>
-      </c>
-      <c r="R1" s="76" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="76" t="s">
-        <v>36</v>
-      </c>
-      <c r="T1" s="79" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="76" t="s">
-        <v>133</v>
-      </c>
-      <c r="V1" s="80" t="s">
-        <v>177</v>
-      </c>
-      <c r="W1" s="76" t="s">
-        <v>178</v>
-      </c>
-      <c r="X1" s="76" t="s">
-        <v>170</v>
-      </c>
-      <c r="Y1" s="76" t="s">
-        <v>152</v>
-      </c>
-      <c r="Z1" s="76" t="s">
-        <v>153</v>
-      </c>
-      <c r="AA1" s="79" t="s">
-        <v>154</v>
-      </c>
-      <c r="AB1" s="79" t="s">
-        <v>168</v>
-      </c>
-      <c r="AC1" s="79" t="s">
-        <v>163</v>
-      </c>
-      <c r="AD1" s="79" t="s">
-        <v>169</v>
+      <c r="X1" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y1" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z1" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>147</v>
       </c>
       <c r="AE1" s="7" t="s">
         <v>22</v>
       </c>
       <c r="AF1" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG1" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="AH1" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI1" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ1" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="AK1" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="AL1" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM1" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="AN1" s="54" t="s">
         <v>156</v>
       </c>
-      <c r="AG1" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH1" s="51" t="s">
+      <c r="AO1" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="AI1" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="AJ1" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="AK1" s="51" t="s">
-        <v>161</v>
-      </c>
-      <c r="AL1" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="AM1" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="AN1" s="51" t="s">
-        <v>166</v>
-      </c>
-      <c r="AO1" s="81" t="s">
-        <v>137</v>
-      </c>
-      <c r="AP1" s="66" t="s">
-        <v>27</v>
+      <c r="AP1" s="70" t="s">
+        <v>26</v>
       </c>
       <c r="BO1" s="8"/>
       <c r="BP1" s="8"/>
@@ -9228,7 +8973,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DH1"/>
+  <dimension ref="A1:DG1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -9241,70 +8986,68 @@
   <cols>
     <col min="1" max="1" width="9.28515625" style="4" customWidth="1"/>
     <col min="2" max="3" width="20.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13" style="5" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="13" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="5" customWidth="1"/>
     <col min="9" max="9" width="15.140625" style="5" customWidth="1"/>
     <col min="10" max="10" width="12.140625" style="5" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" style="5" customWidth="1"/>
     <col min="12" max="12" width="8.85546875" style="5" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" style="5" customWidth="1"/>
-    <col min="14" max="14" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.42578125" style="5" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" style="5" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" style="5" customWidth="1"/>
     <col min="18" max="18" width="18.85546875" style="4" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" style="5" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11" style="5"/>
-    <col min="22" max="22" width="10" style="4" customWidth="1"/>
-    <col min="23" max="23" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" style="4" customWidth="1"/>
-    <col min="25" max="25" width="12.140625" style="5" customWidth="1"/>
-    <col min="26" max="26" width="12" style="6" customWidth="1"/>
-    <col min="27" max="27" width="11" style="6"/>
-    <col min="28" max="28" width="12.85546875" style="5" customWidth="1"/>
-    <col min="29" max="31" width="11" style="5"/>
-    <col min="32" max="32" width="8.85546875" style="5" customWidth="1"/>
-    <col min="33" max="35" width="11" style="5"/>
-    <col min="36" max="37" width="11" style="4"/>
-    <col min="38" max="38" width="12.85546875" style="4" customWidth="1"/>
-    <col min="39" max="40" width="8.5703125" style="4" customWidth="1"/>
-    <col min="41" max="41" width="14" style="4" customWidth="1"/>
-    <col min="42" max="42" width="11.140625" style="4" customWidth="1"/>
-    <col min="43" max="43" width="12.140625" style="68" customWidth="1"/>
-    <col min="44" max="44" width="10.42578125" style="4" customWidth="1"/>
-    <col min="45" max="109" width="9.5703125" style="5" customWidth="1"/>
-    <col min="110" max="110" width="9.5703125" style="4" customWidth="1"/>
-    <col min="111" max="111" width="9.5703125" style="5" customWidth="1"/>
-    <col min="112" max="112" width="9.5703125" style="4" customWidth="1"/>
-    <col min="113" max="140" width="9.5703125" style="5" customWidth="1"/>
-    <col min="141" max="16384" width="11" style="5"/>
+    <col min="19" max="19" width="13.42578125" style="5" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" style="5" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="5" customWidth="1"/>
+    <col min="22" max="22" width="11" style="5"/>
+    <col min="23" max="23" width="10" style="4" customWidth="1"/>
+    <col min="24" max="24" width="11" style="5"/>
+    <col min="25" max="25" width="15.5703125" style="4" customWidth="1"/>
+    <col min="26" max="26" width="12.140625" style="5" customWidth="1"/>
+    <col min="27" max="27" width="12" style="6" customWidth="1"/>
+    <col min="28" max="28" width="11" style="6"/>
+    <col min="29" max="29" width="12.85546875" style="5" customWidth="1"/>
+    <col min="30" max="32" width="11" style="5"/>
+    <col min="33" max="33" width="8.85546875" style="5" customWidth="1"/>
+    <col min="34" max="36" width="11" style="5"/>
+    <col min="37" max="38" width="11" style="4"/>
+    <col min="39" max="39" width="12.85546875" style="4" customWidth="1"/>
+    <col min="40" max="41" width="8.5703125" style="4" customWidth="1"/>
+    <col min="42" max="42" width="14" style="4" customWidth="1"/>
+    <col min="43" max="43" width="12.140625" style="72" customWidth="1"/>
+    <col min="44" max="108" width="9.5703125" style="5" customWidth="1"/>
+    <col min="109" max="109" width="9.5703125" style="4" customWidth="1"/>
+    <col min="110" max="110" width="9.5703125" style="5" customWidth="1"/>
+    <col min="111" max="111" width="9.5703125" style="4" customWidth="1"/>
+    <col min="112" max="139" width="9.5703125" style="5" customWidth="1"/>
+    <col min="140" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="8" customFormat="1" ht="14" customHeight="1">
-      <c r="A1" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="50" t="s">
+    <row r="1" spans="1:43" s="8" customFormat="1">
+      <c r="A1" s="51" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>8</v>
@@ -9313,60 +9056,60 @@
         <v>9</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="K1" s="82" t="s">
-        <v>174</v>
+        <v>161</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>162</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="82" t="s">
-        <v>143</v>
+      <c r="M1" s="8" t="s">
+        <v>163</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="P1" s="82" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q1" s="83" t="s">
+        <v>165</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="V1" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="R1" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="82" t="s">
-        <v>146</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="V1" s="82" t="s">
-        <v>147</v>
-      </c>
-      <c r="W1" s="82" t="s">
+      <c r="W1" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="X1" s="82" t="s">
+      <c r="X1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="82" t="s">
-        <v>140</v>
-      </c>
-      <c r="AA1" s="82" t="s">
+      <c r="Z1" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA1" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="9" t="s">
         <v>16</v>
       </c>
       <c r="AC1" s="8" t="s">
@@ -9376,7 +9119,7 @@
         <v>18</v>
       </c>
       <c r="AE1" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="AF1" s="8" t="s">
         <v>19</v>
@@ -9388,36 +9131,36 @@
         <v>21</v>
       </c>
       <c r="AI1" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="AJ1" s="7" t="s">
-        <v>149</v>
+        <v>173</v>
+      </c>
+      <c r="AJ1" s="8" t="s">
+        <v>174</v>
       </c>
       <c r="AK1" s="7" t="s">
         <v>22</v>
       </c>
       <c r="AL1" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="AM1" s="84" t="s">
+        <v>157</v>
+      </c>
+      <c r="AM1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AN1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AO1" s="82" t="s">
+      <c r="AO1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AP1" s="8" t="s">
+      <c r="AP1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AQ1" s="82" t="s">
-        <v>27</v>
+      <c r="AQ1" s="70" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <autoFilter ref="A1:EJ1"/>
+  <autoFilter ref="A1:EI1"/>
   <pageMargins left="0.25" right="0.25" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>
@@ -9442,76 +9185,75 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="11" customWidth="1"/>
     <col min="2" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="10"/>
-    <col min="8" max="8" width="13.140625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" style="11"/>
-    <col min="11" max="11" width="16.140625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="11"/>
+    <col min="8" max="8" width="16.42578125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="12"/>
+    <col min="11" max="11" width="16.140625" style="12" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" style="10" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" style="10" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" style="30" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" style="11" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="32" customWidth="1"/>
     <col min="18" max="41" width="9.5703125" customWidth="1"/>
-    <col min="42" max="42" width="9.5703125" style="12" customWidth="1"/>
+    <col min="42" max="42" width="9.5703125" style="13" customWidth="1"/>
     <col min="43" max="81" width="9.5703125" customWidth="1"/>
-    <col min="82" max="82" width="9.5703125" style="12"/>
+    <col min="82" max="82" width="9.5703125" style="13"/>
     <col min="84" max="85" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" s="14" customFormat="1" ht="14" customHeight="1">
-      <c r="A1" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="45" t="s">
+    <row r="1" spans="1:113" s="16" customFormat="1">
+      <c r="A1" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="17" t="s">
+      <c r="D1" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="K1" s="18" t="s">
+      <c r="I1" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="14" t="s">
-        <v>133</v>
+      <c r="N1" s="16" t="s">
+        <v>129</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q1" s="66" t="s">
-        <v>27</v>
+      <c r="P1" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q1" s="70" t="s">
+        <v>26</v>
       </c>
       <c r="AP1" s="8"/>
       <c r="AQ1" s="8"/>
@@ -9616,99 +9358,96 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="11" customWidth="1"/>
     <col min="2" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="10"/>
-    <col min="9" max="9" width="14.5703125" style="10" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" style="10" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="21"/>
+    <col min="7" max="7" width="8.5703125" style="11"/>
+    <col min="9" max="9" width="14.5703125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="10" style="12" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="11" customWidth="1"/>
+    <col min="15" max="15" width="12" style="11" customWidth="1"/>
+    <col min="16" max="16" width="12" style="32" customWidth="1"/>
     <col min="17" max="40" width="9.5703125" customWidth="1"/>
-    <col min="41" max="41" width="9.5703125" style="12" customWidth="1"/>
+    <col min="41" max="41" width="9.5703125" style="13" customWidth="1"/>
     <col min="42" max="80" width="9.5703125" customWidth="1"/>
-    <col min="81" max="81" width="9.5703125" style="12" customWidth="1"/>
+    <col min="81" max="81" width="9.5703125" style="13" customWidth="1"/>
     <col min="82" max="112" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" s="14" customFormat="1" ht="14" customHeight="1">
-      <c r="A1" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="45" t="s">
+    <row r="1" spans="1:112" s="16" customFormat="1">
+      <c r="A1" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E1" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="17" t="s">
+      <c r="D1" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="K1" s="16" t="s">
+      <c r="J1" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="16" t="s">
-        <v>133</v>
+      <c r="M1" s="18" t="s">
+        <v>129</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="P1" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="16"/>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="16"/>
-      <c r="AL1" s="16"/>
-      <c r="AM1" s="16"/>
-      <c r="AN1" s="16"/>
+      <c r="O1" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="P1" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="18"/>
+      <c r="AH1" s="18"/>
+      <c r="AI1" s="18"/>
+      <c r="AJ1" s="18"/>
+      <c r="AK1" s="18"/>
+      <c r="AL1" s="18"/>
+      <c r="AM1" s="18"/>
+      <c r="AN1" s="18"/>
       <c r="AO1" s="8"/>
       <c r="AP1" s="8"/>
       <c r="AQ1" s="8"/>
@@ -9806,67 +9545,67 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="8.5703125" style="10"/>
-    <col min="3" max="3" width="13.42578125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="19" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="19" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="19" customWidth="1"/>
+    <col min="1" max="2" width="8.5703125" style="11"/>
+    <col min="3" max="3" width="13.42578125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="21" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="21" customWidth="1"/>
     <col min="9" max="9" width="14.140625" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" customWidth="1"/>
     <col min="11" max="11" width="8.140625" customWidth="1"/>
     <col min="12" max="12" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="23" customFormat="1">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:16" s="25" customFormat="1">
+      <c r="A1" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="F1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="G1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="H1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="J1" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="K1" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="L1" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="71" t="s">
+      <c r="M1" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="71" t="s">
+      <c r="N1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="O1" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="P1" s="25" t="s">
         <v>50</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="O1" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="P1" s="23" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -9895,59 +9634,59 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="10"/>
+    <col min="1" max="1" width="9.5703125" style="11"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="5" width="14.42578125" style="12" customWidth="1"/>
+    <col min="4" max="5" width="14.42578125" style="13" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="7" width="26.42578125" customWidth="1"/>
     <col min="8" max="8" width="21.42578125" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="19.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="25.42578125" style="47" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="47" customWidth="1"/>
+    <col min="12" max="12" width="25.42578125" style="49" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="26" customFormat="1">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:13" s="28" customFormat="1">
+      <c r="A1" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="H1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="I1" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="J1" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="25" t="s">
+      <c r="K1" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="L1" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="M1" s="48" t="s">
         <v>61</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="L1" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="46" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -9980,57 +9719,57 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="11" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="12" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="12" style="12" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="13" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="13" customWidth="1"/>
+    <col min="11" max="11" width="12" style="13" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="25" customFormat="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" s="27" customFormat="1">
+      <c r="A1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="I1" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="25" t="s">
+      <c r="J1" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="27" t="s">
+      <c r="K1" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="L1" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="27" t="s">
         <v>70</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="25" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -10061,13 +9800,13 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="5"/>
-    <col min="2" max="2" width="7.85546875" style="60" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="64" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" style="5"/>
-    <col min="5" max="5" width="8.42578125" style="60" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="64" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" style="5"/>
-    <col min="8" max="8" width="24.140625" style="62" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" style="66" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" style="5"/>
     <col min="10" max="10" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" style="5" customWidth="1"/>
@@ -10076,57 +9815,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="84"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="84" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="65"/>
+      <c r="J1" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="62" customFormat="1">
+      <c r="A2" s="77" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="78" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="88" t="s">
+      <c r="D2" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="61"/>
-      <c r="J1" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="58" customFormat="1">
-      <c r="A2" s="72" t="s">
+      <c r="E2" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="I2" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="J2" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="72" t="s">
+      <c r="K2" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="59" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="57" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="H2" s="59" t="s">
+      <c r="L2" s="61" t="s">
         <v>81</v>
-      </c>
-      <c r="I2" s="57" t="s">
-        <v>82</v>
-      </c>
-      <c r="J2" s="57" t="s">
-        <v>83</v>
-      </c>
-      <c r="K2" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="L2" s="57" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TM-6724 Rearranged the columns in the Asset Export Spreadsheet template
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="13120" tabRatio="782"/>
+    <workbookView xWindow="100" yWindow="0" windowWidth="25760" windowHeight="15620" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Comments!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Databases!$A$1:$DI$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Dependencies!$A$1:$P$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Devices!$A$1:$EI$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Devices!$A$1:$EH$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Rack!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Room!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Storage!$A$1:$DH$1</definedName>
@@ -56,7 +56,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="M1" authorId="0">
+    <comment ref="S1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="T1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -112,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="AC1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="176">
   <si>
     <t>Customer:</t>
   </si>
@@ -839,7 +839,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -885,6 +885,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -975,7 +981,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1568">
+  <cellStyleXfs count="1608">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -5866,6 +5872,46 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -5875,33 +5921,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -5936,76 +5959,105 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1539" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1049"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="17" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="17" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1049"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="1539" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1049" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1568">
+  <cellStyles count="1608">
     <cellStyle name="_JDI DCM Runbook Hour by Hour EMA Comm Systems (Bundle 2) 11-JUL-07" xfId="1"/>
     <cellStyle name="_JDI DCM Runbook Hour by Hour EMA Comm Systems (Bundle 2) 11-JUL-07_Title" xfId="2"/>
     <cellStyle name="_Momentive Migration Runbook Move Event 2B 09-08-2007 v2 31" xfId="3"/>
@@ -6225,6 +6277,26 @@
     <cellStyle name="Followed Hyperlink" xfId="1563" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1565" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1567" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1569" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1571" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1573" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1575" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1577" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1579" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1581" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1583" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1585" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1587" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1589" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1591" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1593" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1595" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1597" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1599" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1601" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1603" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1605" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1607" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1540" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1542" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1544" builtinId="8" hidden="1"/>
@@ -6239,6 +6311,26 @@
     <cellStyle name="Hyperlink" xfId="1562" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1564" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1566" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1568" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1570" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1574" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1576" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1578" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1580" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1582" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1584" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1586" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1588" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1590" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1592" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1600" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1602" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1604" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1606" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 10" xfId="206"/>
     <cellStyle name="Hyperlink 11" xfId="207"/>
     <cellStyle name="Hyperlink 12" xfId="208"/>
@@ -8097,7 +8189,7 @@
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
@@ -8105,7 +8197,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -8113,7 +8205,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="32" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -8121,7 +8213,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="32" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -8129,7 +8221,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="32" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -8137,15 +8229,15 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="11">
         <v>38295</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="32" t="s">
         <v>125</v>
       </c>
       <c r="B9" t="s">
@@ -8153,7 +8245,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="32" t="s">
         <v>126</v>
       </c>
       <c r="B10" t="s">
@@ -8167,102 +8259,102 @@
       <c r="B12" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
         <v>123</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
       <c r="F15" s="82" t="s">
         <v>87</v>
       </c>
       <c r="G15" s="82"/>
     </row>
     <row r="16" spans="1:7" ht="28" customHeight="1">
-      <c r="A16" s="35"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="81" t="s">
         <v>88</v>
       </c>
       <c r="C16" s="81"/>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="60" t="s">
+      <c r="F16" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G16" s="15" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="20" customHeight="1">
-      <c r="A17" s="38">
+      <c r="A17" s="17">
         <f>COUNTA(Applications!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="19">
         <f>COUNTA(Applications!A:A)-1</f>
         <v>0</v>
       </c>
-      <c r="E17" s="40">
+      <c r="E17" s="19">
         <f>A17-D17</f>
         <v>0</v>
       </c>
-      <c r="F17" s="41">
+      <c r="F17" s="20">
         <f>COUNTIF(Applications!B:EH,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="G17" s="41">
+      <c r="G17" s="20">
         <f>COUNTIF(Applications!B:EI,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Applications!B:EI,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Applications!B:EI,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Applications!B:EI,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="I17" s="38" t="s">
+      <c r="I17" s="17" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="20" customHeight="1">
       <c r="A18">
-        <f>COUNTIF(Applications!R:R,"Master")</f>
+        <f>COUNTIF(Applications!D:D,"Master")</f>
         <v>0</v>
       </c>
       <c r="B18" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="42">
-        <f>COUNTIFS(Applications!A:A,"&gt;0",Applications!R:R,"Master")</f>
+      <c r="D18" s="21">
+        <f>COUNTIFS(Applications!A:A,"&gt;0",Applications!D:D,"Master")</f>
         <v>0</v>
       </c>
-      <c r="E18" s="42">
-        <f>COUNTIFS(Applications!B:B,"&lt;&gt;''",Applications!R:R,"Master")-D18</f>
+      <c r="E18" s="21">
+        <f>COUNTIFS(Applications!B:B,"&lt;&gt;''",Applications!D:D,"Master")-D18</f>
         <v>0</v>
       </c>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
       <c r="I18" t="s">
         <v>110</v>
       </c>
@@ -8275,17 +8367,17 @@
       <c r="B19" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="42">
+      <c r="D19" s="21">
         <f>IF(ISNUMBER(D17),D17-D18,"")</f>
         <v>0</v>
       </c>
-      <c r="E19" s="42">
+      <c r="E19" s="21">
         <f>IF(ISNUMBER(E17),E17-E18,"")</f>
         <v>0</v>
       </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="I19" s="57" t="s">
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="I19" s="27" t="s">
         <v>111</v>
       </c>
       <c r="J19" t="s">
@@ -8296,30 +8388,30 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="20" customHeight="1">
-      <c r="A20" s="38">
+      <c r="A20" s="17">
         <f>COUNTA(Devices!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="D20" s="40">
+      <c r="D20" s="19">
         <f>COUNTA(Devices!A:A)-1</f>
         <v>0</v>
       </c>
-      <c r="E20" s="40">
+      <c r="E20" s="19">
         <f>A20-D20</f>
         <v>0</v>
       </c>
-      <c r="F20" s="41">
-        <f>COUNTIF(Devices!B:EI,REPT("?",254)&amp;"*")</f>
+      <c r="F20" s="20">
+        <f>COUNTIF(Devices!B:EH,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="G20" s="41">
-        <f>COUNTIF(Devices!B:EJ,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Devices!B:EJ,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Devices!B:EJ,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Devices!B:EJ,"*"&amp;CHAR(39)&amp;"*")</f>
+      <c r="G20" s="20">
+        <f>COUNTIF(Devices!B:EI,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Devices!B:EI,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Devices!B:EI,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Devices!B:EI,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="I20" s="58" t="s">
+      <c r="I20" s="28" t="s">
         <v>112</v>
       </c>
       <c r="J20" t="s">
@@ -8331,94 +8423,94 @@
     </row>
     <row r="21" spans="1:11" ht="20" customHeight="1">
       <c r="A21">
-        <f>COUNTIF(Devices!J:J,"Server")+COUNTIF(Devices!J:J,"VM")+COUNTIF(Devices!J:J,"Blade")+COUNTIF(Devices!J:J,"Appliance")</f>
+        <f>COUNTIF(Devices!P:P,"Server")+COUNTIF(Devices!P:P,"VM")+COUNTIF(Devices!P:P,"Blade")+COUNTIF(Devices!P:P,"Appliance")</f>
         <v>0</v>
       </c>
       <c r="B21" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="42">
-        <f>COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!J:J,"Server")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!J:J,"Blade")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!J:J,"VM")++COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!J:J,"Appliance")</f>
+      <c r="D21" s="21">
+        <f>COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!P:P,"Server")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!P:P,"Blade")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!P:P,"VM")++COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!P:P,"Appliance")</f>
         <v>0</v>
       </c>
-      <c r="E21" s="42">
-        <f>COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!J:J,"Server")+COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!J:J,"Blade")+COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!J:J,"VM")++COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!J:J,"Appliance")</f>
+      <c r="E21" s="21">
+        <f>COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!P:P,"Server")+COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!P:P,"Blade")+COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!P:P,"VM")++COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!P:P,"Appliance")</f>
         <v>0</v>
       </c>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
     </row>
     <row r="22" spans="1:11" ht="20" customHeight="1">
-      <c r="A22" s="38">
+      <c r="A22" s="17">
         <f>COUNTA(Databases!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="19">
         <f>COUNTA(Databases!A:A)-1</f>
         <v>0</v>
       </c>
-      <c r="E22" s="40">
+      <c r="E22" s="19">
         <f>A22-D22</f>
         <v>0</v>
       </c>
-      <c r="F22" s="41">
+      <c r="F22" s="20">
         <f>COUNTIF(Databases!B:EJ,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="G22" s="41">
+      <c r="G22" s="20">
         <f>COUNTIF(Databases!B:EK,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Databases!B:EK,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Databases!B:EK,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Databases!B:EK,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="20" customHeight="1">
-      <c r="A23" s="38">
+      <c r="A23" s="17">
         <f>COUNTA(Storage!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="40">
+      <c r="D23" s="19">
         <f>COUNTA(Storage!A:A)-1</f>
         <v>0</v>
       </c>
-      <c r="E23" s="40">
+      <c r="E23" s="19">
         <f>A23-D23</f>
         <v>0</v>
       </c>
-      <c r="F23" s="41">
+      <c r="F23" s="20">
         <f>COUNTIF(Storage!B:EI,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="G23" s="41">
+      <c r="G23" s="20">
         <f>COUNTIF(Storage!B:EJ,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Storage!B:EJ,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Storage!B:EJ,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Storage!B:EJ,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="20" customHeight="1">
-      <c r="A24" s="38">
+      <c r="A24" s="17">
         <f>COUNTA(Dependencies!D:D)-1</f>
         <v>0</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="D24" s="40">
+      <c r="D24" s="19">
         <f>COUNTA(Dependencies!A:A)-1</f>
         <v>0</v>
       </c>
-      <c r="E24" s="40">
+      <c r="E24" s="19">
         <f>A24-D24</f>
         <v>0</v>
       </c>
-      <c r="F24" s="41">
+      <c r="F24" s="20">
         <f>COUNTIF(Storage!B:EI,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="G24" s="44">
+      <c r="G24" s="23">
         <f>COUNTIF(Dependencies!B:EL,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Dependencies!B:EL,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Dependencies!B:EL,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Dependencies!B:EL,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
@@ -8431,10 +8523,10 @@
       <c r="B25" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
     </row>
     <row r="26" spans="1:11" ht="20" customHeight="1">
       <c r="A26">
@@ -8444,10 +8536,10 @@
       <c r="B26" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:11" ht="20" customHeight="1">
       <c r="A27">
@@ -8457,10 +8549,10 @@
       <c r="B27" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
     </row>
     <row r="28" spans="1:11" ht="20" customHeight="1">
       <c r="A28">
@@ -8470,10 +8562,10 @@
       <c r="B28" t="s">
         <v>103</v>
       </c>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:11" ht="20" customHeight="1">
       <c r="A29">
@@ -8483,10 +8575,10 @@
       <c r="B29" t="s">
         <v>104</v>
       </c>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
     </row>
     <row r="30" spans="1:11" ht="20" customHeight="1">
       <c r="A30">
@@ -8496,62 +8588,62 @@
       <c r="B30" t="s">
         <v>105</v>
       </c>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
     </row>
     <row r="31" spans="1:11" ht="20" customHeight="1">
-      <c r="A31" s="38">
+      <c r="A31" s="17">
         <f>COUNTA(Room!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
     </row>
     <row r="32" spans="1:11" ht="20" customHeight="1">
-      <c r="A32" s="38">
+      <c r="A32" s="17">
         <f>COUNTA(Rack!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
     </row>
     <row r="33" spans="1:7" ht="20" customHeight="1">
-      <c r="A33" s="38">
+      <c r="A33" s="17">
         <f>COUNTA(Cabling!B:B)-2</f>
         <v>0</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
     </row>
     <row r="34" spans="1:7" ht="20" customHeight="1">
-      <c r="A34" s="39">
+      <c r="A34" s="18">
         <f>COUNTA(Comments!B:B)-1</f>
         <v>0</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
@@ -8619,32 +8711,32 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="16" style="11" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="21" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" style="21" customWidth="1"/>
-    <col min="7" max="16384" width="9.5703125" style="21"/>
+    <col min="1" max="1" width="16.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16" style="7" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" style="10" customWidth="1"/>
+    <col min="7" max="16384" width="9.5703125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:6" s="78" customFormat="1">
+      <c r="A1" s="75" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="75" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="75" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="77" t="s">
         <v>86</v>
       </c>
     </row>
@@ -8675,24 +8767,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="5" width="19.42578125" style="69" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="69"/>
+    <col min="1" max="5" width="19.42578125" style="33" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="68" t="s">
+    <row r="1" spans="1:5" s="80" customFormat="1">
+      <c r="A1" s="79" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="79" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="79" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="79" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="79" t="s">
         <v>131</v>
       </c>
     </row>
@@ -8717,239 +8809,243 @@
   <dimension ref="A1:EH1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="2"/>
-    <col min="15" max="15" width="9.5703125" style="12"/>
-    <col min="16" max="16" width="11.85546875" style="12" customWidth="1"/>
-    <col min="20" max="20" width="11.140625" customWidth="1"/>
-    <col min="22" max="22" width="9.5703125" style="11"/>
-    <col min="31" max="31" width="9.85546875" style="11" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" customWidth="1"/>
-    <col min="33" max="33" width="13.42578125" customWidth="1"/>
-    <col min="34" max="34" width="16.140625" style="11" customWidth="1"/>
-    <col min="35" max="35" width="9.42578125" customWidth="1"/>
-    <col min="36" max="36" width="11.42578125" customWidth="1"/>
-    <col min="37" max="37" width="13.42578125" style="11" customWidth="1"/>
-    <col min="38" max="38" width="8.5703125" customWidth="1"/>
-    <col min="39" max="39" width="10.42578125" customWidth="1"/>
-    <col min="40" max="40" width="13.42578125" style="55" customWidth="1"/>
-    <col min="41" max="41" width="11.85546875" style="11" customWidth="1"/>
-    <col min="42" max="42" width="12.140625" style="71" customWidth="1"/>
+    <col min="4" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" style="34" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="2"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="18" max="20" width="12.85546875" customWidth="1"/>
+    <col min="21" max="21" width="9.5703125" style="8"/>
+    <col min="22" max="22" width="11.85546875" style="8" customWidth="1"/>
+    <col min="25" max="25" width="9.5703125" style="7"/>
+    <col min="34" max="34" width="11.42578125" customWidth="1"/>
+    <col min="35" max="35" width="13.42578125" customWidth="1"/>
+    <col min="36" max="36" width="16.140625" style="7" customWidth="1"/>
+    <col min="37" max="37" width="10.5703125" customWidth="1"/>
+    <col min="38" max="38" width="12.85546875" customWidth="1"/>
+    <col min="39" max="39" width="14.42578125" style="7" customWidth="1"/>
+    <col min="40" max="40" width="10.85546875" customWidth="1"/>
+    <col min="41" max="41" width="11.85546875" customWidth="1"/>
+    <col min="42" max="42" width="13.42578125" style="26" customWidth="1"/>
     <col min="43" max="70" width="9.5703125" customWidth="1"/>
-    <col min="71" max="71" width="9.5703125" style="13" customWidth="1"/>
+    <col min="71" max="71" width="9.5703125" style="9" customWidth="1"/>
     <col min="72" max="106" width="9.5703125" customWidth="1"/>
-    <col min="107" max="107" width="9.5703125" style="13" customWidth="1"/>
+    <col min="107" max="107" width="9.5703125" style="9" customWidth="1"/>
     <col min="108" max="138" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:138" s="16" customFormat="1">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:138" s="47" customFormat="1">
+      <c r="A1" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="54" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="73" t="s">
+      <c r="L1" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="M1" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="N1" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="O1" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="P1" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="Q1" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="L1" s="79" t="s">
+      <c r="R1" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="M1" s="79" t="s">
+      <c r="S1" s="56" t="s">
         <v>134</v>
       </c>
-      <c r="N1" s="79" t="s">
+      <c r="T1" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="80" t="s">
+      <c r="U1" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="P1" s="80" t="s">
+      <c r="V1" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="W1" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="15" t="s">
+      <c r="X1" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="V1" s="53" t="s">
+      <c r="Y1" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="Z1" s="54" t="s">
         <v>140</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="AA1" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="AB1" s="54" t="s">
         <v>142</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="AC1" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="AA1" s="16" t="s">
+      <c r="AD1" s="47" t="s">
         <v>144</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AE1" s="47" t="s">
         <v>145</v>
       </c>
-      <c r="AC1" s="16" t="s">
+      <c r="AF1" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="AD1" s="16" t="s">
+      <c r="AG1" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="AE1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AH1" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AI1" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="AH1" s="54" t="s">
+      <c r="AJ1" s="59" t="s">
         <v>150</v>
       </c>
-      <c r="AI1" s="17" t="s">
+      <c r="AK1" s="60" t="s">
         <v>151</v>
       </c>
-      <c r="AJ1" s="17" t="s">
+      <c r="AL1" s="60" t="s">
         <v>152</v>
       </c>
-      <c r="AK1" s="54" t="s">
+      <c r="AM1" s="59" t="s">
         <v>153</v>
       </c>
-      <c r="AL1" s="17" t="s">
+      <c r="AN1" s="60" t="s">
         <v>154</v>
       </c>
-      <c r="AM1" s="17" t="s">
+      <c r="AO1" s="60" t="s">
         <v>155</v>
       </c>
-      <c r="AN1" s="54" t="s">
+      <c r="AP1" s="59" t="s">
         <v>156</v>
       </c>
-      <c r="AO1" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="AP1" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="BO1" s="8"/>
-      <c r="BP1" s="8"/>
-      <c r="BQ1" s="8"/>
-      <c r="BR1" s="8"/>
-      <c r="BS1" s="8"/>
-      <c r="BT1" s="8"/>
-      <c r="BU1" s="8"/>
-      <c r="BV1" s="8"/>
-      <c r="BW1" s="8"/>
-      <c r="BX1" s="8"/>
-      <c r="BY1" s="8"/>
-      <c r="BZ1" s="8"/>
-      <c r="CA1" s="8"/>
-      <c r="CB1" s="8"/>
-      <c r="CC1" s="8"/>
-      <c r="CD1" s="8"/>
-      <c r="CE1" s="8"/>
-      <c r="CF1" s="8"/>
-      <c r="CG1" s="8"/>
-      <c r="CH1" s="8"/>
-      <c r="CI1" s="8"/>
-      <c r="CJ1" s="8"/>
-      <c r="CK1" s="8"/>
-      <c r="CL1" s="8"/>
-      <c r="CM1" s="8"/>
-      <c r="CN1" s="8"/>
-      <c r="CO1" s="8"/>
-      <c r="CP1" s="8"/>
-      <c r="CQ1" s="8"/>
-      <c r="CR1" s="8"/>
-      <c r="CS1" s="8"/>
-      <c r="CT1" s="8"/>
-      <c r="CU1" s="8"/>
-      <c r="CV1" s="8"/>
-      <c r="CW1" s="8"/>
-      <c r="CX1" s="8"/>
-      <c r="CY1" s="8"/>
-      <c r="CZ1" s="8"/>
-      <c r="DA1" s="8"/>
-      <c r="DB1" s="8"/>
-      <c r="DC1" s="8"/>
-      <c r="DD1" s="8"/>
-      <c r="DE1" s="8"/>
-      <c r="DF1" s="8"/>
-      <c r="DG1" s="8"/>
-      <c r="DH1" s="8"/>
-      <c r="DI1" s="8"/>
-      <c r="DJ1" s="8"/>
-      <c r="DK1" s="8"/>
-      <c r="DL1" s="8"/>
-      <c r="DM1" s="8"/>
-      <c r="DN1" s="8"/>
-      <c r="DO1" s="8"/>
-      <c r="DP1" s="8"/>
-      <c r="DQ1" s="8"/>
-      <c r="DR1" s="8"/>
-      <c r="DS1" s="8"/>
-      <c r="DT1" s="8"/>
-      <c r="DU1" s="8"/>
-      <c r="DV1" s="8"/>
-      <c r="DW1" s="8"/>
-      <c r="DX1" s="8"/>
-      <c r="DY1" s="8"/>
-      <c r="DZ1" s="8"/>
-      <c r="EA1" s="8"/>
-      <c r="EB1" s="8"/>
-      <c r="EC1" s="8"/>
-      <c r="ED1" s="8"/>
-      <c r="EE1" s="8"/>
-      <c r="EF1" s="8"/>
-      <c r="EG1" s="8"/>
-      <c r="EH1" s="8"/>
+      <c r="BO1" s="46"/>
+      <c r="BP1" s="46"/>
+      <c r="BQ1" s="46"/>
+      <c r="BR1" s="46"/>
+      <c r="BS1" s="46"/>
+      <c r="BT1" s="46"/>
+      <c r="BU1" s="46"/>
+      <c r="BV1" s="46"/>
+      <c r="BW1" s="46"/>
+      <c r="BX1" s="46"/>
+      <c r="BY1" s="46"/>
+      <c r="BZ1" s="46"/>
+      <c r="CA1" s="46"/>
+      <c r="CB1" s="46"/>
+      <c r="CC1" s="46"/>
+      <c r="CD1" s="46"/>
+      <c r="CE1" s="46"/>
+      <c r="CF1" s="46"/>
+      <c r="CG1" s="46"/>
+      <c r="CH1" s="46"/>
+      <c r="CI1" s="46"/>
+      <c r="CJ1" s="46"/>
+      <c r="CK1" s="46"/>
+      <c r="CL1" s="46"/>
+      <c r="CM1" s="46"/>
+      <c r="CN1" s="46"/>
+      <c r="CO1" s="46"/>
+      <c r="CP1" s="46"/>
+      <c r="CQ1" s="46"/>
+      <c r="CR1" s="46"/>
+      <c r="CS1" s="46"/>
+      <c r="CT1" s="46"/>
+      <c r="CU1" s="46"/>
+      <c r="CV1" s="46"/>
+      <c r="CW1" s="46"/>
+      <c r="CX1" s="46"/>
+      <c r="CY1" s="46"/>
+      <c r="CZ1" s="46"/>
+      <c r="DA1" s="46"/>
+      <c r="DB1" s="46"/>
+      <c r="DC1" s="46"/>
+      <c r="DD1" s="46"/>
+      <c r="DE1" s="46"/>
+      <c r="DF1" s="46"/>
+      <c r="DG1" s="46"/>
+      <c r="DH1" s="46"/>
+      <c r="DI1" s="46"/>
+      <c r="DJ1" s="46"/>
+      <c r="DK1" s="46"/>
+      <c r="DL1" s="46"/>
+      <c r="DM1" s="46"/>
+      <c r="DN1" s="46"/>
+      <c r="DO1" s="46"/>
+      <c r="DP1" s="46"/>
+      <c r="DQ1" s="46"/>
+      <c r="DR1" s="46"/>
+      <c r="DS1" s="46"/>
+      <c r="DT1" s="46"/>
+      <c r="DU1" s="46"/>
+      <c r="DV1" s="46"/>
+      <c r="DW1" s="46"/>
+      <c r="DX1" s="46"/>
+      <c r="DY1" s="46"/>
+      <c r="DZ1" s="46"/>
+      <c r="EA1" s="46"/>
+      <c r="EB1" s="46"/>
+      <c r="EC1" s="46"/>
+      <c r="ED1" s="46"/>
+      <c r="EE1" s="46"/>
+      <c r="EF1" s="46"/>
+      <c r="EG1" s="46"/>
+      <c r="EH1" s="46"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -8973,7 +9069,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DG1"/>
+  <dimension ref="A1:DF1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -8984,183 +9080,183 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="4" customWidth="1"/>
     <col min="2" max="3" width="20.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13" style="5" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="5" customWidth="1"/>
-    <col min="13" max="14" width="10.42578125" style="5" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" style="5" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="11.42578125" style="5" customWidth="1"/>
-    <col min="18" max="18" width="18.85546875" style="4" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" style="5" customWidth="1"/>
-    <col min="20" max="20" width="8.42578125" style="5" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="5" customWidth="1"/>
-    <col min="22" max="22" width="11" style="5"/>
-    <col min="23" max="23" width="10" style="4" customWidth="1"/>
-    <col min="24" max="24" width="11" style="5"/>
-    <col min="25" max="25" width="15.5703125" style="4" customWidth="1"/>
-    <col min="26" max="26" width="12.140625" style="5" customWidth="1"/>
-    <col min="27" max="27" width="12" style="6" customWidth="1"/>
-    <col min="28" max="28" width="11" style="6"/>
-    <col min="29" max="29" width="12.85546875" style="5" customWidth="1"/>
-    <col min="30" max="32" width="11" style="5"/>
-    <col min="33" max="33" width="8.85546875" style="5" customWidth="1"/>
-    <col min="34" max="36" width="11" style="5"/>
-    <col min="37" max="38" width="11" style="4"/>
-    <col min="39" max="39" width="12.85546875" style="4" customWidth="1"/>
-    <col min="40" max="41" width="8.5703125" style="4" customWidth="1"/>
-    <col min="42" max="42" width="14" style="4" customWidth="1"/>
-    <col min="43" max="43" width="12.140625" style="72" customWidth="1"/>
-    <col min="44" max="108" width="9.5703125" style="5" customWidth="1"/>
-    <col min="109" max="109" width="9.5703125" style="4" customWidth="1"/>
-    <col min="110" max="110" width="9.5703125" style="5" customWidth="1"/>
-    <col min="111" max="111" width="9.5703125" style="4" customWidth="1"/>
-    <col min="112" max="139" width="9.5703125" style="5" customWidth="1"/>
-    <col min="140" max="16384" width="11" style="5"/>
+    <col min="4" max="4" width="15.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="36" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="13" style="5" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" style="5" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" style="5" customWidth="1"/>
+    <col min="19" max="20" width="10.42578125" style="5" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" style="5" customWidth="1"/>
+    <col min="22" max="22" width="10.42578125" style="4" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" style="5" customWidth="1"/>
+    <col min="24" max="24" width="18.85546875" style="4" customWidth="1"/>
+    <col min="25" max="25" width="13.42578125" style="5" customWidth="1"/>
+    <col min="26" max="26" width="8.42578125" style="5" customWidth="1"/>
+    <col min="27" max="27" width="11.42578125" style="5" customWidth="1"/>
+    <col min="28" max="28" width="11" style="5"/>
+    <col min="29" max="29" width="10" style="4" customWidth="1"/>
+    <col min="30" max="30" width="11" style="5"/>
+    <col min="31" max="31" width="15.5703125" style="4" customWidth="1"/>
+    <col min="32" max="32" width="12.140625" style="5" customWidth="1"/>
+    <col min="33" max="33" width="12" style="6" customWidth="1"/>
+    <col min="34" max="34" width="9.28515625" style="5" customWidth="1"/>
+    <col min="35" max="35" width="11" style="5"/>
+    <col min="36" max="36" width="8.85546875" style="5" customWidth="1"/>
+    <col min="37" max="39" width="11" style="5"/>
+    <col min="40" max="40" width="12.85546875" style="4" customWidth="1"/>
+    <col min="41" max="41" width="8.5703125" style="4" customWidth="1"/>
+    <col min="42" max="42" width="10.140625" style="4" customWidth="1"/>
+    <col min="43" max="107" width="9.5703125" style="5" customWidth="1"/>
+    <col min="108" max="108" width="9.5703125" style="4" customWidth="1"/>
+    <col min="109" max="109" width="9.5703125" style="5" customWidth="1"/>
+    <col min="110" max="110" width="9.5703125" style="4" customWidth="1"/>
+    <col min="111" max="138" width="9.5703125" style="5" customWidth="1"/>
+    <col min="139" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="8" customFormat="1">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:42" s="46" customFormat="1">
+      <c r="A1" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="L1" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="M1" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="N1" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="O1" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="P1" s="46" t="s">
         <v>161</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="Q1" s="46" t="s">
         <v>162</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="R1" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="S1" s="46" t="s">
         <v>163</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="T1" s="46" t="s">
         <v>164</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="U1" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="V1" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="W1" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="X1" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="Y1" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="Z1" s="46" t="s">
         <v>169</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="AA1" s="46" t="s">
         <v>170</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="AB1" s="46" t="s">
         <v>171</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="AC1" s="51" t="s">
         <v>172</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="AD1" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AE1" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AF1" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AG1" s="50" t="s">
         <v>138</v>
       </c>
-      <c r="AB1" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AH1" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="AD1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE1" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AI1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AJ1" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AK1" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AL1" s="46" t="s">
         <v>173</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AM1" s="46" t="s">
         <v>174</v>
       </c>
-      <c r="AK1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL1" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AN1" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="AN1" s="10" t="s">
+      <c r="AO1" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AP1" s="46" t="s">
         <v>25</v>
-      </c>
-      <c r="AP1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="AQ1" s="70" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <autoFilter ref="A1:EI1"/>
+  <autoFilter ref="A1:EH1"/>
   <pageMargins left="0.25" right="0.25" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>
@@ -9177,156 +9273,157 @@
   <dimension ref="A1:DI1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="11"/>
-    <col min="8" max="8" width="16.42578125" style="11" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" style="12"/>
-    <col min="11" max="11" width="16.140625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" style="11" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" style="11" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" style="32" customWidth="1"/>
+    <col min="4" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="7"/>
+    <col min="13" max="13" width="7.140625" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="7" customWidth="1"/>
+    <col min="16" max="17" width="12.85546875" style="8" customWidth="1"/>
     <col min="18" max="41" width="9.5703125" customWidth="1"/>
-    <col min="42" max="42" width="9.5703125" style="13" customWidth="1"/>
+    <col min="42" max="42" width="9.5703125" style="9" customWidth="1"/>
     <col min="43" max="81" width="9.5703125" customWidth="1"/>
-    <col min="82" max="82" width="9.5703125" style="13"/>
+    <col min="82" max="82" width="9.5703125" style="9"/>
     <col min="84" max="85" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" s="16" customFormat="1">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:113" s="47" customFormat="1">
+      <c r="A1" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="L1" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="M1" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="N1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="O1" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="P1" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="Q1" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="L1" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q1" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="AP1" s="8"/>
-      <c r="AQ1" s="8"/>
-      <c r="AR1" s="8"/>
-      <c r="AS1" s="8"/>
-      <c r="AT1" s="8"/>
-      <c r="AU1" s="8"/>
-      <c r="AV1" s="8"/>
-      <c r="AW1" s="8"/>
-      <c r="AX1" s="8"/>
-      <c r="AY1" s="8"/>
-      <c r="AZ1" s="8"/>
-      <c r="BA1" s="8"/>
-      <c r="BB1" s="8"/>
-      <c r="BC1" s="8"/>
-      <c r="BD1" s="8"/>
-      <c r="BE1" s="8"/>
-      <c r="BF1" s="8"/>
-      <c r="BG1" s="8"/>
-      <c r="BH1" s="8"/>
-      <c r="BI1" s="8"/>
-      <c r="BJ1" s="8"/>
-      <c r="BK1" s="8"/>
-      <c r="BL1" s="8"/>
-      <c r="BM1" s="8"/>
-      <c r="BN1" s="8"/>
-      <c r="BO1" s="8"/>
-      <c r="BP1" s="8"/>
-      <c r="BQ1" s="8"/>
-      <c r="BR1" s="8"/>
-      <c r="BS1" s="8"/>
-      <c r="BT1" s="8"/>
-      <c r="BU1" s="8"/>
-      <c r="BV1" s="8"/>
-      <c r="BW1" s="8"/>
-      <c r="BX1" s="8"/>
-      <c r="BY1" s="8"/>
-      <c r="BZ1" s="8"/>
-      <c r="CA1" s="8"/>
-      <c r="CB1" s="8"/>
-      <c r="CC1" s="8"/>
-      <c r="CD1" s="8"/>
-      <c r="CE1" s="8"/>
-      <c r="CF1" s="8"/>
-      <c r="CG1" s="8"/>
-      <c r="CH1" s="8"/>
-      <c r="CI1" s="8"/>
-      <c r="CJ1" s="8"/>
-      <c r="CK1" s="8"/>
-      <c r="CL1" s="8"/>
-      <c r="CM1" s="8"/>
-      <c r="CN1" s="8"/>
-      <c r="CO1" s="8"/>
-      <c r="CP1" s="8"/>
-      <c r="CQ1" s="8"/>
-      <c r="CR1" s="8"/>
-      <c r="CS1" s="8"/>
-      <c r="CT1" s="8"/>
-      <c r="CU1" s="8"/>
-      <c r="CV1" s="8"/>
-      <c r="CW1" s="8"/>
-      <c r="CX1" s="8"/>
-      <c r="CY1" s="8"/>
-      <c r="CZ1" s="8"/>
-      <c r="DA1" s="8"/>
-      <c r="DB1" s="8"/>
-      <c r="DC1" s="8"/>
-      <c r="DD1" s="8"/>
-      <c r="DE1" s="8"/>
-      <c r="DF1" s="8"/>
-      <c r="DG1" s="8"/>
-      <c r="DH1" s="8"/>
-      <c r="DI1" s="8"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
+      <c r="AW1" s="46"/>
+      <c r="AX1" s="46"/>
+      <c r="AY1" s="46"/>
+      <c r="AZ1" s="46"/>
+      <c r="BA1" s="46"/>
+      <c r="BB1" s="46"/>
+      <c r="BC1" s="46"/>
+      <c r="BD1" s="46"/>
+      <c r="BE1" s="46"/>
+      <c r="BF1" s="46"/>
+      <c r="BG1" s="46"/>
+      <c r="BH1" s="46"/>
+      <c r="BI1" s="46"/>
+      <c r="BJ1" s="46"/>
+      <c r="BK1" s="46"/>
+      <c r="BL1" s="46"/>
+      <c r="BM1" s="46"/>
+      <c r="BN1" s="46"/>
+      <c r="BO1" s="46"/>
+      <c r="BP1" s="46"/>
+      <c r="BQ1" s="46"/>
+      <c r="BR1" s="46"/>
+      <c r="BS1" s="46"/>
+      <c r="BT1" s="46"/>
+      <c r="BU1" s="46"/>
+      <c r="BV1" s="46"/>
+      <c r="BW1" s="46"/>
+      <c r="BX1" s="46"/>
+      <c r="BY1" s="46"/>
+      <c r="BZ1" s="46"/>
+      <c r="CA1" s="46"/>
+      <c r="CB1" s="46"/>
+      <c r="CC1" s="46"/>
+      <c r="CD1" s="46"/>
+      <c r="CE1" s="46"/>
+      <c r="CF1" s="46"/>
+      <c r="CG1" s="46"/>
+      <c r="CH1" s="46"/>
+      <c r="CI1" s="46"/>
+      <c r="CJ1" s="46"/>
+      <c r="CK1" s="46"/>
+      <c r="CL1" s="46"/>
+      <c r="CM1" s="46"/>
+      <c r="CN1" s="46"/>
+      <c r="CO1" s="46"/>
+      <c r="CP1" s="46"/>
+      <c r="CQ1" s="46"/>
+      <c r="CR1" s="46"/>
+      <c r="CS1" s="46"/>
+      <c r="CT1" s="46"/>
+      <c r="CU1" s="46"/>
+      <c r="CV1" s="46"/>
+      <c r="CW1" s="46"/>
+      <c r="CX1" s="46"/>
+      <c r="CY1" s="46"/>
+      <c r="CZ1" s="46"/>
+      <c r="DA1" s="46"/>
+      <c r="DB1" s="46"/>
+      <c r="DC1" s="46"/>
+      <c r="DD1" s="46"/>
+      <c r="DE1" s="46"/>
+      <c r="DF1" s="46"/>
+      <c r="DG1" s="46"/>
+      <c r="DH1" s="46"/>
+      <c r="DI1" s="46"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -9350,176 +9447,179 @@
   <dimension ref="A1:DH1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="21"/>
-    <col min="7" max="7" width="8.5703125" style="11"/>
-    <col min="9" max="9" width="14.5703125" style="11" customWidth="1"/>
-    <col min="11" max="11" width="10" style="12" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="12" style="11" customWidth="1"/>
-    <col min="16" max="16" width="12" style="32" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="10"/>
+    <col min="13" max="13" width="8.5703125" style="7"/>
+    <col min="14" max="14" width="7.140625" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" style="7" customWidth="1"/>
     <col min="17" max="40" width="9.5703125" customWidth="1"/>
-    <col min="41" max="41" width="9.5703125" style="13" customWidth="1"/>
+    <col min="41" max="41" width="9.5703125" style="9" customWidth="1"/>
     <col min="42" max="80" width="9.5703125" customWidth="1"/>
-    <col min="81" max="81" width="9.5703125" style="13" customWidth="1"/>
+    <col min="81" max="81" width="9.5703125" style="9" customWidth="1"/>
     <col min="82" max="112" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" s="16" customFormat="1">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:112" s="47" customFormat="1">
+      <c r="A1" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="F1" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="L1" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="M1" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="N1" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="O1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="P1" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="P1" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="8"/>
-      <c r="AP1" s="8"/>
-      <c r="AQ1" s="8"/>
-      <c r="AR1" s="8"/>
-      <c r="AS1" s="8"/>
-      <c r="AT1" s="8"/>
-      <c r="AU1" s="8"/>
-      <c r="AV1" s="8"/>
-      <c r="AW1" s="8"/>
-      <c r="AX1" s="8"/>
-      <c r="AY1" s="8"/>
-      <c r="AZ1" s="8"/>
-      <c r="BA1" s="8"/>
-      <c r="BB1" s="8"/>
-      <c r="BC1" s="8"/>
-      <c r="BD1" s="8"/>
-      <c r="BE1" s="8"/>
-      <c r="BF1" s="8"/>
-      <c r="BG1" s="8"/>
-      <c r="BH1" s="8"/>
-      <c r="BI1" s="8"/>
-      <c r="BJ1" s="8"/>
-      <c r="BK1" s="8"/>
-      <c r="BL1" s="8"/>
-      <c r="BM1" s="8"/>
-      <c r="BN1" s="8"/>
-      <c r="BO1" s="8"/>
-      <c r="BP1" s="8"/>
-      <c r="BQ1" s="8"/>
-      <c r="BR1" s="8"/>
-      <c r="BS1" s="8"/>
-      <c r="BT1" s="8"/>
-      <c r="BU1" s="8"/>
-      <c r="BV1" s="8"/>
-      <c r="BW1" s="8"/>
-      <c r="BX1" s="8"/>
-      <c r="BY1" s="8"/>
-      <c r="BZ1" s="8"/>
-      <c r="CA1" s="8"/>
-      <c r="CB1" s="8"/>
-      <c r="CC1" s="8"/>
-      <c r="CD1" s="8"/>
-      <c r="CE1" s="8"/>
-      <c r="CF1" s="8"/>
-      <c r="CG1" s="8"/>
-      <c r="CH1" s="8"/>
-      <c r="CI1" s="8"/>
-      <c r="CJ1" s="8"/>
-      <c r="CK1" s="8"/>
-      <c r="CL1" s="8"/>
-      <c r="CM1" s="8"/>
-      <c r="CN1" s="8"/>
-      <c r="CO1" s="8"/>
-      <c r="CP1" s="8"/>
-      <c r="CQ1" s="8"/>
-      <c r="CR1" s="8"/>
-      <c r="CS1" s="8"/>
-      <c r="CT1" s="8"/>
-      <c r="CU1" s="8"/>
-      <c r="CV1" s="8"/>
-      <c r="CW1" s="8"/>
-      <c r="CX1" s="8"/>
-      <c r="CY1" s="8"/>
-      <c r="CZ1" s="8"/>
-      <c r="DA1" s="8"/>
-      <c r="DB1" s="8"/>
-      <c r="DC1" s="8"/>
-      <c r="DD1" s="8"/>
-      <c r="DE1" s="8"/>
-      <c r="DF1" s="8"/>
-      <c r="DG1" s="8"/>
-      <c r="DH1" s="8"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="39"/>
+      <c r="AD1" s="39"/>
+      <c r="AE1" s="39"/>
+      <c r="AF1" s="39"/>
+      <c r="AG1" s="39"/>
+      <c r="AH1" s="39"/>
+      <c r="AI1" s="39"/>
+      <c r="AJ1" s="39"/>
+      <c r="AK1" s="39"/>
+      <c r="AL1" s="39"/>
+      <c r="AM1" s="39"/>
+      <c r="AN1" s="39"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
+      <c r="AW1" s="46"/>
+      <c r="AX1" s="46"/>
+      <c r="AY1" s="46"/>
+      <c r="AZ1" s="46"/>
+      <c r="BA1" s="46"/>
+      <c r="BB1" s="46"/>
+      <c r="BC1" s="46"/>
+      <c r="BD1" s="46"/>
+      <c r="BE1" s="46"/>
+      <c r="BF1" s="46"/>
+      <c r="BG1" s="46"/>
+      <c r="BH1" s="46"/>
+      <c r="BI1" s="46"/>
+      <c r="BJ1" s="46"/>
+      <c r="BK1" s="46"/>
+      <c r="BL1" s="46"/>
+      <c r="BM1" s="46"/>
+      <c r="BN1" s="46"/>
+      <c r="BO1" s="46"/>
+      <c r="BP1" s="46"/>
+      <c r="BQ1" s="46"/>
+      <c r="BR1" s="46"/>
+      <c r="BS1" s="46"/>
+      <c r="BT1" s="46"/>
+      <c r="BU1" s="46"/>
+      <c r="BV1" s="46"/>
+      <c r="BW1" s="46"/>
+      <c r="BX1" s="46"/>
+      <c r="BY1" s="46"/>
+      <c r="BZ1" s="46"/>
+      <c r="CA1" s="46"/>
+      <c r="CB1" s="46"/>
+      <c r="CC1" s="46"/>
+      <c r="CD1" s="46"/>
+      <c r="CE1" s="46"/>
+      <c r="CF1" s="46"/>
+      <c r="CG1" s="46"/>
+      <c r="CH1" s="46"/>
+      <c r="CI1" s="46"/>
+      <c r="CJ1" s="46"/>
+      <c r="CK1" s="46"/>
+      <c r="CL1" s="46"/>
+      <c r="CM1" s="46"/>
+      <c r="CN1" s="46"/>
+      <c r="CO1" s="46"/>
+      <c r="CP1" s="46"/>
+      <c r="CQ1" s="46"/>
+      <c r="CR1" s="46"/>
+      <c r="CS1" s="46"/>
+      <c r="CT1" s="46"/>
+      <c r="CU1" s="46"/>
+      <c r="CV1" s="46"/>
+      <c r="CW1" s="46"/>
+      <c r="CX1" s="46"/>
+      <c r="CY1" s="46"/>
+      <c r="CZ1" s="46"/>
+      <c r="DA1" s="46"/>
+      <c r="DB1" s="46"/>
+      <c r="DC1" s="46"/>
+      <c r="DD1" s="46"/>
+      <c r="DE1" s="46"/>
+      <c r="DF1" s="46"/>
+      <c r="DG1" s="46"/>
+      <c r="DH1" s="46"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -9545,66 +9645,66 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="8.5703125" style="11"/>
-    <col min="3" max="3" width="13.42578125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="21" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="21" customWidth="1"/>
+    <col min="1" max="2" width="8.5703125" style="7"/>
+    <col min="3" max="3" width="13.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="10" customWidth="1"/>
     <col min="9" max="9" width="14.140625" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" customWidth="1"/>
     <col min="11" max="11" width="8.140625" customWidth="1"/>
     <col min="12" max="12" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="25" customFormat="1">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:16" s="39" customFormat="1">
+      <c r="A1" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="76" t="s">
+      <c r="I1" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="76" t="s">
+      <c r="J1" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="O1" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="P1" s="39" t="s">
         <v>50</v>
       </c>
     </row>
@@ -9634,58 +9734,58 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="11"/>
+    <col min="1" max="1" width="9.5703125" style="7"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="5" width="14.42578125" style="13" customWidth="1"/>
+    <col min="4" max="5" width="14.42578125" style="9" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="7" width="26.42578125" customWidth="1"/>
     <col min="8" max="8" width="21.42578125" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="19.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="25.42578125" style="49" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="49" customWidth="1"/>
+    <col min="12" max="12" width="25.42578125" style="25" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="28" customFormat="1">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:13" s="67" customFormat="1">
+      <c r="A1" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="48" t="s">
+      <c r="M1" s="66" t="s">
         <v>61</v>
       </c>
     </row>
@@ -9719,56 +9819,56 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="7" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="13" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="12" style="13" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="12" style="9" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="27" customFormat="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:13" s="64" customFormat="1">
+      <c r="A1" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="64" t="s">
         <v>70</v>
       </c>
     </row>
@@ -9800,13 +9900,13 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="5"/>
-    <col min="2" max="2" width="7.85546875" style="64" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="30" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" style="5"/>
-    <col min="5" max="5" width="8.42578125" style="64" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="30" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" style="5"/>
-    <col min="8" max="8" width="24.140625" style="66" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" style="31" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" style="5"/>
     <col min="10" max="10" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" style="5" customWidth="1"/>
@@ -9814,7 +9914,7 @@
     <col min="13" max="16384" width="9.5703125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" s="47" customFormat="1">
       <c r="B1" s="83" t="s">
         <v>71</v>
       </c>
@@ -9825,46 +9925,46 @@
       </c>
       <c r="F1" s="84"/>
       <c r="G1" s="84"/>
-      <c r="H1" s="65"/>
-      <c r="J1" s="5" t="s">
+      <c r="H1" s="69"/>
+      <c r="J1" s="47" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="62" customFormat="1">
-      <c r="A2" s="77" t="s">
+    <row r="2" spans="1:12" s="74" customFormat="1">
+      <c r="A2" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="63" t="s">
+      <c r="E2" s="72" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="61" t="s">
+      <c r="G2" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="63" t="s">
+      <c r="H2" s="72" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="61" t="s">
+      <c r="I2" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="61" t="s">
+      <c r="J2" s="73" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="61" t="s">
+      <c r="K2" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="L2" s="61" t="s">
+      <c r="L2" s="73" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TM-6715 Dropped the Usize column from the spreadsheet template
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Comments!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Databases!$A$1:$DI$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Dependencies!$A$1:$P$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Devices!$A$1:$EH$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Devices!$A$1:$EG$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Rack!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Room!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Storage!$A$1:$DH$1</definedName>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="175">
   <si>
     <t>Customer:</t>
   </si>
@@ -654,9 +654,6 @@
   </si>
   <si>
     <t>Rail Type</t>
-  </si>
-  <si>
-    <t>Usize</t>
   </si>
   <si>
     <t>Id</t>
@@ -8404,11 +8401,11 @@
         <v>0</v>
       </c>
       <c r="F20" s="20">
-        <f>COUNTIF(Devices!B:EH,REPT("?",254)&amp;"*")</f>
+        <f>COUNTIF(Devices!B:EG,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
       <c r="G20" s="20">
-        <f>COUNTIF(Devices!B:EI,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Devices!B:EI,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Devices!B:EI,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Devices!B:EI,"*"&amp;CHAR(39)&amp;"*")</f>
+        <f>COUNTIF(Devices!B:EH,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Devices!B:EH,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Devices!B:EH,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Devices!B:EH,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
       <c r="I20" s="28" t="s">
@@ -8849,7 +8846,7 @@
   <sheetData>
     <row r="1" spans="1:138" s="47" customFormat="1">
       <c r="A1" s="37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B1" s="53" t="s">
         <v>7</v>
@@ -9069,7 +9066,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DF1"/>
+  <dimension ref="A1:DE1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -9114,21 +9111,21 @@
     <col min="34" max="34" width="9.28515625" style="5" customWidth="1"/>
     <col min="35" max="35" width="11" style="5"/>
     <col min="36" max="36" width="8.85546875" style="5" customWidth="1"/>
-    <col min="37" max="39" width="11" style="5"/>
-    <col min="40" max="40" width="12.85546875" style="4" customWidth="1"/>
-    <col min="41" max="41" width="8.5703125" style="4" customWidth="1"/>
-    <col min="42" max="42" width="10.140625" style="4" customWidth="1"/>
-    <col min="43" max="107" width="9.5703125" style="5" customWidth="1"/>
-    <col min="108" max="108" width="9.5703125" style="4" customWidth="1"/>
-    <col min="109" max="109" width="9.5703125" style="5" customWidth="1"/>
-    <col min="110" max="110" width="9.5703125" style="4" customWidth="1"/>
-    <col min="111" max="138" width="9.5703125" style="5" customWidth="1"/>
-    <col min="139" max="16384" width="11" style="5"/>
+    <col min="37" max="38" width="11" style="5"/>
+    <col min="39" max="39" width="12.85546875" style="4" customWidth="1"/>
+    <col min="40" max="40" width="8.5703125" style="4" customWidth="1"/>
+    <col min="41" max="41" width="10.140625" style="4" customWidth="1"/>
+    <col min="42" max="106" width="9.5703125" style="5" customWidth="1"/>
+    <col min="107" max="107" width="9.5703125" style="4" customWidth="1"/>
+    <col min="108" max="108" width="9.5703125" style="5" customWidth="1"/>
+    <col min="109" max="109" width="9.5703125" style="4" customWidth="1"/>
+    <col min="110" max="137" width="9.5703125" style="5" customWidth="1"/>
+    <col min="138" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="46" customFormat="1">
+    <row r="1" spans="1:41" s="46" customFormat="1">
       <c r="A1" s="48" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B1" s="49" t="s">
         <v>7</v>
@@ -9241,22 +9238,19 @@
       <c r="AL1" s="46" t="s">
         <v>173</v>
       </c>
-      <c r="AM1" s="46" t="s">
-        <v>174</v>
-      </c>
-      <c r="AN1" s="51" t="s">
+      <c r="AM1" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="AO1" s="52" t="s">
+      <c r="AN1" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="AP1" s="46" t="s">
+      <c r="AO1" s="46" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <autoFilter ref="A1:EH1"/>
+  <autoFilter ref="A1:EG1"/>
   <pageMargins left="0.25" right="0.25" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>
@@ -9302,7 +9296,7 @@
   <sheetData>
     <row r="1" spans="1:113" s="47" customFormat="1">
       <c r="A1" s="37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>7</v>
@@ -9477,7 +9471,7 @@
   <sheetData>
     <row r="1" spans="1:112" s="47" customFormat="1">
       <c r="A1" s="37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
TM-6741 Fixed two tabs where the first row was row 3 thereby hiding row 2 in the Export Template Spreadsheet.
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -8809,10 +8809,10 @@
   <dimension ref="A1:EH1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -9273,10 +9273,10 @@
   <dimension ref="A1:DI1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
TM-6932 Fix Asset Export/Import Spreadsheet to address format types and some width issues.
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -978,7 +978,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1608">
+  <cellStyleXfs count="1610">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -5909,8 +5909,10 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -5983,7 +5985,6 @@
     <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6027,17 +6028,12 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="1539" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1049" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -6053,8 +6049,16 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1049" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1608">
+  <cellStyles count="1610">
     <cellStyle name="_JDI DCM Runbook Hour by Hour EMA Comm Systems (Bundle 2) 11-JUL-07" xfId="1"/>
     <cellStyle name="_JDI DCM Runbook Hour by Hour EMA Comm Systems (Bundle 2) 11-JUL-07_Title" xfId="2"/>
     <cellStyle name="_Momentive Migration Runbook Move Event 2B 09-08-2007 v2 31" xfId="3"/>
@@ -6294,6 +6298,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1603" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1605" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1607" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1609" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1540" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1542" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1544" builtinId="8" hidden="1"/>
@@ -6328,6 +6333,7 @@
     <cellStyle name="Hyperlink" xfId="1602" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1604" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1606" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1608" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 10" xfId="206"/>
     <cellStyle name="Hyperlink 11" xfId="207"/>
     <cellStyle name="Hyperlink 12" xfId="208"/>
@@ -8282,17 +8288,17 @@
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
-      <c r="F15" s="82" t="s">
+      <c r="F15" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="82"/>
+      <c r="G15" s="78"/>
     </row>
     <row r="16" spans="1:7" ht="28" customHeight="1">
       <c r="A16" s="14"/>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="81"/>
+      <c r="C16" s="77"/>
       <c r="D16" s="15" t="s">
         <v>116</v>
       </c>
@@ -8708,32 +8714,32 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="16" style="7" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="10" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" style="8" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="88.85546875" style="10" customWidth="1"/>
     <col min="7" max="16384" width="9.5703125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="78" customFormat="1">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:6" s="85" customFormat="1">
+      <c r="A1" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="75" t="s">
+      <c r="E1" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="75" t="s">
         <v>86</v>
       </c>
     </row>
@@ -8768,20 +8774,20 @@
     <col min="6" max="16384" width="11.42578125" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="80" customFormat="1">
-      <c r="A1" s="79" t="s">
+    <row r="1" spans="1:5" s="86" customFormat="1">
+      <c r="A1" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="76" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="76" t="s">
         <v>131</v>
       </c>
     </row>
@@ -8809,12 +8815,12 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" style="35" customWidth="1"/>
@@ -8844,205 +8850,205 @@
     <col min="108" max="138" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:138" s="47" customFormat="1">
+    <row r="1" spans="1:138" s="46" customFormat="1">
       <c r="A1" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="53" t="s">
         <v>132</v>
       </c>
       <c r="F1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="82" t="s">
         <v>157</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="54" t="s">
+      <c r="N1" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="54" t="s">
+      <c r="O1" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="54" t="s">
+      <c r="P1" s="53" t="s">
         <v>133</v>
       </c>
-      <c r="Q1" s="56" t="s">
+      <c r="Q1" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="R1" s="56" t="s">
+      <c r="R1" s="55" t="s">
         <v>136</v>
       </c>
-      <c r="S1" s="56" t="s">
+      <c r="S1" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="T1" s="56" t="s">
+      <c r="T1" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="57" t="s">
+      <c r="U1" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="V1" s="57" t="s">
+      <c r="V1" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="W1" s="54" t="s">
+      <c r="W1" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="54" t="s">
+      <c r="X1" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" s="58" t="s">
+      <c r="Y1" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="Z1" s="54" t="s">
+      <c r="Z1" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="AA1" s="54" t="s">
+      <c r="AA1" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="AB1" s="54" t="s">
+      <c r="AB1" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="AC1" s="54" t="s">
+      <c r="AC1" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="AD1" s="47" t="s">
+      <c r="AD1" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="AE1" s="47" t="s">
+      <c r="AE1" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="AF1" s="47" t="s">
+      <c r="AF1" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="AG1" s="47" t="s">
+      <c r="AG1" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="AH1" s="46" t="s">
+      <c r="AH1" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="AI1" s="46" t="s">
+      <c r="AI1" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="AJ1" s="59" t="s">
+      <c r="AJ1" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="AK1" s="60" t="s">
+      <c r="AK1" s="59" t="s">
         <v>151</v>
       </c>
-      <c r="AL1" s="60" t="s">
+      <c r="AL1" s="59" t="s">
         <v>152</v>
       </c>
-      <c r="AM1" s="59" t="s">
+      <c r="AM1" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="AN1" s="60" t="s">
+      <c r="AN1" s="59" t="s">
         <v>154</v>
       </c>
-      <c r="AO1" s="60" t="s">
+      <c r="AO1" s="59" t="s">
         <v>155</v>
       </c>
-      <c r="AP1" s="59" t="s">
+      <c r="AP1" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="BO1" s="46"/>
-      <c r="BP1" s="46"/>
-      <c r="BQ1" s="46"/>
-      <c r="BR1" s="46"/>
-      <c r="BS1" s="46"/>
-      <c r="BT1" s="46"/>
-      <c r="BU1" s="46"/>
-      <c r="BV1" s="46"/>
-      <c r="BW1" s="46"/>
-      <c r="BX1" s="46"/>
-      <c r="BY1" s="46"/>
-      <c r="BZ1" s="46"/>
-      <c r="CA1" s="46"/>
-      <c r="CB1" s="46"/>
-      <c r="CC1" s="46"/>
-      <c r="CD1" s="46"/>
-      <c r="CE1" s="46"/>
-      <c r="CF1" s="46"/>
-      <c r="CG1" s="46"/>
-      <c r="CH1" s="46"/>
-      <c r="CI1" s="46"/>
-      <c r="CJ1" s="46"/>
-      <c r="CK1" s="46"/>
-      <c r="CL1" s="46"/>
-      <c r="CM1" s="46"/>
-      <c r="CN1" s="46"/>
-      <c r="CO1" s="46"/>
-      <c r="CP1" s="46"/>
-      <c r="CQ1" s="46"/>
-      <c r="CR1" s="46"/>
-      <c r="CS1" s="46"/>
-      <c r="CT1" s="46"/>
-      <c r="CU1" s="46"/>
-      <c r="CV1" s="46"/>
-      <c r="CW1" s="46"/>
-      <c r="CX1" s="46"/>
-      <c r="CY1" s="46"/>
-      <c r="CZ1" s="46"/>
-      <c r="DA1" s="46"/>
-      <c r="DB1" s="46"/>
-      <c r="DC1" s="46"/>
-      <c r="DD1" s="46"/>
-      <c r="DE1" s="46"/>
-      <c r="DF1" s="46"/>
-      <c r="DG1" s="46"/>
-      <c r="DH1" s="46"/>
-      <c r="DI1" s="46"/>
-      <c r="DJ1" s="46"/>
-      <c r="DK1" s="46"/>
-      <c r="DL1" s="46"/>
-      <c r="DM1" s="46"/>
-      <c r="DN1" s="46"/>
-      <c r="DO1" s="46"/>
-      <c r="DP1" s="46"/>
-      <c r="DQ1" s="46"/>
-      <c r="DR1" s="46"/>
-      <c r="DS1" s="46"/>
-      <c r="DT1" s="46"/>
-      <c r="DU1" s="46"/>
-      <c r="DV1" s="46"/>
-      <c r="DW1" s="46"/>
-      <c r="DX1" s="46"/>
-      <c r="DY1" s="46"/>
-      <c r="DZ1" s="46"/>
-      <c r="EA1" s="46"/>
-      <c r="EB1" s="46"/>
-      <c r="EC1" s="46"/>
-      <c r="ED1" s="46"/>
-      <c r="EE1" s="46"/>
-      <c r="EF1" s="46"/>
-      <c r="EG1" s="46"/>
-      <c r="EH1" s="46"/>
+      <c r="BO1" s="45"/>
+      <c r="BP1" s="45"/>
+      <c r="BQ1" s="45"/>
+      <c r="BR1" s="45"/>
+      <c r="BS1" s="45"/>
+      <c r="BT1" s="45"/>
+      <c r="BU1" s="45"/>
+      <c r="BV1" s="45"/>
+      <c r="BW1" s="45"/>
+      <c r="BX1" s="45"/>
+      <c r="BY1" s="45"/>
+      <c r="BZ1" s="45"/>
+      <c r="CA1" s="45"/>
+      <c r="CB1" s="45"/>
+      <c r="CC1" s="45"/>
+      <c r="CD1" s="45"/>
+      <c r="CE1" s="45"/>
+      <c r="CF1" s="45"/>
+      <c r="CG1" s="45"/>
+      <c r="CH1" s="45"/>
+      <c r="CI1" s="45"/>
+      <c r="CJ1" s="45"/>
+      <c r="CK1" s="45"/>
+      <c r="CL1" s="45"/>
+      <c r="CM1" s="45"/>
+      <c r="CN1" s="45"/>
+      <c r="CO1" s="45"/>
+      <c r="CP1" s="45"/>
+      <c r="CQ1" s="45"/>
+      <c r="CR1" s="45"/>
+      <c r="CS1" s="45"/>
+      <c r="CT1" s="45"/>
+      <c r="CU1" s="45"/>
+      <c r="CV1" s="45"/>
+      <c r="CW1" s="45"/>
+      <c r="CX1" s="45"/>
+      <c r="CY1" s="45"/>
+      <c r="CZ1" s="45"/>
+      <c r="DA1" s="45"/>
+      <c r="DB1" s="45"/>
+      <c r="DC1" s="45"/>
+      <c r="DD1" s="45"/>
+      <c r="DE1" s="45"/>
+      <c r="DF1" s="45"/>
+      <c r="DG1" s="45"/>
+      <c r="DH1" s="45"/>
+      <c r="DI1" s="45"/>
+      <c r="DJ1" s="45"/>
+      <c r="DK1" s="45"/>
+      <c r="DL1" s="45"/>
+      <c r="DM1" s="45"/>
+      <c r="DN1" s="45"/>
+      <c r="DO1" s="45"/>
+      <c r="DP1" s="45"/>
+      <c r="DQ1" s="45"/>
+      <c r="DR1" s="45"/>
+      <c r="DS1" s="45"/>
+      <c r="DT1" s="45"/>
+      <c r="DU1" s="45"/>
+      <c r="DV1" s="45"/>
+      <c r="DW1" s="45"/>
+      <c r="DX1" s="45"/>
+      <c r="DY1" s="45"/>
+      <c r="DZ1" s="45"/>
+      <c r="EA1" s="45"/>
+      <c r="EB1" s="45"/>
+      <c r="EC1" s="45"/>
+      <c r="ED1" s="45"/>
+      <c r="EE1" s="45"/>
+      <c r="EF1" s="45"/>
+      <c r="EG1" s="45"/>
+      <c r="EH1" s="45"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -9072,12 +9078,12 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="4" customWidth="1"/>
     <col min="2" max="3" width="20.5703125" style="5" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="6" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" style="5" customWidth="1"/>
@@ -9085,7 +9091,7 @@
     <col min="7" max="7" width="15.42578125" style="5" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" style="5" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" style="87" customWidth="1"/>
     <col min="11" max="11" width="15.85546875" style="5" customWidth="1"/>
     <col min="12" max="12" width="13" style="5" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" style="5" customWidth="1"/>
@@ -9108,7 +9114,7 @@
     <col min="31" max="31" width="15.5703125" style="4" customWidth="1"/>
     <col min="32" max="32" width="12.140625" style="5" customWidth="1"/>
     <col min="33" max="33" width="12" style="6" customWidth="1"/>
-    <col min="34" max="34" width="9.28515625" style="5" customWidth="1"/>
+    <col min="34" max="34" width="9.28515625" style="4" customWidth="1"/>
     <col min="35" max="35" width="11" style="5"/>
     <col min="36" max="36" width="8.85546875" style="5" customWidth="1"/>
     <col min="37" max="38" width="11" style="5"/>
@@ -9123,128 +9129,128 @@
     <col min="138" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="46" customFormat="1">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:41" s="45" customFormat="1">
+      <c r="A1" s="47" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="45" t="s">
         <v>132</v>
       </c>
       <c r="F1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="50" t="s">
         <v>157</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="46" t="s">
+      <c r="K1" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="N1" s="46" t="s">
+      <c r="N1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="46" t="s">
+      <c r="O1" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="46" t="s">
+      <c r="P1" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="Q1" s="46" t="s">
+      <c r="Q1" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="R1" s="46" t="s">
+      <c r="R1" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="46" t="s">
+      <c r="S1" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="T1" s="46" t="s">
+      <c r="T1" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="U1" s="46" t="s">
+      <c r="U1" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="V1" s="51" t="s">
+      <c r="V1" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="W1" s="46" t="s">
+      <c r="W1" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="X1" s="51" t="s">
+      <c r="X1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="46" t="s">
+      <c r="Y1" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="Z1" s="46" t="s">
+      <c r="Z1" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="AA1" s="46" t="s">
+      <c r="AA1" s="45" t="s">
         <v>170</v>
       </c>
-      <c r="AB1" s="46" t="s">
+      <c r="AB1" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="AC1" s="51" t="s">
+      <c r="AC1" s="50" t="s">
         <v>172</v>
       </c>
-      <c r="AD1" s="46" t="s">
+      <c r="AD1" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="AE1" s="51" t="s">
+      <c r="AE1" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="AF1" s="46" t="s">
+      <c r="AF1" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="AG1" s="50" t="s">
+      <c r="AG1" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="AH1" s="46" t="s">
+      <c r="AH1" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="46" t="s">
+      <c r="AI1" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="AJ1" s="46" t="s">
+      <c r="AJ1" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="AK1" s="46" t="s">
+      <c r="AK1" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="AL1" s="46" t="s">
+      <c r="AL1" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="AM1" s="51" t="s">
+      <c r="AM1" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="AN1" s="52" t="s">
+      <c r="AN1" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="AO1" s="46" t="s">
+      <c r="AO1" s="45" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9270,12 +9276,12 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" style="35" customWidth="1"/>
@@ -9286,7 +9292,8 @@
     <col min="12" max="12" width="9.5703125" style="7"/>
     <col min="13" max="13" width="7.140625" customWidth="1"/>
     <col min="14" max="14" width="12.85546875" style="7" customWidth="1"/>
-    <col min="16" max="17" width="12.85546875" style="8" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" style="8" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="25" customWidth="1"/>
     <col min="18" max="41" width="9.5703125" customWidth="1"/>
     <col min="42" max="42" width="9.5703125" style="9" customWidth="1"/>
     <col min="43" max="81" width="9.5703125" customWidth="1"/>
@@ -9294,7 +9301,7 @@
     <col min="84" max="85" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" s="47" customFormat="1">
+    <row r="1" spans="1:113" s="46" customFormat="1">
       <c r="A1" s="37" t="s">
         <v>174</v>
       </c>
@@ -9313,28 +9320,28 @@
       <c r="F1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="82" t="s">
         <v>157</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="42" t="s">
         <v>26</v>
       </c>
       <c r="K1" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="44" t="s">
         <v>23</v>
       </c>
       <c r="M1" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="N1" s="44" t="s">
         <v>25</v>
       </c>
       <c r="O1" s="39" t="s">
@@ -9343,81 +9350,81 @@
       <c r="P1" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="Q1" s="40" t="s">
+      <c r="Q1" s="65" t="s">
         <v>138</v>
       </c>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
-      <c r="AW1" s="46"/>
-      <c r="AX1" s="46"/>
-      <c r="AY1" s="46"/>
-      <c r="AZ1" s="46"/>
-      <c r="BA1" s="46"/>
-      <c r="BB1" s="46"/>
-      <c r="BC1" s="46"/>
-      <c r="BD1" s="46"/>
-      <c r="BE1" s="46"/>
-      <c r="BF1" s="46"/>
-      <c r="BG1" s="46"/>
-      <c r="BH1" s="46"/>
-      <c r="BI1" s="46"/>
-      <c r="BJ1" s="46"/>
-      <c r="BK1" s="46"/>
-      <c r="BL1" s="46"/>
-      <c r="BM1" s="46"/>
-      <c r="BN1" s="46"/>
-      <c r="BO1" s="46"/>
-      <c r="BP1" s="46"/>
-      <c r="BQ1" s="46"/>
-      <c r="BR1" s="46"/>
-      <c r="BS1" s="46"/>
-      <c r="BT1" s="46"/>
-      <c r="BU1" s="46"/>
-      <c r="BV1" s="46"/>
-      <c r="BW1" s="46"/>
-      <c r="BX1" s="46"/>
-      <c r="BY1" s="46"/>
-      <c r="BZ1" s="46"/>
-      <c r="CA1" s="46"/>
-      <c r="CB1" s="46"/>
-      <c r="CC1" s="46"/>
-      <c r="CD1" s="46"/>
-      <c r="CE1" s="46"/>
-      <c r="CF1" s="46"/>
-      <c r="CG1" s="46"/>
-      <c r="CH1" s="46"/>
-      <c r="CI1" s="46"/>
-      <c r="CJ1" s="46"/>
-      <c r="CK1" s="46"/>
-      <c r="CL1" s="46"/>
-      <c r="CM1" s="46"/>
-      <c r="CN1" s="46"/>
-      <c r="CO1" s="46"/>
-      <c r="CP1" s="46"/>
-      <c r="CQ1" s="46"/>
-      <c r="CR1" s="46"/>
-      <c r="CS1" s="46"/>
-      <c r="CT1" s="46"/>
-      <c r="CU1" s="46"/>
-      <c r="CV1" s="46"/>
-      <c r="CW1" s="46"/>
-      <c r="CX1" s="46"/>
-      <c r="CY1" s="46"/>
-      <c r="CZ1" s="46"/>
-      <c r="DA1" s="46"/>
-      <c r="DB1" s="46"/>
-      <c r="DC1" s="46"/>
-      <c r="DD1" s="46"/>
-      <c r="DE1" s="46"/>
-      <c r="DF1" s="46"/>
-      <c r="DG1" s="46"/>
-      <c r="DH1" s="46"/>
-      <c r="DI1" s="46"/>
+      <c r="AP1" s="45"/>
+      <c r="AQ1" s="45"/>
+      <c r="AR1" s="45"/>
+      <c r="AS1" s="45"/>
+      <c r="AT1" s="45"/>
+      <c r="AU1" s="45"/>
+      <c r="AV1" s="45"/>
+      <c r="AW1" s="45"/>
+      <c r="AX1" s="45"/>
+      <c r="AY1" s="45"/>
+      <c r="AZ1" s="45"/>
+      <c r="BA1" s="45"/>
+      <c r="BB1" s="45"/>
+      <c r="BC1" s="45"/>
+      <c r="BD1" s="45"/>
+      <c r="BE1" s="45"/>
+      <c r="BF1" s="45"/>
+      <c r="BG1" s="45"/>
+      <c r="BH1" s="45"/>
+      <c r="BI1" s="45"/>
+      <c r="BJ1" s="45"/>
+      <c r="BK1" s="45"/>
+      <c r="BL1" s="45"/>
+      <c r="BM1" s="45"/>
+      <c r="BN1" s="45"/>
+      <c r="BO1" s="45"/>
+      <c r="BP1" s="45"/>
+      <c r="BQ1" s="45"/>
+      <c r="BR1" s="45"/>
+      <c r="BS1" s="45"/>
+      <c r="BT1" s="45"/>
+      <c r="BU1" s="45"/>
+      <c r="BV1" s="45"/>
+      <c r="BW1" s="45"/>
+      <c r="BX1" s="45"/>
+      <c r="BY1" s="45"/>
+      <c r="BZ1" s="45"/>
+      <c r="CA1" s="45"/>
+      <c r="CB1" s="45"/>
+      <c r="CC1" s="45"/>
+      <c r="CD1" s="45"/>
+      <c r="CE1" s="45"/>
+      <c r="CF1" s="45"/>
+      <c r="CG1" s="45"/>
+      <c r="CH1" s="45"/>
+      <c r="CI1" s="45"/>
+      <c r="CJ1" s="45"/>
+      <c r="CK1" s="45"/>
+      <c r="CL1" s="45"/>
+      <c r="CM1" s="45"/>
+      <c r="CN1" s="45"/>
+      <c r="CO1" s="45"/>
+      <c r="CP1" s="45"/>
+      <c r="CQ1" s="45"/>
+      <c r="CR1" s="45"/>
+      <c r="CS1" s="45"/>
+      <c r="CT1" s="45"/>
+      <c r="CU1" s="45"/>
+      <c r="CV1" s="45"/>
+      <c r="CW1" s="45"/>
+      <c r="CX1" s="45"/>
+      <c r="CY1" s="45"/>
+      <c r="CZ1" s="45"/>
+      <c r="DA1" s="45"/>
+      <c r="DB1" s="45"/>
+      <c r="DC1" s="45"/>
+      <c r="DD1" s="45"/>
+      <c r="DE1" s="45"/>
+      <c r="DF1" s="45"/>
+      <c r="DG1" s="45"/>
+      <c r="DH1" s="45"/>
+      <c r="DI1" s="45"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -9444,12 +9451,12 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="8" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
@@ -9469,7 +9476,7 @@
     <col min="82" max="112" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" s="47" customFormat="1">
+    <row r="1" spans="1:112" s="46" customFormat="1">
       <c r="A1" s="37" t="s">
         <v>174</v>
       </c>
@@ -9494,25 +9501,25 @@
       <c r="H1" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="82" t="s">
         <v>157</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="43" t="s">
         <v>115</v>
       </c>
       <c r="L1" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="44" t="s">
         <v>23</v>
       </c>
       <c r="N1" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="45" t="s">
+      <c r="O1" s="44" t="s">
         <v>25</v>
       </c>
       <c r="P1" s="39" t="s">
@@ -9542,78 +9549,78 @@
       <c r="AL1" s="39"/>
       <c r="AM1" s="39"/>
       <c r="AN1" s="39"/>
-      <c r="AO1" s="46"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
-      <c r="AW1" s="46"/>
-      <c r="AX1" s="46"/>
-      <c r="AY1" s="46"/>
-      <c r="AZ1" s="46"/>
-      <c r="BA1" s="46"/>
-      <c r="BB1" s="46"/>
-      <c r="BC1" s="46"/>
-      <c r="BD1" s="46"/>
-      <c r="BE1" s="46"/>
-      <c r="BF1" s="46"/>
-      <c r="BG1" s="46"/>
-      <c r="BH1" s="46"/>
-      <c r="BI1" s="46"/>
-      <c r="BJ1" s="46"/>
-      <c r="BK1" s="46"/>
-      <c r="BL1" s="46"/>
-      <c r="BM1" s="46"/>
-      <c r="BN1" s="46"/>
-      <c r="BO1" s="46"/>
-      <c r="BP1" s="46"/>
-      <c r="BQ1" s="46"/>
-      <c r="BR1" s="46"/>
-      <c r="BS1" s="46"/>
-      <c r="BT1" s="46"/>
-      <c r="BU1" s="46"/>
-      <c r="BV1" s="46"/>
-      <c r="BW1" s="46"/>
-      <c r="BX1" s="46"/>
-      <c r="BY1" s="46"/>
-      <c r="BZ1" s="46"/>
-      <c r="CA1" s="46"/>
-      <c r="CB1" s="46"/>
-      <c r="CC1" s="46"/>
-      <c r="CD1" s="46"/>
-      <c r="CE1" s="46"/>
-      <c r="CF1" s="46"/>
-      <c r="CG1" s="46"/>
-      <c r="CH1" s="46"/>
-      <c r="CI1" s="46"/>
-      <c r="CJ1" s="46"/>
-      <c r="CK1" s="46"/>
-      <c r="CL1" s="46"/>
-      <c r="CM1" s="46"/>
-      <c r="CN1" s="46"/>
-      <c r="CO1" s="46"/>
-      <c r="CP1" s="46"/>
-      <c r="CQ1" s="46"/>
-      <c r="CR1" s="46"/>
-      <c r="CS1" s="46"/>
-      <c r="CT1" s="46"/>
-      <c r="CU1" s="46"/>
-      <c r="CV1" s="46"/>
-      <c r="CW1" s="46"/>
-      <c r="CX1" s="46"/>
-      <c r="CY1" s="46"/>
-      <c r="CZ1" s="46"/>
-      <c r="DA1" s="46"/>
-      <c r="DB1" s="46"/>
-      <c r="DC1" s="46"/>
-      <c r="DD1" s="46"/>
-      <c r="DE1" s="46"/>
-      <c r="DF1" s="46"/>
-      <c r="DG1" s="46"/>
-      <c r="DH1" s="46"/>
+      <c r="AO1" s="45"/>
+      <c r="AP1" s="45"/>
+      <c r="AQ1" s="45"/>
+      <c r="AR1" s="45"/>
+      <c r="AS1" s="45"/>
+      <c r="AT1" s="45"/>
+      <c r="AU1" s="45"/>
+      <c r="AV1" s="45"/>
+      <c r="AW1" s="45"/>
+      <c r="AX1" s="45"/>
+      <c r="AY1" s="45"/>
+      <c r="AZ1" s="45"/>
+      <c r="BA1" s="45"/>
+      <c r="BB1" s="45"/>
+      <c r="BC1" s="45"/>
+      <c r="BD1" s="45"/>
+      <c r="BE1" s="45"/>
+      <c r="BF1" s="45"/>
+      <c r="BG1" s="45"/>
+      <c r="BH1" s="45"/>
+      <c r="BI1" s="45"/>
+      <c r="BJ1" s="45"/>
+      <c r="BK1" s="45"/>
+      <c r="BL1" s="45"/>
+      <c r="BM1" s="45"/>
+      <c r="BN1" s="45"/>
+      <c r="BO1" s="45"/>
+      <c r="BP1" s="45"/>
+      <c r="BQ1" s="45"/>
+      <c r="BR1" s="45"/>
+      <c r="BS1" s="45"/>
+      <c r="BT1" s="45"/>
+      <c r="BU1" s="45"/>
+      <c r="BV1" s="45"/>
+      <c r="BW1" s="45"/>
+      <c r="BX1" s="45"/>
+      <c r="BY1" s="45"/>
+      <c r="BZ1" s="45"/>
+      <c r="CA1" s="45"/>
+      <c r="CB1" s="45"/>
+      <c r="CC1" s="45"/>
+      <c r="CD1" s="45"/>
+      <c r="CE1" s="45"/>
+      <c r="CF1" s="45"/>
+      <c r="CG1" s="45"/>
+      <c r="CH1" s="45"/>
+      <c r="CI1" s="45"/>
+      <c r="CJ1" s="45"/>
+      <c r="CK1" s="45"/>
+      <c r="CL1" s="45"/>
+      <c r="CM1" s="45"/>
+      <c r="CN1" s="45"/>
+      <c r="CO1" s="45"/>
+      <c r="CP1" s="45"/>
+      <c r="CQ1" s="45"/>
+      <c r="CR1" s="45"/>
+      <c r="CS1" s="45"/>
+      <c r="CT1" s="45"/>
+      <c r="CU1" s="45"/>
+      <c r="CV1" s="45"/>
+      <c r="CW1" s="45"/>
+      <c r="CX1" s="45"/>
+      <c r="CY1" s="45"/>
+      <c r="CZ1" s="45"/>
+      <c r="DA1" s="45"/>
+      <c r="DB1" s="45"/>
+      <c r="DC1" s="45"/>
+      <c r="DD1" s="45"/>
+      <c r="DE1" s="45"/>
+      <c r="DF1" s="45"/>
+      <c r="DG1" s="45"/>
+      <c r="DH1" s="45"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -9639,7 +9646,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="8.5703125" style="7"/>
+    <col min="1" max="1" width="8.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="7"/>
     <col min="3" max="3" width="13.42578125" style="7" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" style="10" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" style="7" customWidth="1"/>
@@ -9649,32 +9657,32 @@
     <col min="9" max="9" width="14.140625" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" customWidth="1"/>
     <col min="11" max="11" width="8.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="39" customFormat="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="43" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="38" t="s">
@@ -9723,7 +9731,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -9742,8 +9750,8 @@
     <col min="13" max="13" width="16.85546875" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="67" customFormat="1">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:13" s="66" customFormat="1">
+      <c r="A1" s="44" t="s">
         <v>51</v>
       </c>
       <c r="B1" s="39" t="s">
@@ -9752,16 +9760,16 @@
       <c r="C1" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="62" t="s">
         <v>54</v>
       </c>
       <c r="F1" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="63" t="s">
         <v>55</v>
       </c>
       <c r="H1" s="39" t="s">
@@ -9773,13 +9781,13 @@
       <c r="J1" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="65" t="s">
+      <c r="K1" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="65" t="s">
         <v>61</v>
       </c>
     </row>
@@ -9808,7 +9816,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -9825,44 +9833,44 @@
     <col min="12" max="12" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="64" customFormat="1">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:13" s="63" customFormat="1">
+      <c r="A1" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="68" t="s">
+      <c r="I1" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="J1" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="68" t="s">
+      <c r="K1" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="64" t="s">
+      <c r="L1" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="63" t="s">
         <v>70</v>
       </c>
     </row>
@@ -9894,71 +9902,75 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="5"/>
-    <col min="2" max="2" width="7.85546875" style="30" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="30" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" style="5"/>
-    <col min="5" max="5" width="8.42578125" style="30" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="30" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" style="5"/>
     <col min="8" max="8" width="24.140625" style="31" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" style="5"/>
+    <col min="9" max="9" width="10.7109375" style="5" customWidth="1"/>
     <col min="10" max="10" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" style="5" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" style="5" customWidth="1"/>
     <col min="13" max="16384" width="9.5703125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="47" customFormat="1">
-      <c r="B1" s="83" t="s">
+    <row r="1" spans="1:12" s="83" customFormat="1">
+      <c r="A1" s="46"/>
+      <c r="B1" s="79" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="84" t="s">
+      <c r="C1" s="80"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="69"/>
-      <c r="J1" s="47" t="s">
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46" t="s">
         <v>124</v>
       </c>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
     </row>
-    <row r="2" spans="1:12" s="74" customFormat="1">
-      <c r="A2" s="70" t="s">
+    <row r="2" spans="1:12" s="84" customFormat="1">
+      <c r="A2" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="72" t="s">
+      <c r="E2" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="73" t="s">
+      <c r="F2" s="72" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="73" t="s">
+      <c r="G2" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="72" t="s">
+      <c r="H2" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="73" t="s">
+      <c r="I2" s="72" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="73" t="s">
+      <c r="J2" s="72" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="73" t="s">
+      <c r="K2" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="L2" s="73" t="s">
+      <c r="L2" s="72" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TM-6932 adding the format of the spreadsheet cells using the original header in the Template
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/octavio/Documents/TDS/tranman/git-tdstm/web-app/templates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="100" yWindow="0" windowWidth="25760" windowHeight="15620" tabRatio="782"/>
+    <workbookView xWindow="1100" yWindow="460" windowWidth="25520" windowHeight="14900" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -38,13 +43,13 @@
     <definedName name="ProjectManager">Title!$B$5</definedName>
     <definedName name="ProjectName">Title!$C$4</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -663,11 +668,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="d\ mmm\ yy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="168" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -5910,7 +5916,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -5956,7 +5962,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -6006,12 +6011,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="17" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6038,6 +6040,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1049" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -8096,7 +8104,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8140,7 +8148,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8164,95 +8172,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="38.42578125" customWidth="1"/>
-    <col min="10" max="10" width="2.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="9" max="9" width="38.5" customWidth="1"/>
+    <col min="10" max="10" width="2.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="31" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="32" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="32" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="31" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="32" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="31" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="32" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="31" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="11">
         <v>38295</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="32" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="31" t="s">
         <v>125</v>
       </c>
       <c r="B9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="32" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="31" t="s">
         <v>126</v>
       </c>
       <c r="B10" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>90</v>
       </c>
@@ -8261,7 +8267,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>123</v>
       </c>
@@ -8270,43 +8276,43 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
-      <c r="F15" s="82" t="s">
+      <c r="F15" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="82"/>
+      <c r="G15" s="84"/>
     </row>
-    <row r="16" spans="1:7" ht="28" customHeight="1">
+    <row r="16" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="83" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="81"/>
+      <c r="C16" s="83"/>
       <c r="D16" s="15" t="s">
         <v>116</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="28" t="s">
         <v>118</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="20" customHeight="1">
+    <row r="17" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17">
         <f>COUNTA(Applications!B:B)-1</f>
         <v>0</v>
@@ -8334,7 +8340,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="20" customHeight="1">
+    <row r="18" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18">
         <f>COUNTIF(Applications!D:D,"Master")</f>
         <v>0</v>
@@ -8356,7 +8362,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="20" customHeight="1">
+    <row r="19" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19">
         <f>A17-A18</f>
         <v>0</v>
@@ -8374,7 +8380,7 @@
       </c>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="I19" s="27" t="s">
+      <c r="I19" s="26" t="s">
         <v>111</v>
       </c>
       <c r="J19" t="s">
@@ -8384,7 +8390,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="20" customHeight="1">
+    <row r="20" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17">
         <f>COUNTA(Devices!B:B)-1</f>
         <v>0</v>
@@ -8408,7 +8414,7 @@
         <f>COUNTIF(Devices!B:EH,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Devices!B:EH,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Devices!B:EH,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Devices!B:EH,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="I20" s="28" t="s">
+      <c r="I20" s="27" t="s">
         <v>112</v>
       </c>
       <c r="J20" t="s">
@@ -8418,7 +8424,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="20" customHeight="1">
+    <row r="21" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21">
         <f>COUNTIF(Devices!P:P,"Server")+COUNTIF(Devices!P:P,"VM")+COUNTIF(Devices!P:P,"Blade")+COUNTIF(Devices!P:P,"Appliance")</f>
         <v>0</v>
@@ -8437,7 +8443,7 @@
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
     </row>
-    <row r="22" spans="1:11" ht="20" customHeight="1">
+    <row r="22" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17">
         <f>COUNTA(Databases!B:B)-1</f>
         <v>0</v>
@@ -8462,7 +8468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="20" customHeight="1">
+    <row r="23" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17">
         <f>COUNTA(Storage!B:B)-1</f>
         <v>0</v>
@@ -8487,7 +8493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="20" customHeight="1">
+    <row r="24" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17">
         <f>COUNTA(Dependencies!D:D)-1</f>
         <v>0</v>
@@ -8512,7 +8518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="20" customHeight="1">
+    <row r="25" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25">
         <f>COUNTIF(Dependencies!H:H,"Master")</f>
         <v>0</v>
@@ -8525,7 +8531,7 @@
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="1:11" ht="20" customHeight="1">
+    <row r="26" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Application")-A25</f>
         <v>0</v>
@@ -8538,7 +8544,7 @@
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
     </row>
-    <row r="27" spans="1:11" ht="20" customHeight="1">
+    <row r="27" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!H:H,"Runs On")</f>
         <v>0</v>
@@ -8551,7 +8557,7 @@
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
     </row>
-    <row r="28" spans="1:11" ht="20" customHeight="1">
+    <row r="28" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Database")</f>
         <v>0</v>
@@ -8564,7 +8570,7 @@
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
     </row>
-    <row r="29" spans="1:11" ht="20" customHeight="1">
+    <row r="29" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29">
         <f>COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Server")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Blade")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"VM")</f>
         <v>0</v>
@@ -8577,7 +8583,7 @@
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
     </row>
-    <row r="30" spans="1:11" ht="20" customHeight="1">
+    <row r="30" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30">
         <f>COUNTIF(Dependencies!H:H,"Storage")</f>
         <v>0</v>
@@ -8590,7 +8596,7 @@
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
     </row>
-    <row r="31" spans="1:11" ht="20" customHeight="1">
+    <row r="31" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17">
         <f>COUNTA(Room!B:B)-1</f>
         <v>0</v>
@@ -8603,7 +8609,7 @@
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
     </row>
-    <row r="32" spans="1:11" ht="20" customHeight="1">
+    <row r="32" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17">
         <f>COUNTA(Rack!B:B)-1</f>
         <v>0</v>
@@ -8616,7 +8622,7 @@
       <c r="F32" s="24"/>
       <c r="G32" s="24"/>
     </row>
-    <row r="33" spans="1:7" ht="20" customHeight="1">
+    <row r="33" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17">
         <f>COUNTA(Cabling!B:B)-2</f>
         <v>0</v>
@@ -8629,7 +8635,7 @@
       <c r="F33" s="24"/>
       <c r="G33" s="24"/>
     </row>
-    <row r="34" spans="1:7" ht="20" customHeight="1">
+    <row r="34" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
         <f>COUNTA(Comments!B:B)-1</f>
         <v>0</v>
@@ -8642,21 +8648,21 @@
       <c r="F34" s="24"/>
       <c r="G34" s="24"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="21" customHeight="1"/>
-    <row r="46" spans="1:7" ht="21" customHeight="1"/>
-    <row r="47" spans="1:7" ht="21" customHeight="1"/>
-    <row r="48" spans="1:7" ht="21" customHeight="1"/>
-    <row r="49" ht="21" customHeight="1"/>
+    <row r="45" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="46" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="47" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="48" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataConsolidate/>
@@ -8690,11 +8696,6 @@
     <ignoredError sqref="D17:D24 E18 F17:F24 G17:G24 A17:A34" emptyCellReference="1"/>
     <ignoredError sqref="E21" formula="1" emptyCellReference="1"/>
   </ignoredErrors>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8703,37 +8704,37 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="16.5" style="7" customWidth="1"/>
     <col min="2" max="2" width="16" style="7" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" style="10" customWidth="1"/>
-    <col min="7" max="16384" width="9.5703125" style="10"/>
+    <col min="3" max="3" width="20.1640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="17.5" style="11" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="10" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" style="10" customWidth="1"/>
+    <col min="7" max="16384" width="9.5" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="78" customFormat="1">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:6" s="74" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="72" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="75" t="s">
+      <c r="E1" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="73" t="s">
         <v>86</v>
       </c>
     </row>
@@ -8746,11 +8747,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8762,26 +8758,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="19.42578125" style="33" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="33"/>
+    <col min="1" max="5" width="19.5" style="32" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="80" customFormat="1">
-      <c r="A1" s="79" t="s">
+    <row r="1" spans="1:5" s="76" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="75" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="75" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="75" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="75" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="75" t="s">
         <v>131</v>
       </c>
     </row>
@@ -8793,11 +8789,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8812,237 +8803,237 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="7" customWidth="1"/>
-    <col min="2" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="35" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" style="34" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="2"/>
-    <col min="17" max="17" width="13.42578125" customWidth="1"/>
-    <col min="18" max="20" width="12.85546875" customWidth="1"/>
-    <col min="21" max="21" width="9.5703125" style="8"/>
-    <col min="22" max="22" width="11.85546875" style="8" customWidth="1"/>
-    <col min="25" max="25" width="9.5703125" style="7"/>
-    <col min="34" max="34" width="11.42578125" customWidth="1"/>
-    <col min="35" max="35" width="13.42578125" customWidth="1"/>
-    <col min="36" max="36" width="16.140625" style="7" customWidth="1"/>
-    <col min="37" max="37" width="10.5703125" customWidth="1"/>
-    <col min="38" max="38" width="12.85546875" customWidth="1"/>
-    <col min="39" max="39" width="14.42578125" style="7" customWidth="1"/>
-    <col min="40" max="40" width="10.85546875" customWidth="1"/>
-    <col min="41" max="41" width="11.85546875" customWidth="1"/>
-    <col min="42" max="42" width="13.42578125" style="26" customWidth="1"/>
-    <col min="43" max="70" width="9.5703125" customWidth="1"/>
-    <col min="71" max="71" width="9.5703125" style="9" customWidth="1"/>
-    <col min="72" max="106" width="9.5703125" customWidth="1"/>
-    <col min="107" max="107" width="9.5703125" style="9" customWidth="1"/>
-    <col min="108" max="138" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="7" customWidth="1"/>
+    <col min="2" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="34" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="33" customWidth="1"/>
+    <col min="12" max="12" width="9.5" style="2"/>
+    <col min="17" max="17" width="13.5" customWidth="1"/>
+    <col min="18" max="20" width="12.83203125" customWidth="1"/>
+    <col min="21" max="21" width="9.5" style="8"/>
+    <col min="22" max="22" width="11.83203125" style="8" customWidth="1"/>
+    <col min="25" max="25" width="9.5" style="7"/>
+    <col min="34" max="34" width="11.5" customWidth="1"/>
+    <col min="35" max="35" width="13.5" customWidth="1"/>
+    <col min="36" max="36" width="16.1640625" style="7" customWidth="1"/>
+    <col min="37" max="37" width="10.5" customWidth="1"/>
+    <col min="38" max="38" width="12.83203125" customWidth="1"/>
+    <col min="39" max="39" width="14.5" style="7" customWidth="1"/>
+    <col min="40" max="40" width="10.83203125" customWidth="1"/>
+    <col min="41" max="41" width="11.83203125" customWidth="1"/>
+    <col min="42" max="42" width="13.5" style="25" customWidth="1"/>
+    <col min="43" max="70" width="9.5" customWidth="1"/>
+    <col min="71" max="71" width="9.5" style="9" customWidth="1"/>
+    <col min="72" max="106" width="9.5" customWidth="1"/>
+    <col min="107" max="107" width="9.5" style="9" customWidth="1"/>
+    <col min="108" max="138" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:138" s="47" customFormat="1">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:138" s="46" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="54" t="s">
+      <c r="N1" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="54" t="s">
+      <c r="O1" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="54" t="s">
+      <c r="P1" s="53" t="s">
         <v>133</v>
       </c>
-      <c r="Q1" s="56" t="s">
+      <c r="Q1" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="R1" s="56" t="s">
+      <c r="R1" s="55" t="s">
         <v>136</v>
       </c>
-      <c r="S1" s="56" t="s">
+      <c r="S1" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="T1" s="56" t="s">
+      <c r="T1" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="57" t="s">
+      <c r="U1" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="V1" s="57" t="s">
+      <c r="V1" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="W1" s="54" t="s">
+      <c r="W1" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="54" t="s">
+      <c r="X1" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" s="58" t="s">
+      <c r="Y1" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="Z1" s="54" t="s">
+      <c r="Z1" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="AA1" s="54" t="s">
+      <c r="AA1" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="AB1" s="54" t="s">
+      <c r="AB1" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="AC1" s="54" t="s">
+      <c r="AC1" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="AD1" s="47" t="s">
+      <c r="AD1" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="AE1" s="47" t="s">
+      <c r="AE1" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="AF1" s="47" t="s">
+      <c r="AF1" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="AG1" s="47" t="s">
+      <c r="AG1" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="AH1" s="46" t="s">
+      <c r="AH1" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="AI1" s="46" t="s">
+      <c r="AI1" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="AJ1" s="59" t="s">
+      <c r="AJ1" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="AK1" s="60" t="s">
+      <c r="AK1" s="59" t="s">
         <v>151</v>
       </c>
-      <c r="AL1" s="60" t="s">
+      <c r="AL1" s="59" t="s">
         <v>152</v>
       </c>
-      <c r="AM1" s="59" t="s">
+      <c r="AM1" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="AN1" s="60" t="s">
+      <c r="AN1" s="59" t="s">
         <v>154</v>
       </c>
-      <c r="AO1" s="60" t="s">
+      <c r="AO1" s="59" t="s">
         <v>155</v>
       </c>
-      <c r="AP1" s="59" t="s">
+      <c r="AP1" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="BO1" s="46"/>
-      <c r="BP1" s="46"/>
-      <c r="BQ1" s="46"/>
-      <c r="BR1" s="46"/>
-      <c r="BS1" s="46"/>
-      <c r="BT1" s="46"/>
-      <c r="BU1" s="46"/>
-      <c r="BV1" s="46"/>
-      <c r="BW1" s="46"/>
-      <c r="BX1" s="46"/>
-      <c r="BY1" s="46"/>
-      <c r="BZ1" s="46"/>
-      <c r="CA1" s="46"/>
-      <c r="CB1" s="46"/>
-      <c r="CC1" s="46"/>
-      <c r="CD1" s="46"/>
-      <c r="CE1" s="46"/>
-      <c r="CF1" s="46"/>
-      <c r="CG1" s="46"/>
-      <c r="CH1" s="46"/>
-      <c r="CI1" s="46"/>
-      <c r="CJ1" s="46"/>
-      <c r="CK1" s="46"/>
-      <c r="CL1" s="46"/>
-      <c r="CM1" s="46"/>
-      <c r="CN1" s="46"/>
-      <c r="CO1" s="46"/>
-      <c r="CP1" s="46"/>
-      <c r="CQ1" s="46"/>
-      <c r="CR1" s="46"/>
-      <c r="CS1" s="46"/>
-      <c r="CT1" s="46"/>
-      <c r="CU1" s="46"/>
-      <c r="CV1" s="46"/>
-      <c r="CW1" s="46"/>
-      <c r="CX1" s="46"/>
-      <c r="CY1" s="46"/>
-      <c r="CZ1" s="46"/>
-      <c r="DA1" s="46"/>
-      <c r="DB1" s="46"/>
-      <c r="DC1" s="46"/>
-      <c r="DD1" s="46"/>
-      <c r="DE1" s="46"/>
-      <c r="DF1" s="46"/>
-      <c r="DG1" s="46"/>
-      <c r="DH1" s="46"/>
-      <c r="DI1" s="46"/>
-      <c r="DJ1" s="46"/>
-      <c r="DK1" s="46"/>
-      <c r="DL1" s="46"/>
-      <c r="DM1" s="46"/>
-      <c r="DN1" s="46"/>
-      <c r="DO1" s="46"/>
-      <c r="DP1" s="46"/>
-      <c r="DQ1" s="46"/>
-      <c r="DR1" s="46"/>
-      <c r="DS1" s="46"/>
-      <c r="DT1" s="46"/>
-      <c r="DU1" s="46"/>
-      <c r="DV1" s="46"/>
-      <c r="DW1" s="46"/>
-      <c r="DX1" s="46"/>
-      <c r="DY1" s="46"/>
-      <c r="DZ1" s="46"/>
-      <c r="EA1" s="46"/>
-      <c r="EB1" s="46"/>
-      <c r="EC1" s="46"/>
-      <c r="ED1" s="46"/>
-      <c r="EE1" s="46"/>
-      <c r="EF1" s="46"/>
-      <c r="EG1" s="46"/>
-      <c r="EH1" s="46"/>
+      <c r="BO1" s="45"/>
+      <c r="BP1" s="45"/>
+      <c r="BQ1" s="45"/>
+      <c r="BR1" s="45"/>
+      <c r="BS1" s="45"/>
+      <c r="BT1" s="45"/>
+      <c r="BU1" s="45"/>
+      <c r="BV1" s="45"/>
+      <c r="BW1" s="45"/>
+      <c r="BX1" s="45"/>
+      <c r="BY1" s="45"/>
+      <c r="BZ1" s="45"/>
+      <c r="CA1" s="45"/>
+      <c r="CB1" s="45"/>
+      <c r="CC1" s="45"/>
+      <c r="CD1" s="45"/>
+      <c r="CE1" s="45"/>
+      <c r="CF1" s="45"/>
+      <c r="CG1" s="45"/>
+      <c r="CH1" s="45"/>
+      <c r="CI1" s="45"/>
+      <c r="CJ1" s="45"/>
+      <c r="CK1" s="45"/>
+      <c r="CL1" s="45"/>
+      <c r="CM1" s="45"/>
+      <c r="CN1" s="45"/>
+      <c r="CO1" s="45"/>
+      <c r="CP1" s="45"/>
+      <c r="CQ1" s="45"/>
+      <c r="CR1" s="45"/>
+      <c r="CS1" s="45"/>
+      <c r="CT1" s="45"/>
+      <c r="CU1" s="45"/>
+      <c r="CV1" s="45"/>
+      <c r="CW1" s="45"/>
+      <c r="CX1" s="45"/>
+      <c r="CY1" s="45"/>
+      <c r="CZ1" s="45"/>
+      <c r="DA1" s="45"/>
+      <c r="DB1" s="45"/>
+      <c r="DC1" s="45"/>
+      <c r="DD1" s="45"/>
+      <c r="DE1" s="45"/>
+      <c r="DF1" s="45"/>
+      <c r="DG1" s="45"/>
+      <c r="DH1" s="45"/>
+      <c r="DI1" s="45"/>
+      <c r="DJ1" s="45"/>
+      <c r="DK1" s="45"/>
+      <c r="DL1" s="45"/>
+      <c r="DM1" s="45"/>
+      <c r="DN1" s="45"/>
+      <c r="DO1" s="45"/>
+      <c r="DP1" s="45"/>
+      <c r="DQ1" s="45"/>
+      <c r="DR1" s="45"/>
+      <c r="DS1" s="45"/>
+      <c r="DT1" s="45"/>
+      <c r="DU1" s="45"/>
+      <c r="DV1" s="45"/>
+      <c r="DW1" s="45"/>
+      <c r="DX1" s="45"/>
+      <c r="DY1" s="45"/>
+      <c r="DZ1" s="45"/>
+      <c r="EA1" s="45"/>
+      <c r="EB1" s="45"/>
+      <c r="EC1" s="45"/>
+      <c r="ED1" s="45"/>
+      <c r="EE1" s="45"/>
+      <c r="EF1" s="45"/>
+      <c r="EG1" s="45"/>
+      <c r="EH1" s="45"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -9053,11 +9044,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9066,7 +9052,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DE1"/>
+  <dimension ref="A1:AO1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -9075,176 +9061,172 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="4" customWidth="1"/>
-    <col min="2" max="3" width="20.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="36" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="20.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="6" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="35" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="5" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="77" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" style="5" customWidth="1"/>
     <col min="12" max="12" width="13" style="5" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" style="5" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" style="5" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" style="5" customWidth="1"/>
-    <col min="19" max="20" width="10.42578125" style="5" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" style="5" customWidth="1"/>
-    <col min="22" max="22" width="10.42578125" style="4" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" style="5" customWidth="1"/>
-    <col min="24" max="24" width="18.85546875" style="4" customWidth="1"/>
-    <col min="25" max="25" width="13.42578125" style="5" customWidth="1"/>
-    <col min="26" max="26" width="8.42578125" style="5" customWidth="1"/>
-    <col min="27" max="27" width="11.42578125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="11.5" style="5" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="9.5" style="5" customWidth="1"/>
+    <col min="18" max="18" width="8.83203125" style="5" customWidth="1"/>
+    <col min="19" max="20" width="10.5" style="5" customWidth="1"/>
+    <col min="21" max="21" width="9.83203125" style="5" customWidth="1"/>
+    <col min="22" max="22" width="10.5" style="4" customWidth="1"/>
+    <col min="23" max="23" width="11.5" style="5" customWidth="1"/>
+    <col min="24" max="24" width="18.83203125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="13.5" style="5" customWidth="1"/>
+    <col min="26" max="26" width="8.5" style="5" customWidth="1"/>
+    <col min="27" max="27" width="11.5" style="5" customWidth="1"/>
     <col min="28" max="28" width="11" style="5"/>
     <col min="29" max="29" width="10" style="4" customWidth="1"/>
     <col min="30" max="30" width="11" style="5"/>
-    <col min="31" max="31" width="15.5703125" style="4" customWidth="1"/>
-    <col min="32" max="32" width="12.140625" style="5" customWidth="1"/>
-    <col min="33" max="33" width="12" style="6" customWidth="1"/>
-    <col min="34" max="34" width="9.28515625" style="5" customWidth="1"/>
+    <col min="31" max="31" width="15.5" style="4" customWidth="1"/>
+    <col min="32" max="32" width="12.1640625" style="79" customWidth="1"/>
+    <col min="33" max="33" width="12" style="79" customWidth="1"/>
+    <col min="34" max="34" width="9.33203125" style="5" customWidth="1"/>
     <col min="35" max="35" width="11" style="5"/>
-    <col min="36" max="36" width="8.85546875" style="5" customWidth="1"/>
+    <col min="36" max="36" width="8.83203125" style="5" customWidth="1"/>
     <col min="37" max="38" width="11" style="5"/>
-    <col min="39" max="39" width="12.85546875" style="4" customWidth="1"/>
-    <col min="40" max="40" width="8.5703125" style="4" customWidth="1"/>
-    <col min="41" max="41" width="10.140625" style="4" customWidth="1"/>
-    <col min="42" max="106" width="9.5703125" style="5" customWidth="1"/>
-    <col min="107" max="107" width="9.5703125" style="4" customWidth="1"/>
-    <col min="108" max="108" width="9.5703125" style="5" customWidth="1"/>
-    <col min="109" max="109" width="9.5703125" style="4" customWidth="1"/>
-    <col min="110" max="137" width="9.5703125" style="5" customWidth="1"/>
+    <col min="39" max="39" width="12.83203125" style="4" customWidth="1"/>
+    <col min="40" max="40" width="8.5" style="4" customWidth="1"/>
+    <col min="41" max="41" width="10.1640625" style="4" customWidth="1"/>
+    <col min="42" max="137" width="9.5" style="5" customWidth="1"/>
     <col min="138" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="46" customFormat="1">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:41" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="47" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="50" t="s">
         <v>157</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="46" t="s">
+      <c r="K1" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="N1" s="46" t="s">
+      <c r="N1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="46" t="s">
+      <c r="O1" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="46" t="s">
+      <c r="P1" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="Q1" s="46" t="s">
+      <c r="Q1" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="R1" s="46" t="s">
+      <c r="R1" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="46" t="s">
+      <c r="S1" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="T1" s="46" t="s">
+      <c r="T1" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="U1" s="46" t="s">
+      <c r="U1" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="V1" s="51" t="s">
+      <c r="V1" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="W1" s="46" t="s">
+      <c r="W1" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="X1" s="51" t="s">
+      <c r="X1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="46" t="s">
+      <c r="Y1" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="Z1" s="46" t="s">
+      <c r="Z1" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="AA1" s="46" t="s">
+      <c r="AA1" s="45" t="s">
         <v>170</v>
       </c>
-      <c r="AB1" s="46" t="s">
+      <c r="AB1" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="AC1" s="51" t="s">
+      <c r="AC1" s="50" t="s">
         <v>172</v>
       </c>
-      <c r="AD1" s="46" t="s">
+      <c r="AD1" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="AE1" s="51" t="s">
+      <c r="AE1" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="AF1" s="46" t="s">
+      <c r="AF1" s="78" t="s">
         <v>137</v>
       </c>
-      <c r="AG1" s="50" t="s">
+      <c r="AG1" s="78" t="s">
         <v>138</v>
       </c>
-      <c r="AH1" s="46" t="s">
+      <c r="AH1" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="46" t="s">
+      <c r="AI1" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="AJ1" s="46" t="s">
+      <c r="AJ1" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="AK1" s="46" t="s">
+      <c r="AK1" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="AL1" s="46" t="s">
+      <c r="AL1" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="AM1" s="51" t="s">
+      <c r="AM1" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="AN1" s="52" t="s">
+      <c r="AN1" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="AO1" s="46" t="s">
+      <c r="AO1" s="45" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9254,11 +9236,6 @@
   <pageMargins left="0.25" right="0.25" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9273,151 +9250,151 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="7" customWidth="1"/>
-    <col min="2" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="35" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" style="11" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="7"/>
-    <col min="13" max="13" width="7.140625" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="7" customWidth="1"/>
-    <col min="16" max="17" width="12.85546875" style="8" customWidth="1"/>
-    <col min="18" max="41" width="9.5703125" customWidth="1"/>
-    <col min="42" max="42" width="9.5703125" style="9" customWidth="1"/>
-    <col min="43" max="81" width="9.5703125" customWidth="1"/>
-    <col min="82" max="82" width="9.5703125" style="9"/>
-    <col min="84" max="85" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="7" customWidth="1"/>
+    <col min="2" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="34" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="11" customWidth="1"/>
+    <col min="12" max="12" width="9.5" style="7"/>
+    <col min="13" max="13" width="7.1640625" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" style="7" customWidth="1"/>
+    <col min="16" max="17" width="12.83203125" style="8" customWidth="1"/>
+    <col min="18" max="41" width="9.5" customWidth="1"/>
+    <col min="42" max="42" width="9.5" style="9" customWidth="1"/>
+    <col min="43" max="81" width="9.5" customWidth="1"/>
+    <col min="82" max="82" width="9.5" style="9"/>
+    <col min="84" max="85" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" s="47" customFormat="1">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:113" s="46" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="N1" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="P1" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="Q1" s="40" t="s">
+      <c r="Q1" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
-      <c r="AW1" s="46"/>
-      <c r="AX1" s="46"/>
-      <c r="AY1" s="46"/>
-      <c r="AZ1" s="46"/>
-      <c r="BA1" s="46"/>
-      <c r="BB1" s="46"/>
-      <c r="BC1" s="46"/>
-      <c r="BD1" s="46"/>
-      <c r="BE1" s="46"/>
-      <c r="BF1" s="46"/>
-      <c r="BG1" s="46"/>
-      <c r="BH1" s="46"/>
-      <c r="BI1" s="46"/>
-      <c r="BJ1" s="46"/>
-      <c r="BK1" s="46"/>
-      <c r="BL1" s="46"/>
-      <c r="BM1" s="46"/>
-      <c r="BN1" s="46"/>
-      <c r="BO1" s="46"/>
-      <c r="BP1" s="46"/>
-      <c r="BQ1" s="46"/>
-      <c r="BR1" s="46"/>
-      <c r="BS1" s="46"/>
-      <c r="BT1" s="46"/>
-      <c r="BU1" s="46"/>
-      <c r="BV1" s="46"/>
-      <c r="BW1" s="46"/>
-      <c r="BX1" s="46"/>
-      <c r="BY1" s="46"/>
-      <c r="BZ1" s="46"/>
-      <c r="CA1" s="46"/>
-      <c r="CB1" s="46"/>
-      <c r="CC1" s="46"/>
-      <c r="CD1" s="46"/>
-      <c r="CE1" s="46"/>
-      <c r="CF1" s="46"/>
-      <c r="CG1" s="46"/>
-      <c r="CH1" s="46"/>
-      <c r="CI1" s="46"/>
-      <c r="CJ1" s="46"/>
-      <c r="CK1" s="46"/>
-      <c r="CL1" s="46"/>
-      <c r="CM1" s="46"/>
-      <c r="CN1" s="46"/>
-      <c r="CO1" s="46"/>
-      <c r="CP1" s="46"/>
-      <c r="CQ1" s="46"/>
-      <c r="CR1" s="46"/>
-      <c r="CS1" s="46"/>
-      <c r="CT1" s="46"/>
-      <c r="CU1" s="46"/>
-      <c r="CV1" s="46"/>
-      <c r="CW1" s="46"/>
-      <c r="CX1" s="46"/>
-      <c r="CY1" s="46"/>
-      <c r="CZ1" s="46"/>
-      <c r="DA1" s="46"/>
-      <c r="DB1" s="46"/>
-      <c r="DC1" s="46"/>
-      <c r="DD1" s="46"/>
-      <c r="DE1" s="46"/>
-      <c r="DF1" s="46"/>
-      <c r="DG1" s="46"/>
-      <c r="DH1" s="46"/>
-      <c r="DI1" s="46"/>
+      <c r="AP1" s="45"/>
+      <c r="AQ1" s="45"/>
+      <c r="AR1" s="45"/>
+      <c r="AS1" s="45"/>
+      <c r="AT1" s="45"/>
+      <c r="AU1" s="45"/>
+      <c r="AV1" s="45"/>
+      <c r="AW1" s="45"/>
+      <c r="AX1" s="45"/>
+      <c r="AY1" s="45"/>
+      <c r="AZ1" s="45"/>
+      <c r="BA1" s="45"/>
+      <c r="BB1" s="45"/>
+      <c r="BC1" s="45"/>
+      <c r="BD1" s="45"/>
+      <c r="BE1" s="45"/>
+      <c r="BF1" s="45"/>
+      <c r="BG1" s="45"/>
+      <c r="BH1" s="45"/>
+      <c r="BI1" s="45"/>
+      <c r="BJ1" s="45"/>
+      <c r="BK1" s="45"/>
+      <c r="BL1" s="45"/>
+      <c r="BM1" s="45"/>
+      <c r="BN1" s="45"/>
+      <c r="BO1" s="45"/>
+      <c r="BP1" s="45"/>
+      <c r="BQ1" s="45"/>
+      <c r="BR1" s="45"/>
+      <c r="BS1" s="45"/>
+      <c r="BT1" s="45"/>
+      <c r="BU1" s="45"/>
+      <c r="BV1" s="45"/>
+      <c r="BW1" s="45"/>
+      <c r="BX1" s="45"/>
+      <c r="BY1" s="45"/>
+      <c r="BZ1" s="45"/>
+      <c r="CA1" s="45"/>
+      <c r="CB1" s="45"/>
+      <c r="CC1" s="45"/>
+      <c r="CD1" s="45"/>
+      <c r="CE1" s="45"/>
+      <c r="CF1" s="45"/>
+      <c r="CG1" s="45"/>
+      <c r="CH1" s="45"/>
+      <c r="CI1" s="45"/>
+      <c r="CJ1" s="45"/>
+      <c r="CK1" s="45"/>
+      <c r="CL1" s="45"/>
+      <c r="CM1" s="45"/>
+      <c r="CN1" s="45"/>
+      <c r="CO1" s="45"/>
+      <c r="CP1" s="45"/>
+      <c r="CQ1" s="45"/>
+      <c r="CR1" s="45"/>
+      <c r="CS1" s="45"/>
+      <c r="CT1" s="45"/>
+      <c r="CU1" s="45"/>
+      <c r="CV1" s="45"/>
+      <c r="CW1" s="45"/>
+      <c r="CX1" s="45"/>
+      <c r="CY1" s="45"/>
+      <c r="CZ1" s="45"/>
+      <c r="DA1" s="45"/>
+      <c r="DB1" s="45"/>
+      <c r="DC1" s="45"/>
+      <c r="DD1" s="45"/>
+      <c r="DE1" s="45"/>
+      <c r="DF1" s="45"/>
+      <c r="DG1" s="45"/>
+      <c r="DH1" s="45"/>
+      <c r="DI1" s="45"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -9428,11 +9405,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9447,184 +9419,179 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="7" customWidth="1"/>
-    <col min="2" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="35" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" style="11" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="10"/>
-    <col min="13" max="13" width="8.5703125" style="7"/>
-    <col min="14" max="14" width="7.140625" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" style="7" customWidth="1"/>
-    <col min="17" max="40" width="9.5703125" customWidth="1"/>
-    <col min="41" max="41" width="9.5703125" style="9" customWidth="1"/>
-    <col min="42" max="80" width="9.5703125" customWidth="1"/>
-    <col min="81" max="81" width="9.5703125" style="9" customWidth="1"/>
-    <col min="82" max="112" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="7" customWidth="1"/>
+    <col min="2" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="34" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="11" customWidth="1"/>
+    <col min="11" max="11" width="8.5" style="10"/>
+    <col min="13" max="13" width="8.5" style="7"/>
+    <col min="14" max="14" width="7.1640625" customWidth="1"/>
+    <col min="15" max="15" width="14.5" style="7" customWidth="1"/>
+    <col min="17" max="40" width="9.5" customWidth="1"/>
+    <col min="41" max="41" width="9.5" style="9" customWidth="1"/>
+    <col min="42" max="80" width="9.5" customWidth="1"/>
+    <col min="81" max="81" width="9.5" style="9" customWidth="1"/>
+    <col min="82" max="112" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" s="47" customFormat="1">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:112" s="46" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="45" t="s">
+      <c r="O1" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="39"/>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="39"/>
-      <c r="AC1" s="39"/>
-      <c r="AD1" s="39"/>
-      <c r="AE1" s="39"/>
-      <c r="AF1" s="39"/>
-      <c r="AG1" s="39"/>
-      <c r="AH1" s="39"/>
-      <c r="AI1" s="39"/>
-      <c r="AJ1" s="39"/>
-      <c r="AK1" s="39"/>
-      <c r="AL1" s="39"/>
-      <c r="AM1" s="39"/>
-      <c r="AN1" s="39"/>
-      <c r="AO1" s="46"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
-      <c r="AW1" s="46"/>
-      <c r="AX1" s="46"/>
-      <c r="AY1" s="46"/>
-      <c r="AZ1" s="46"/>
-      <c r="BA1" s="46"/>
-      <c r="BB1" s="46"/>
-      <c r="BC1" s="46"/>
-      <c r="BD1" s="46"/>
-      <c r="BE1" s="46"/>
-      <c r="BF1" s="46"/>
-      <c r="BG1" s="46"/>
-      <c r="BH1" s="46"/>
-      <c r="BI1" s="46"/>
-      <c r="BJ1" s="46"/>
-      <c r="BK1" s="46"/>
-      <c r="BL1" s="46"/>
-      <c r="BM1" s="46"/>
-      <c r="BN1" s="46"/>
-      <c r="BO1" s="46"/>
-      <c r="BP1" s="46"/>
-      <c r="BQ1" s="46"/>
-      <c r="BR1" s="46"/>
-      <c r="BS1" s="46"/>
-      <c r="BT1" s="46"/>
-      <c r="BU1" s="46"/>
-      <c r="BV1" s="46"/>
-      <c r="BW1" s="46"/>
-      <c r="BX1" s="46"/>
-      <c r="BY1" s="46"/>
-      <c r="BZ1" s="46"/>
-      <c r="CA1" s="46"/>
-      <c r="CB1" s="46"/>
-      <c r="CC1" s="46"/>
-      <c r="CD1" s="46"/>
-      <c r="CE1" s="46"/>
-      <c r="CF1" s="46"/>
-      <c r="CG1" s="46"/>
-      <c r="CH1" s="46"/>
-      <c r="CI1" s="46"/>
-      <c r="CJ1" s="46"/>
-      <c r="CK1" s="46"/>
-      <c r="CL1" s="46"/>
-      <c r="CM1" s="46"/>
-      <c r="CN1" s="46"/>
-      <c r="CO1" s="46"/>
-      <c r="CP1" s="46"/>
-      <c r="CQ1" s="46"/>
-      <c r="CR1" s="46"/>
-      <c r="CS1" s="46"/>
-      <c r="CT1" s="46"/>
-      <c r="CU1" s="46"/>
-      <c r="CV1" s="46"/>
-      <c r="CW1" s="46"/>
-      <c r="CX1" s="46"/>
-      <c r="CY1" s="46"/>
-      <c r="CZ1" s="46"/>
-      <c r="DA1" s="46"/>
-      <c r="DB1" s="46"/>
-      <c r="DC1" s="46"/>
-      <c r="DD1" s="46"/>
-      <c r="DE1" s="46"/>
-      <c r="DF1" s="46"/>
-      <c r="DG1" s="46"/>
-      <c r="DH1" s="46"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="45"/>
+      <c r="AP1" s="45"/>
+      <c r="AQ1" s="45"/>
+      <c r="AR1" s="45"/>
+      <c r="AS1" s="45"/>
+      <c r="AT1" s="45"/>
+      <c r="AU1" s="45"/>
+      <c r="AV1" s="45"/>
+      <c r="AW1" s="45"/>
+      <c r="AX1" s="45"/>
+      <c r="AY1" s="45"/>
+      <c r="AZ1" s="45"/>
+      <c r="BA1" s="45"/>
+      <c r="BB1" s="45"/>
+      <c r="BC1" s="45"/>
+      <c r="BD1" s="45"/>
+      <c r="BE1" s="45"/>
+      <c r="BF1" s="45"/>
+      <c r="BG1" s="45"/>
+      <c r="BH1" s="45"/>
+      <c r="BI1" s="45"/>
+      <c r="BJ1" s="45"/>
+      <c r="BK1" s="45"/>
+      <c r="BL1" s="45"/>
+      <c r="BM1" s="45"/>
+      <c r="BN1" s="45"/>
+      <c r="BO1" s="45"/>
+      <c r="BP1" s="45"/>
+      <c r="BQ1" s="45"/>
+      <c r="BR1" s="45"/>
+      <c r="BS1" s="45"/>
+      <c r="BT1" s="45"/>
+      <c r="BU1" s="45"/>
+      <c r="BV1" s="45"/>
+      <c r="BW1" s="45"/>
+      <c r="BX1" s="45"/>
+      <c r="BY1" s="45"/>
+      <c r="BZ1" s="45"/>
+      <c r="CA1" s="45"/>
+      <c r="CB1" s="45"/>
+      <c r="CC1" s="45"/>
+      <c r="CD1" s="45"/>
+      <c r="CE1" s="45"/>
+      <c r="CF1" s="45"/>
+      <c r="CG1" s="45"/>
+      <c r="CH1" s="45"/>
+      <c r="CI1" s="45"/>
+      <c r="CJ1" s="45"/>
+      <c r="CK1" s="45"/>
+      <c r="CL1" s="45"/>
+      <c r="CM1" s="45"/>
+      <c r="CN1" s="45"/>
+      <c r="CO1" s="45"/>
+      <c r="CP1" s="45"/>
+      <c r="CQ1" s="45"/>
+      <c r="CR1" s="45"/>
+      <c r="CS1" s="45"/>
+      <c r="CT1" s="45"/>
+      <c r="CU1" s="45"/>
+      <c r="CV1" s="45"/>
+      <c r="CW1" s="45"/>
+      <c r="CX1" s="45"/>
+      <c r="CY1" s="45"/>
+      <c r="CZ1" s="45"/>
+      <c r="DA1" s="45"/>
+      <c r="DB1" s="45"/>
+      <c r="DC1" s="45"/>
+      <c r="DD1" s="45"/>
+      <c r="DE1" s="45"/>
+      <c r="DF1" s="45"/>
+      <c r="DG1" s="45"/>
+      <c r="DH1" s="45"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <autoFilter ref="A1:DH1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9634,71 +9601,72 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="8.5703125" style="7"/>
-    <col min="3" max="3" width="13.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="7" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="10" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="7" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="10" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" customWidth="1"/>
+    <col min="11" max="11" width="8.1640625" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="39" customFormat="1">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="38" t="s">
         <v>50</v>
       </c>
     </row>
@@ -9707,11 +9675,6 @@
   <autoFilter ref="A1:P1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9726,60 +9689,60 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="7"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="5" width="14.42578125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="7"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="4" max="5" width="14.5" style="7" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="26.5" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="25.42578125" style="25" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="25" customWidth="1"/>
+    <col min="11" max="11" width="19.5" style="2" customWidth="1"/>
+    <col min="12" max="12" width="25.5" style="11" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="67" customFormat="1">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="65" t="s">
+      <c r="K1" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="82" t="s">
         <v>61</v>
       </c>
     </row>
@@ -9792,11 +9755,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9811,58 +9769,57 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="12" style="9" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="5" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="7" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="7" customWidth="1"/>
+    <col min="9" max="10" width="13.5" style="7" customWidth="1"/>
+    <col min="11" max="11" width="12" style="7" customWidth="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="64" customFormat="1">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:13" s="62" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="68" t="s">
+      <c r="I1" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="J1" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="68" t="s">
+      <c r="K1" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="64" t="s">
+      <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="62" t="s">
         <v>70</v>
       </c>
     </row>
@@ -9875,11 +9832,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9888,77 +9840,77 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="5"/>
-    <col min="2" max="2" width="7.85546875" style="30" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="5"/>
-    <col min="5" max="5" width="8.42578125" style="30" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="5"/>
-    <col min="8" max="8" width="24.140625" style="31" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" style="5"/>
-    <col min="10" max="10" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="9.5703125" style="5"/>
+    <col min="1" max="1" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.5" style="5"/>
+    <col min="5" max="5" width="8.5" style="29" customWidth="1"/>
+    <col min="6" max="6" width="24.5" style="5" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="5"/>
+    <col min="8" max="8" width="24.1640625" style="30" customWidth="1"/>
+    <col min="9" max="9" width="9.5" style="5"/>
+    <col min="10" max="10" width="14.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="15.5" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="9.5" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="47" customFormat="1">
-      <c r="B1" s="83" t="s">
+    <row r="1" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="84" t="s">
+      <c r="C1" s="86"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="69"/>
-      <c r="J1" s="47" t="s">
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="65"/>
+      <c r="J1" s="46" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="74" customFormat="1">
-      <c r="A2" s="70" t="s">
+    <row r="2" spans="1:12" s="70" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="72" t="s">
+      <c r="E2" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="73" t="s">
+      <c r="F2" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="73" t="s">
+      <c r="G2" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="72" t="s">
+      <c r="H2" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="73" t="s">
+      <c r="I2" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="73" t="s">
+      <c r="J2" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="73" t="s">
+      <c r="K2" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="L2" s="73" t="s">
+      <c r="L2" s="69" t="s">
         <v>81</v>
       </c>
     </row>
@@ -9975,10 +9927,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TM-6932 last changes approved by Craig: 'External Ref Id' sould be text
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="460" windowWidth="25520" windowHeight="14900" tabRatio="782"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -668,12 +668,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="d\ mmm\ yy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="168" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -5916,7 +5915,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -5962,6 +5961,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -5988,7 +5988,6 @@
     <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6004,16 +6003,18 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="17" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6040,12 +6041,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1049" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -8104,7 +8102,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8148,7 +8146,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8192,7 +8190,7 @@
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
@@ -8200,7 +8198,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -8208,7 +8206,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -8216,7 +8214,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="32" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -8224,7 +8222,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="32" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -8232,7 +8230,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="32" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="11">
@@ -8240,7 +8238,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>125</v>
       </c>
       <c r="B9" t="s">
@@ -8248,7 +8246,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="32" t="s">
         <v>126</v>
       </c>
       <c r="B10" t="s">
@@ -8288,24 +8286,24 @@
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
-      <c r="F15" s="84" t="s">
+      <c r="F15" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="84"/>
+      <c r="G15" s="83"/>
     </row>
     <row r="16" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
-      <c r="B16" s="83" t="s">
+      <c r="B16" s="82" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="83"/>
+      <c r="C16" s="82"/>
       <c r="D16" s="15" t="s">
         <v>116</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="29" t="s">
         <v>118</v>
       </c>
       <c r="G16" s="15" t="s">
@@ -8380,7 +8378,7 @@
       </c>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="I19" s="26" t="s">
+      <c r="I19" s="27" t="s">
         <v>111</v>
       </c>
       <c r="J19" t="s">
@@ -8414,7 +8412,7 @@
         <f>COUNTIF(Devices!B:EH,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Devices!B:EH,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Devices!B:EH,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Devices!B:EH,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
-      <c r="I20" s="27" t="s">
+      <c r="I20" s="28" t="s">
         <v>112</v>
       </c>
       <c r="J20" t="s">
@@ -8704,37 +8702,37 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.5" style="9" customWidth="1"/>
     <col min="2" max="2" width="16" style="7" customWidth="1"/>
     <col min="3" max="3" width="20.1640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="11" customWidth="1"/>
+    <col min="4" max="4" width="17.5" style="8" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="10" customWidth="1"/>
     <col min="6" max="6" width="51.83203125" style="10" customWidth="1"/>
     <col min="7" max="16384" width="9.5" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="74" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="81" t="s">
+    <row r="1" spans="1:6" s="76" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="73" t="s">
+      <c r="F1" s="75" t="s">
         <v>86</v>
       </c>
     </row>
@@ -8760,24 +8758,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="19.5" style="32" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="32"/>
+    <col min="1" max="5" width="19.5" style="33" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="76" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:5" s="78" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="75" t="s">
+      <c r="E1" s="77" t="s">
         <v>131</v>
       </c>
     </row>
@@ -8797,7 +8795,7 @@
   <dimension ref="A1:EH1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
@@ -8808,17 +8806,17 @@
     <col min="1" max="1" width="6.6640625" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="34" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="35" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="33" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="34" customWidth="1"/>
     <col min="12" max="12" width="9.5" style="2"/>
     <col min="17" max="17" width="13.5" customWidth="1"/>
     <col min="18" max="20" width="12.83203125" customWidth="1"/>
     <col min="21" max="21" width="9.5" style="8"/>
     <col min="22" max="22" width="11.83203125" style="8" customWidth="1"/>
-    <col min="25" max="25" width="9.5" style="7"/>
+    <col min="25" max="25" width="9.5" style="2"/>
     <col min="34" max="34" width="11.5" customWidth="1"/>
     <col min="35" max="35" width="13.5" customWidth="1"/>
     <col min="36" max="36" width="16.1640625" style="7" customWidth="1"/>
@@ -8827,7 +8825,7 @@
     <col min="39" max="39" width="14.5" style="7" customWidth="1"/>
     <col min="40" max="40" width="10.83203125" customWidth="1"/>
     <col min="41" max="41" width="11.83203125" customWidth="1"/>
-    <col min="42" max="42" width="13.5" style="25" customWidth="1"/>
+    <col min="42" max="42" width="13.5" style="26" customWidth="1"/>
     <col min="43" max="70" width="9.5" customWidth="1"/>
     <col min="71" max="71" width="9.5" style="9" customWidth="1"/>
     <col min="72" max="106" width="9.5" customWidth="1"/>
@@ -8836,7 +8834,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:138" s="46" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>174</v>
       </c>
       <c r="B1" s="52" t="s">
@@ -8851,7 +8849,7 @@
       <c r="E1" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="41" t="s">
         <v>22</v>
       </c>
       <c r="G1" s="46" t="s">
@@ -8860,7 +8858,7 @@
       <c r="H1" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="79" t="s">
         <v>157</v>
       </c>
       <c r="J1" s="42" t="s">
@@ -8908,7 +8906,7 @@
       <c r="X1" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" s="57" t="s">
+      <c r="Y1" s="54" t="s">
         <v>139</v>
       </c>
       <c r="Z1" s="53" t="s">
@@ -8941,25 +8939,25 @@
       <c r="AI1" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="AJ1" s="58" t="s">
+      <c r="AJ1" s="57" t="s">
         <v>150</v>
       </c>
-      <c r="AK1" s="59" t="s">
+      <c r="AK1" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="AL1" s="59" t="s">
+      <c r="AL1" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="AM1" s="58" t="s">
+      <c r="AM1" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="AN1" s="59" t="s">
+      <c r="AN1" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="AO1" s="59" t="s">
+      <c r="AO1" s="58" t="s">
         <v>155</v>
       </c>
-      <c r="AP1" s="58" t="s">
+      <c r="AP1" s="57" t="s">
         <v>156</v>
       </c>
       <c r="BO1" s="45"/>
@@ -9067,11 +9065,11 @@
     <col min="2" max="3" width="20.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="6" customWidth="1"/>
     <col min="5" max="5" width="15.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="35" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="36" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="5" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="77" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="81" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="4" customWidth="1"/>
     <col min="11" max="11" width="15.83203125" style="5" customWidth="1"/>
     <col min="12" max="12" width="13" style="5" customWidth="1"/>
     <col min="13" max="13" width="11.5" style="5" customWidth="1"/>
@@ -9092,8 +9090,8 @@
     <col min="29" max="29" width="10" style="4" customWidth="1"/>
     <col min="30" max="30" width="11" style="5"/>
     <col min="31" max="31" width="15.5" style="4" customWidth="1"/>
-    <col min="32" max="32" width="12.1640625" style="79" customWidth="1"/>
-    <col min="33" max="33" width="12" style="79" customWidth="1"/>
+    <col min="32" max="32" width="12.1640625" style="5" customWidth="1"/>
+    <col min="33" max="33" width="12" style="6" customWidth="1"/>
     <col min="34" max="34" width="9.33203125" style="5" customWidth="1"/>
     <col min="35" max="35" width="11" style="5"/>
     <col min="36" max="36" width="8.83203125" style="5" customWidth="1"/>
@@ -9121,7 +9119,7 @@
       <c r="E1" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="41" t="s">
         <v>22</v>
       </c>
       <c r="G1" s="45" t="s">
@@ -9130,10 +9128,10 @@
       <c r="H1" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="80" t="s">
         <v>157</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="50" t="s">
         <v>26</v>
       </c>
       <c r="K1" s="45" t="s">
@@ -9199,10 +9197,10 @@
       <c r="AE1" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="AF1" s="78" t="s">
+      <c r="AF1" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="AG1" s="78" t="s">
+      <c r="AG1" s="49" t="s">
         <v>138</v>
       </c>
       <c r="AH1" s="45" t="s">
@@ -9255,10 +9253,10 @@
     <col min="1" max="1" width="6.6640625" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="34" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="35" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.5" style="11" customWidth="1"/>
     <col min="12" max="12" width="9.5" style="7"/>
     <col min="13" max="13" width="7.1640625" customWidth="1"/>
@@ -9272,22 +9270,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:113" s="46" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="41" t="s">
         <v>22</v>
       </c>
       <c r="G1" s="46" t="s">
@@ -9296,31 +9294,31 @@
       <c r="H1" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="79" t="s">
         <v>157</v>
       </c>
       <c r="J1" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="39" t="s">
         <v>35</v>
       </c>
       <c r="L1" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="39" t="s">
         <v>24</v>
       </c>
       <c r="N1" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="38" t="s">
+      <c r="O1" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="40" t="s">
         <v>138</v>
       </c>
       <c r="AP1" s="45"/>
@@ -9425,10 +9423,10 @@
     <col min="2" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="8" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="34" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="35" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.5" style="11" customWidth="1"/>
     <col min="11" max="11" width="8.5" style="10"/>
     <col min="13" max="13" width="8.5" style="7"/>
@@ -9442,31 +9440,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:112" s="46" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="79" t="s">
         <v>157</v>
       </c>
       <c r="J1" s="42" t="s">
@@ -9475,45 +9473,45 @@
       <c r="K1" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="39" t="s">
         <v>35</v>
       </c>
       <c r="M1" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="N1" s="39" t="s">
         <v>24</v>
       </c>
       <c r="O1" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="38" t="s">
+      <c r="P1" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38"/>
-      <c r="AB1" s="38"/>
-      <c r="AC1" s="38"/>
-      <c r="AD1" s="38"/>
-      <c r="AE1" s="38"/>
-      <c r="AF1" s="38"/>
-      <c r="AG1" s="38"/>
-      <c r="AH1" s="38"/>
-      <c r="AI1" s="38"/>
-      <c r="AJ1" s="38"/>
-      <c r="AK1" s="38"/>
-      <c r="AL1" s="38"/>
-      <c r="AM1" s="38"/>
-      <c r="AN1" s="38"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="39"/>
+      <c r="AD1" s="39"/>
+      <c r="AE1" s="39"/>
+      <c r="AF1" s="39"/>
+      <c r="AG1" s="39"/>
+      <c r="AH1" s="39"/>
+      <c r="AI1" s="39"/>
+      <c r="AJ1" s="39"/>
+      <c r="AK1" s="39"/>
+      <c r="AL1" s="39"/>
+      <c r="AM1" s="39"/>
+      <c r="AN1" s="39"/>
       <c r="AO1" s="45"/>
       <c r="AP1" s="45"/>
       <c r="AQ1" s="45"/>
@@ -9601,13 +9599,12 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.5" style="7"/>
     <col min="3" max="3" width="13.5" style="7" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="10" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="7" customWidth="1"/>
@@ -9620,14 +9617,14 @@
     <col min="12" max="12" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="59" t="s">
         <v>38</v>
       </c>
       <c r="D1" s="43" t="s">
@@ -9636,7 +9633,7 @@
       <c r="E1" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="F1" s="60" t="s">
         <v>41</v>
       </c>
       <c r="G1" s="43" t="s">
@@ -9645,28 +9642,28 @@
       <c r="H1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="N1" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="38" t="s">
+      <c r="O1" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="38" t="s">
+      <c r="P1" s="39" t="s">
         <v>50</v>
       </c>
     </row>
@@ -9694,55 +9691,55 @@
     <col min="1" max="1" width="9.5" style="7"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
     <col min="3" max="3" width="22.1640625" customWidth="1"/>
-    <col min="4" max="5" width="14.5" style="7" customWidth="1"/>
+    <col min="4" max="5" width="14.5" style="9" customWidth="1"/>
     <col min="6" max="6" width="10.5" customWidth="1"/>
     <col min="7" max="7" width="26.5" customWidth="1"/>
     <col min="8" max="8" width="21.5" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="19.5" style="2" customWidth="1"/>
-    <col min="12" max="12" width="25.5" style="11" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="25.5" style="25" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" s="65" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="39" t="s">
         <v>30</v>
       </c>
       <c r="G1" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="39" t="s">
         <v>58</v>
       </c>
       <c r="K1" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="82" t="s">
+      <c r="L1" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="82" t="s">
+      <c r="M1" s="64" t="s">
         <v>61</v>
       </c>
     </row>
@@ -9775,10 +9772,10 @@
     <col min="2" max="2" width="19.5" customWidth="1"/>
     <col min="3" max="5" width="16.5" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="7" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="7" customWidth="1"/>
-    <col min="9" max="10" width="13.5" style="7" customWidth="1"/>
-    <col min="11" max="11" width="12" style="7" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="9" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="9" customWidth="1"/>
+    <col min="9" max="10" width="13.5" style="9" customWidth="1"/>
+    <col min="11" max="11" width="12" style="9" customWidth="1"/>
     <col min="12" max="12" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9801,19 +9798,19 @@
       <c r="F1" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="66" t="s">
         <v>69</v>
       </c>
       <c r="L1" s="62" t="s">
@@ -9840,19 +9837,19 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="5"/>
+    <col min="2" max="2" width="7.83203125" style="30" customWidth="1"/>
     <col min="3" max="3" width="22.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="5"/>
-    <col min="5" max="5" width="8.5" style="29" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="30" customWidth="1"/>
     <col min="6" max="6" width="24.5" style="5" customWidth="1"/>
     <col min="7" max="7" width="9.5" style="5"/>
-    <col min="8" max="8" width="24.1640625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" style="31" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="5"/>
     <col min="10" max="10" width="14.5" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.83203125" style="5" customWidth="1"/>
@@ -9861,56 +9858,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="86" t="s">
+      <c r="C1" s="85"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="65"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="67"/>
       <c r="J1" s="46" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="70" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="66" t="s">
+    <row r="2" spans="1:12" s="72" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="69" t="s">
+      <c r="F2" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="69" t="s">
+      <c r="G2" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="68" t="s">
+      <c r="H2" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="69" t="s">
+      <c r="I2" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="69" t="s">
+      <c r="J2" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="69" t="s">
+      <c r="K2" s="71" t="s">
         <v>80</v>
       </c>
-      <c r="L2" s="69" t="s">
+      <c r="L2" s="71" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TM-6932 adding missing formats to the Devices and Database Sheets
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="782"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="14900" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -8102,7 +8102,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8146,7 +8146,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -9086,13 +9086,13 @@
     <col min="25" max="25" width="13.5" style="5" customWidth="1"/>
     <col min="26" max="26" width="8.5" style="5" customWidth="1"/>
     <col min="27" max="27" width="11.5" style="5" customWidth="1"/>
-    <col min="28" max="28" width="11" style="5"/>
+    <col min="28" max="28" width="11" style="4"/>
     <col min="29" max="29" width="10" style="4" customWidth="1"/>
-    <col min="30" max="30" width="11" style="5"/>
+    <col min="30" max="30" width="11" style="4"/>
     <col min="31" max="31" width="15.5" style="4" customWidth="1"/>
     <col min="32" max="32" width="12.1640625" style="5" customWidth="1"/>
     <col min="33" max="33" width="12" style="6" customWidth="1"/>
-    <col min="34" max="34" width="9.33203125" style="5" customWidth="1"/>
+    <col min="34" max="34" width="9.33203125" style="4" customWidth="1"/>
     <col min="35" max="35" width="11" style="5"/>
     <col min="36" max="36" width="8.83203125" style="5" customWidth="1"/>
     <col min="37" max="38" width="11" style="5"/>
@@ -9185,13 +9185,13 @@
       <c r="AA1" s="45" t="s">
         <v>170</v>
       </c>
-      <c r="AB1" s="45" t="s">
+      <c r="AB1" s="50" t="s">
         <v>171</v>
       </c>
       <c r="AC1" s="50" t="s">
         <v>172</v>
       </c>
-      <c r="AD1" s="45" t="s">
+      <c r="AD1" s="50" t="s">
         <v>14</v>
       </c>
       <c r="AE1" s="50" t="s">
@@ -9203,7 +9203,7 @@
       <c r="AG1" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="AH1" s="45" t="s">
+      <c r="AH1" s="50" t="s">
         <v>17</v>
       </c>
       <c r="AI1" s="45" t="s">
@@ -9224,7 +9224,7 @@
       <c r="AN1" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="AO1" s="45" t="s">
+      <c r="AO1" s="50" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TM-1097 Excel Export Template Cursor position view not fully left
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/octavio/Documents/TDS/tranman/git-tdstm/web-app/templates/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="14900" tabRatio="782"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -45,9 +40,6 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -6266,74 +6258,74 @@
     <cellStyle name="EMC Table Text Example" xfId="203"/>
     <cellStyle name="EMC Table Text_Title" xfId="204"/>
     <cellStyle name="EMC Title" xfId="205"/>
-    <cellStyle name="Followed Hyperlink" xfId="1541" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1543" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1545" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1547" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1549" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1551" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1553" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1555" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1557" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1559" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1561" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1563" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1565" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1567" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1569" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1571" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1573" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1575" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1577" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1579" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1581" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1583" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1585" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1587" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1589" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1591" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1593" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1595" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1597" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1599" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1601" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1603" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1605" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1607" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1540" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1542" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1544" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1546" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1548" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1550" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1552" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1554" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1556" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1558" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1560" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1562" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1564" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1566" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1568" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1570" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1572" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1574" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1576" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1578" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1580" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1582" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1584" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1586" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1588" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1590" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1592" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1594" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1596" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1598" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1600" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1602" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1604" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1606" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1540" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1542" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1544" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1546" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1548" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1550" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1552" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1554" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1556" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1558" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1560" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1562" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1564" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1566" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1568" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1570" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1574" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1576" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1578" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1580" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1582" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1584" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1586" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1588" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1590" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1592" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1600" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1602" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1604" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1606" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1541" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1543" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1545" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1547" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1549" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1551" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1553" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1555" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1557" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1559" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1561" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1563" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1565" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1567" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1569" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1571" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1573" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1575" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1577" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1579" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1581" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1583" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1585" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1587" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1589" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1591" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1593" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1595" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1597" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1599" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1601" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1603" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1605" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1607" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink 10" xfId="206"/>
     <cellStyle name="Hyperlink 11" xfId="207"/>
     <cellStyle name="Hyperlink 12" xfId="208"/>
@@ -8101,8 +8093,8 @@
         </a:ln>
         <a:effectLst/>
         <a:extLst>
-          <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8145,8 +8137,8 @@
         </a:ln>
         <a:effectLst/>
         <a:extLst>
-          <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -8172,24 +8164,24 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="11.5" customWidth="1"/>
     <col min="9" max="9" width="38.5" customWidth="1"/>
     <col min="10" max="10" width="2.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
@@ -8197,7 +8189,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>1</v>
       </c>
@@ -8205,7 +8197,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>2</v>
       </c>
@@ -8213,7 +8205,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>5</v>
       </c>
@@ -8221,7 +8213,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>4</v>
       </c>
@@ -8229,7 +8221,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>3</v>
       </c>
@@ -8237,7 +8229,7 @@
         <v>38295</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>125</v>
       </c>
@@ -8245,7 +8237,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>126</v>
       </c>
@@ -8253,10 +8245,10 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>90</v>
       </c>
@@ -8265,7 +8257,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>123</v>
       </c>
@@ -8274,13 +8266,13 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -8291,7 +8283,7 @@
       </c>
       <c r="G15" s="83"/>
     </row>
-    <row r="16" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="82" t="s">
         <v>88</v>
@@ -8310,7 +8302,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17">
         <f>COUNTA(Applications!B:B)-1</f>
         <v>0</v>
@@ -8338,7 +8330,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <f>COUNTIF(Applications!D:D,"Master")</f>
         <v>0</v>
@@ -8360,7 +8352,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <f>A17-A18</f>
         <v>0</v>
@@ -8388,7 +8380,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17">
         <f>COUNTA(Devices!B:B)-1</f>
         <v>0</v>
@@ -8422,7 +8414,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <f>COUNTIF(Devices!P:P,"Server")+COUNTIF(Devices!P:P,"VM")+COUNTIF(Devices!P:P,"Blade")+COUNTIF(Devices!P:P,"Appliance")</f>
         <v>0</v>
@@ -8441,7 +8433,7 @@
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
     </row>
-    <row r="22" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17">
         <f>COUNTA(Databases!B:B)-1</f>
         <v>0</v>
@@ -8466,7 +8458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17">
         <f>COUNTA(Storage!B:B)-1</f>
         <v>0</v>
@@ -8491,7 +8483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17">
         <f>COUNTA(Dependencies!D:D)-1</f>
         <v>0</v>
@@ -8516,7 +8508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <f>COUNTIF(Dependencies!H:H,"Master")</f>
         <v>0</v>
@@ -8529,7 +8521,7 @@
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Application")-A25</f>
         <v>0</v>
@@ -8542,7 +8534,7 @@
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
     </row>
-    <row r="27" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!H:H,"Runs On")</f>
         <v>0</v>
@@ -8555,7 +8547,7 @@
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
     </row>
-    <row r="28" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Database")</f>
         <v>0</v>
@@ -8568,7 +8560,7 @@
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
     </row>
-    <row r="29" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <f>COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Server")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Blade")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"VM")</f>
         <v>0</v>
@@ -8581,7 +8573,7 @@
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
     </row>
-    <row r="30" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <f>COUNTIF(Dependencies!H:H,"Storage")</f>
         <v>0</v>
@@ -8594,7 +8586,7 @@
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
     </row>
-    <row r="31" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17">
         <f>COUNTA(Room!B:B)-1</f>
         <v>0</v>
@@ -8607,7 +8599,7 @@
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
     </row>
-    <row r="32" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17">
         <f>COUNTA(Rack!B:B)-1</f>
         <v>0</v>
@@ -8620,7 +8612,7 @@
       <c r="F32" s="24"/>
       <c r="G32" s="24"/>
     </row>
-    <row r="33" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17">
         <f>COUNTA(Cabling!B:B)-2</f>
         <v>0</v>
@@ -8633,7 +8625,7 @@
       <c r="F33" s="24"/>
       <c r="G33" s="24"/>
     </row>
-    <row r="34" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
         <f>COUNTA(Comments!B:B)-1</f>
         <v>0</v>
@@ -8646,21 +8638,21 @@
       <c r="F34" s="24"/>
       <c r="G34" s="24"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="46" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="47" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="48" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="45" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataConsolidate/>
@@ -8705,18 +8697,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" style="9" customWidth="1"/>
     <col min="2" max="2" width="16" style="7" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="20.125" style="10" customWidth="1"/>
     <col min="4" max="4" width="17.5" style="8" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="10" customWidth="1"/>
-    <col min="6" max="6" width="51.83203125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="51.875" style="10" customWidth="1"/>
     <col min="7" max="16384" width="9.5" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="76" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="73" t="s">
         <v>82</v>
       </c>
@@ -8756,13 +8748,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="5" width="19.5" style="33" customWidth="1"/>
     <col min="6" max="16384" width="11.5" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="78" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="77" t="s">
         <v>127</v>
       </c>
@@ -8795,36 +8787,36 @@
   <dimension ref="A1:EH1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="6.625" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="35" customWidth="1"/>
+    <col min="6" max="6" width="9.375" style="35" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.375" customWidth="1"/>
+    <col min="9" max="9" width="12.875" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.5" style="34" customWidth="1"/>
     <col min="12" max="12" width="9.5" style="2"/>
     <col min="17" max="17" width="13.5" customWidth="1"/>
-    <col min="18" max="20" width="12.83203125" customWidth="1"/>
+    <col min="18" max="20" width="12.875" customWidth="1"/>
     <col min="21" max="21" width="9.5" style="8"/>
-    <col min="22" max="22" width="11.83203125" style="8" customWidth="1"/>
+    <col min="22" max="22" width="11.875" style="8" customWidth="1"/>
     <col min="25" max="25" width="9.5" style="2"/>
     <col min="34" max="34" width="11.5" customWidth="1"/>
     <col min="35" max="35" width="13.5" customWidth="1"/>
-    <col min="36" max="36" width="16.1640625" style="7" customWidth="1"/>
+    <col min="36" max="36" width="16.125" style="7" customWidth="1"/>
     <col min="37" max="37" width="10.5" customWidth="1"/>
-    <col min="38" max="38" width="12.83203125" customWidth="1"/>
+    <col min="38" max="38" width="12.875" customWidth="1"/>
     <col min="39" max="39" width="14.5" style="7" customWidth="1"/>
-    <col min="40" max="40" width="10.83203125" customWidth="1"/>
-    <col min="41" max="41" width="11.83203125" customWidth="1"/>
+    <col min="40" max="40" width="10.875" customWidth="1"/>
+    <col min="41" max="41" width="11.875" customWidth="1"/>
     <col min="42" max="42" width="13.5" style="26" customWidth="1"/>
     <col min="43" max="70" width="9.5" customWidth="1"/>
     <col min="71" max="71" width="9.5" style="9" customWidth="1"/>
@@ -8833,7 +8825,7 @@
     <col min="108" max="138" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:138" s="46" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:138" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
         <v>174</v>
       </c>
@@ -9059,30 +9051,30 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="6.625" style="4" customWidth="1"/>
     <col min="2" max="3" width="20.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="6" customWidth="1"/>
     <col min="5" max="5" width="15.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="36" customWidth="1"/>
+    <col min="6" max="6" width="9.375" style="36" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="5" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="81" customWidth="1"/>
+    <col min="8" max="8" width="10.375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="12.875" style="81" customWidth="1"/>
     <col min="10" max="10" width="17.5" style="4" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="15.875" style="5" customWidth="1"/>
     <col min="12" max="12" width="13" style="5" customWidth="1"/>
     <col min="13" max="13" width="11.5" style="5" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="15.1640625" style="5" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="11.125" style="5" customWidth="1"/>
+    <col min="15" max="15" width="15.125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="12.125" style="5" customWidth="1"/>
     <col min="17" max="17" width="9.5" style="5" customWidth="1"/>
-    <col min="18" max="18" width="8.83203125" style="5" customWidth="1"/>
+    <col min="18" max="18" width="8.875" style="5" customWidth="1"/>
     <col min="19" max="20" width="10.5" style="5" customWidth="1"/>
-    <col min="21" max="21" width="9.83203125" style="5" customWidth="1"/>
+    <col min="21" max="21" width="9.875" style="5" customWidth="1"/>
     <col min="22" max="22" width="10.5" style="4" customWidth="1"/>
     <col min="23" max="23" width="11.5" style="5" customWidth="1"/>
-    <col min="24" max="24" width="18.83203125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="18.875" style="4" customWidth="1"/>
     <col min="25" max="25" width="13.5" style="5" customWidth="1"/>
     <col min="26" max="26" width="8.5" style="5" customWidth="1"/>
     <col min="27" max="27" width="11.5" style="5" customWidth="1"/>
@@ -9090,20 +9082,20 @@
     <col min="29" max="29" width="10" style="4" customWidth="1"/>
     <col min="30" max="30" width="11" style="4"/>
     <col min="31" max="31" width="15.5" style="4" customWidth="1"/>
-    <col min="32" max="32" width="12.1640625" style="5" customWidth="1"/>
+    <col min="32" max="32" width="12.125" style="5" customWidth="1"/>
     <col min="33" max="33" width="12" style="6" customWidth="1"/>
-    <col min="34" max="34" width="9.33203125" style="4" customWidth="1"/>
+    <col min="34" max="34" width="9.375" style="4" customWidth="1"/>
     <col min="35" max="35" width="11" style="5"/>
-    <col min="36" max="36" width="8.83203125" style="5" customWidth="1"/>
+    <col min="36" max="36" width="8.875" style="5" customWidth="1"/>
     <col min="37" max="38" width="11" style="5"/>
-    <col min="39" max="39" width="12.83203125" style="4" customWidth="1"/>
+    <col min="39" max="39" width="12.875" style="4" customWidth="1"/>
     <col min="40" max="40" width="8.5" style="4" customWidth="1"/>
-    <col min="41" max="41" width="10.1640625" style="4" customWidth="1"/>
+    <col min="41" max="41" width="10.125" style="4" customWidth="1"/>
     <col min="42" max="137" width="9.5" style="5" customWidth="1"/>
     <col min="138" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="45" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:41" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
         <v>174</v>
       </c>
@@ -9248,20 +9240,20 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="6.625" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="35" customWidth="1"/>
+    <col min="6" max="6" width="9.375" style="35" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.375" customWidth="1"/>
+    <col min="9" max="9" width="12.875" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.5" style="11" customWidth="1"/>
     <col min="12" max="12" width="9.5" style="7"/>
-    <col min="13" max="13" width="7.1640625" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" style="7" customWidth="1"/>
-    <col min="16" max="17" width="12.83203125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="7.125" customWidth="1"/>
+    <col min="14" max="14" width="12.875" style="7" customWidth="1"/>
+    <col min="16" max="17" width="12.875" style="8" customWidth="1"/>
     <col min="18" max="41" width="9.5" customWidth="1"/>
     <col min="42" max="42" width="9.5" style="9" customWidth="1"/>
     <col min="43" max="81" width="9.5" customWidth="1"/>
@@ -9269,7 +9261,7 @@
     <col min="84" max="85" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" s="46" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:113" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
         <v>174</v>
       </c>
@@ -9417,20 +9409,20 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="6.625" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="8" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="35" customWidth="1"/>
+    <col min="6" max="6" width="9.375" style="35" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.375" customWidth="1"/>
+    <col min="9" max="9" width="12.875" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.5" style="11" customWidth="1"/>
     <col min="11" max="11" width="8.5" style="10"/>
     <col min="13" max="13" width="8.5" style="7"/>
-    <col min="14" max="14" width="7.1640625" customWidth="1"/>
+    <col min="14" max="14" width="7.125" customWidth="1"/>
     <col min="15" max="15" width="14.5" style="7" customWidth="1"/>
     <col min="17" max="40" width="9.5" customWidth="1"/>
     <col min="41" max="41" width="9.5" style="9" customWidth="1"/>
@@ -9439,7 +9431,7 @@
     <col min="82" max="112" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" s="46" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:112" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
         <v>174</v>
       </c>
@@ -9602,22 +9594,22 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="8.5" style="7"/>
     <col min="3" max="3" width="13.5" style="7" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="10" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="7" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="16.125" style="10" customWidth="1"/>
     <col min="7" max="7" width="14.5" style="10" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" customWidth="1"/>
-    <col min="11" max="11" width="8.1640625" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="14.125" customWidth="1"/>
+    <col min="10" max="10" width="17.875" customWidth="1"/>
+    <col min="11" max="11" width="8.125" customWidth="1"/>
+    <col min="12" max="12" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
         <v>36</v>
       </c>
@@ -9686,23 +9678,23 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" style="7"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.125" customWidth="1"/>
     <col min="4" max="5" width="14.5" style="9" customWidth="1"/>
     <col min="6" max="6" width="10.5" customWidth="1"/>
     <col min="7" max="7" width="26.5" customWidth="1"/>
     <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="13.125" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="19.5" style="2" customWidth="1"/>
     <col min="12" max="12" width="25.5" style="25" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" style="25" customWidth="1"/>
+    <col min="13" max="13" width="16.875" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="65" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
         <v>51</v>
       </c>
@@ -9766,20 +9758,20 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" style="7" customWidth="1"/>
     <col min="2" max="2" width="19.5" customWidth="1"/>
     <col min="3" max="5" width="16.5" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="12.5" style="9" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="12.875" style="9" customWidth="1"/>
     <col min="9" max="10" width="13.5" style="9" customWidth="1"/>
     <col min="11" max="11" width="12" style="9" customWidth="1"/>
     <col min="12" max="12" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="62" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="51" t="s">
         <v>62</v>
       </c>
@@ -9840,24 +9832,24 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" style="5"/>
-    <col min="2" max="2" width="7.83203125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="7.875" style="30" customWidth="1"/>
     <col min="3" max="3" width="22.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="5"/>
     <col min="5" max="5" width="8.5" style="30" customWidth="1"/>
     <col min="6" max="6" width="24.5" style="5" customWidth="1"/>
     <col min="7" max="7" width="9.5" style="5"/>
-    <col min="8" max="8" width="24.1640625" style="31" customWidth="1"/>
+    <col min="8" max="8" width="24.125" style="31" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="5"/>
     <col min="10" max="10" width="14.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="11.875" style="5" customWidth="1"/>
     <col min="12" max="12" width="15.5" style="5" customWidth="1"/>
     <col min="13" max="16384" width="9.5" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="84" t="s">
         <v>71</v>
       </c>
@@ -9873,7 +9865,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="72" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" s="72" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="68" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
TM-10977 Excel Export Template Cursor position view not fully left
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -8790,7 +8790,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9048,7 +9048,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9237,7 +9237,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9406,7 +9406,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9675,7 +9675,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9755,7 +9755,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
TM-11229 Refactor DEVICE.supportType field label in Setting domain class
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/git/repo/tds/tdstm/web-app/templates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="782"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="20740" windowHeight="11760" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -128,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="174">
   <si>
     <t>Customer:</t>
   </si>
@@ -173,9 +178,6 @@
   </si>
   <si>
     <t>Target Blade Position</t>
-  </si>
-  <si>
-    <t>SupportType</t>
   </si>
   <si>
     <t>Environment</t>
@@ -660,11 +662,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="d\ mmm\ yy"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -5911,15 +5912,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5966,7 +5967,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1049"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -5976,25 +5977,25 @@
     <xf numFmtId="1" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="17" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="1316" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="1316" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6258,74 +6259,74 @@
     <cellStyle name="EMC Table Text Example" xfId="203"/>
     <cellStyle name="EMC Table Text_Title" xfId="204"/>
     <cellStyle name="EMC Title" xfId="205"/>
-    <cellStyle name="Hipervínculo" xfId="1540" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1542" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1544" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1546" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1548" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1550" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1552" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1554" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1556" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1558" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1560" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1562" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1564" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1566" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1568" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1570" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1572" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1574" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1576" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1578" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1580" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1582" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1584" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1586" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1588" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1590" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1592" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1594" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1596" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1598" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1600" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1602" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1604" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1606" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1541" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1543" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1545" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1547" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1549" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1551" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1553" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1555" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1557" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1559" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1561" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1563" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1565" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1567" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1569" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1571" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1573" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1575" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1577" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1579" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1581" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1583" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1585" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1587" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1589" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1591" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1593" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1595" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1597" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1599" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1601" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1603" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1605" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="1607" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1541" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1543" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1545" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1547" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1549" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1551" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1553" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1555" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1557" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1559" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1561" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1563" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1565" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1567" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1569" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1571" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1573" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1575" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1577" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1579" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1581" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1583" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1585" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1587" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1589" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1591" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1593" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1595" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1597" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1599" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1601" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1603" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1605" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1607" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1540" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1542" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1544" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1546" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1548" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1550" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1552" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1554" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1556" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1558" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1560" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1562" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1564" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1566" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1568" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1570" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1574" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1576" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1578" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1580" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1582" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1584" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1586" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1588" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1590" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1592" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1600" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1602" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1604" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1606" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 10" xfId="206"/>
     <cellStyle name="Hyperlink 11" xfId="207"/>
     <cellStyle name="Hyperlink 12" xfId="208"/>
@@ -8164,64 +8165,64 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="11.5" customWidth="1"/>
     <col min="9" max="9" width="38.5" customWidth="1"/>
     <col min="10" max="10" width="2.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="32" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="32" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="32" t="s">
         <v>3</v>
       </c>
@@ -8229,86 +8230,86 @@
         <v>38295</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="B9" t="s">
-        <v>122</v>
+      <c r="B10" t="s">
+        <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="B10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="83" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G15" s="83"/>
     </row>
-    <row r="16" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="B16" s="82" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C16" s="82"/>
       <c r="D16" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F16" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="G16" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G16" s="15" t="s">
-        <v>119</v>
-      </c>
     </row>
-    <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17">
         <f>COUNTA(Applications!B:B)-1</f>
         <v>0</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D17" s="19">
         <f>COUNTA(Applications!A:A)-1</f>
@@ -8327,16 +8328,16 @@
         <v>0</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18">
         <f>COUNTIF(Applications!D:D,"Master")</f>
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D18" s="21">
         <f>COUNTIFS(Applications!A:A,"&gt;0",Applications!D:D,"Master")</f>
@@ -8349,16 +8350,16 @@
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
       <c r="I18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19">
         <f>A17-A18</f>
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D19" s="21">
         <f>IF(ISNUMBER(D17),D17-D18,"")</f>
@@ -8371,22 +8372,22 @@
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
       <c r="I19" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17">
         <f>COUNTA(Devices!B:B)-1</f>
         <v>0</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D20" s="19">
         <f>COUNTA(Devices!A:A)-1</f>
@@ -8405,22 +8406,22 @@
         <v>0</v>
       </c>
       <c r="I20" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21">
         <f>COUNTIF(Devices!P:P,"Server")+COUNTIF(Devices!P:P,"VM")+COUNTIF(Devices!P:P,"Blade")+COUNTIF(Devices!P:P,"Appliance")</f>
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D21" s="21">
         <f>COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!P:P,"Server")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!P:P,"Blade")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!P:P,"VM")++COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!P:P,"Appliance")</f>
@@ -8433,13 +8434,13 @@
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
     </row>
-    <row r="22" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17">
         <f>COUNTA(Databases!B:B)-1</f>
         <v>0</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" s="19">
         <f>COUNTA(Databases!A:A)-1</f>
@@ -8458,13 +8459,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17">
         <f>COUNTA(Storage!B:B)-1</f>
         <v>0</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" s="19">
         <f>COUNTA(Storage!A:A)-1</f>
@@ -8483,13 +8484,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17">
         <f>COUNTA(Dependencies!D:D)-1</f>
         <v>0</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D24" s="19">
         <f>COUNTA(Dependencies!A:A)-1</f>
@@ -8508,151 +8509,151 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25">
         <f>COUNTIF(Dependencies!H:H,"Master")</f>
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Application")-A25</f>
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
     </row>
-    <row r="27" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!H:H,"Runs On")</f>
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
     </row>
-    <row r="28" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Database")</f>
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
     </row>
-    <row r="29" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29">
         <f>COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Server")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Blade")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"VM")</f>
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
     </row>
-    <row r="30" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30">
         <f>COUNTIF(Dependencies!H:H,"Storage")</f>
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
     </row>
-    <row r="31" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17">
         <f>COUNTA(Room!B:B)-1</f>
         <v>0</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
     </row>
-    <row r="32" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17">
         <f>COUNTA(Rack!B:B)-1</f>
         <v>0</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D32" s="24"/>
       <c r="E32" s="24"/>
       <c r="F32" s="24"/>
       <c r="G32" s="24"/>
     </row>
-    <row r="33" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17">
         <f>COUNTA(Cabling!B:B)-2</f>
         <v>0</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D33" s="24"/>
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
       <c r="G33" s="24"/>
     </row>
-    <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
         <f>COUNTA(Comments!B:B)-1</f>
         <v>0</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D34" s="24"/>
       <c r="E34" s="24"/>
       <c r="F34" s="24"/>
       <c r="G34" s="24"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="46" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="47" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="48" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataConsolidate/>
@@ -8697,35 +8698,35 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.5" style="9" customWidth="1"/>
     <col min="2" max="2" width="16" style="7" customWidth="1"/>
-    <col min="3" max="3" width="20.125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="10" customWidth="1"/>
     <col min="4" max="4" width="17.5" style="8" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="10" customWidth="1"/>
-    <col min="6" max="6" width="51.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" style="10" customWidth="1"/>
     <col min="7" max="16384" width="9.5" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="76" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="74" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="74" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="E1" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="F1" s="75" t="s">
         <v>85</v>
-      </c>
-      <c r="F1" s="75" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -8748,27 +8749,27 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="5" width="19.5" style="33" customWidth="1"/>
     <col min="6" max="16384" width="11.5" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="78" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="78" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="77" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="C1" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="D1" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="E1" s="77" t="s">
         <v>130</v>
-      </c>
-      <c r="E1" s="77" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -8793,30 +8794,30 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="9.375" style="35" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="35" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="10.375" customWidth="1"/>
-    <col min="9" max="9" width="12.875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.5" style="34" customWidth="1"/>
     <col min="12" max="12" width="9.5" style="2"/>
     <col min="17" max="17" width="13.5" customWidth="1"/>
-    <col min="18" max="20" width="12.875" customWidth="1"/>
+    <col min="18" max="20" width="12.83203125" customWidth="1"/>
     <col min="21" max="21" width="9.5" style="8"/>
-    <col min="22" max="22" width="11.875" style="8" customWidth="1"/>
+    <col min="22" max="22" width="11.83203125" style="8" customWidth="1"/>
     <col min="25" max="25" width="9.5" style="2"/>
     <col min="34" max="34" width="11.5" customWidth="1"/>
     <col min="35" max="35" width="13.5" customWidth="1"/>
-    <col min="36" max="36" width="16.125" style="7" customWidth="1"/>
+    <col min="36" max="36" width="16.1640625" style="7" customWidth="1"/>
     <col min="37" max="37" width="10.5" customWidth="1"/>
-    <col min="38" max="38" width="12.875" customWidth="1"/>
+    <col min="38" max="38" width="12.83203125" customWidth="1"/>
     <col min="39" max="39" width="14.5" style="7" customWidth="1"/>
-    <col min="40" max="40" width="10.875" customWidth="1"/>
-    <col min="41" max="41" width="11.875" customWidth="1"/>
+    <col min="40" max="40" width="10.83203125" customWidth="1"/>
+    <col min="41" max="41" width="11.83203125" customWidth="1"/>
     <col min="42" max="42" width="13.5" style="26" customWidth="1"/>
     <col min="43" max="70" width="9.5" customWidth="1"/>
     <col min="71" max="71" width="9.5" style="9" customWidth="1"/>
@@ -8825,9 +8826,9 @@
     <col min="108" max="138" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:138" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:138" s="46" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>7</v>
@@ -8836,121 +8837,121 @@
         <v>11</v>
       </c>
       <c r="D1" s="53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="79" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="53" t="s">
-        <v>129</v>
-      </c>
-      <c r="I1" s="79" t="s">
-        <v>157</v>
-      </c>
-      <c r="J1" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="54" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="53" t="s">
+      <c r="Q1" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="R1" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="S1" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="T1" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="53" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q1" s="55" t="s">
-        <v>135</v>
-      </c>
-      <c r="R1" s="55" t="s">
+      <c r="U1" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="S1" s="55" t="s">
-        <v>134</v>
-      </c>
-      <c r="T1" s="55" t="s">
+      <c r="V1" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="W1" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="56" t="s">
-        <v>137</v>
-      </c>
-      <c r="V1" s="56" t="s">
+      <c r="X1" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="W1" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="X1" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y1" s="54" t="s">
+      <c r="Z1" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="Z1" s="53" t="s">
+      <c r="AA1" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="AA1" s="53" t="s">
+      <c r="AB1" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="AB1" s="53" t="s">
+      <c r="AC1" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="AC1" s="53" t="s">
+      <c r="AD1" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="AD1" s="46" t="s">
+      <c r="AE1" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="AE1" s="46" t="s">
+      <c r="AF1" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="AF1" s="46" t="s">
+      <c r="AG1" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="AG1" s="46" t="s">
+      <c r="AH1" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="AH1" s="45" t="s">
+      <c r="AI1" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="AI1" s="45" t="s">
+      <c r="AJ1" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="AJ1" s="57" t="s">
+      <c r="AK1" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="AK1" s="58" t="s">
+      <c r="AL1" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="AL1" s="58" t="s">
+      <c r="AM1" s="57" t="s">
         <v>152</v>
       </c>
-      <c r="AM1" s="57" t="s">
+      <c r="AN1" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="AN1" s="58" t="s">
+      <c r="AO1" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="AO1" s="58" t="s">
+      <c r="AP1" s="57" t="s">
         <v>155</v>
-      </c>
-      <c r="AP1" s="57" t="s">
-        <v>156</v>
       </c>
       <c r="BO1" s="45"/>
       <c r="BP1" s="45"/>
@@ -9051,30 +9052,30 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="4" customWidth="1"/>
     <col min="2" max="3" width="20.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="6" customWidth="1"/>
     <col min="5" max="5" width="15.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.375" style="36" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="36" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="5" customWidth="1"/>
-    <col min="8" max="8" width="10.375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="12.875" style="81" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="81" customWidth="1"/>
     <col min="10" max="10" width="17.5" style="4" customWidth="1"/>
-    <col min="11" max="11" width="15.875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" style="5" customWidth="1"/>
     <col min="12" max="12" width="13" style="5" customWidth="1"/>
     <col min="13" max="13" width="11.5" style="5" customWidth="1"/>
-    <col min="14" max="14" width="11.125" style="5" customWidth="1"/>
-    <col min="15" max="15" width="15.125" style="5" customWidth="1"/>
-    <col min="16" max="16" width="12.125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" style="5" customWidth="1"/>
     <col min="17" max="17" width="9.5" style="5" customWidth="1"/>
-    <col min="18" max="18" width="8.875" style="5" customWidth="1"/>
+    <col min="18" max="18" width="8.83203125" style="5" customWidth="1"/>
     <col min="19" max="20" width="10.5" style="5" customWidth="1"/>
-    <col min="21" max="21" width="9.875" style="5" customWidth="1"/>
+    <col min="21" max="21" width="9.83203125" style="5" customWidth="1"/>
     <col min="22" max="22" width="10.5" style="4" customWidth="1"/>
     <col min="23" max="23" width="11.5" style="5" customWidth="1"/>
-    <col min="24" max="24" width="18.875" style="4" customWidth="1"/>
+    <col min="24" max="24" width="18.83203125" style="4" customWidth="1"/>
     <col min="25" max="25" width="13.5" style="5" customWidth="1"/>
     <col min="26" max="26" width="8.5" style="5" customWidth="1"/>
     <col min="27" max="27" width="11.5" style="5" customWidth="1"/>
@@ -9082,22 +9083,22 @@
     <col min="29" max="29" width="10" style="4" customWidth="1"/>
     <col min="30" max="30" width="11" style="4"/>
     <col min="31" max="31" width="15.5" style="4" customWidth="1"/>
-    <col min="32" max="32" width="12.125" style="5" customWidth="1"/>
+    <col min="32" max="32" width="12.1640625" style="5" customWidth="1"/>
     <col min="33" max="33" width="12" style="6" customWidth="1"/>
-    <col min="34" max="34" width="9.375" style="4" customWidth="1"/>
+    <col min="34" max="34" width="9.33203125" style="4" customWidth="1"/>
     <col min="35" max="35" width="11" style="5"/>
-    <col min="36" max="36" width="8.875" style="5" customWidth="1"/>
+    <col min="36" max="36" width="8.83203125" style="5" customWidth="1"/>
     <col min="37" max="38" width="11" style="5"/>
-    <col min="39" max="39" width="12.875" style="4" customWidth="1"/>
+    <col min="39" max="39" width="12.83203125" style="4" customWidth="1"/>
     <col min="40" max="40" width="8.5" style="4" customWidth="1"/>
-    <col min="41" max="41" width="10.125" style="4" customWidth="1"/>
+    <col min="41" max="41" width="10.1640625" style="4" customWidth="1"/>
     <col min="42" max="137" width="9.5" style="5" customWidth="1"/>
     <col min="138" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="45" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" s="45" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="47" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B1" s="48" t="s">
         <v>7</v>
@@ -9106,34 +9107,34 @@
         <v>11</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I1" s="80" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="J1" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="45" t="s">
+      <c r="L1" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="M1" s="45" t="s">
         <v>159</v>
-      </c>
-      <c r="M1" s="45" t="s">
-        <v>160</v>
       </c>
       <c r="N1" s="45" t="s">
         <v>8</v>
@@ -9142,82 +9143,82 @@
         <v>9</v>
       </c>
       <c r="P1" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q1" s="45" t="s">
         <v>161</v>
-      </c>
-      <c r="Q1" s="45" t="s">
-        <v>162</v>
       </c>
       <c r="R1" s="45" t="s">
         <v>12</v>
       </c>
       <c r="S1" s="45" t="s">
+        <v>162</v>
+      </c>
+      <c r="T1" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="T1" s="45" t="s">
+      <c r="U1" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="U1" s="45" t="s">
+      <c r="V1" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="V1" s="50" t="s">
+      <c r="W1" s="45" t="s">
         <v>166</v>
-      </c>
-      <c r="W1" s="45" t="s">
-        <v>167</v>
       </c>
       <c r="X1" s="50" t="s">
         <v>13</v>
       </c>
       <c r="Y1" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z1" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="Z1" s="45" t="s">
+      <c r="AA1" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="AA1" s="45" t="s">
+      <c r="AB1" s="50" t="s">
         <v>170</v>
       </c>
-      <c r="AB1" s="50" t="s">
+      <c r="AC1" s="50" t="s">
         <v>171</v>
-      </c>
-      <c r="AC1" s="50" t="s">
-        <v>172</v>
       </c>
       <c r="AD1" s="50" t="s">
         <v>14</v>
       </c>
       <c r="AE1" s="50" t="s">
-        <v>15</v>
+        <v>132</v>
       </c>
       <c r="AF1" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG1" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="AG1" s="49" t="s">
-        <v>138</v>
-      </c>
       <c r="AH1" s="50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI1" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ1" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="AJ1" s="45" t="s">
+      <c r="AK1" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="AK1" s="45" t="s">
-        <v>21</v>
-      </c>
       <c r="AL1" s="45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AM1" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN1" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="AN1" s="51" t="s">
+      <c r="AO1" s="50" t="s">
         <v>24</v>
-      </c>
-      <c r="AO1" s="50" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -9240,20 +9241,20 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="9.375" style="35" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="35" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="10.375" customWidth="1"/>
-    <col min="9" max="9" width="12.875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.5" style="11" customWidth="1"/>
     <col min="12" max="12" width="9.5" style="7"/>
-    <col min="13" max="13" width="7.125" customWidth="1"/>
-    <col min="14" max="14" width="12.875" style="7" customWidth="1"/>
-    <col min="16" max="17" width="12.875" style="8" customWidth="1"/>
+    <col min="13" max="13" width="7.1640625" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" style="7" customWidth="1"/>
+    <col min="16" max="17" width="12.83203125" style="8" customWidth="1"/>
     <col min="18" max="41" width="9.5" customWidth="1"/>
     <col min="42" max="42" width="9.5" style="9" customWidth="1"/>
     <col min="43" max="81" width="9.5" customWidth="1"/>
@@ -9261,9 +9262,9 @@
     <col min="84" max="85" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:113" s="46" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>7</v>
@@ -9272,46 +9273,46 @@
         <v>11</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="79" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="46" t="s">
-        <v>129</v>
-      </c>
-      <c r="I1" s="79" t="s">
-        <v>157</v>
-      </c>
-      <c r="J1" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="39" t="s">
-        <v>133</v>
-      </c>
       <c r="P1" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q1" s="40" t="s">
         <v>137</v>
-      </c>
-      <c r="Q1" s="40" t="s">
-        <v>138</v>
       </c>
       <c r="AP1" s="45"/>
       <c r="AQ1" s="45"/>
@@ -9409,20 +9410,20 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="8" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="9.375" style="35" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="35" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="10.375" customWidth="1"/>
-    <col min="9" max="9" width="12.875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.5" style="11" customWidth="1"/>
     <col min="11" max="11" width="8.5" style="10"/>
     <col min="13" max="13" width="8.5" style="7"/>
-    <col min="14" max="14" width="7.125" customWidth="1"/>
+    <col min="14" max="14" width="7.1640625" customWidth="1"/>
     <col min="15" max="15" width="14.5" style="7" customWidth="1"/>
     <col min="17" max="40" width="9.5" customWidth="1"/>
     <col min="41" max="41" width="9.5" style="9" customWidth="1"/>
@@ -9431,9 +9432,9 @@
     <col min="82" max="112" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:112" s="46" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>7</v>
@@ -9442,43 +9443,43 @@
         <v>11</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="79" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="39" t="s">
         <v>132</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="I1" s="79" t="s">
-        <v>157</v>
-      </c>
-      <c r="J1" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="L1" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" s="39" t="s">
-        <v>133</v>
       </c>
       <c r="Q1" s="39"/>
       <c r="R1" s="39"/>
@@ -9594,69 +9595,69 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="8.5" style="7"/>
     <col min="3" max="3" width="13.5" style="7" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="10" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="7" customWidth="1"/>
-    <col min="6" max="6" width="16.125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" style="10" customWidth="1"/>
     <col min="7" max="7" width="14.5" style="10" customWidth="1"/>
-    <col min="8" max="8" width="14.125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="14.125" customWidth="1"/>
-    <col min="10" max="10" width="17.875" customWidth="1"/>
-    <col min="11" max="11" width="8.125" customWidth="1"/>
-    <col min="12" max="12" width="12.125" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" customWidth="1"/>
+    <col min="11" max="11" width="8.1640625" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="C1" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="D1" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="F1" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="G1" s="43" t="s">
         <v>41</v>
-      </c>
-      <c r="G1" s="43" t="s">
-        <v>42</v>
       </c>
       <c r="H1" s="43" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="K1" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="L1" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="M1" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="N1" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="O1" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="P1" s="39" t="s">
         <v>49</v>
-      </c>
-      <c r="P1" s="39" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -9678,61 +9679,61 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" style="7"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="22.125" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
     <col min="4" max="5" width="14.5" style="9" customWidth="1"/>
     <col min="6" max="6" width="10.5" customWidth="1"/>
     <col min="7" max="7" width="26.5" customWidth="1"/>
     <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="9" width="13.125" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="19.5" style="2" customWidth="1"/>
     <col min="12" max="12" width="25.5" style="25" customWidth="1"/>
-    <col min="13" max="13" width="16.875" style="25" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="65" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="39" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="E1" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="F1" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="62" t="s">
+      <c r="H1" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="I1" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="J1" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="K1" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="63" t="s">
+      <c r="L1" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="64" t="s">
+      <c r="M1" s="64" t="s">
         <v>60</v>
-      </c>
-      <c r="M1" s="64" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -9758,58 +9759,58 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" style="7" customWidth="1"/>
     <col min="2" max="2" width="19.5" customWidth="1"/>
     <col min="3" max="5" width="16.5" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="12.5" style="9" customWidth="1"/>
-    <col min="8" max="8" width="12.875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="9" customWidth="1"/>
     <col min="9" max="10" width="13.5" style="9" customWidth="1"/>
     <col min="11" max="11" width="12" style="9" customWidth="1"/>
     <col min="12" max="12" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="62" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="62" t="s">
-        <v>63</v>
-      </c>
       <c r="C1" s="62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D1" s="62" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="66" t="s">
+      <c r="H1" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="I1" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="J1" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="66" t="s">
+      <c r="K1" s="66" t="s">
         <v>68</v>
-      </c>
-      <c r="K1" s="66" t="s">
-        <v>69</v>
       </c>
       <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
       <c r="M1" s="62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -9832,75 +9833,75 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" style="5"/>
-    <col min="2" max="2" width="7.875" style="30" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" style="30" customWidth="1"/>
     <col min="3" max="3" width="22.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="5"/>
     <col min="5" max="5" width="8.5" style="30" customWidth="1"/>
     <col min="6" max="6" width="24.5" style="5" customWidth="1"/>
     <col min="7" max="7" width="9.5" style="5"/>
-    <col min="8" max="8" width="24.125" style="31" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" style="31" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="5"/>
     <col min="10" max="10" width="14.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" style="5" customWidth="1"/>
     <col min="12" max="12" width="15.5" style="5" customWidth="1"/>
     <col min="13" max="16384" width="9.5" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B1" s="84" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" s="85"/>
       <c r="D1" s="86"/>
       <c r="E1" s="85" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F1" s="85"/>
       <c r="G1" s="85"/>
       <c r="H1" s="67"/>
       <c r="J1" s="46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="72" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="72" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="C2" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="68" t="s">
+      <c r="D2" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="E2" s="70" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="71" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="70" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="71" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="71" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" s="70" t="s">
+      <c r="I2" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="71" t="s">
+      <c r="J2" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="71" t="s">
+      <c r="K2" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="71" t="s">
+      <c r="L2" s="71" t="s">
         <v>80</v>
-      </c>
-      <c r="L2" s="71" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TM-11518 Asset Export not able to export assets
</commit_message>
<xml_diff>
--- a/web-app/templates/TDSMaster_template.xlsx
+++ b/web-app/templates/TDSMaster_template.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/git/repo/tds/tdstm/web-app/templates/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="20740" windowHeight="11760" tabRatio="782"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -25,15 +20,15 @@
     <sheet name="Validation" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Applications!$A$1:$EH$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Applications!$A$1:$EI$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Cabling!$A$2:$L$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Comments!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Databases!$A$1:$DI$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Databases!$A$1:$DJ$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Dependencies!$A$1:$P$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Devices!$A$1:$EG$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Devices!$A$1:$EH$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Rack!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Room!$A$1:$M$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Storage!$A$1:$DH$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Storage!$A$1:$DI$1</definedName>
     <definedName name="_xlfn_COUNTIFS">#N/A</definedName>
     <definedName name="CustomerName">Title!$B$3</definedName>
     <definedName name="ExportDatetime">Title!$B$8</definedName>
@@ -43,7 +38,7 @@
     <definedName name="ProjectManager">Title!$B$5</definedName>
     <definedName name="ProjectName">Title!$C$4</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -58,7 +53,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="S1" authorId="0">
+    <comment ref="T1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="W1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -114,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0">
+    <comment ref="AD1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -133,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="175">
   <si>
     <t>Customer:</t>
   </si>
@@ -656,6 +651,9 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>Tags</t>
   </si>
 </sst>
 </file>
@@ -6259,74 +6257,74 @@
     <cellStyle name="EMC Table Text Example" xfId="203"/>
     <cellStyle name="EMC Table Text_Title" xfId="204"/>
     <cellStyle name="EMC Title" xfId="205"/>
-    <cellStyle name="Followed Hyperlink" xfId="1541" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1543" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1545" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1547" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1549" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1551" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1553" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1555" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1557" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1559" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1561" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1563" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1565" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1567" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1569" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1571" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1573" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1575" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1577" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1579" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1581" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1583" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1585" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1587" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1589" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1591" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1593" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1595" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1597" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1599" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1601" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1603" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1605" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1607" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1540" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1542" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1544" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1546" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1548" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1550" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1552" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1554" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1556" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1558" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1560" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1562" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1564" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1566" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1568" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1570" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1572" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1574" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1576" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1578" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1580" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1582" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1584" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1586" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1588" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1590" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1592" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1594" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1596" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1598" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1600" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1602" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1604" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1606" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1540" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1542" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1544" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1546" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1548" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1550" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1552" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1554" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1556" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1558" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1560" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1562" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1564" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1566" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1568" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1570" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1574" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1576" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1578" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1580" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1582" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1584" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1586" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1588" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1590" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1592" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1600" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1602" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1604" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1606" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1541" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1543" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1545" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1547" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1549" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1551" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1553" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1555" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1557" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1559" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1561" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1563" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1565" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1567" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1569" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1571" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1573" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1575" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1577" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1579" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1581" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1583" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1585" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1587" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1589" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1591" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1593" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1595" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1597" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1599" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1601" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1603" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1605" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="1607" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink 10" xfId="206"/>
     <cellStyle name="Hyperlink 11" xfId="207"/>
     <cellStyle name="Hyperlink 12" xfId="208"/>
@@ -8165,24 +8163,24 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="11.5" customWidth="1"/>
     <col min="9" max="9" width="38.5" customWidth="1"/>
     <col min="10" max="10" width="2.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
@@ -8190,7 +8188,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>1</v>
       </c>
@@ -8198,7 +8196,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>2</v>
       </c>
@@ -8206,7 +8204,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>5</v>
       </c>
@@ -8214,7 +8212,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>4</v>
       </c>
@@ -8222,7 +8220,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>3</v>
       </c>
@@ -8230,7 +8228,7 @@
         <v>38295</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>124</v>
       </c>
@@ -8238,7 +8236,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>125</v>
       </c>
@@ -8246,10 +8244,10 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>89</v>
       </c>
@@ -8258,7 +8256,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>122</v>
       </c>
@@ -8267,13 +8265,13 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -8284,7 +8282,7 @@
       </c>
       <c r="G15" s="83"/>
     </row>
-    <row r="16" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="82" t="s">
         <v>87</v>
@@ -8303,7 +8301,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17">
         <f>COUNTA(Applications!B:B)-1</f>
         <v>0</v>
@@ -8320,18 +8318,18 @@
         <v>0</v>
       </c>
       <c r="F17" s="20">
-        <f>COUNTIF(Applications!B:EH,REPT("?",254)&amp;"*")</f>
+        <f>COUNTIF(Applications!B:EI,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
       <c r="G17" s="20">
-        <f>COUNTIF(Applications!B:EI,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Applications!B:EI,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Applications!B:EI,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Applications!B:EI,"*"&amp;CHAR(39)&amp;"*")</f>
+        <f>COUNTIF(Applications!B:EJ,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Applications!B:EJ,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Applications!B:EJ,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Applications!B:EJ,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
       <c r="I17" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <f>COUNTIF(Applications!D:D,"Master")</f>
         <v>0</v>
@@ -8353,7 +8351,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <f>A17-A18</f>
         <v>0</v>
@@ -8381,7 +8379,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17">
         <f>COUNTA(Devices!B:B)-1</f>
         <v>0</v>
@@ -8398,11 +8396,11 @@
         <v>0</v>
       </c>
       <c r="F20" s="20">
-        <f>COUNTIF(Devices!B:EG,REPT("?",254)&amp;"*")</f>
+        <f>COUNTIF(Devices!B:EH,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
       <c r="G20" s="20">
-        <f>COUNTIF(Devices!B:EH,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Devices!B:EH,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Devices!B:EH,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Devices!B:EH,"*"&amp;CHAR(39)&amp;"*")</f>
+        <f>COUNTIF(Devices!B:EI,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Devices!B:EI,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Devices!B:EI,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Devices!B:EI,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
       <c r="I20" s="28" t="s">
@@ -8415,26 +8413,26 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
-        <f>COUNTIF(Devices!P:P,"Server")+COUNTIF(Devices!P:P,"VM")+COUNTIF(Devices!P:P,"Blade")+COUNTIF(Devices!P:P,"Appliance")</f>
+        <f>COUNTIF(Devices!Q:Q,"Server")+COUNTIF(Devices!Q:Q,"VM")+COUNTIF(Devices!Q:Q,"Blade")+COUNTIF(Devices!Q:Q,"Appliance")</f>
         <v>0</v>
       </c>
       <c r="B21" t="s">
         <v>95</v>
       </c>
       <c r="D21" s="21">
-        <f>COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!P:P,"Server")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!P:P,"Blade")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!P:P,"VM")++COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!P:P,"Appliance")</f>
+        <f>COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!Q:Q,"Server")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!Q:Q,"Blade")+COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!Q:Q,"VM")++COUNTIFS(Devices!A:A,"&lt;&gt;''",Devices!Q:Q,"Appliance")</f>
         <v>0</v>
       </c>
       <c r="E21" s="21">
-        <f>COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!P:P,"Server")+COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!P:P,"Blade")+COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!P:P,"VM")++COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!P:P,"Appliance")</f>
+        <f>COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!Q:Q,"Server")+COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!Q:Q,"Blade")+COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!Q:Q,"VM")++COUNTIFS(Devices!A:A,"",Devices!B:B,"&lt;&gt;''",Devices!Q:Q,"Appliance")</f>
         <v>0</v>
       </c>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
     </row>
-    <row r="22" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17">
         <f>COUNTA(Databases!B:B)-1</f>
         <v>0</v>
@@ -8451,15 +8449,15 @@
         <v>0</v>
       </c>
       <c r="F22" s="20">
-        <f>COUNTIF(Databases!B:EJ,REPT("?",254)&amp;"*")</f>
+        <f>COUNTIF(Databases!B:EK,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
       <c r="G22" s="20">
-        <f>COUNTIF(Databases!B:EK,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Databases!B:EK,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Databases!B:EK,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Databases!B:EK,"*"&amp;CHAR(39)&amp;"*")</f>
+        <f>COUNTIF(Databases!B:EL,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Databases!B:EL,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Databases!B:EL,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Databases!B:EL,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17">
         <f>COUNTA(Storage!B:B)-1</f>
         <v>0</v>
@@ -8476,15 +8474,15 @@
         <v>0</v>
       </c>
       <c r="F23" s="20">
-        <f>COUNTIF(Storage!B:EI,REPT("?",254)&amp;"*")</f>
+        <f>COUNTIF(Storage!B:EJ,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
       <c r="G23" s="20">
-        <f>COUNTIF(Storage!B:EJ,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Storage!B:EJ,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Storage!B:EJ,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Storage!B:EJ,"*"&amp;CHAR(39)&amp;"*")</f>
+        <f>COUNTIF(Storage!B:EK,"*"&amp;CHAR(12)&amp;"*")+COUNTIF(Storage!B:EK,"*"&amp;CHAR(13)&amp;"*")+COUNTIF(Storage!B:EK,"*"&amp;CHAR(34)&amp;"*")+COUNTIF(Storage!B:EK,"*"&amp;CHAR(39)&amp;"*")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17">
         <f>COUNTA(Dependencies!D:D)-1</f>
         <v>0</v>
@@ -8501,7 +8499,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="20">
-        <f>COUNTIF(Storage!B:EI,REPT("?",254)&amp;"*")</f>
+        <f>COUNTIF(Storage!B:EJ,REPT("?",254)&amp;"*")</f>
         <v>0</v>
       </c>
       <c r="G24" s="23">
@@ -8509,7 +8507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <f>COUNTIF(Dependencies!H:H,"Master")</f>
         <v>0</v>
@@ -8522,7 +8520,7 @@
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Application")-A25</f>
         <v>0</v>
@@ -8535,7 +8533,7 @@
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
     </row>
-    <row r="27" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!H:H,"Runs On")</f>
         <v>0</v>
@@ -8548,7 +8546,7 @@
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
     </row>
-    <row r="28" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <f>COUNTIFS(Dependencies!D:D,"Application",Dependencies!G:G,"Database")</f>
         <v>0</v>
@@ -8561,7 +8559,7 @@
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
     </row>
-    <row r="29" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <f>COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Server")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"Blade")+COUNTIFS(Dependencies!D:D,"Database",Dependencies!G:G,"VM")</f>
         <v>0</v>
@@ -8574,7 +8572,7 @@
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
     </row>
-    <row r="30" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <f>COUNTIF(Dependencies!H:H,"Storage")</f>
         <v>0</v>
@@ -8587,7 +8585,7 @@
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
     </row>
-    <row r="31" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17">
         <f>COUNTA(Room!B:B)-1</f>
         <v>0</v>
@@ -8600,7 +8598,7 @@
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
     </row>
-    <row r="32" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17">
         <f>COUNTA(Rack!B:B)-1</f>
         <v>0</v>
@@ -8613,7 +8611,7 @@
       <c r="F32" s="24"/>
       <c r="G32" s="24"/>
     </row>
-    <row r="33" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17">
         <f>COUNTA(Cabling!B:B)-2</f>
         <v>0</v>
@@ -8626,7 +8624,7 @@
       <c r="F33" s="24"/>
       <c r="G33" s="24"/>
     </row>
-    <row r="34" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
         <f>COUNTA(Comments!B:B)-1</f>
         <v>0</v>
@@ -8639,21 +8637,21 @@
       <c r="F34" s="24"/>
       <c r="G34" s="24"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="46" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="47" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="48" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="45" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataConsolidate/>
@@ -8698,18 +8696,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" style="9" customWidth="1"/>
     <col min="2" max="2" width="16" style="7" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="20.125" style="10" customWidth="1"/>
     <col min="4" max="4" width="17.5" style="8" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="10" customWidth="1"/>
-    <col min="6" max="6" width="51.83203125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="51.875" style="10" customWidth="1"/>
     <col min="7" max="16384" width="9.5" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="76" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="73" t="s">
         <v>81</v>
       </c>
@@ -8749,13 +8747,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="5" width="19.5" style="33" customWidth="1"/>
     <col min="6" max="16384" width="11.5" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="78" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="77" t="s">
         <v>126</v>
       </c>
@@ -8785,7 +8783,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EH1"/>
+  <dimension ref="A1:EI1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -8794,39 +8792,39 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="6.625" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="35" customWidth="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="34" customWidth="1"/>
-    <col min="12" max="12" width="9.5" style="2"/>
-    <col min="17" max="17" width="13.5" customWidth="1"/>
-    <col min="18" max="20" width="12.83203125" customWidth="1"/>
-    <col min="21" max="21" width="9.5" style="8"/>
-    <col min="22" max="22" width="11.83203125" style="8" customWidth="1"/>
-    <col min="25" max="25" width="9.5" style="2"/>
-    <col min="34" max="34" width="11.5" customWidth="1"/>
-    <col min="35" max="35" width="13.5" customWidth="1"/>
-    <col min="36" max="36" width="16.1640625" style="7" customWidth="1"/>
-    <col min="37" max="37" width="10.5" customWidth="1"/>
-    <col min="38" max="38" width="12.83203125" customWidth="1"/>
-    <col min="39" max="39" width="14.5" style="7" customWidth="1"/>
-    <col min="40" max="40" width="10.83203125" customWidth="1"/>
-    <col min="41" max="41" width="11.83203125" customWidth="1"/>
-    <col min="42" max="42" width="13.5" style="26" customWidth="1"/>
-    <col min="43" max="70" width="9.5" customWidth="1"/>
-    <col min="71" max="71" width="9.5" style="9" customWidth="1"/>
-    <col min="72" max="106" width="9.5" customWidth="1"/>
-    <col min="107" max="107" width="9.5" style="9" customWidth="1"/>
-    <col min="108" max="138" width="9.5" customWidth="1"/>
+    <col min="4" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="9.375" style="35" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="9" width="10.375" customWidth="1"/>
+    <col min="10" max="10" width="12.875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17.5" style="34" customWidth="1"/>
+    <col min="13" max="13" width="9.5" style="2"/>
+    <col min="18" max="18" width="13.5" customWidth="1"/>
+    <col min="19" max="21" width="12.875" customWidth="1"/>
+    <col min="22" max="22" width="21.125" style="8" customWidth="1"/>
+    <col min="23" max="23" width="11.875" style="8" customWidth="1"/>
+    <col min="26" max="26" width="9.5" style="2"/>
+    <col min="35" max="35" width="11.5" customWidth="1"/>
+    <col min="36" max="36" width="13.5" customWidth="1"/>
+    <col min="37" max="37" width="16.125" style="7" customWidth="1"/>
+    <col min="38" max="38" width="10.5" customWidth="1"/>
+    <col min="39" max="39" width="12.875" customWidth="1"/>
+    <col min="40" max="40" width="14.5" style="7" customWidth="1"/>
+    <col min="41" max="41" width="10.875" customWidth="1"/>
+    <col min="42" max="42" width="11.875" customWidth="1"/>
+    <col min="43" max="43" width="13.5" style="26" customWidth="1"/>
+    <col min="44" max="71" width="9.5" customWidth="1"/>
+    <col min="72" max="72" width="9.5" style="9" customWidth="1"/>
+    <col min="73" max="107" width="9.5" customWidth="1"/>
+    <col min="108" max="108" width="9.5" style="9" customWidth="1"/>
+    <col min="109" max="139" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:138" s="46" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:139" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
         <v>173</v>
       </c>
@@ -8842,118 +8840,120 @@
       <c r="E1" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="53" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="H1" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="I1" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="79" t="s">
+      <c r="J1" s="79" t="s">
         <v>156</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="K1" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="L1" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="54" t="s">
+      <c r="M1" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="N1" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="53" t="s">
+      <c r="O1" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="53" t="s">
+      <c r="P1" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="53" t="s">
+      <c r="Q1" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="Q1" s="55" t="s">
+      <c r="R1" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="R1" s="55" t="s">
+      <c r="S1" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="S1" s="55" t="s">
+      <c r="T1" s="55" t="s">
         <v>133</v>
       </c>
-      <c r="T1" s="55" t="s">
+      <c r="U1" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="U1" s="56" t="s">
+      <c r="V1" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="V1" s="56" t="s">
+      <c r="W1" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="W1" s="53" t="s">
+      <c r="X1" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="53" t="s">
+      <c r="Y1" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" s="54" t="s">
+      <c r="Z1" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="Z1" s="53" t="s">
+      <c r="AA1" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="AA1" s="53" t="s">
+      <c r="AB1" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="AB1" s="53" t="s">
+      <c r="AC1" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="AC1" s="53" t="s">
+      <c r="AD1" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="AD1" s="46" t="s">
+      <c r="AE1" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="AE1" s="46" t="s">
+      <c r="AF1" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="AF1" s="46" t="s">
+      <c r="AG1" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="AG1" s="46" t="s">
+      <c r="AH1" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="AH1" s="45" t="s">
+      <c r="AI1" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="AI1" s="45" t="s">
+      <c r="AJ1" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="AJ1" s="57" t="s">
+      <c r="AK1" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="AK1" s="58" t="s">
+      <c r="AL1" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="AL1" s="58" t="s">
+      <c r="AM1" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="AM1" s="57" t="s">
+      <c r="AN1" s="57" t="s">
         <v>152</v>
       </c>
-      <c r="AN1" s="58" t="s">
+      <c r="AO1" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="AO1" s="58" t="s">
+      <c r="AP1" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="AP1" s="57" t="s">
+      <c r="AQ1" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="BO1" s="45"/>
       <c r="BP1" s="45"/>
       <c r="BQ1" s="45"/>
       <c r="BR1" s="45"/>
@@ -9025,10 +9025,11 @@
       <c r="EF1" s="45"/>
       <c r="EG1" s="45"/>
       <c r="EH1" s="45"/>
+      <c r="EI1" s="45"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <autoFilter ref="A1:EH1"/>
+  <autoFilter ref="A1:EI1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -9043,7 +9044,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AO1"/>
+  <dimension ref="A1:AP1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -9052,51 +9053,51 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="6.625" style="4" customWidth="1"/>
     <col min="2" max="3" width="20.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="6" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="36" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="5" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="81" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="4" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="13" style="5" customWidth="1"/>
-    <col min="13" max="13" width="11.5" style="5" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="15.1640625" style="5" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="9.5" style="5" customWidth="1"/>
-    <col min="18" max="18" width="8.83203125" style="5" customWidth="1"/>
-    <col min="19" max="20" width="10.5" style="5" customWidth="1"/>
-    <col min="21" max="21" width="9.83203125" style="5" customWidth="1"/>
-    <col min="22" max="22" width="10.5" style="4" customWidth="1"/>
-    <col min="23" max="23" width="11.5" style="5" customWidth="1"/>
-    <col min="24" max="24" width="18.83203125" style="4" customWidth="1"/>
-    <col min="25" max="25" width="13.5" style="5" customWidth="1"/>
-    <col min="26" max="26" width="8.5" style="5" customWidth="1"/>
-    <col min="27" max="27" width="11.5" style="5" customWidth="1"/>
-    <col min="28" max="28" width="11" style="4"/>
-    <col min="29" max="29" width="10" style="4" customWidth="1"/>
-    <col min="30" max="30" width="11" style="4"/>
-    <col min="31" max="31" width="15.5" style="4" customWidth="1"/>
-    <col min="32" max="32" width="12.1640625" style="5" customWidth="1"/>
-    <col min="33" max="33" width="12" style="6" customWidth="1"/>
-    <col min="34" max="34" width="9.33203125" style="4" customWidth="1"/>
-    <col min="35" max="35" width="11" style="5"/>
-    <col min="36" max="36" width="8.83203125" style="5" customWidth="1"/>
-    <col min="37" max="38" width="11" style="5"/>
-    <col min="39" max="39" width="12.83203125" style="4" customWidth="1"/>
-    <col min="40" max="40" width="8.5" style="4" customWidth="1"/>
-    <col min="41" max="41" width="10.1640625" style="4" customWidth="1"/>
-    <col min="42" max="137" width="9.5" style="5" customWidth="1"/>
-    <col min="138" max="16384" width="11" style="5"/>
+    <col min="5" max="6" width="15.5" style="5" customWidth="1"/>
+    <col min="7" max="7" width="9.375" style="36" customWidth="1"/>
+    <col min="8" max="8" width="15.5" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="12.875" style="81" customWidth="1"/>
+    <col min="11" max="11" width="17.5" style="4" customWidth="1"/>
+    <col min="12" max="12" width="15.875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="13" style="5" customWidth="1"/>
+    <col min="14" max="14" width="11.5" style="5" customWidth="1"/>
+    <col min="15" max="15" width="11.125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="15.125" style="5" customWidth="1"/>
+    <col min="17" max="17" width="12.125" style="5" customWidth="1"/>
+    <col min="18" max="18" width="9.5" style="5" customWidth="1"/>
+    <col min="19" max="19" width="8.875" style="5" customWidth="1"/>
+    <col min="20" max="21" width="10.5" style="5" customWidth="1"/>
+    <col min="22" max="22" width="9.875" style="5" customWidth="1"/>
+    <col min="23" max="23" width="10.5" style="4" customWidth="1"/>
+    <col min="24" max="24" width="11.5" style="5" customWidth="1"/>
+    <col min="25" max="25" width="18.875" style="4" customWidth="1"/>
+    <col min="26" max="26" width="13.5" style="5" customWidth="1"/>
+    <col min="27" max="27" width="8.5" style="5" customWidth="1"/>
+    <col min="28" max="28" width="11.5" style="5" customWidth="1"/>
+    <col min="29" max="29" width="11" style="4"/>
+    <col min="30" max="30" width="10" style="4" customWidth="1"/>
+    <col min="31" max="31" width="11" style="4"/>
+    <col min="32" max="32" width="15.5" style="4" customWidth="1"/>
+    <col min="33" max="33" width="12.125" style="5" customWidth="1"/>
+    <col min="34" max="34" width="12" style="6" customWidth="1"/>
+    <col min="35" max="35" width="9.375" style="4" customWidth="1"/>
+    <col min="36" max="36" width="11" style="5"/>
+    <col min="37" max="37" width="8.875" style="5" customWidth="1"/>
+    <col min="38" max="39" width="11" style="5"/>
+    <col min="40" max="40" width="12.875" style="4" customWidth="1"/>
+    <col min="41" max="41" width="8.5" style="4" customWidth="1"/>
+    <col min="42" max="42" width="15.75" style="4" customWidth="1"/>
+    <col min="43" max="138" width="9.5" style="5" customWidth="1"/>
+    <col min="139" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="45" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:42" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
         <v>173</v>
       </c>
@@ -9112,118 +9113,121 @@
       <c r="E1" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="H1" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="I1" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="80" t="s">
+      <c r="J1" s="80" t="s">
         <v>156</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="K1" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="L1" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="M1" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="N1" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="O1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="45" t="s">
+      <c r="P1" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="45" t="s">
+      <c r="Q1" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="Q1" s="45" t="s">
+      <c r="R1" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="R1" s="45" t="s">
+      <c r="S1" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="45" t="s">
+      <c r="T1" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="T1" s="45" t="s">
+      <c r="U1" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="U1" s="45" t="s">
+      <c r="V1" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="V1" s="50" t="s">
+      <c r="W1" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="W1" s="45" t="s">
+      <c r="X1" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="X1" s="50" t="s">
+      <c r="Y1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="45" t="s">
+      <c r="Z1" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="Z1" s="45" t="s">
+      <c r="AA1" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="AA1" s="45" t="s">
+      <c r="AB1" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="AB1" s="50" t="s">
+      <c r="AC1" s="50" t="s">
         <v>170</v>
       </c>
-      <c r="AC1" s="50" t="s">
+      <c r="AD1" s="50" t="s">
         <v>171</v>
       </c>
-      <c r="AD1" s="50" t="s">
+      <c r="AE1" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="AE1" s="50" t="s">
+      <c r="AF1" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="AF1" s="45" t="s">
+      <c r="AG1" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="AG1" s="49" t="s">
+      <c r="AH1" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="AH1" s="50" t="s">
+      <c r="AI1" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="AI1" s="45" t="s">
+      <c r="AJ1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="AJ1" s="45" t="s">
+      <c r="AK1" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="AK1" s="45" t="s">
+      <c r="AL1" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="AL1" s="45" t="s">
+      <c r="AM1" s="45" t="s">
         <v>172</v>
       </c>
-      <c r="AM1" s="50" t="s">
+      <c r="AN1" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="AN1" s="51" t="s">
+      <c r="AO1" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="AO1" s="50" t="s">
+      <c r="AP1" s="50" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <autoFilter ref="A1:EG1"/>
+  <autoFilter ref="A1:EH1"/>
   <pageMargins left="0.25" right="0.25" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>
@@ -9231,6 +9235,178 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:DJ1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.625" style="7" customWidth="1"/>
+    <col min="2" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="9.375" style="35" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="9" width="10.375" customWidth="1"/>
+    <col min="10" max="10" width="12.875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17.5" style="11" customWidth="1"/>
+    <col min="13" max="13" width="9.5" style="7"/>
+    <col min="14" max="14" width="7.125" customWidth="1"/>
+    <col min="15" max="15" width="12.875" style="7" customWidth="1"/>
+    <col min="17" max="18" width="12.875" style="8" customWidth="1"/>
+    <col min="19" max="42" width="9.5" customWidth="1"/>
+    <col min="43" max="43" width="9.5" style="9" customWidth="1"/>
+    <col min="44" max="82" width="9.5" customWidth="1"/>
+    <col min="83" max="83" width="9.5" style="9"/>
+    <col min="85" max="86" width="9.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:114" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" s="79" t="s">
+        <v>156</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q1" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="R1" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="AQ1" s="45"/>
+      <c r="AR1" s="45"/>
+      <c r="AS1" s="45"/>
+      <c r="AT1" s="45"/>
+      <c r="AU1" s="45"/>
+      <c r="AV1" s="45"/>
+      <c r="AW1" s="45"/>
+      <c r="AX1" s="45"/>
+      <c r="AY1" s="45"/>
+      <c r="AZ1" s="45"/>
+      <c r="BA1" s="45"/>
+      <c r="BB1" s="45"/>
+      <c r="BC1" s="45"/>
+      <c r="BD1" s="45"/>
+      <c r="BE1" s="45"/>
+      <c r="BF1" s="45"/>
+      <c r="BG1" s="45"/>
+      <c r="BH1" s="45"/>
+      <c r="BI1" s="45"/>
+      <c r="BJ1" s="45"/>
+      <c r="BK1" s="45"/>
+      <c r="BL1" s="45"/>
+      <c r="BM1" s="45"/>
+      <c r="BN1" s="45"/>
+      <c r="BO1" s="45"/>
+      <c r="BP1" s="45"/>
+      <c r="BQ1" s="45"/>
+      <c r="BR1" s="45"/>
+      <c r="BS1" s="45"/>
+      <c r="BT1" s="45"/>
+      <c r="BU1" s="45"/>
+      <c r="BV1" s="45"/>
+      <c r="BW1" s="45"/>
+      <c r="BX1" s="45"/>
+      <c r="BY1" s="45"/>
+      <c r="BZ1" s="45"/>
+      <c r="CA1" s="45"/>
+      <c r="CB1" s="45"/>
+      <c r="CC1" s="45"/>
+      <c r="CD1" s="45"/>
+      <c r="CE1" s="45"/>
+      <c r="CF1" s="45"/>
+      <c r="CG1" s="45"/>
+      <c r="CH1" s="45"/>
+      <c r="CI1" s="45"/>
+      <c r="CJ1" s="45"/>
+      <c r="CK1" s="45"/>
+      <c r="CL1" s="45"/>
+      <c r="CM1" s="45"/>
+      <c r="CN1" s="45"/>
+      <c r="CO1" s="45"/>
+      <c r="CP1" s="45"/>
+      <c r="CQ1" s="45"/>
+      <c r="CR1" s="45"/>
+      <c r="CS1" s="45"/>
+      <c r="CT1" s="45"/>
+      <c r="CU1" s="45"/>
+      <c r="CV1" s="45"/>
+      <c r="CW1" s="45"/>
+      <c r="CX1" s="45"/>
+      <c r="CY1" s="45"/>
+      <c r="CZ1" s="45"/>
+      <c r="DA1" s="45"/>
+      <c r="DB1" s="45"/>
+      <c r="DC1" s="45"/>
+      <c r="DD1" s="45"/>
+      <c r="DE1" s="45"/>
+      <c r="DF1" s="45"/>
+      <c r="DG1" s="45"/>
+      <c r="DH1" s="45"/>
+      <c r="DI1" s="45"/>
+      <c r="DJ1" s="45"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <autoFilter ref="A1:DJ1"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DI1"/>
   <sheetViews>
@@ -9241,28 +9417,29 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="6.625" style="7" customWidth="1"/>
     <col min="2" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="35" customWidth="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="11" customWidth="1"/>
-    <col min="12" max="12" width="9.5" style="7"/>
-    <col min="13" max="13" width="7.1640625" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" style="7" customWidth="1"/>
-    <col min="16" max="17" width="12.83203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="8" customWidth="1"/>
+    <col min="5" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="9.375" style="35" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="9" width="10.375" customWidth="1"/>
+    <col min="10" max="10" width="12.875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17.5" style="11" customWidth="1"/>
+    <col min="12" max="12" width="8.5" style="10"/>
+    <col min="14" max="14" width="8.5" style="7"/>
+    <col min="15" max="15" width="7.125" customWidth="1"/>
+    <col min="16" max="16" width="14.5" style="7" customWidth="1"/>
     <col min="18" max="41" width="9.5" customWidth="1"/>
     <col min="42" max="42" width="9.5" style="9" customWidth="1"/>
     <col min="43" max="81" width="9.5" customWidth="1"/>
-    <col min="82" max="82" width="9.5" style="9"/>
-    <col min="84" max="85" width="9.5" customWidth="1"/>
+    <col min="82" max="82" width="9.5" style="9" customWidth="1"/>
+    <col min="83" max="113" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" s="46" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:113" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
         <v>173</v>
       </c>
@@ -9272,48 +9449,72 @@
       <c r="C1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="40" t="s">
         <v>15</v>
       </c>
       <c r="E1" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="H1" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="I1" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="79" t="s">
+      <c r="J1" s="79" t="s">
         <v>156</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="K1" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="L1" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="N1" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="O1" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="44" t="s">
+      <c r="P1" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="Q1" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="P1" s="40" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q1" s="40" t="s">
-        <v>137</v>
-      </c>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="39"/>
+      <c r="AD1" s="39"/>
+      <c r="AE1" s="39"/>
+      <c r="AF1" s="39"/>
+      <c r="AG1" s="39"/>
+      <c r="AH1" s="39"/>
+      <c r="AI1" s="39"/>
+      <c r="AJ1" s="39"/>
+      <c r="AK1" s="39"/>
+      <c r="AL1" s="39"/>
+      <c r="AM1" s="39"/>
+      <c r="AN1" s="39"/>
+      <c r="AO1" s="39"/>
       <c r="AP1" s="45"/>
       <c r="AQ1" s="45"/>
       <c r="AR1" s="45"/>
@@ -9390,197 +9591,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <autoFilter ref="A1:DI1"/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DH1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="6.6640625" style="7" customWidth="1"/>
-    <col min="2" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="8" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="35" customWidth="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="11" customWidth="1"/>
-    <col min="11" max="11" width="8.5" style="10"/>
-    <col min="13" max="13" width="8.5" style="7"/>
-    <col min="14" max="14" width="7.1640625" customWidth="1"/>
-    <col min="15" max="15" width="14.5" style="7" customWidth="1"/>
-    <col min="17" max="40" width="9.5" customWidth="1"/>
-    <col min="41" max="41" width="9.5" style="9" customWidth="1"/>
-    <col min="42" max="80" width="9.5" customWidth="1"/>
-    <col min="81" max="81" width="9.5" style="9" customWidth="1"/>
-    <col min="82" max="112" width="9.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:112" s="46" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="37" t="s">
-        <v>173</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="I1" s="79" t="s">
-        <v>156</v>
-      </c>
-      <c r="J1" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>114</v>
-      </c>
-      <c r="L1" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="39"/>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="39"/>
-      <c r="AC1" s="39"/>
-      <c r="AD1" s="39"/>
-      <c r="AE1" s="39"/>
-      <c r="AF1" s="39"/>
-      <c r="AG1" s="39"/>
-      <c r="AH1" s="39"/>
-      <c r="AI1" s="39"/>
-      <c r="AJ1" s="39"/>
-      <c r="AK1" s="39"/>
-      <c r="AL1" s="39"/>
-      <c r="AM1" s="39"/>
-      <c r="AN1" s="39"/>
-      <c r="AO1" s="45"/>
-      <c r="AP1" s="45"/>
-      <c r="AQ1" s="45"/>
-      <c r="AR1" s="45"/>
-      <c r="AS1" s="45"/>
-      <c r="AT1" s="45"/>
-      <c r="AU1" s="45"/>
-      <c r="AV1" s="45"/>
-      <c r="AW1" s="45"/>
-      <c r="AX1" s="45"/>
-      <c r="AY1" s="45"/>
-      <c r="AZ1" s="45"/>
-      <c r="BA1" s="45"/>
-      <c r="BB1" s="45"/>
-      <c r="BC1" s="45"/>
-      <c r="BD1" s="45"/>
-      <c r="BE1" s="45"/>
-      <c r="BF1" s="45"/>
-      <c r="BG1" s="45"/>
-      <c r="BH1" s="45"/>
-      <c r="BI1" s="45"/>
-      <c r="BJ1" s="45"/>
-      <c r="BK1" s="45"/>
-      <c r="BL1" s="45"/>
-      <c r="BM1" s="45"/>
-      <c r="BN1" s="45"/>
-      <c r="BO1" s="45"/>
-      <c r="BP1" s="45"/>
-      <c r="BQ1" s="45"/>
-      <c r="BR1" s="45"/>
-      <c r="BS1" s="45"/>
-      <c r="BT1" s="45"/>
-      <c r="BU1" s="45"/>
-      <c r="BV1" s="45"/>
-      <c r="BW1" s="45"/>
-      <c r="BX1" s="45"/>
-      <c r="BY1" s="45"/>
-      <c r="BZ1" s="45"/>
-      <c r="CA1" s="45"/>
-      <c r="CB1" s="45"/>
-      <c r="CC1" s="45"/>
-      <c r="CD1" s="45"/>
-      <c r="CE1" s="45"/>
-      <c r="CF1" s="45"/>
-      <c r="CG1" s="45"/>
-      <c r="CH1" s="45"/>
-      <c r="CI1" s="45"/>
-      <c r="CJ1" s="45"/>
-      <c r="CK1" s="45"/>
-      <c r="CL1" s="45"/>
-      <c r="CM1" s="45"/>
-      <c r="CN1" s="45"/>
-      <c r="CO1" s="45"/>
-      <c r="CP1" s="45"/>
-      <c r="CQ1" s="45"/>
-      <c r="CR1" s="45"/>
-      <c r="CS1" s="45"/>
-      <c r="CT1" s="45"/>
-      <c r="CU1" s="45"/>
-      <c r="CV1" s="45"/>
-      <c r="CW1" s="45"/>
-      <c r="CX1" s="45"/>
-      <c r="CY1" s="45"/>
-      <c r="CZ1" s="45"/>
-      <c r="DA1" s="45"/>
-      <c r="DB1" s="45"/>
-      <c r="DC1" s="45"/>
-      <c r="DD1" s="45"/>
-      <c r="DE1" s="45"/>
-      <c r="DF1" s="45"/>
-      <c r="DG1" s="45"/>
-      <c r="DH1" s="45"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <autoFilter ref="A1:DH1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -9595,22 +9605,22 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="8.5" style="7"/>
     <col min="3" max="3" width="13.5" style="7" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="10" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="7" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="16.125" style="10" customWidth="1"/>
     <col min="7" max="7" width="14.5" style="10" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" customWidth="1"/>
-    <col min="11" max="11" width="8.1640625" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="14.125" customWidth="1"/>
+    <col min="10" max="10" width="17.875" customWidth="1"/>
+    <col min="11" max="11" width="8.125" customWidth="1"/>
+    <col min="12" max="12" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
         <v>35</v>
       </c>
@@ -9679,23 +9689,23 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" style="7"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.125" customWidth="1"/>
     <col min="4" max="5" width="14.5" style="9" customWidth="1"/>
     <col min="6" max="6" width="10.5" customWidth="1"/>
     <col min="7" max="7" width="26.5" customWidth="1"/>
     <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="13.125" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="19.5" style="2" customWidth="1"/>
     <col min="12" max="12" width="25.5" style="25" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" style="25" customWidth="1"/>
+    <col min="13" max="13" width="16.875" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="65" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
         <v>50</v>
       </c>
@@ -9759,20 +9769,20 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" style="7" customWidth="1"/>
     <col min="2" max="2" width="19.5" customWidth="1"/>
     <col min="3" max="5" width="16.5" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="12.5" style="9" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="12.875" style="9" customWidth="1"/>
     <col min="9" max="10" width="13.5" style="9" customWidth="1"/>
     <col min="11" max="11" width="12" style="9" customWidth="1"/>
     <col min="12" max="12" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="62" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="51" t="s">
         <v>61</v>
       </c>
@@ -9833,24 +9843,24 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" style="5"/>
-    <col min="2" max="2" width="7.83203125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="7.875" style="30" customWidth="1"/>
     <col min="3" max="3" width="22.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="5"/>
     <col min="5" max="5" width="8.5" style="30" customWidth="1"/>
     <col min="6" max="6" width="24.5" style="5" customWidth="1"/>
     <col min="7" max="7" width="9.5" style="5"/>
-    <col min="8" max="8" width="24.1640625" style="31" customWidth="1"/>
+    <col min="8" max="8" width="24.125" style="31" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="5"/>
     <col min="10" max="10" width="14.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="11.875" style="5" customWidth="1"/>
     <col min="12" max="12" width="15.5" style="5" customWidth="1"/>
     <col min="13" max="16384" width="9.5" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="84" t="s">
         <v>70</v>
       </c>
@@ -9866,7 +9876,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="72" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" s="72" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="68" t="s">
         <v>72</v>
       </c>

</xml_diff>